<commit_message>
Update portfolios at 2024-09-15 12:19:20
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +481,34 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Portfolio_2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2024-09-15</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[{'id': 32981, 'symbol': 'CATE', 'name': 'Cate', 'price': 0.04622151630505624, 'change_24h': 15.65927489, 'change_7d': 525.26505339, 'market_cap': 46221516.305056244}, {'id': 32902, 'symbol': 'BRUH', 'name': 'Bruh', 'price': 0.00031770425887260134, 'change_24h': -11.81050116, 'change_7d': -54.21449484, 'market_cap': 317704.2588726013}, {'id': 32862, 'symbol': 'MUNCAT', 'name': 'MUNCAT', 'price': 0.020332950047081428, 'change_24h': 0.04479229, 'change_7d': 24.47954696, 'market_cap': 20332950.04708143}, {'id': 32844, 'symbol': 'WIWI', 'name': 'Wiggly Willy', 'price': 1.2794438148911169e-06, 'change_24h': 0.36519617, 'change_7d': -25.90473384, 'market_cap': 832663.1003376707}, {'id': 32698, 'symbol': 'DOGS', 'name': 'DOGS', 'price': 0.001070001016141869, 'change_24h': -2.1870609, 'change_7d': 5.78861839, 'market_cap': 552923025.0913107}, {'id': 32821, 'symbol': 'BULLS', 'name': 'BULLS', 'price': 0.0003010673566050869, 'change_24h': -0.31866993, 'change_7d': -72.53269195, 'market_cap': 301067.3566050869}, {'id': 32797, 'symbol': 'IVfun', 'name': 'Invest Zone', 'price': 0.018351533177714856, 'change_24h': -5.90489481, 'change_7d': -33.83488965, 'market_cap': 17254458.447773766}, {'id': 32790, 'symbol': 'EBULL', 'name': 'ETHEREUM IS GOOD', 'price': 0.0002474804052799423, 'change_24h': 0.9636044, 'change_7d': -45.5373862, 'market_cap': 2474804.052799423}, {'id': 32732, 'symbol': 'SUNPEPE', 'name': 'sunpepe', 'price': 0.000897168648582681, 'change_24h': 1.58911547, 'change_7d': -23.06688199, 'market_cap': 897168.648582681}, {'id': 32727, 'symbol': 'FOFAR', 'name': 'Fofar (fofar.meme)', 'price': 0.005994983027720214, 'change_24h': 0.5843079, 'change_7d': 2.52146706, 'market_cap': 5695188.11063377}, {'id': 32724, 'symbol': 'CAT', 'name': "Simon's Cat", 'price': 3.500854798810511e-05, 'change_24h': 5.00455684, 'change_7d': 21.68004737, 'market_cap': 236306135.10035145}, {'id': 32717, 'symbol': 'SUNDOG', 'name': 'SUNDOG', 'price': 0.34380402988132813, 'change_24h': 0.42014554, 'change_7d': 41.40471499, 'market_cap': 342943334.3703298}, {'id': 32638, 'symbol': 'CATDOG', 'name': 'CatDog', 'price': 7.402990858692653e-05, 'change_24h': -10.65482375, 'change_7d': 3.12557669, 'market_cap': 7402990.858692653}, {'id': 32625, 'symbol': 'FUKU', 'name': 'Fuku-Kun', 'price': 1.5877577345751996e-06, 'change_24h': -9.703381, 'change_7d': -47.90988549, 'market_cap': 510971.83034441207}, {'id': 32618, 'symbol': 'WDOG', 'name': 'Wrapped Dog', 'price': 0.013227097510162796, 'change_24h': -10.1036857, 'change_7d': -24.8197901, 'market_cap': 13227076.862663582}, {'id': 32598, 'symbol': 'GODCAT', 'name': 'Godcat Exploding Kittens', 'price': 0.0001428806379538942, 'change_24h': -19.76930028, 'change_7d': 76.51318518, 'market_cap': 113865.6434821598}, {'id': 32590, 'symbol': 'DOGY', 'name': 'Dogy', 'price': 1.1893418755613293e-07, 'change_24h': -0.5283509, 'change_7d': -29.43293235, 'market_cap': 103457.79178549594}, {'id': 32524, 'symbol': 'GINNAN', 'name': 'Ginnan The Cat', 'price': 2.9331244838977883e-06, 'change_24h': -10.2501768, 'change_7d': -15.88496351, 'market_cap': 20238554.134991195}, {'id': 32521, 'symbol': 'NEIRO', 'name': 'First Neiro On Ethereum', 'price': 4.208864094761428e-05, 'change_24h': 0.02630109, 'change_7d': -25.71518583, 'market_cap': 17411948.878136143}, {'id': 32495, 'symbol': '$YAWN', 'name': 'YAWN', 'price': 3.691291491467053e-05, 'change_24h': -1.13594427, 'change_7d': -8.88183076, 'market_cap': 236816.17226191767}, {'id': 32464, 'symbol': 'NEIRO', 'name': 'Neiro (neiro.lol)', 'price': 0.003357283483090154, 'change_24h': -9.83454865, 'change_7d': -24.45073389, 'market_cap': 3357283.379014366}, {'id': 32462, 'symbol': 'YOUNES', 'name': 'YOUNES', 'price': 0.0019201691760439004, 'change_24h': 0.04371067, 'change_7d': 4.47551325, 'market_cap': 1920165.7216595528}, {'id': 32461, 'symbol': 'NEIRO', 'name': 'Neiro Ethereum', 'price': 0.13394809708361538, 'change_24h': -19.45958405, 'change_7d': -8.80093972, 'market_cap': 133948097.08361538}, {'id': 32448, 'symbol': 'BRAINLET', 'name': 'Brainlet', 'price': 0.015264458273555239, 'change_24h': -11.10895338, 'change_7d': -22.56562209, 'market_cap': 14545586.869234081}, {'id': 32415, 'symbol': 'SKBDI', 'name': 'Skibidi Toilet', 'price': 0.05019684172868577, 'change_24h': -3.35381365, 'change_7d': -18.52161743, 'market_cap': 3515720.1332713356}, {'id': 32350, 'symbol': 'SOY', 'name': 'Soyjak', 'price': 0.0006979898173231251, 'change_24h': -12.64424242, 'change_7d': -39.59443819, 'market_cap': 646728.0414813921}, {'id': 32310, 'symbol': 'SAITAMA', 'name': 'SAITAMA INU', 'price': 0.00033670238715070605, 'change_24h': -4.92073736, 'change_7d': 51.23960976, 'market_cap': 224403.18071201874}, {'id': 32297, 'symbol': 'BILL', 'name': 'BILL THE BEAR', 'price': 2.105708232664283e-06, 'change_24h': -10.0729372, 'change_7d': 2.45341264, 'market_cap': 1871734.1356051096}, {'id': 32288, 'symbol': 'torsy', 'name': 'TORSY', 'price': 0.003067949816923183, 'change_24h': -1.07737468, 'change_7d': 9.19390548, 'market_cap': 2147563.868626638}, {'id': 32259, 'symbol': 'MOBY', 'name': 'Moby', 'price': 0.00014163620888763475, 'change_24h': -6.02447285, 'change_7d': 20.19311015, 'market_cap': 1416362.0888763475}, {'id': 32128, 'symbol': 'MSI', 'name': 'monkey shit inu', 'price': 1.6455146724593568e-06, 'change_24h': 17.82578479, 'change_7d': 30.23824405, 'market_cap': 4844839.220083151}, {'id': 32125, 'symbol': 'COIN', 'name': '8-Bit Coin', 'price': 0.0006392985397571367, 'change_24h': -3.72990149, 'change_7d': -16.293883, 'market_cap': 19178956.192714103}, {'id': 32074, 'symbol': 'FEG', 'name': 'FEED EVERY GORILLA', 'price': 0.00032864666641601437, 'change_24h': -6.86729081, 'change_7d': -14.19314604, 'market_cap': 26469704.97511844}, {'id': 32019, 'symbol': 'CRASH', 'name': 'Crash', 'price': 0.0035908137716047415, 'change_24h': 4.74084861, 'change_7d': 6.93844363, 'market_cap': 3512668.1015975485}, {'id': 31923, 'symbol': 'HAWKTUAH', 'name': 'Hawk Tuah', 'price': 0.0008897625533380383, 'change_24h': -6.65733615, 'change_7d': 10.34980199, 'market_cap': 764056.5777083959}, {'id': 31921, 'symbol': 'RETARDIO', 'name': 'RETARDIO', 'price': 0.040150477657181494, 'change_24h': 2.87572677, 'change_7d': 7.38531031, 'market_cap': 39173667.32613651}, {'id': 31914, 'symbol': 'BILLY', 'name': 'Billy', 'price': 0.02036048834136512, 'change_24h': -12.99161381, 'change_7d': -12.71696274, 'market_cap': 19060219.85126136}, {'id': 31908, 'symbol': 'WAT', 'name': 'Wat', 'price': 7.900638295374549e-06, 'change_24h': -3.89456196, 'change_7d': 34.25522638, 'market_cap': 3305511.7276330935}, {'id': 31847, 'symbol': 'WOLF', 'name': 'LandWolf (SOL)', 'price': 0.002000247992751642, 'change_24h': -5.10306212, 'change_7d': 27.89328079, 'market_cap': 20002166.270074576}, {'id': 31830, 'symbol': 'DADDY', 'name': 'Daddy Tate', 'price': 0.07541035601469624, 'change_24h': 2.3400481, 'change_7d': 0.79026391, 'market_cap': 45222710.38962473}, {'id': 31798, 'symbol': 'JENNER', 'name': 'Caitlyn Jenner (ETH)', 'price': 0.0002215635197330867, 'change_24h': 3.22030906, 'change_7d': 3.81997045, 'market_cap': 213714.15834373693}, {'id': 31770, 'symbol': 'HONK', 'name': 'Pepoclown', 'price': 2.474355501280837e-09, 'change_24h': -9.45214316, 'change_7d': 85.55821414, 'market_cap': 992845.525569602}, {'id': 31678, 'symbol': 'MAGAA', 'name': 'MAGA AGAIN', 'price': 0.007149135149749142, 'change_24h': -7.00163058, 'change_7d': -6.05357947, 'market_cap': 7149135.149749142}, {'id': 31632, 'symbol': 'PEIPEI', 'name': 'PeiPei (ETH)', 'price': 1.1149213635392922e-07, 'change_24h': -1.19243483, 'change_7d': -12.35441257, 'market_cap': 45840699.13043585}, {'id': 31569, 'symbol': 'TROG', 'name': 'Trog', 'price': 2.249779085048139e-06, 'change_24h': 1.43307773, 'change_7d': 48.51745419, 'market_cap': 946459.5632889016}, {'id': 31561, 'symbol': 'SOLCAT', 'name': 'CatSolHat', 'price': 0.012559164084184048, 'change_24h': -0.17625545, 'change_7d': 6.068356, 'market_cap': 830901.2845156254}, {'id': 31510, 'symbol': 'MOTHER', 'name': 'Mother Iggy', 'price': 0.05950302362871237, 'change_24h': 9.13057155, 'change_7d': 66.53466622, 'market_cap': 58678499.412200876}, {'id': 31496, 'symbol': 'PAPU', 'name': 'Papu Token', 'price': 8.127591752575577e-09, 'change_24h': 3.32237823, 'change_7d': 84.29785943, 'market_cap': 257687.8581491088}, {'id': 31317, 'symbol': 'MEOW', 'name': 'MeowCat', 'price': 0.008027174921922751, 'change_24h': -1.93791851, 'change_7d': -4.6879953, 'market_cap': 802717.4921922751}, {'id': 31305, 'symbol': 'MAGA', 'name': 'MAGA', 'price': 6.45821541829669e-05, 'change_24h': 2.61448697, 'change_7d': -33.55051374, 'market_cap': 25203760.182413302}, {'id': 31284, 'symbol': 'HAMMY', 'name': 'SAD HAMSTER', 'price': 0.012036529348068124, 'change_24h': -7.93810938, 'change_7d': 16.15741239, 'market_cap': 11337222.038607052}, {'id': 31267, 'symbol': 'UTYAB', 'name': 'UTYABSWAP', 'price': 0.0013080123797746539, 'change_24h': 12.87982157, 'change_7d': 90.98739274, 'market_cap': 1308012.3797746538}, {'id': 31259, 'symbol': 'FOXSY', 'name': 'Foxsy AI', 'price': 0.09002360660849407, 'change_24h': -1.0132708, 'change_7d': 15.70748931, 'market_cap': 18296466.67516939}, {'id': 31163, 'symbol': 'SLOTH', 'name': 'Slothana', 'price': 0.006046333945347184, 'change_24h': -2.7642754, 'change_7d': 2.40574951, 'market_cap': 10249250.423811788}, {'id': 31152, 'symbol': 'KENDU', 'name': 'Kendu Inu', 'price': 5.4935096559914444e-05, 'change_24h': -0.97786411, 'change_7d': 20.00854328, 'market_cap': 52101991.84975898}, {'id': 31121, 'symbol': 'LABZ', 'name': 'Insane Labz', 'price': 0.01918521121245546, 'change_24h': -3.11082122, 'change_7d': 3.79800696, 'market_cap': 949806.9599914897}, {'id': 31106, 'symbol': 'DOKY', 'name': 'Donkey King', 'price': 2.2075139455454384e-05, 'change_24h': -5.01876988, 'change_7d': -28.3249804, 'market_cap': 191492.16518065598}, {'id': 31061, 'symbol': 'DUREV', 'name': 'Povel Durev', 'price': 0.035918555440704596, 'change_24h': -0.4457259, 'change_7d': 2.74063729, 'market_cap': 3412262.766866937}, {'id': 31051, 'symbol': 'LOBO', 'name': 'LOBO•THE•WOLF•PUP', 'price': 0.0005446515319582705, 'change_24h': -4.39495922, 'change_7d': -14.72250201, 'market_cap': 8925630.381070133}, {'id': 31044, 'symbol': 'HEGE', 'name': 'Hege', 'price': 0.015461313982300686, 'change_24h': 1.49023661, 'change_7d': 17.33684212, 'market_cap': 15459031.843962986}, {'id': 31036, 'symbol': 'CARLO', 'name': 'Carlo', 'price': 0.0009803795167569037, 'change_24h': -4.01065896, 'change_7d': -12.71171748, 'market_cap': 908744.9658366792}, {'id': 30979, 'symbol': 'ELON', 'name': 'Elon MemeLord', 'price': 4.842346651796097e-06, 'change_24h': 13.13773278, 'change_7d': 20.27182781, 'market_cap': 3318071.7158579836}, {'id': 30968, 'symbol': 'LONG', 'name': 'Long', 'price': 1.1058038310879761e-06, 'change_24h': -0.43797833, 'change_7d': 32.47623643, 'market_cap': 866633.7614739848}, {'id': 30953, 'symbol': 'SHIBTC', 'name': 'ShibaBitcoin', 'price': 0.6975613166927364, 'change_24h': -0.09149543, 'change_7d': -0.10271175, 'market_cap': 60311902.01723075}, {'id': 30943, 'symbol': '$MICHI', 'name': 'michi (SOL)', 'price': 0.117911869351425, 'change_24h': -2.72345559, 'change_7d': 14.56403438, 'market_cap': 65531812.063366674}, {'id': 30933, 'symbol': 'DOG', 'name': 'Dog (Runes)', 'price': 0.0021882683829385547, 'change_24h': -7.30841919, 'change_7d': -13.16273772, 'market_cap': 218826838.29385546}, {'id': 30912, 'symbol': 'MANEKI', 'name': 'MANEKI', 'price': 0.005424160880608815, 'change_24h': -1.55428908, 'change_7d': 27.75077777, 'market_cap': 45687095.31711064}, {'id': 30867, 'symbol': 'WHY', 'name': 'WHY', 'price': 2.678935018639163e-07, 'change_24h': -2.09424985, 'change_7d': -1.6444193, 'market_cap': 112515270.78284486}, {'id': 30859, 'symbol': 'HOPPY', 'name': 'Hoppy', 'price': 5.7326445931293125e-05, 'change_24h': -8.5522925, 'change_7d': 19.82919212, 'market_cap': 24116662.538835704}, {'id': 30828, 'symbol': 'CATA', 'name': 'CATAMOTO', 'price': 0.00027747981086225166, 'change_24h': -1.00979801, 'change_7d': 19.74747714, 'market_cap': 5376911.293642551}, {'id': 30647, 'symbol': 'GOAT', 'name': 'Sonic The Goat', 'price': 3.2588968825515676e-07, 'change_24h': 0.33699756, 'change_7d': -5.31891005, 'market_cap': 288771.7766670043}, {'id': 30645, 'symbol': 'POWSCHE', 'name': 'Powsche', 'price': 0.017237224992953708, 'change_24h': -1.21393757, 'change_7d': 30.59615048, 'market_cap': 1638391.9267559026}, {'id': 30629, 'symbol': 'KITTENWIF', 'name': 'KittenWifHat', 'price': 0.0008244819696452965, 'change_24h': 0.55046486, 'change_7d': 3.14689902, 'market_cap': 805996.554023717}, {'id': 30601, 'symbol': 'MOUTAI', 'name': 'Moutai', 'price': 0.006432758184363277, 'change_24h': -6.29420006, 'change_7d': -6.73813125, 'market_cap': 4481814.836773734}, {'id': 30550, 'symbol': 'HAMI', 'name': 'HAMI', 'price': 0.001750194661509419, 'change_24h': 2.40717766, 'change_7d': 8.38800081, 'market_cap': 1684101.8947695398}, {'id': 30493, 'symbol': 'NUB', 'name': 'nubcat', 'price': 0.008602029181940361, 'change_24h': -5.96381558, 'change_7d': -13.65462854, 'market_cap': 8171929.899156726}, {'id': 30484, 'symbol': 'PUPS', 'name': 'PUPS (Ordinals)', 'price': 2.719228707186724, 'change_24h': 0.37133471, 'change_7d': -6.98688497, 'market_cap': 21128407.054840844}, {'id': 30409, 'symbol': 'NSO', 'name': "NeverSurrenderOne's", 'price': 0.00019396208554128963, 'change_24h': -2.26618058, 'change_7d': 3.35814086, 'market_cap': 124758.63040679523}, {'id': 30407, 'symbol': 'ROOST', 'name': 'Roost Coin', 'price': 0.0020775869321590043, 'change_24h': 16.27924256, 'change_7d': 50.55261981, 'market_cap': 1946997.6521838105}, {'id': 30402, 'symbol': 'CAW', 'name': 'crow with knife', 'price': 3.766828728058379e-08, 'change_24h': -3.21365199, 'change_7d': 4.23995501, 'market_cap': 28999360.29598486}, {'id': 30361, 'symbol': 'DOGEMOB', 'name': 'DOGEMOB', 'price': 0.00034782268006846326, 'change_24h': -4.12544203, 'change_7d': -1.35392858, 'market_cap': 173720.06955988053}, {'id': 30309, 'symbol': 'SC', 'name': 'Shark Cat', 'price': 0.012052976711005805, 'change_24h': -6.4461373, 'change_7d': -11.71048065, 'market_cap': 11931187.636836004}, {'id': 30303, 'symbol': 'GB', 'name': 'Gary Banking', 'price': 9.672085807112003e-05, 'change_24h': -3.01620481, 'change_7d': -37.39824308, 'market_cap': 1015569.0097467602}, {'id': 30285, 'symbol': 'MUMU', 'name': 'Mumu the Bull', 'price': 3.651115704661971e-05, 'change_24h': -5.92629023, 'change_7d': 2.78724668, 'market_cap': 83362435.03807513}, {'id': 30270, 'symbol': 'FOMO', 'name': 'FOMO BULL CLUB', 'price': 9.464007213768345e-06, 'change_24h': -1.05740597, 'change_7d': -39.27013238, 'market_cap': 316699.0380232343}, {'id': 30218, 'symbol': 'MABA', 'name': 'Make America Based Again', 'price': 0.00024460005932453263, 'change_24h': 0.27982023, 'change_7d': 14.86484953, 'market_cap': 225620.62689572052}, {'id': 30193, 'symbol': 'BENJI', 'name': 'Basenji', 'price': 0.015489738445553111, 'change_24h': -1.60147188, 'change_7d': -13.33552972, 'market_cap': 14282233.87136402}, {'id': 30133, 'symbol': 'COINYE', 'name': 'Coinye West', 'price': 0.0008938532605026727, 'change_24h': 0.58480217, 'change_7d': 26.76437029, 'market_cap': 716195.2107956706}, {'id': 30126, 'symbol': 'MEW', 'name': 'cat in a dogs world', 'price': 0.0042752317408956565, 'change_24h': -3.83502265, 'change_7d': 3.98341454, 'market_cap': 380020599.1869248}, {'id': 30119, 'symbol': 'WIF', 'name': 'DOGWIFHOOD', 'price': 0.00042830709499371516, 'change_24h': -4.85299443, 'change_7d': 9.96572314, 'market_cap': 427844.59742824937}, {'id': 30096, 'symbol': 'DEGEN', 'name': 'Degen', 'price': 0.003245256240496699, 'change_24h': -0.5219058, 'change_7d': 8.02685185, 'market_cap': 46016464.202377155}, {'id': 30071, 'symbol': 'LADYF', 'name': 'Milady Wif Hat', 'price': 1.3713102368460841e-05, 'change_24h': -1.23880289, 'change_7d': 3.96667031, 'market_cap': 3428251.539550532}, {'id': 30063, 'symbol': 'GIGA', 'name': 'Gigachad', 'price': 0.016779323169116272, 'change_24h': -7.15490186, 'change_7d': 12.10071658, 'market_cap': 156088175.32098106}, {'id': 30011, 'symbol': 'SKID', 'name': 'Success Kid', 'price': 0.026644795348589937, 'change_24h': 1.68115728, 'change_7d': 4.83207344, 'market_cap': 2311241.436194542}, {'id': 30008, 'symbol': 'APU', 'name': 'Apu Apustaja', 'price': 0.00018752558223819106, 'change_24h': -14.60615612, 'change_7d': 3.59312395, 'market_cap': 59698114.894198336}, {'id': 30007, 'symbol': 'HUND', 'name': 'HUND', 'price': 0.006624933004839104, 'change_24h': -4.23012646, 'change_7d': 18.80458653, 'market_cap': 2529579.0666696564}, {'id': 29999, 'symbol': 'CHKN', 'name': 'Chickencoin', 'price': 5.1618896538034534e-08, 'change_24h': 0.21755199, 'change_7d': 2.94907457, 'market_cap': 3315946.2947068005}, {'id': 29932, 'symbol': 'BSHIB', 'name': 'Based Shiba Inu', 'price': 2.0759965209992277e-05, 'change_24h': 4.54541767, 'change_7d': 9.29667141, 'market_cap': 187698.96483125357}, {'id': 29920, 'symbol': 'SLERF', 'name': 'SLERF', 'price': 0.13567370591902544, 'change_24h': -2.6148509, 'change_7d': 3.48513591, 'market_cap': 67836547.6936744}, {'id': 29879, 'symbol': 'ANDY', 'name': 'ANDY (ETH)', 'price': 7.275078363694599e-05, 'change_24h': -7.99221739, 'change_7d': 33.40693501, 'market_cap': 72750783.636946}]</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>59981.8</v>
+      </c>
+      <c r="E3" t="n">
+        <v>135.2</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolios at 2024-09-16 12:22:10
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,6 +509,34 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Portfolio_3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[{'id': 32981, 'symbol': 'CATE', 'name': 'Cate', 'price': 0.029139323930875163, 'change_24h': -36.08711097, 'change_7d': 294.18440566, 'market_cap': 29139323.930875164}, {'id': 32902, 'symbol': 'BRUH', 'name': 'Bruh', 'price': 0.0002525611914506638, 'change_24h': -20.74363296, 'change_7d': -64.96657158, 'market_cap': 252561.1914506638}, {'id': 32862, 'symbol': 'MUNCAT', 'name': 'MUNCAT', 'price': 0.019374330182423315, 'change_24h': -4.60176334, 'change_7d': 8.75089258, 'market_cap': 19374330.182423316}, {'id': 32844, 'symbol': 'WIWI', 'name': 'Wiggly Willy', 'price': 1.1970992615880443e-06, 'change_24h': -6.43596478, 'change_7d': -30.49371301, 'market_cap': 779073.1964659699}, {'id': 32698, 'symbol': 'DOGS', 'name': 'DOGS', 'price': 0.000974934022244226, 'change_24h': -8.84416531, 'change_7d': -4.42049895, 'market_cap': 503797155.99470377}, {'id': 32821, 'symbol': 'BULLS', 'name': 'BULLS', 'price': 0.0003321096010086998, 'change_24h': 10.31073071, 'change_7d': -69.08446803, 'market_cap': 332109.6010086998}, {'id': 32797, 'symbol': 'IVfun', 'name': 'Invest Zone', 'price': 0.01509359367209487, 'change_24h': -17.72769307, 'change_7d': -43.50275799, 'market_cap': 14191282.129985562}, {'id': 32790, 'symbol': 'EBULL', 'name': 'ETHEREUM IS GOOD', 'price': 0.0002195472998804108, 'change_24h': -11.28277107, 'change_7d': -47.72450816, 'market_cap': 2195472.998804108}, {'id': 32732, 'symbol': 'SUNPEPE', 'name': 'sunpepe', 'price': 0.0007073959010905591, 'change_24h': -22.32759297, 'change_7d': -15.13403981, 'market_cap': 707395.9010905592}, {'id': 32727, 'symbol': 'FOFAR', 'name': 'Fofar (fofar.meme)', 'price': 0.004762916399806206, 'change_24h': -20.60774427, 'change_7d': -22.81827769, 'market_cap': 4524734.2197121}, {'id': 32724, 'symbol': 'CAT', 'name': "Simon's Cat", 'price': 3.128230254831375e-05, 'change_24h': -10.57951281, 'change_7d': 12.07102345, 'market_cap': 211154144.82625225}, {'id': 32717, 'symbol': 'SUNDOG', 'name': 'SUNDOG', 'price': 0.32350882367672973, 'change_24h': -6.11142331, 'change_7d': 11.17595893, 'market_cap': 322697710.70768976}, {'id': 32638, 'symbol': 'CATDOG', 'name': 'CatDog', 'price': 6.376179414161324e-05, 'change_24h': -13.70645916, 'change_7d': 10.80027526, 'market_cap': 6376179.4141613245}, {'id': 32625, 'symbol': 'FUKU', 'name': 'Fuku-Kun', 'price': 1.8667628802515917e-06, 'change_24h': 17.41560241, 'change_7d': -17.07599284, 'market_cap': 600761.2023986556}, {'id': 32618, 'symbol': 'WDOG', 'name': 'Wrapped Dog', 'price': 0.013036393535211509, 'change_24h': -1.46995629, 'change_7d': -11.93829317, 'market_cap': 13036373.185401201}, {'id': 32598, 'symbol': 'GODCAT', 'name': 'Godcat Exploding Kittens', 'price': 0.00012854647107292624, 'change_24h': -10.03226685, 'change_7d': 1.96281608, 'market_cap': 102442.33827401283}, {'id': 32524, 'symbol': 'GINNAN', 'name': 'Ginnan The Cat', 'price': 3.1159333185215106e-06, 'change_24h': 6.07614516, 'change_7d': -12.29124678, 'market_cap': 21499934.79448856}, {'id': 32521, 'symbol': 'NEIRO', 'name': 'First Neiro On Ethereum', 'price': 0.00031501157832759856, 'change_24h': 650.9717983, 'change_7d': 573.24760554, 'market_cap': 131812785.08008216}, {'id': 32495, 'symbol': '$YAWN', 'name': 'YAWN', 'price': 3.590853100253668e-05, 'change_24h': -2.61457542, 'change_7d': -17.57092872, 'market_cap': 230372.5100883174}, {'id': 32464, 'symbol': 'NEIRO', 'name': 'Neiro (neiro.lol)', 'price': 0.004294003486495922, 'change_24h': 28.80036116, 'change_7d': 10.66580436, 'market_cap': 4294003.3533818135}, {'id': 32462, 'symbol': 'YOUNES', 'name': 'YOUNES', 'price': 0.0015603198612713744, 'change_24h': -18.73639977, 'change_7d': -5.37927022, 'market_cap': 1560317.054255944}, {'id': 32461, 'symbol': 'NEIRO', 'name': 'Neiro Ethereum', 'price': 0.08901291215736677, 'change_24h': -33.68366943, 'change_7d': -46.54167583, 'market_cap': 89012912.15736677}, {'id': 32448, 'symbol': 'BRAINLET', 'name': 'Brainlet', 'price': 0.013371055846627362, 'change_24h': -12.36710061, 'change_7d': -36.54155982, 'market_cap': 12741353.20527166}, {'id': 32415, 'symbol': 'SKBDI', 'name': 'Skibidi Toilet', 'price': 0.04473303942948299, 'change_24h': -10.90531428, 'change_7d': -22.92623991, 'market_cap': 3133042.6761646266}, {'id': 32350, 'symbol': 'SOY', 'name': 'Soyjak', 'price': 0.0006795624706939648, 'change_24h': -2.64842734, 'change_7d': -35.54658999, 'market_cap': 629654.0362460715}, {'id': 32310, 'symbol': 'SAITAMA', 'name': 'SAITAMA INU', 'price': 0.00027430996870847366, 'change_24h': -18.53043543, 'change_7d': 23.72363344, 'market_cap': 182820.29420731042}, {'id': 32297, 'symbol': 'BILL', 'name': 'BILL THE BEAR', 'price': 1.979811310241725e-06, 'change_24h': -6.00642017, 'change_7d': 5.29085747, 'market_cap': 1759826.1496376554}, {'id': 32288, 'symbol': 'torsy', 'name': 'TORSY', 'price': 0.003005750585596339, 'change_24h': -1.82467013, 'change_7d': 6.5042258, 'market_cap': 2104024.427036996}, {'id': 32259, 'symbol': 'MOBY', 'name': 'Moby', 'price': 0.00013450244292354262, 'change_24h': -5.03668237, 'change_7d': 11.54955673, 'market_cap': 1345024.4292354262}, {'id': 32128, 'symbol': 'MSI', 'name': 'monkey shit inu', 'price': 1.8098729385003677e-06, 'change_24h': 9.95461635, 'change_7d': 45.91601572, 'market_cap': 5328754.305610909}, {'id': 32125, 'symbol': 'COIN', 'name': '8-Bit Coin', 'price': 0.0006319251620375989, 'change_24h': -1.15136583, 'change_7d': -15.6718967, 'market_cap': 18957754.86112797}, {'id': 32074, 'symbol': 'FEG', 'name': 'FEED EVERY GORILLA', 'price': 0.00030113265003483, 'change_24h': -8.35137175, 'change_7d': -19.63470506, 'market_cap': 24253684.03009346}, {'id': 32019, 'symbol': 'CRASH', 'name': 'Crash', 'price': 0.003306616540248982, 'change_24h': -7.91456337, 'change_7d': 3.14937666, 'market_cap': 3234655.7588133174}, {'id': 31923, 'symbol': 'HAWKTUAH', 'name': 'Hawk Tuah', 'price': 0.0009020855931686253, 'change_24h': 1.38498241, 'change_7d': 11.43846528, 'market_cap': 774638.6140107772}, {'id': 31921, 'symbol': 'RETARDIO', 'name': 'RETARDIO', 'price': 0.035894365968676796, 'change_24h': -10.60680773, 'change_7d': -5.89337012, 'market_cap': 35021101.45103184}, {'id': 31914, 'symbol': 'BILLY', 'name': 'Billy', 'price': 0.02019622322252712, 'change_24h': -0.77008517, 'change_7d': -18.87591525, 'market_cap': 18906445.087785527}, {'id': 31908, 'symbol': 'WAT', 'name': 'Wat', 'price': 6.434700983075277e-06, 'change_24h': -18.66694023, 'change_7d': -0.02011322, 'market_cap': 2692184.956223106}, {'id': 31847, 'symbol': 'WOLF', 'name': 'LandWolf (SOL)', 'price': 0.0017975557046317865, 'change_24h': -9.84772067, 'change_7d': 13.26939103, 'market_cap': 17975275.154204458}, {'id': 31830, 'symbol': 'DADDY', 'name': 'Daddy Tate', 'price': 0.07349639130174392, 'change_24h': -2.40572335, 'change_7d': 0.92716441, 'market_cap': 44074928.089101754}, {'id': 31798, 'symbol': 'JENNER', 'name': 'Caitlyn Jenner (ETH)', 'price': 0.00019243234131918272, 'change_24h': -12.99314125, 'change_7d': -16.94863288, 'market_cap': 185615.01420760492}, {'id': 31770, 'symbol': 'HONK', 'name': 'Pepoclown', 'price': 2.068912460203536e-09, 'change_24h': -16.38580393, 'change_7d': 49.56251288, 'market_cap': 830159.8043793539}, {'id': 31678, 'symbol': 'MAGAA', 'name': 'MAGA AGAIN', 'price': 0.00687644569218029, 'change_24h': -3.06701461, 'change_7d': -10.03807586, 'market_cap': 6876445.69218029}, {'id': 31632, 'symbol': 'PEIPEI', 'name': 'PeiPei (ETH)', 'price': 1.0483626872196531e-07, 'change_24h': -5.82396976, 'change_7d': -14.50373131, 'market_cap': 43104096.930973984}, {'id': 31569, 'symbol': 'TROG', 'name': 'Trog', 'price': 1.9000862937687478e-06, 'change_24h': -15.54342796, 'change_7d': 24.62627876, 'market_cap': 799347.3029255745}, {'id': 31561, 'symbol': 'SOLCAT', 'name': 'CatSolHat', 'price': 0.012440070426778086, 'change_24h': -0.84177775, 'change_7d': 6.55731762, 'market_cap': 823022.171522676}, {'id': 31510, 'symbol': 'MOTHER', 'name': 'Mother Iggy', 'price': 0.05428805790894996, 'change_24h': -8.61527654, 'change_7d': 53.69338084, 'market_cap': 53535796.66769585}, {'id': 31496, 'symbol': 'PAPU', 'name': 'Papu Token', 'price': 8.63254434919503e-09, 'change_24h': 6.35814711, 'change_7d': 85.70910873, 'market_cap': 273697.5393746039}, {'id': 31317, 'symbol': 'MEOW', 'name': 'MeowCat', 'price': 0.007325005223657749, 'change_24h': -8.74740746, 'change_7d': -17.20302316, 'market_cap': 732500.522365775}, {'id': 31305, 'symbol': 'MAGA', 'name': 'MAGA', 'price': 6.375211512978745e-05, 'change_24h': -0.95305309, 'change_7d': -27.25946893, 'market_cap': 24879830.05801541}, {'id': 31284, 'symbol': 'HAMMY', 'name': 'SAD HAMSTER', 'price': 0.011266577684823262, 'change_24h': -6.34657659, 'change_7d': -4.08111829, 'market_cap': 10612003.604557136}, {'id': 31267, 'symbol': 'UTYAB', 'name': 'UTYABSWAP', 'price': 0.0011104591165764781, 'change_24h': -15.10572874, 'change_7d': 51.251048, 'market_cap': 1110459.1165764781}, {'id': 31259, 'symbol': 'FOXSY', 'name': 'Foxsy AI', 'price': 0.08529040891276468, 'change_24h': -5.26974331, 'change_7d': 7.83199334, 'market_cap': 17334487.95459311}, {'id': 31163, 'symbol': 'SLOTH', 'name': 'Slothana', 'price': 0.00593063885816661, 'change_24h': -1.49380992, 'change_7d': 2.18500391, 'market_cap': 10053133.581434773}, {'id': 31152, 'symbol': 'KENDU', 'name': 'Kendu Inu', 'price': 5.5953786970426215e-05, 'change_24h': 2.67499453, 'change_7d': 25.07916241, 'market_cap': 53068146.50843015}, {'id': 31121, 'symbol': 'LABZ', 'name': 'Insane Labz', 'price': 0.017456755559443735, 'change_24h': -9.01472971, 'change_7d': 4.32482207, 'market_cap': 864235.8817746732}, {'id': 31106, 'symbol': 'DOKY', 'name': 'Donkey King', 'price': 2.1838017714979863e-05, 'change_24h': -1.07148149, 'change_7d': -21.9366622, 'market_cap': 189435.2379487126}, {'id': 31061, 'symbol': 'DUREV', 'name': 'Povel Durev', 'price': 0.03528661976631283, 'change_24h': -2.0411243, 'change_7d': -7.14347822, 'market_cap': 3352228.877799719}, {'id': 31051, 'symbol': 'LOBO', 'name': 'LOBO•THE•WOLF•PUP', 'price': 0.000510869249058204, 'change_24h': -6.46887891, 'change_7d': -19.80979546, 'market_cap': 8372013.705265315}, {'id': 31044, 'symbol': 'HEGE', 'name': 'Hege', 'price': 0.01528185216378374, 'change_24h': -1.1678672, 'change_7d': 3.00578079, 'market_cap': 15279596.514572168}, {'id': 31036, 'symbol': 'CARLO', 'name': 'Carlo', 'price': 0.0008650162782807935, 'change_24h': -11.76720204, 'change_7d': -25.17629652, 'market_cap': 801811.1096963773}, {'id': 30979, 'symbol': 'ELON', 'name': 'Elon MemeLord', 'price': 4.536133694681866e-06, 'change_24h': -6.32402697, 'change_7d': 12.44899525, 'market_cap': 3108248.540217904}, {'id': 30968, 'symbol': 'LONG', 'name': 'Long', 'price': 1.0422856620233421e-06, 'change_24h': -5.74407207, 'change_7d': 23.08945372, 'market_cap': 816853.693589553}, {'id': 30953, 'symbol': 'SHIBTC', 'name': 'ShibaBitcoin', 'price': 0.6970305061463759, 'change_24h': -0.07714365, 'change_7d': -0.15680246, 'market_cap': 60266007.566240266}, {'id': 30943, 'symbol': '$MICHI', 'name': 'michi (SOL)', 'price': 0.11288322873985437, 'change_24h': -4.39640829, 'change_7d': 2.13794535, 'market_cap': 62737047.35219478}, {'id': 30933, 'symbol': 'DOG', 'name': 'Dog (Runes)', 'price': 0.0021400667517258573, 'change_24h': -2.44059291, 'change_7d': -14.80441103, 'market_cap': 214006675.17258573}, {'id': 30912, 'symbol': 'MANEKI', 'name': 'MANEKI', 'price': 0.00565028992493853, 'change_24h': 4.40875026, 'change_7d': 30.09895904, 'market_cap': 47591754.75285718}, {'id': 30867, 'symbol': 'WHY', 'name': 'WHY', 'price': 2.692710739893155e-07, 'change_24h': 0.49866255, 'change_7d': 4.01470162, 'market_cap': 113093851.0755125}, {'id': 30859, 'symbol': 'HOPPY', 'name': 'Hoppy', 'price': 5.368310561811881e-05, 'change_24h': -6.35613079, 'change_7d': 1.05730674, 'market_cap': 22583945.702486403}, {'id': 30828, 'symbol': 'CATA', 'name': 'CATAMOTO', 'price': 0.00026764432395804066, 'change_24h': -3.47241182, 'change_7d': 16.08540717, 'market_cap': 5186322.50648218}, {'id': 30647, 'symbol': 'GOAT', 'name': 'Sonic The Goat', 'price': 3.1491388254117285e-07, 'change_24h': -3.36795121, 'change_7d': -6.36869642, 'market_cap': 279046.08410720347}, {'id': 30645, 'symbol': 'POWSCHE', 'name': 'Powsche', 'price': 0.015752725261451144, 'change_24h': -8.62687032, 'change_7d': 21.47726974, 'market_cap': 1497290.7706034856}, {'id': 30629, 'symbol': 'KITTENWIF', 'name': 'KittenWifHat', 'price': 0.0008044336871728509, 'change_24h': -2.44670259, 'change_7d': 2.28799903, 'market_cap': 786397.7067117799}, {'id': 30601, 'symbol': 'MOUTAI', 'name': 'Moutai', 'price': 0.005497809688962206, 'change_24h': -14.527483, 'change_7d': -11.69149726, 'market_cap': 3830419.7406890998}, {'id': 30550, 'symbol': 'HAMI', 'name': 'HAMI', 'price': 0.0016212390216391401, 'change_24h': -7.37546275, 'change_7d': 0.31642221, 'market_cap': 1560015.4545347888}, {'id': 30493, 'symbol': 'NUB', 'name': 'nubcat', 'price': 0.008871408835112867, 'change_24h': 3.39199983, 'change_7d': -8.28930856, 'market_cap': 8427840.637823658}, {'id': 30484, 'symbol': 'PUPS', 'name': 'PUPS (Ordinals)', 'price': 2.507201534089858, 'change_24h': -5.80841652, 'change_7d': -6.86848297, 'market_cap': 19480955.919878196}, {'id': 30409, 'symbol': 'NSO', 'name': "NeverSurrenderOne's", 'price': 0.00018821080490818678, 'change_24h': -2.97789603, 'change_7d': 2.97455753, 'market_cap': 121059.34096644583}, {'id': 30407, 'symbol': 'ROOST', 'name': 'Roost Coin', 'price': 0.0017491617219330038, 'change_24h': -15.80491292, 'change_7d': 24.08285034, 'market_cap': 1639216.0121811486}, {'id': 30402, 'symbol': 'CAW', 'name': 'crow with knife', 'price': 3.6141720897967874e-08, 'change_24h': -4.32496404, 'change_7d': -0.92919839, 'market_cap': 27824115.76693413}, {'id': 30361, 'symbol': 'DOGEMOB', 'name': 'DOGEMOB', 'price': 0.00034513339900209126, 'change_24h': -0.77270971, 'change_7d': -3.85510172, 'market_cap': 172376.90788386718}, {'id': 30309, 'symbol': 'SC', 'name': 'Shark Cat', 'price': 0.011597929638090474, 'change_24h': -3.60634632, 'change_7d': -9.5873231, 'market_cap': 11480738.578423053}, {'id': 30303, 'symbol': 'GB', 'name': 'Gary Banking', 'price': 9.603228198005154e-05, 'change_24h': -0.71192099, 'change_7d': -36.68830043, 'market_cap': 1008338.9607905411}, {'id': 30285, 'symbol': 'MUMU', 'name': 'Mumu the Bull', 'price': 3.311633143858145e-05, 'change_24h': -9.35557125, 'change_7d': -5.18532352, 'market_cap': 75611354.21490838}, {'id': 30270, 'symbol': 'FOMO', 'name': 'FOMO BULL CLUB', 'price': 9.32242505811339e-06, 'change_24h': -1.72464896, 'change_7d': -37.68931312, 'market_cap': 311961.20007738535}, {'id': 30218, 'symbol': 'MABA', 'name': 'Make America Based Again', 'price': 0.00021710814260935348, 'change_24h': -11.23953804, 'change_7d': -5.23313165, 'market_cap': 200261.91070827295}, {'id': 30193, 'symbol': 'BENJI', 'name': 'Basenji', 'price': 0.014691124333341283, 'change_24h': -4.97266429, 'change_7d': -19.38632383, 'market_cap': 13545875.8260895}, {'id': 30133, 'symbol': 'COINYE', 'name': 'Coinye West', 'price': 0.0009798889975638088, 'change_24h': 9.80172775, 'change_7d': 31.7042877, 'market_cap': 785130.8913634287}, {'id': 30126, 'symbol': 'MEW', 'name': 'cat in a dogs world', 'price': 0.0042210796171238745, 'change_24h': -1.23964412, 'change_7d': 1.715932, 'market_cap': 375207077.0739257}, {'id': 30119, 'symbol': 'WIF', 'name': 'DOGWIFHOOD', 'price': 0.000458884941988761, 'change_24h': 7.13712257, 'change_7d': 11.69619647, 'market_cap': 458389.4256385081}, {'id': 30096, 'symbol': 'DEGEN', 'name': 'Degen', 'price': 0.002952136717829938, 'change_24h': -9.03085859, 'change_7d': -1.365551, 'market_cap': 41860144.016163304}, {'id': 30071, 'symbol': 'LADYF', 'name': 'Milady Wif Hat', 'price': 1.332583878802956e-05, 'change_24h': -3.66171163, 'change_7d': 2.52262203, 'market_cap': 3331436.323696907}, {'id': 30063, 'symbol': 'GIGA', 'name': 'Gigachad', 'price': 0.0164742932798592, 'change_24h': -1.80681799, 'change_7d': 2.76960118, 'market_cap': 153250661.65296072}, {'id': 30011, 'symbol': 'SKID', 'name': 'Success Kid', 'price': 0.025331225184864834, 'change_24h': -4.81351327, 'change_7d': 0.56263472, 'market_cap': 2197298.8161807247}, {'id': 30008, 'symbol': 'APU', 'name': 'Apu Apustaja', 'price': 0.00018650718384005105, 'change_24h': -0.72103611, 'change_7d': 6.62478854, 'market_cap': 59373911.31698716}, {'id': 30007, 'symbol': 'HUND', 'name': 'HUND', 'price': 0.006278814398861651, 'change_24h': -5.22448462, 'change_7d': 13.23043212, 'market_cap': 2397421.5669479524}, {'id': 29999, 'symbol': 'CHKN', 'name': 'Chickencoin', 'price': 4.834561903759423e-08, 'change_24h': -6.19775309, 'change_7d': -8.30257855, 'market_cap': 3105674.2213560157}, {'id': 29932, 'symbol': 'BSHIB', 'name': 'Based Shiba Inu', 'price': 2.0321708154334188e-05, 'change_24h': -2.11104076, 'change_7d': 6.98052083, 'market_cap': 183736.5113856465}, {'id': 29920, 'symbol': 'SLERF', 'name': 'SLERF', 'price': 0.13511996743584379, 'change_24h': -0.37994926, 'change_7d': 3.28035753, 'market_cap': 67559679.69799516}, {'id': 29879, 'symbol': 'ANDY', 'name': 'ANDY (ETH)', 'price': 6.502301923744789e-05, 'change_24h': -10.48923845, 'change_7d': 11.66785725, 'market_cap': 65023019.23744789}, {'id': 29870, 'symbol': 'BOME', 'name': 'BOOK OF MEME', 'price': 0.005999715543528559, 'change_24h': -4.49814322, 'change_7d': -3.97460541, 'market_cap': 413750959.9093467}]</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>58743.11</v>
+      </c>
+      <c r="E4" t="n">
+        <v>132.09</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolios at 2024-09-18 12:20:55
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Portfolio_2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Portfolio_3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3822,4 +3823,3285 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0314601681884711</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-9.01374285</v>
+      </c>
+      <c r="F2" t="n">
+        <v>85.2934731</v>
+      </c>
+      <c r="G2" t="n">
+        <v>31460168.1884711</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0002886987239681734</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.86581467</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-25.33639039</v>
+      </c>
+      <c r="G3" t="n">
+        <v>288698.7239681734</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.01565988190351425</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-14.83332758</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-22.85597253</v>
+      </c>
+      <c r="G4" t="n">
+        <v>15659881.90351425</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1.169665596201949e-06</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.23191891</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-21.21404312</v>
+      </c>
+      <c r="G5" t="n">
+        <v>761219.3441841047</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0009391527221152177</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-1.87185195</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-7.69974167</v>
+      </c>
+      <c r="G6" t="n">
+        <v>485307169.1530387</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0003337235965788325</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-0.49696215</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-63.42900894</v>
+      </c>
+      <c r="G7" t="n">
+        <v>333723.5965788325</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.01688242758061729</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.27707106</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-30.8150752</v>
+      </c>
+      <c r="G8" t="n">
+        <v>15873177.59047221</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0002259580858537046</v>
+      </c>
+      <c r="E9" t="n">
+        <v>18.19734041</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-47.215013</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2259580.858537046</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.004382857711044227</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-28.25640368</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-22.2530333</v>
+      </c>
+      <c r="G10" t="n">
+        <v>4291403.691445079</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0007083754844751799</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-11.38241714</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-32.51688975</v>
+      </c>
+      <c r="G11" t="n">
+        <v>708375.4844751799</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.005316141406463372</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.01289087</v>
+      </c>
+      <c r="F12" t="n">
+        <v>34.04808885</v>
+      </c>
+      <c r="G12" t="n">
+        <v>5050293.752716706</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3.393288611656429e-05</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1.95952058</v>
+      </c>
+      <c r="F13" t="n">
+        <v>35.17158518</v>
+      </c>
+      <c r="G13" t="n">
+        <v>229045465.5048298</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.3256105563192074</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.01779238</v>
+      </c>
+      <c r="F14" t="n">
+        <v>13.26198823</v>
+      </c>
+      <c r="G14" t="n">
+        <v>324790980.547698</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>6.95125227201352e-05</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-9.179092880000001</v>
+      </c>
+      <c r="F15" t="n">
+        <v>74.95834044999999</v>
+      </c>
+      <c r="G15" t="n">
+        <v>6951252.27201352</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>4.331783572745723e-06</v>
+      </c>
+      <c r="E16" t="n">
+        <v>56.87065468</v>
+      </c>
+      <c r="F16" t="n">
+        <v>119.04107264</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1394053.596856785</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.01469504195329923</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1.30495262</v>
+      </c>
+      <c r="F17" t="n">
+        <v>8.26840617</v>
+      </c>
+      <c r="G17" t="n">
+        <v>14695019.01433874</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>2.79099550285755e-06</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-2.21657753</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-2.48385258</v>
+      </c>
+      <c r="G18" t="n">
+        <v>19257864.39859396</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0008020343017450083</v>
+      </c>
+      <c r="E19" t="n">
+        <v>110.79565452</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1580.85069329</v>
+      </c>
+      <c r="G19" t="n">
+        <v>336568957.2594691</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>3.645992960202539e-05</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.0975472</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.98055169</v>
+      </c>
+      <c r="G20" t="n">
+        <v>233910.0282177676</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.004182625582189715</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4.60361776</v>
+      </c>
+      <c r="F21" t="n">
+        <v>13.27160641</v>
+      </c>
+      <c r="G21" t="n">
+        <v>4182625.452528322</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0012790772829485</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-2.15171418</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-31.30450495</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1279074.981888468</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.07781026185109709</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.71395745</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-53.99453383</v>
+      </c>
+      <c r="G23" t="n">
+        <v>77810261.85109709</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.01227787745127043</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-8.91255896</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-26.50012129</v>
+      </c>
+      <c r="G24" t="n">
+        <v>11699657.45503455</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.05399580492970803</v>
+      </c>
+      <c r="E25" t="n">
+        <v>36.92797496</v>
+      </c>
+      <c r="F25" t="n">
+        <v>14.09844404</v>
+      </c>
+      <c r="G25" t="n">
+        <v>3781794.470847804</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.0006289791457013893</v>
+      </c>
+      <c r="E26" t="n">
+        <v>20.12941931</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-37.54956996</v>
+      </c>
+      <c r="G26" t="n">
+        <v>582785.6523640173</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.0002847002686253574</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.04533244</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-3.5451007</v>
+      </c>
+      <c r="G27" t="n">
+        <v>189745.1525952521</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>1.977867940256163e-06</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-6.28887991</v>
+      </c>
+      <c r="F28" t="n">
+        <v>5.25246618</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1758098.709463046</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.002959440805797831</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-1.53607296</v>
+      </c>
+      <c r="F29" t="n">
+        <v>4.63953348</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2071607.596321339</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0001305356765073596</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.25612968</v>
+      </c>
+      <c r="F30" t="n">
+        <v>13.66729039</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1305356.765073596</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>2.500783542120415e-06</v>
+      </c>
+      <c r="E31" t="n">
+        <v>9.57996829</v>
+      </c>
+      <c r="F31" t="n">
+        <v>107.63067562</v>
+      </c>
+      <c r="G31" t="n">
+        <v>7362981.55743288</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.0006263216707293956</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1.19787235</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-18.14602673</v>
+      </c>
+      <c r="G32" t="n">
+        <v>18789650.12188187</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.0003150350542591964</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-0.22021841</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-14.83725321</v>
+      </c>
+      <c r="G33" t="n">
+        <v>25373404.9214595</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.002950113112072576</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-10.72636955</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.71480979</v>
+      </c>
+      <c r="G34" t="n">
+        <v>2885910.794602659</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.000999047023478528</v>
+      </c>
+      <c r="E35" t="n">
+        <v>6.72525056</v>
+      </c>
+      <c r="F35" t="n">
+        <v>22.59590565</v>
+      </c>
+      <c r="G35" t="n">
+        <v>857901.2983464591</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.03692185752194251</v>
+      </c>
+      <c r="E36" t="n">
+        <v>4.66768036</v>
+      </c>
+      <c r="F36" t="n">
+        <v>9.65485425</v>
+      </c>
+      <c r="G36" t="n">
+        <v>36023595.43458342</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.03291116846330668</v>
+      </c>
+      <c r="E37" t="n">
+        <v>57.08649026</v>
+      </c>
+      <c r="F37" t="n">
+        <v>14.78076935</v>
+      </c>
+      <c r="G37" t="n">
+        <v>30809384.1343722</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>9.010684869328252e-06</v>
+      </c>
+      <c r="E38" t="n">
+        <v>16.28564521</v>
+      </c>
+      <c r="F38" t="n">
+        <v>37.34533363</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3769939.009485888</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.001634869605256261</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-9.724336660000001</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-24.75672347</v>
+      </c>
+      <c r="G39" t="n">
+        <v>16348439.47431751</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.07335348416904103</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3.83720953</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.64876624</v>
+      </c>
+      <c r="G40" t="n">
+        <v>43989228.34948543</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.0002041630550085357</v>
+      </c>
+      <c r="E41" t="n">
+        <v>15.03779695</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-1.10763796</v>
+      </c>
+      <c r="G41" t="n">
+        <v>196930.1422842467</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>1.806246144444392e-09</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-6.53321896</v>
+      </c>
+      <c r="F42" t="n">
+        <v>42.86392023</v>
+      </c>
+      <c r="G42" t="n">
+        <v>724763.8432151949</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.006563223165946595</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-10.45728612</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-11.00746281</v>
+      </c>
+      <c r="G43" t="n">
+        <v>6563223.165946595</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>1.090704464620433e-07</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.6819984100000001</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-0.5414021999999999</v>
+      </c>
+      <c r="G44" t="n">
+        <v>44845005.96900287</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>1.903987450908757e-06</v>
+      </c>
+      <c r="E45" t="n">
+        <v>3.75722983</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-32.42878012</v>
+      </c>
+      <c r="G45" t="n">
+        <v>800988.4807228051</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.01191029717108162</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-7.42290091</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2.86200755</v>
+      </c>
+      <c r="G46" t="n">
+        <v>787972.9217708906</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.04975034686677482</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-9.950782930000001</v>
+      </c>
+      <c r="F47" t="n">
+        <v>26.33470636</v>
+      </c>
+      <c r="G47" t="n">
+        <v>49060963.98721794</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>8.973677775149259e-09</v>
+      </c>
+      <c r="E48" t="n">
+        <v>3.14574396</v>
+      </c>
+      <c r="F48" t="n">
+        <v>28.96984082</v>
+      </c>
+      <c r="G48" t="n">
+        <v>284513.2821620484</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.007503613859507431</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.54573405</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-4.57738775</v>
+      </c>
+      <c r="G49" t="n">
+        <v>750361.3859507431</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>7.12010943708051e-05</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.51437703</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-2.51953004</v>
+      </c>
+      <c r="G50" t="n">
+        <v>27786860.47175004</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.01475965778995445</v>
+      </c>
+      <c r="E51" t="n">
+        <v>8.5404631</v>
+      </c>
+      <c r="F51" t="n">
+        <v>37.09683155</v>
+      </c>
+      <c r="G51" t="n">
+        <v>13902140.12193033</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.001042933169549669</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.0419948</v>
+      </c>
+      <c r="F52" t="n">
+        <v>43.50698742</v>
+      </c>
+      <c r="G52" t="n">
+        <v>1042933.169549669</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.08810828857794795</v>
+      </c>
+      <c r="E53" t="n">
+        <v>2.34848782</v>
+      </c>
+      <c r="F53" t="n">
+        <v>3.96405829</v>
+      </c>
+      <c r="G53" t="n">
+        <v>17907195.9734229</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.00596258765581896</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-1.866448</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-2.28403949</v>
+      </c>
+      <c r="G54" t="n">
+        <v>10107290.56826985</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>5.035564476582168e-05</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-0.26655235</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-2.24010142</v>
+      </c>
+      <c r="G55" t="n">
+        <v>47758710.86923026</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>1.789371119163758e-05</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-16.59941457</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-31.6599135</v>
+      </c>
+      <c r="G56" t="n">
+        <v>155220.106587249</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.0345300623681213</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.04455114</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-10.52073661</v>
+      </c>
+      <c r="G57" t="n">
+        <v>3280355.924971524</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.0005618652740571069</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-1.64729544</v>
+      </c>
+      <c r="F58" t="n">
+        <v>-8.71470373</v>
+      </c>
+      <c r="G58" t="n">
+        <v>9207725.427965278</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.0137341823630507</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-9.96721327</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-11.65736507</v>
+      </c>
+      <c r="G59" t="n">
+        <v>13732155.15474593</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.0009371206867663618</v>
+      </c>
+      <c r="E60" t="n">
+        <v>8.052700919999999</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-6.30034406</v>
+      </c>
+      <c r="G60" t="n">
+        <v>868646.9799955109</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Elon MemeLord</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>3.950756716716704e-06</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-10.29530765</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-2.6637726</v>
+      </c>
+      <c r="G61" t="n">
+        <v>2707136.65514041</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>1.061510110193848e-06</v>
+      </c>
+      <c r="E62" t="n">
+        <v>1.8155364</v>
+      </c>
+      <c r="F62" t="n">
+        <v>7.21870478</v>
+      </c>
+      <c r="G62" t="n">
+        <v>831920.1595954403</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.6972390593984787</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.23872061</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-0.06841147</v>
+      </c>
+      <c r="G63" t="n">
+        <v>60284039.30482039</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.1085482061958874</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1.71021111</v>
+      </c>
+      <c r="F64" t="n">
+        <v>5.34536653</v>
+      </c>
+      <c r="G64" t="n">
+        <v>60327774.23221217</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.002247117856898261</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-4.10754196</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-13.78399914</v>
+      </c>
+      <c r="G65" t="n">
+        <v>224711785.689826</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.005446211915267155</v>
+      </c>
+      <c r="E66" t="n">
+        <v>2.20256638</v>
+      </c>
+      <c r="F66" t="n">
+        <v>12.24423898</v>
+      </c>
+      <c r="G66" t="n">
+        <v>45872828.69494575</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>2.894818960875689e-07</v>
+      </c>
+      <c r="E67" t="n">
+        <v>8.17283119</v>
+      </c>
+      <c r="F67" t="n">
+        <v>11.65263361</v>
+      </c>
+      <c r="G67" t="n">
+        <v>121582396.3567789</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>6.368839998949808e-05</v>
+      </c>
+      <c r="E68" t="n">
+        <v>15.25778962</v>
+      </c>
+      <c r="F68" t="n">
+        <v>11.65925826</v>
+      </c>
+      <c r="G68" t="n">
+        <v>26793072.99158195</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.0002510389536923054</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-0.30468197</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-6.27508645</v>
+      </c>
+      <c r="G69" t="n">
+        <v>4864549.175876617</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>3.164908259989256e-07</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-1.20813637</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-4.57364175</v>
+      </c>
+      <c r="G70" t="n">
+        <v>280443.418175786</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.01478544228269673</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-6.08177164</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-11.23312056</v>
+      </c>
+      <c r="G71" t="n">
+        <v>1405350.877498449</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.0008005669461844754</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-0.08312374</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.16908524</v>
+      </c>
+      <c r="G72" t="n">
+        <v>782617.6068677446</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.005908695584661424</v>
+      </c>
+      <c r="E73" t="n">
+        <v>4.78688987</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-14.47229934</v>
+      </c>
+      <c r="G73" t="n">
+        <v>4116690.945492102</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.001669982390422543</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-1.12131877</v>
+      </c>
+      <c r="F74" t="n">
+        <v>3.76834499</v>
+      </c>
+      <c r="G74" t="n">
+        <v>1606918.007610079</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.009333791370312367</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-1.62086416</v>
+      </c>
+      <c r="F75" t="n">
+        <v>-7.38747183</v>
+      </c>
+      <c r="G75" t="n">
+        <v>8867104.163245965</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>2.656358951818236</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-2.30207796</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-0.57238089</v>
+      </c>
+      <c r="G76" t="n">
+        <v>20639909.0556277</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.0001817902052960551</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-2.31130197</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-4.51664315</v>
+      </c>
+      <c r="G77" t="n">
+        <v>116929.5379084692</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.001751161631468445</v>
+      </c>
+      <c r="E78" t="n">
+        <v>7.39964468</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-4.58659071</v>
+      </c>
+      <c r="G78" t="n">
+        <v>1641090.214944851</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>3.437123268932534e-08</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-3.65848572</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-2.35630013</v>
+      </c>
+      <c r="G79" t="n">
+        <v>26461085.23996131</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.0003345465578027703</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-1.36183101</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-8.22092752</v>
+      </c>
+      <c r="G80" t="n">
+        <v>167089.3090728769</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.01146226250435498</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-1.46377569</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-14.95611434</v>
+      </c>
+      <c r="G81" t="n">
+        <v>11346442.29066272</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>9.598662237281627e-05</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-0.20523386</v>
+      </c>
+      <c r="F82" t="n">
+        <v>-26.88158685</v>
+      </c>
+      <c r="G82" t="n">
+        <v>1007859.534914571</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>3.215202695029135e-05</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-5.55249161</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-9.746086679999999</v>
+      </c>
+      <c r="G83" t="n">
+        <v>73409649.94792597</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>1.081271465472599e-05</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.10741188</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-17.81827678</v>
+      </c>
+      <c r="G84" t="n">
+        <v>361831.5426249495</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.0002117436470511266</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.10399629</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-13.13306514</v>
+      </c>
+      <c r="G85" t="n">
+        <v>195313.6664021643</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.01658829756846764</v>
+      </c>
+      <c r="E86" t="n">
+        <v>2.76474232</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-8.13312108</v>
+      </c>
+      <c r="G86" t="n">
+        <v>15295154.67503906</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.0008172473643167118</v>
+      </c>
+      <c r="E87" t="n">
+        <v>1.95284595</v>
+      </c>
+      <c r="F87" t="n">
+        <v>-1.50842183</v>
+      </c>
+      <c r="G87" t="n">
+        <v>654815.140496166</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.004194940807870186</v>
+      </c>
+      <c r="E88" t="n">
+        <v>2.56044853</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-0.20749354</v>
+      </c>
+      <c r="G88" t="n">
+        <v>372883627.3625099</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.0005002977519767561</v>
+      </c>
+      <c r="E89" t="n">
+        <v>14.84248737</v>
+      </c>
+      <c r="F89" t="n">
+        <v>16.49837124</v>
+      </c>
+      <c r="G89" t="n">
+        <v>499757.5169561323</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.00292806259357018</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-1.24576009</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-3.03823221</v>
+      </c>
+      <c r="G90" t="n">
+        <v>41518782.3500555</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>1.290142717203994e-05</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-4.71681427</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-3.79218007</v>
+      </c>
+      <c r="G91" t="n">
+        <v>3225332.224082065</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.01393660239570502</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-12.32988749</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-14.62944131</v>
+      </c>
+      <c r="G92" t="n">
+        <v>129644015.8041357</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30011</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>SKID</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Success Kid</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.0227018088585945</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-5.64056008</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-15.77107284</v>
+      </c>
+      <c r="G93" t="n">
+        <v>1969216.149874787</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-20T13:27:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30008</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>APU</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Apu Apustaja</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.000242474847581794</v>
+      </c>
+      <c r="E94" t="n">
+        <v>4.99767269</v>
+      </c>
+      <c r="F94" t="n">
+        <v>27.6450939</v>
+      </c>
+      <c r="G94" t="n">
+        <v>77433496.66510083</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:03:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30007</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.006174465981086641</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-3.21692829</v>
+      </c>
+      <c r="F95" t="n">
+        <v>9.48465994</v>
+      </c>
+      <c r="G95" t="n">
+        <v>2360665.744966834</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:00:29.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>29999</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>CHKN</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Chickencoin</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>4.73342767200681e-08</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-0.12833356</v>
+      </c>
+      <c r="F96" t="n">
+        <v>-6.09919596</v>
+      </c>
+      <c r="G96" t="n">
+        <v>3040706.602220454</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-20T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>29932</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>BSHIB</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Based Shiba Inu</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>1.878662229735234e-05</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-5.27768967</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-1.09805893</v>
+      </c>
+      <c r="G97" t="n">
+        <v>169857.1997698493</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-19T05:05:42.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>29920</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>SLERF</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>SLERF</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.1554236085839686</v>
+      </c>
+      <c r="E98" t="n">
+        <v>3.13677652</v>
+      </c>
+      <c r="F98" t="n">
+        <v>18.11793386</v>
+      </c>
+      <c r="G98" t="n">
+        <v>77711454.58886498</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-18T09:28:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>29879</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>ANDY</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>ANDY (ETH)</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>6.097675191845948e-05</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-4.22686831</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0.98946746</v>
+      </c>
+      <c r="G99" t="n">
+        <v>60976751.91845948</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-15T05:18:29.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>29870</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>BOME</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>BOOK OF MEME</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.005937033750967241</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-0.3350107</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-5.06354778</v>
+      </c>
+      <c r="G100" t="n">
+        <v>409428312.94565</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-14T11:43:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>29855</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>PAJAMAS</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>The First Youtube Cat</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.004055611640748521</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-0.17369403</v>
+      </c>
+      <c r="F101" t="n">
+        <v>-8.101800150000001</v>
+      </c>
+      <c r="G101" t="n">
+        <v>3974154.911708389</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-14T08:28:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>59767.76</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>129.17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update portfolios at 2024-09-19 12:21:21
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Portfolio_2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Portfolio_3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Portfolio_4" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -7104,4 +7105,3285 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0241391120371036</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-23.27087417</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-22.72557505</v>
+      </c>
+      <c r="G2" t="n">
+        <v>24139112.0371036</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0002783230872006439</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-3.59393233</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-31.4600829</v>
+      </c>
+      <c r="G3" t="n">
+        <v>278323.0872006438</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.01609638672606264</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.78740814</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-27.56191352</v>
+      </c>
+      <c r="G4" t="n">
+        <v>16096386.72606264</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1.180061577527536e-06</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.88879944</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-20.9728054</v>
+      </c>
+      <c r="G5" t="n">
+        <v>767985.0574892664</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0009860145402632403</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4.9897974</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-5.34632004</v>
+      </c>
+      <c r="G6" t="n">
+        <v>509523013.6810294</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0003335509276341079</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-0.05174011</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.49988214</v>
+      </c>
+      <c r="G7" t="n">
+        <v>333550.9276341079</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0158678882134565</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-6.00944007</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-33.48608529</v>
+      </c>
+      <c r="G8" t="n">
+        <v>14919288.49658637</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0002049917973226787</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-9.278839680000001</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-41.03631575</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2049917.973226787</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.004088459828744923</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-6.71703034</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-19.76514428</v>
+      </c>
+      <c r="G10" t="n">
+        <v>4003148.803391265</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.000713639694918847</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.74313843</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-37.51633551</v>
+      </c>
+      <c r="G11" t="n">
+        <v>713639.6949188471</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.006036341750167286</v>
+      </c>
+      <c r="E12" t="n">
+        <v>13.54742639</v>
+      </c>
+      <c r="F12" t="n">
+        <v>24.63506386</v>
+      </c>
+      <c r="G12" t="n">
+        <v>5734478.581226001</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3.434903879256661e-05</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1.22639929</v>
+      </c>
+      <c r="F13" t="n">
+        <v>6.89339398</v>
+      </c>
+      <c r="G13" t="n">
+        <v>231854477.4783059</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.3418227983932659</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4.9790284</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10.2146109</v>
+      </c>
+      <c r="G14" t="n">
+        <v>340960861.7848882</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>8.137082329876266e-05</v>
+      </c>
+      <c r="E15" t="n">
+        <v>17.05922921</v>
+      </c>
+      <c r="F15" t="n">
+        <v>46.1384787</v>
+      </c>
+      <c r="G15" t="n">
+        <v>8137082.329876266</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>2.989185352919025e-06</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-30.99412049</v>
+      </c>
+      <c r="F16" t="n">
+        <v>64.11646379</v>
+      </c>
+      <c r="G16" t="n">
+        <v>961978.9453763174</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.01782864688452978</v>
+      </c>
+      <c r="E17" t="n">
+        <v>21.32423263</v>
+      </c>
+      <c r="F17" t="n">
+        <v>23.76029236</v>
+      </c>
+      <c r="G17" t="n">
+        <v>17828619.05401199</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32598</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>GODCAT</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Godcat Exploding Kittens</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0001299239041049616</v>
+      </c>
+      <c r="E18" t="n">
+        <v>20.57613696</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-28.6773289</v>
+      </c>
+      <c r="G18" t="n">
+        <v>103540.0538273049</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-08T06:06:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>3.214998936265179e-06</v>
+      </c>
+      <c r="E19" t="n">
+        <v>15.19183506</v>
+      </c>
+      <c r="F19" t="n">
+        <v>4.09492513</v>
+      </c>
+      <c r="G19" t="n">
+        <v>22183487.39466911</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0008760707540191858</v>
+      </c>
+      <c r="E20" t="n">
+        <v>9.23108302</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1999.57523171</v>
+      </c>
+      <c r="G20" t="n">
+        <v>367645065.8291774</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>3.675110108932476e-05</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.79860683</v>
+      </c>
+      <c r="F21" t="n">
+        <v>5.54865131</v>
+      </c>
+      <c r="G21" t="n">
+        <v>235778.0496745786</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.001571187584333894</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-62.43537574</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-64.26789497</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1571187.535627079</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.001422620213766862</v>
+      </c>
+      <c r="E23" t="n">
+        <v>11.22238138</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-32.23565183</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1422617.654473098</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.1171945398858833</v>
+      </c>
+      <c r="E24" t="n">
+        <v>50.6157891</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-26.19951049</v>
+      </c>
+      <c r="G24" t="n">
+        <v>117194539.8858833</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0156615497314043</v>
+      </c>
+      <c r="E25" t="n">
+        <v>27.55909801</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-11.74824557</v>
+      </c>
+      <c r="G25" t="n">
+        <v>14923977.51970222</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.05751423221760855</v>
+      </c>
+      <c r="E26" t="n">
+        <v>6.5161123</v>
+      </c>
+      <c r="F26" t="n">
+        <v>19.05817879</v>
+      </c>
+      <c r="G26" t="n">
+        <v>4028220.445620918</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.0006378672499417592</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.41309999</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-29.24352295</v>
+      </c>
+      <c r="G27" t="n">
+        <v>591020.9963549968</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.000273814110251071</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-3.82372606</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2.09324261</v>
+      </c>
+      <c r="G28" t="n">
+        <v>182489.8177412368</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>1.779749221488207e-06</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-10.01678195</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-10.57975554</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1581993.794483359</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.003135846202659585</v>
+      </c>
+      <c r="E30" t="n">
+        <v>5.96076788</v>
+      </c>
+      <c r="F30" t="n">
+        <v>9.507925119999999</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2195091.316440001</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.0001371464431928025</v>
+      </c>
+      <c r="E31" t="n">
+        <v>5.06433709</v>
+      </c>
+      <c r="F31" t="n">
+        <v>15.74034556</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1371464.431928025</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2.3172188699378e-06</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-7.34028632</v>
+      </c>
+      <c r="F32" t="n">
+        <v>90.43652745999999</v>
+      </c>
+      <c r="G32" t="n">
+        <v>6822517.629582972</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.00063717427253484</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1.73275208</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-17.72474016</v>
+      </c>
+      <c r="G33" t="n">
+        <v>19115228.1760452</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0003187932259099712</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1.19293761</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-13.91943058</v>
+      </c>
+      <c r="G34" t="n">
+        <v>25676093.81201389</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.003273205961439895</v>
+      </c>
+      <c r="E35" t="n">
+        <v>10.95188005</v>
+      </c>
+      <c r="F35" t="n">
+        <v>12.06189873</v>
+      </c>
+      <c r="G35" t="n">
+        <v>3201972.283171487</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.001193788321492143</v>
+      </c>
+      <c r="E36" t="n">
+        <v>19.49270589</v>
+      </c>
+      <c r="F36" t="n">
+        <v>41.62486844</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1025129.475280361</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.04334360611278716</v>
+      </c>
+      <c r="E37" t="n">
+        <v>17.39281017</v>
+      </c>
+      <c r="F37" t="n">
+        <v>16.23960887</v>
+      </c>
+      <c r="G37" t="n">
+        <v>42289111.00572478</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.04730284073531683</v>
+      </c>
+      <c r="E38" t="n">
+        <v>43.72884022</v>
+      </c>
+      <c r="F38" t="n">
+        <v>72.26170140000001</v>
+      </c>
+      <c r="G38" t="n">
+        <v>44281970.49540365</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>9.694134580978432e-06</v>
+      </c>
+      <c r="E39" t="n">
+        <v>7.58488086</v>
+      </c>
+      <c r="F39" t="n">
+        <v>51.25808557</v>
+      </c>
+      <c r="G39" t="n">
+        <v>4055884.391700102</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.002080686304568462</v>
+      </c>
+      <c r="E40" t="n">
+        <v>27.26925119</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-10.66047724</v>
+      </c>
+      <c r="G40" t="n">
+        <v>20806532.18277593</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.07461611757771384</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1.72129984</v>
+      </c>
+      <c r="F41" t="n">
+        <v>3.62912313</v>
+      </c>
+      <c r="G41" t="n">
+        <v>44746414.86850342</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.000200086443040548</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-1.99674322</v>
+      </c>
+      <c r="F42" t="n">
+        <v>2.13712255</v>
+      </c>
+      <c r="G42" t="n">
+        <v>192997.9530110213</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>2.359681006941444e-09</v>
+      </c>
+      <c r="E43" t="n">
+        <v>30.64005779</v>
+      </c>
+      <c r="F43" t="n">
+        <v>67.40453347</v>
+      </c>
+      <c r="G43" t="n">
+        <v>946831.903621225</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.007057979196925839</v>
+      </c>
+      <c r="E44" t="n">
+        <v>7.53830882</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1.82735759</v>
+      </c>
+      <c r="G44" t="n">
+        <v>7057979.196925839</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>1.554736536915151e-07</v>
+      </c>
+      <c r="E45" t="n">
+        <v>42.54425349</v>
+      </c>
+      <c r="F45" t="n">
+        <v>37.34490962</v>
+      </c>
+      <c r="G45" t="n">
+        <v>63923978.98769967</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>2.020074304848472e-06</v>
+      </c>
+      <c r="E46" t="n">
+        <v>6.09703882</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-23.15601681</v>
+      </c>
+      <c r="G46" t="n">
+        <v>849825.0593067036</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.01207896430070073</v>
+      </c>
+      <c r="E47" t="n">
+        <v>1.41614543</v>
+      </c>
+      <c r="F47" t="n">
+        <v>3.78925552</v>
+      </c>
+      <c r="G47" t="n">
+        <v>799131.7643273451</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.05936529284781026</v>
+      </c>
+      <c r="E48" t="n">
+        <v>19.32638984</v>
+      </c>
+      <c r="F48" t="n">
+        <v>43.69140905</v>
+      </c>
+      <c r="G48" t="n">
+        <v>58542677.14547649</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>8.563409795821157e-09</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-4.57190451</v>
+      </c>
+      <c r="F49" t="n">
+        <v>19.53390698</v>
+      </c>
+      <c r="G49" t="n">
+        <v>271505.6065702325</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.008662274041594874</v>
+      </c>
+      <c r="E50" t="n">
+        <v>15.44136204</v>
+      </c>
+      <c r="F50" t="n">
+        <v>13.04612359</v>
+      </c>
+      <c r="G50" t="n">
+        <v>866227.4041594875</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>7.282069449636388e-05</v>
+      </c>
+      <c r="E51" t="n">
+        <v>2.27468431</v>
+      </c>
+      <c r="F51" t="n">
+        <v>11.02811341</v>
+      </c>
+      <c r="G51" t="n">
+        <v>28418923.82845293</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.01745658647708884</v>
+      </c>
+      <c r="E52" t="n">
+        <v>18.27229822</v>
+      </c>
+      <c r="F52" t="n">
+        <v>50.52180729</v>
+      </c>
+      <c r="G52" t="n">
+        <v>16442380.62350308</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.001148241288422507</v>
+      </c>
+      <c r="E53" t="n">
+        <v>10.09730268</v>
+      </c>
+      <c r="F53" t="n">
+        <v>52.77136526</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1148241.288422507</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.09602424098523926</v>
+      </c>
+      <c r="E54" t="n">
+        <v>8.984344760000001</v>
+      </c>
+      <c r="F54" t="n">
+        <v>9.43776853</v>
+      </c>
+      <c r="G54" t="n">
+        <v>19516040.19638438</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.00650062058672816</v>
+      </c>
+      <c r="E55" t="n">
+        <v>9.02348044</v>
+      </c>
+      <c r="F55" t="n">
+        <v>5.45018088</v>
+      </c>
+      <c r="G55" t="n">
+        <v>11019319.95582779</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>5.480750402608753e-05</v>
+      </c>
+      <c r="E56" t="n">
+        <v>8.84083459</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-3.37613914</v>
+      </c>
+      <c r="G56" t="n">
+        <v>51980979.49929757</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>2.145502343537914e-05</v>
+      </c>
+      <c r="E57" t="n">
+        <v>19.90259151</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-22.75789961</v>
+      </c>
+      <c r="G57" t="n">
+        <v>186112.9303365436</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.04119970752159186</v>
+      </c>
+      <c r="E58" t="n">
+        <v>19.31547381</v>
+      </c>
+      <c r="F58" t="n">
+        <v>17.88950854</v>
+      </c>
+      <c r="G58" t="n">
+        <v>3913972.214551226</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.0006155224010482291</v>
+      </c>
+      <c r="E59" t="n">
+        <v>9.54982083</v>
+      </c>
+      <c r="F59" t="n">
+        <v>3.56398673</v>
+      </c>
+      <c r="G59" t="n">
+        <v>10087046.70906211</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.01510897467443581</v>
+      </c>
+      <c r="E60" t="n">
+        <v>10.01000478</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-3.4075892</v>
+      </c>
+      <c r="G60" t="n">
+        <v>15106744.54248277</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.0003318648190070666</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-64.58675775</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-67.18569832999999</v>
+      </c>
+      <c r="G61" t="n">
+        <v>307616.0593487316</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Elon MemeLord</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>4.1348816422344e-06</v>
+      </c>
+      <c r="E62" t="n">
+        <v>4.66049769</v>
+      </c>
+      <c r="F62" t="n">
+        <v>1.14422838</v>
+      </c>
+      <c r="G62" t="n">
+        <v>2833302.696416724</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>1.128950834659707e-06</v>
+      </c>
+      <c r="E63" t="n">
+        <v>6.35328141</v>
+      </c>
+      <c r="F63" t="n">
+        <v>5.34038924</v>
+      </c>
+      <c r="G63" t="n">
+        <v>884774.3884172683</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.6955839585105761</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-0.23737926</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-0.4243808</v>
+      </c>
+      <c r="G64" t="n">
+        <v>60140937.50116377</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.1502941578821133</v>
+      </c>
+      <c r="E65" t="n">
+        <v>38.45844455</v>
+      </c>
+      <c r="F65" t="n">
+        <v>40.14160996</v>
+      </c>
+      <c r="G65" t="n">
+        <v>83528897.72583935</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.002575146288990027</v>
+      </c>
+      <c r="E66" t="n">
+        <v>14.59774044</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.10485938</v>
+      </c>
+      <c r="G66" t="n">
+        <v>257514628.8990027</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.005902100090956508</v>
+      </c>
+      <c r="E67" t="n">
+        <v>8.370738830000001</v>
+      </c>
+      <c r="F67" t="n">
+        <v>6.43318632</v>
+      </c>
+      <c r="G67" t="n">
+        <v>49712723.38006161</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>2.924057119772309e-07</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1.01001684</v>
+      </c>
+      <c r="F68" t="n">
+        <v>5.4612405</v>
+      </c>
+      <c r="G68" t="n">
+        <v>122810399.030437</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>6.829751031972718e-05</v>
+      </c>
+      <c r="E69" t="n">
+        <v>7.23696989</v>
+      </c>
+      <c r="F69" t="n">
+        <v>13.21828637</v>
+      </c>
+      <c r="G69" t="n">
+        <v>28732079.61640603</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.0002553201651228121</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1.70539726</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-7.63978224</v>
+      </c>
+      <c r="G70" t="n">
+        <v>4947509.06409202</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>3.280182616788801e-07</v>
+      </c>
+      <c r="E71" t="n">
+        <v>3.64226535</v>
+      </c>
+      <c r="F71" t="n">
+        <v>1.08107214</v>
+      </c>
+      <c r="G71" t="n">
+        <v>290657.9116123159</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.01456745690732093</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-1.47432435</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-12.9477123</v>
+      </c>
+      <c r="G72" t="n">
+        <v>1384631.447351627</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0008491758446030972</v>
+      </c>
+      <c r="E73" t="n">
+        <v>6.07180932</v>
+      </c>
+      <c r="F73" t="n">
+        <v>1.38715406</v>
+      </c>
+      <c r="G73" t="n">
+        <v>830136.6073234406</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.007257991845755354</v>
+      </c>
+      <c r="E74" t="n">
+        <v>22.83577216</v>
+      </c>
+      <c r="F74" t="n">
+        <v>2.12352422</v>
+      </c>
+      <c r="G74" t="n">
+        <v>5056769.043834147</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.00216441403450807</v>
+      </c>
+      <c r="E75" t="n">
+        <v>29.60699747</v>
+      </c>
+      <c r="F75" t="n">
+        <v>37.63014944</v>
+      </c>
+      <c r="G75" t="n">
+        <v>2082678.102189858</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.01210440619641099</v>
+      </c>
+      <c r="E76" t="n">
+        <v>29.68370211</v>
+      </c>
+      <c r="F76" t="n">
+        <v>3.75059545</v>
+      </c>
+      <c r="G76" t="n">
+        <v>11499188.94900521</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>2.743889048173041</v>
+      </c>
+      <c r="E77" t="n">
+        <v>3.29511553</v>
+      </c>
+      <c r="F77" t="n">
+        <v>1.53195725</v>
+      </c>
+      <c r="G77" t="n">
+        <v>21320017.90430453</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.0001889865636767937</v>
+      </c>
+      <c r="E78" t="n">
+        <v>3.95860622</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-3.6900911</v>
+      </c>
+      <c r="G78" t="n">
+        <v>121558.3178733365</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.001929881108416636</v>
+      </c>
+      <c r="E79" t="n">
+        <v>10.20576706</v>
+      </c>
+      <c r="F79" t="n">
+        <v>1.11589631</v>
+      </c>
+      <c r="G79" t="n">
+        <v>1808576.059523226</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>3.623904867988064e-08</v>
+      </c>
+      <c r="E80" t="n">
+        <v>5.43424208</v>
+      </c>
+      <c r="F80" t="n">
+        <v>3.43433397</v>
+      </c>
+      <c r="G80" t="n">
+        <v>27899044.66915561</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0003606646648320809</v>
+      </c>
+      <c r="E81" t="n">
+        <v>7.80701712</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-9.25413384</v>
+      </c>
+      <c r="G81" t="n">
+        <v>180134.000031532</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.01483855765273086</v>
+      </c>
+      <c r="E82" t="n">
+        <v>29.45574791</v>
+      </c>
+      <c r="F82" t="n">
+        <v>5.76077292</v>
+      </c>
+      <c r="G82" t="n">
+        <v>14688621.72886144</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>9.243936477260208e-05</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-3.69557498</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-13.07289624</v>
+      </c>
+      <c r="G83" t="n">
+        <v>970613.3301123219</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>4.093235032431671e-05</v>
+      </c>
+      <c r="E84" t="n">
+        <v>27.30877088</v>
+      </c>
+      <c r="F84" t="n">
+        <v>11.71930926</v>
+      </c>
+      <c r="G84" t="n">
+        <v>93456923.05805731</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>1.090022250402197e-05</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.80930508</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-10.02462384</v>
+      </c>
+      <c r="G85" t="n">
+        <v>364759.8636908083</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.0002325957161684661</v>
+      </c>
+      <c r="E86" t="n">
+        <v>9.84778972</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-5.49769387</v>
+      </c>
+      <c r="G86" t="n">
+        <v>214547.7455733592</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.02389648183167215</v>
+      </c>
+      <c r="E87" t="n">
+        <v>44.05626456</v>
+      </c>
+      <c r="F87" t="n">
+        <v>35.07284556</v>
+      </c>
+      <c r="G87" t="n">
+        <v>22033628.48394151</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.0008743990844675139</v>
+      </c>
+      <c r="E88" t="n">
+        <v>6.99319724</v>
+      </c>
+      <c r="F88" t="n">
+        <v>5.83152577</v>
+      </c>
+      <c r="G88" t="n">
+        <v>700607.654848824</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.005253280369079436</v>
+      </c>
+      <c r="E89" t="n">
+        <v>25.22895101</v>
+      </c>
+      <c r="F89" t="n">
+        <v>22.7770202</v>
+      </c>
+      <c r="G89" t="n">
+        <v>466958255.0246136</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.0004876129565878597</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-2.53544921</v>
+      </c>
+      <c r="F90" t="n">
+        <v>14.00424985</v>
+      </c>
+      <c r="G90" t="n">
+        <v>487086.4189517863</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.003408398757243598</v>
+      </c>
+      <c r="E91" t="n">
+        <v>16.40457293</v>
+      </c>
+      <c r="F91" t="n">
+        <v>6.8634605</v>
+      </c>
+      <c r="G91" t="n">
+        <v>48329761.28138389</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>1.447985479246109e-05</v>
+      </c>
+      <c r="E92" t="n">
+        <v>12.23451948</v>
+      </c>
+      <c r="F92" t="n">
+        <v>5.6180579</v>
+      </c>
+      <c r="G92" t="n">
+        <v>3619936.123297079</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.01771227971477517</v>
+      </c>
+      <c r="E93" t="n">
+        <v>27.09180625</v>
+      </c>
+      <c r="F93" t="n">
+        <v>1.92336177</v>
+      </c>
+      <c r="G93" t="n">
+        <v>164766921.3823058</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30011</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>SKID</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Success Kid</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.02596139059662225</v>
+      </c>
+      <c r="E94" t="n">
+        <v>14.35824677</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-6.41956587</v>
+      </c>
+      <c r="G94" t="n">
+        <v>2251961.064182844</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-20T13:27:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30008</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>APU</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Apu Apustaja</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.0003084552023387137</v>
+      </c>
+      <c r="E95" t="n">
+        <v>27.2112161</v>
+      </c>
+      <c r="F95" t="n">
+        <v>44.84614766</v>
+      </c>
+      <c r="G95" t="n">
+        <v>98504092.77428558</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:03:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30007</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.006879597790596105</v>
+      </c>
+      <c r="E96" t="n">
+        <v>11.42012624</v>
+      </c>
+      <c r="F96" t="n">
+        <v>18.14338417</v>
+      </c>
+      <c r="G96" t="n">
+        <v>2630256.753079008</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:00:29.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>29999</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>CHKN</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Chickencoin</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>5.097163193229697e-08</v>
+      </c>
+      <c r="E97" t="n">
+        <v>7.68440011</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0.51472373</v>
+      </c>
+      <c r="G97" t="n">
+        <v>3274366.663698825</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-20T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>29932</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>BSHIB</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Based Shiba Inu</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>2.129536355696072e-05</v>
+      </c>
+      <c r="E98" t="n">
+        <v>13.35387075</v>
+      </c>
+      <c r="F98" t="n">
+        <v>12.16387898</v>
+      </c>
+      <c r="G98" t="n">
+        <v>192539.7106842365</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-19T05:05:42.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>29920</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>SLERF</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>SLERF</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.1617622623830797</v>
+      </c>
+      <c r="E99" t="n">
+        <v>4.07830822</v>
+      </c>
+      <c r="F99" t="n">
+        <v>20.31290241</v>
+      </c>
+      <c r="G99" t="n">
+        <v>80880767.22644947</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-18T09:28:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>29879</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>ANDY</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>ANDY (ETH)</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>8.606207090208068e-05</v>
+      </c>
+      <c r="E100" t="n">
+        <v>41.13915254</v>
+      </c>
+      <c r="F100" t="n">
+        <v>24.49197716</v>
+      </c>
+      <c r="G100" t="n">
+        <v>86062070.90208068</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-15T05:18:29.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>29870</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>BOME</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>BOOK OF MEME</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.00673537809436876</v>
+      </c>
+      <c r="E101" t="n">
+        <v>13.4468554</v>
+      </c>
+      <c r="F101" t="n">
+        <v>7.62123291</v>
+      </c>
+      <c r="G101" t="n">
+        <v>464483545.8444197</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-14T11:43:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>63102.5</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>140.71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update portfolios at 2024-09-20 12:21:09
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Portfolio_2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Portfolio_3" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Portfolio_4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Portfolio_5" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -10386,4 +10387,3285 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.02304325516994139</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-4.53975633</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-1.70297816</v>
+      </c>
+      <c r="G2" t="n">
+        <v>23043255.16994138</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.000462145265149915</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-9.64750402</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-1.59325453</v>
+      </c>
+      <c r="G3" t="n">
+        <v>439038.0018924192</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0002247835474751389</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-19.23647092</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-32.28475324</v>
+      </c>
+      <c r="G4" t="n">
+        <v>224783.5474751389</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.01438792841277052</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-10.61392437</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-38.89236066</v>
+      </c>
+      <c r="G5" t="n">
+        <v>14387928.41277052</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1.095639226642465e-06</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-7.15406319</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-23.26595066</v>
+      </c>
+      <c r="G6" t="n">
+        <v>713042.9212206717</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0009390555224644326</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-4.76250764</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-7.04406952</v>
+      </c>
+      <c r="G7" t="n">
+        <v>485256941.2334955</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0003043485623855309</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-8.754994460000001</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-1.73948718</v>
+      </c>
+      <c r="G8" t="n">
+        <v>304348.5623855309</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4.633273774776166e-07</v>
+      </c>
+      <c r="E9" t="n">
+        <v>115.40645656</v>
+      </c>
+      <c r="F9" t="n">
+        <v>143.08095373</v>
+      </c>
+      <c r="G9" t="n">
+        <v>191018.7004266837</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.008040861961192546</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-49.32619985</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-60.19453752</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7560170.43644947</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0002154185579310101</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5.08642821</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-27.09689215</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2154185.579310101</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.009157953014373664</v>
+      </c>
+      <c r="E12" t="n">
+        <v>123.99518151</v>
+      </c>
+      <c r="F12" t="n">
+        <v>21.14191144</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8966860.428284423</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0006353014073688536</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-10.97728841</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-37.523209</v>
+      </c>
+      <c r="G13" t="n">
+        <v>635301.4073688536</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0049339039006555</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-18.26334385</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-21.27546991</v>
+      </c>
+      <c r="G14" t="n">
+        <v>4687171.040200347</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>3.852502652009814e-05</v>
+      </c>
+      <c r="E15" t="n">
+        <v>12.15750971</v>
+      </c>
+      <c r="F15" t="n">
+        <v>16.73407116</v>
+      </c>
+      <c r="G15" t="n">
+        <v>260042207.9534247</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.3242089357951974</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-5.15292212</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-5.41534099</v>
+      </c>
+      <c r="G16" t="n">
+        <v>323390559.1700308</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>6.960512622784461e-05</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-14.45935606</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-20.54404549</v>
+      </c>
+      <c r="G17" t="n">
+        <v>6960512.622784461</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>3.002310311020473e-06</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.43908144</v>
+      </c>
+      <c r="F18" t="n">
+        <v>61.07367548</v>
+      </c>
+      <c r="G18" t="n">
+        <v>966202.8163852561</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.01734033244607828</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-2.73893157</v>
+      </c>
+      <c r="F19" t="n">
+        <v>39.35965748</v>
+      </c>
+      <c r="G19" t="n">
+        <v>17340305.37781933</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32598</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>GODCAT</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Godcat Exploding Kittens</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0001418477246623067</v>
+      </c>
+      <c r="E20" t="n">
+        <v>9.17754176</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-11.57090859</v>
+      </c>
+      <c r="G20" t="n">
+        <v>113042.4855071385</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-08T06:06:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>3.222633064716399e-06</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.23745353</v>
+      </c>
+      <c r="F21" t="n">
+        <v>22.57973823</v>
+      </c>
+      <c r="G21" t="n">
+        <v>22236162.86847927</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.000809907279833917</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-7.55229802</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2145.94887928</v>
+      </c>
+      <c r="G22" t="n">
+        <v>340033746.3179542</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>3.787048342682832e-05</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.04584707</v>
+      </c>
+      <c r="F23" t="n">
+        <v>13.87764816</v>
+      </c>
+      <c r="G23" t="n">
+        <v>242959.488503725</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0009067254701288322</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-42.29043819</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-75.68860131</v>
+      </c>
+      <c r="G24" t="n">
+        <v>906725.4420203426</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.001373999020388382</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-3.41772125</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-27.3105195</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1373996.548564145</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.09101881479794886</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-22.33527698</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-44.50924456</v>
+      </c>
+      <c r="G26" t="n">
+        <v>91018814.79794887</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.01663157973680262</v>
+      </c>
+      <c r="E27" t="n">
+        <v>6.19370383</v>
+      </c>
+      <c r="F27" t="n">
+        <v>8.834481520000001</v>
+      </c>
+      <c r="G27" t="n">
+        <v>15848324.48678254</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.07039103789552188</v>
+      </c>
+      <c r="E28" t="n">
+        <v>22.38890303</v>
+      </c>
+      <c r="F28" t="n">
+        <v>33.81790785</v>
+      </c>
+      <c r="G28" t="n">
+        <v>4930094.814904028</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.0006231126355762082</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-2.31311678</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1.93884198</v>
+      </c>
+      <c r="G29" t="n">
+        <v>577349.9905399813</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0004896141825383644</v>
+      </c>
+      <c r="E30" t="n">
+        <v>78.81261929</v>
+      </c>
+      <c r="F30" t="n">
+        <v>79.57322083</v>
+      </c>
+      <c r="G30" t="n">
+        <v>326314.8230491942</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>1.790741656207389e-06</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.61763953</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-32.73559114</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1591764.813513483</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.002820334660168499</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-10.06144824</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-5.56143306</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1974233.339868515</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.0001441829352451213</v>
+      </c>
+      <c r="E33" t="n">
+        <v>5.1306413</v>
+      </c>
+      <c r="F33" t="n">
+        <v>10.41836122</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1441829.352451213</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>2.442612572374239e-06</v>
+      </c>
+      <c r="E34" t="n">
+        <v>5.41138794</v>
+      </c>
+      <c r="F34" t="n">
+        <v>102.87141353</v>
+      </c>
+      <c r="G34" t="n">
+        <v>7191710.525692197</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.0006807544013230981</v>
+      </c>
+      <c r="E35" t="n">
+        <v>6.83959329</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-4.40472844</v>
+      </c>
+      <c r="G35" t="n">
+        <v>20422632.03969294</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0003259388155485371</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.24144965</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-5.25733703</v>
+      </c>
+      <c r="G36" t="n">
+        <v>26251610.52626737</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.003987522758165427</v>
+      </c>
+      <c r="E37" t="n">
+        <v>21.82315458</v>
+      </c>
+      <c r="F37" t="n">
+        <v>23.92320101</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3900743.644174643</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.001158857961840435</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-2.9260095</v>
+      </c>
+      <c r="F38" t="n">
+        <v>5.86821289</v>
+      </c>
+      <c r="G38" t="n">
+        <v>995134.0894850361</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.05339273221153498</v>
+      </c>
+      <c r="E39" t="n">
+        <v>23.18479471</v>
+      </c>
+      <c r="F39" t="n">
+        <v>32.95548958</v>
+      </c>
+      <c r="G39" t="n">
+        <v>52093754.57863458</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.05327875107522625</v>
+      </c>
+      <c r="E40" t="n">
+        <v>12.63330119</v>
+      </c>
+      <c r="F40" t="n">
+        <v>135.18535426</v>
+      </c>
+      <c r="G40" t="n">
+        <v>49876245.19944853</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>1.185385148897545e-05</v>
+      </c>
+      <c r="E41" t="n">
+        <v>22.27859424</v>
+      </c>
+      <c r="F41" t="n">
+        <v>80.0156544</v>
+      </c>
+      <c r="G41" t="n">
+        <v>4959478.41801202</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.001863183199512939</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-10.4534309</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-9.14231635</v>
+      </c>
+      <c r="G42" t="n">
+        <v>18631535.56972941</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.07263382704536162</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-2.65665194</v>
+      </c>
+      <c r="F43" t="n">
+        <v>3.4276155</v>
+      </c>
+      <c r="G43" t="n">
+        <v>43557658.37151527</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.0002172370521313247</v>
+      </c>
+      <c r="E44" t="n">
+        <v>8.571599770000001</v>
+      </c>
+      <c r="F44" t="n">
+        <v>6.16169684</v>
+      </c>
+      <c r="G44" t="n">
+        <v>209540.9651067551</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>2.780341373889653e-09</v>
+      </c>
+      <c r="E45" t="n">
+        <v>17.82700143</v>
+      </c>
+      <c r="F45" t="n">
+        <v>38.3019841</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1115623.640658527</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.006355734786776583</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-9.949652589999999</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-13.9334407</v>
+      </c>
+      <c r="G46" t="n">
+        <v>6355734.786776583</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1.700676459306408e-07</v>
+      </c>
+      <c r="E47" t="n">
+        <v>9.38679441</v>
+      </c>
+      <c r="F47" t="n">
+        <v>53.46296755</v>
+      </c>
+      <c r="G47" t="n">
+        <v>69924391.47618188</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>2.33913809804783e-06</v>
+      </c>
+      <c r="E48" t="n">
+        <v>15.79465629</v>
+      </c>
+      <c r="F48" t="n">
+        <v>6.98175924</v>
+      </c>
+      <c r="G48" t="n">
+        <v>984052.0064677418</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.01194696532041746</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-1.09280048</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1.34196218</v>
+      </c>
+      <c r="G49" t="n">
+        <v>790398.8485427474</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.07391994766574227</v>
+      </c>
+      <c r="E50" t="n">
+        <v>24.51711113</v>
+      </c>
+      <c r="F50" t="n">
+        <v>76.80152339</v>
+      </c>
+      <c r="G50" t="n">
+        <v>72895650.3575252</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>8.891157061818678e-09</v>
+      </c>
+      <c r="E51" t="n">
+        <v>3.82729863</v>
+      </c>
+      <c r="F51" t="n">
+        <v>15.37389585</v>
+      </c>
+      <c r="G51" t="n">
+        <v>281896.9369372337</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.009900574474823499</v>
+      </c>
+      <c r="E52" t="n">
+        <v>14.29532738</v>
+      </c>
+      <c r="F52" t="n">
+        <v>31.57120659</v>
+      </c>
+      <c r="G52" t="n">
+        <v>990057.4474823499</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>7.054690956282356e-05</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-3.12244335</v>
+      </c>
+      <c r="F53" t="n">
+        <v>17.01101066</v>
+      </c>
+      <c r="G53" t="n">
+        <v>27531559.03091186</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.01636905373053268</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-6.22992787</v>
+      </c>
+      <c r="F54" t="n">
+        <v>28.90295165</v>
+      </c>
+      <c r="G54" t="n">
+        <v>15418032.1701059</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.00111783314155919</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-2.64823667</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-9.815117069999999</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1117833.14155919</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.09650175096795484</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.49728066</v>
+      </c>
+      <c r="F56" t="n">
+        <v>7.41935096</v>
+      </c>
+      <c r="G56" t="n">
+        <v>19613089.69056663</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.007292654563735125</v>
+      </c>
+      <c r="E57" t="n">
+        <v>12.04702908</v>
+      </c>
+      <c r="F57" t="n">
+        <v>21.36130834</v>
+      </c>
+      <c r="G57" t="n">
+        <v>12361911.12725305</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>5.697055529298894e-05</v>
+      </c>
+      <c r="E58" t="n">
+        <v>3.94663341</v>
+      </c>
+      <c r="F58" t="n">
+        <v>-0.63790634</v>
+      </c>
+      <c r="G58" t="n">
+        <v>54032478.20478895</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>1.630203938856424e-05</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-24.0176109</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-34.73855016</v>
+      </c>
+      <c r="G59" t="n">
+        <v>141413.0508971794</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.03767923195757433</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-8.544904259999999</v>
+      </c>
+      <c r="F60" t="n">
+        <v>7.30729699</v>
+      </c>
+      <c r="G60" t="n">
+        <v>3579527.035969561</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.0005058478483371282</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-17.81812531</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-10.96569169</v>
+      </c>
+      <c r="G61" t="n">
+        <v>8289724.086671173</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.01503642394769866</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-0.48018299</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.21906037</v>
+      </c>
+      <c r="G62" t="n">
+        <v>15034204.52445997</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.0004780174714627627</v>
+      </c>
+      <c r="E63" t="n">
+        <v>44.03981503</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-56.96305393</v>
+      </c>
+      <c r="G63" t="n">
+        <v>443089.6029027068</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Elon MemeLord</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>5.112783909148222e-06</v>
+      </c>
+      <c r="E64" t="n">
+        <v>23.65006671</v>
+      </c>
+      <c r="F64" t="n">
+        <v>25.83151321</v>
+      </c>
+      <c r="G64" t="n">
+        <v>3503380.674315441</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>1.176222933514288e-06</v>
+      </c>
+      <c r="E65" t="n">
+        <v>4.1872593</v>
+      </c>
+      <c r="F65" t="n">
+        <v>9.925683660000001</v>
+      </c>
+      <c r="G65" t="n">
+        <v>921822.1863099638</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.530492561123675</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-23.73421574</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-24.07702818</v>
+      </c>
+      <c r="G66" t="n">
+        <v>45866957.64474871</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.1528997168649368</v>
+      </c>
+      <c r="E67" t="n">
+        <v>1.73363956</v>
+      </c>
+      <c r="F67" t="n">
+        <v>46.55088937</v>
+      </c>
+      <c r="G67" t="n">
+        <v>84976987.7094156</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.00246912632449801</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-4.11704628</v>
+      </c>
+      <c r="F68" t="n">
+        <v>4.12509061</v>
+      </c>
+      <c r="G68" t="n">
+        <v>246912632.449801</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.0061748323632294</v>
+      </c>
+      <c r="E69" t="n">
+        <v>4.62093607</v>
+      </c>
+      <c r="F69" t="n">
+        <v>11.82546051</v>
+      </c>
+      <c r="G69" t="n">
+        <v>52009916.54848865</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>2.61846337365052e-07</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-10.45101835</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-1.0488875</v>
+      </c>
+      <c r="G70" t="n">
+        <v>109975461.6933219</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>7.368239535206992e-05</v>
+      </c>
+      <c r="E71" t="n">
+        <v>7.8844529</v>
+      </c>
+      <c r="F71" t="n">
+        <v>20.33684795</v>
+      </c>
+      <c r="G71" t="n">
+        <v>30997446.9006623</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.0002710289019194041</v>
+      </c>
+      <c r="E72" t="n">
+        <v>6.15256409</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-2.3382283</v>
+      </c>
+      <c r="G72" t="n">
+        <v>5251907.730171491</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>3.519742317871451e-07</v>
+      </c>
+      <c r="E73" t="n">
+        <v>7.30324281</v>
+      </c>
+      <c r="F73" t="n">
+        <v>8.36807333</v>
+      </c>
+      <c r="G73" t="n">
+        <v>311885.3646409278</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.01519915638611245</v>
+      </c>
+      <c r="E74" t="n">
+        <v>4.33637445</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-1.2654753</v>
+      </c>
+      <c r="G74" t="n">
+        <v>1444674.251608751</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.0008841036034664271</v>
+      </c>
+      <c r="E75" t="n">
+        <v>4.11313618</v>
+      </c>
+      <c r="F75" t="n">
+        <v>8.24125083</v>
+      </c>
+      <c r="G75" t="n">
+        <v>864281.2151292393</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.00791173700568519</v>
+      </c>
+      <c r="E76" t="n">
+        <v>9.00724572</v>
+      </c>
+      <c r="F76" t="n">
+        <v>22.81676648</v>
+      </c>
+      <c r="G76" t="n">
+        <v>5512244.645928015</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.002456957653429036</v>
+      </c>
+      <c r="E77" t="n">
+        <v>13.51606552</v>
+      </c>
+      <c r="F77" t="n">
+        <v>71.84362689</v>
+      </c>
+      <c r="G77" t="n">
+        <v>2364174.177875817</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.01261457444141295</v>
+      </c>
+      <c r="E78" t="n">
+        <v>4.2147317</v>
+      </c>
+      <c r="F78" t="n">
+        <v>19.98352247</v>
+      </c>
+      <c r="G78" t="n">
+        <v>11983848.91082964</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>3.064277239681981</v>
+      </c>
+      <c r="E79" t="n">
+        <v>11.67642663</v>
+      </c>
+      <c r="F79" t="n">
+        <v>13.17300291</v>
+      </c>
+      <c r="G79" t="n">
+        <v>23809434.15232899</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.0001953501632120366</v>
+      </c>
+      <c r="E80" t="n">
+        <v>3.36722326</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.41871703</v>
+      </c>
+      <c r="G80" t="n">
+        <v>125651.4578303474</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.002041477411190705</v>
+      </c>
+      <c r="E81" t="n">
+        <v>5.78254807</v>
+      </c>
+      <c r="F81" t="n">
+        <v>16.21702756</v>
+      </c>
+      <c r="G81" t="n">
+        <v>1913157.839534575</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>3.799197489924472e-08</v>
+      </c>
+      <c r="E82" t="n">
+        <v>4.83711986</v>
+      </c>
+      <c r="F82" t="n">
+        <v>1.41084197</v>
+      </c>
+      <c r="G82" t="n">
+        <v>29248554.89851557</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.0003594333347111273</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-0.34140581</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-7.78825259</v>
+      </c>
+      <c r="G83" t="n">
+        <v>179519.0120893393</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.01853841997983431</v>
+      </c>
+      <c r="E84" t="n">
+        <v>24.93411027</v>
+      </c>
+      <c r="F84" t="n">
+        <v>51.59420538</v>
+      </c>
+      <c r="G84" t="n">
+        <v>18351098.86737806</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>9.606010693079896e-05</v>
+      </c>
+      <c r="E85" t="n">
+        <v>3.91688343</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-0.9361137899999999</v>
+      </c>
+      <c r="G85" t="n">
+        <v>1008631.122773389</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>4.101828100018722e-05</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.2099334</v>
+      </c>
+      <c r="F86" t="n">
+        <v>12.01080255</v>
+      </c>
+      <c r="G86" t="n">
+        <v>93653120.35675935</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>1.093555330088236e-05</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.32412913</v>
+      </c>
+      <c r="F87" t="n">
+        <v>8.00442872</v>
+      </c>
+      <c r="G87" t="n">
+        <v>365942.1566799768</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.000225756043313248</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-2.94058419</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-8.031191209999999</v>
+      </c>
+      <c r="G88" t="n">
+        <v>208238.7884879953</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.02303011739094655</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-3.6254895</v>
+      </c>
+      <c r="F89" t="n">
+        <v>35.03246054</v>
+      </c>
+      <c r="G89" t="n">
+        <v>21234801.59582005</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.0008830695211790717</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.99158804</v>
+      </c>
+      <c r="F90" t="n">
+        <v>2.10753784</v>
+      </c>
+      <c r="G90" t="n">
+        <v>707554.7965360765</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.005516894430706665</v>
+      </c>
+      <c r="E91" t="n">
+        <v>5.01808476</v>
+      </c>
+      <c r="F91" t="n">
+        <v>31.27536805</v>
+      </c>
+      <c r="G91" t="n">
+        <v>490390616.0579108</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.0004416830538572118</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-9.41933599</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-3.25929403</v>
+      </c>
+      <c r="G92" t="n">
+        <v>441206.1125702144</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.005045370150124975</v>
+      </c>
+      <c r="E93" t="n">
+        <v>48.02757862</v>
+      </c>
+      <c r="F93" t="n">
+        <v>61.30908704</v>
+      </c>
+      <c r="G93" t="n">
+        <v>71541375.37855366</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>1.512286870460443e-05</v>
+      </c>
+      <c r="E94" t="n">
+        <v>4.44074835</v>
+      </c>
+      <c r="F94" t="n">
+        <v>11.93517548</v>
+      </c>
+      <c r="G94" t="n">
+        <v>3780688.367056252</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.02326732956908757</v>
+      </c>
+      <c r="E95" t="n">
+        <v>31.36270398</v>
+      </c>
+      <c r="F95" t="n">
+        <v>31.00450108</v>
+      </c>
+      <c r="G95" t="n">
+        <v>216442283.1854941</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30011</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>SKID</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Success Kid</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.02674273188743071</v>
+      </c>
+      <c r="E96" t="n">
+        <v>3.00962804</v>
+      </c>
+      <c r="F96" t="n">
+        <v>5.79362987</v>
+      </c>
+      <c r="G96" t="n">
+        <v>2319736.715806372</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-20T13:27:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30008</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>APU</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Apu Apustaja</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.0002788148564047882</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-9.60928709</v>
+      </c>
+      <c r="F97" t="n">
+        <v>22.49284799</v>
+      </c>
+      <c r="G97" t="n">
+        <v>89038551.70511207</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:03:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30007</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.007347608093979947</v>
+      </c>
+      <c r="E98" t="n">
+        <v>6.80287304</v>
+      </c>
+      <c r="F98" t="n">
+        <v>22.75534156</v>
+      </c>
+      <c r="G98" t="n">
+        <v>2809189.777305937</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:00:29.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>29999</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>CHKN</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Chickencoin</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>5.454068454438208e-08</v>
+      </c>
+      <c r="E99" t="n">
+        <v>7.00203717</v>
+      </c>
+      <c r="F99" t="n">
+        <v>7.31422592</v>
+      </c>
+      <c r="G99" t="n">
+        <v>3503639.034446561</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-20T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>29932</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>BSHIB</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Based Shiba Inu</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>2.530972156885919e-05</v>
+      </c>
+      <c r="E100" t="n">
+        <v>18.85085456</v>
+      </c>
+      <c r="F100" t="n">
+        <v>33.24248093</v>
+      </c>
+      <c r="G100" t="n">
+        <v>228835.0915133296</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-19T05:05:42.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>29920</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>SLERF</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>SLERF</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.1646572547476717</v>
+      </c>
+      <c r="E101" t="n">
+        <v>1.78965868</v>
+      </c>
+      <c r="F101" t="n">
+        <v>23.65413625</v>
+      </c>
+      <c r="G101" t="n">
+        <v>82328256.89501268</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-18T09:28:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>63382.31</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>150.58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update portfolios at 2024-09-21 12:19:09
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Portfolio_3" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Portfolio_4" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Portfolio_5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Portfolio_6" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -13668,4 +13669,3285 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0192379007892039</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-17.05704906</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-51.86134438</v>
+      </c>
+      <c r="G2" t="n">
+        <v>19237900.7892039</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0004361743791909329</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-5.62150555</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-24.83146136</v>
+      </c>
+      <c r="G3" t="n">
+        <v>414365.6602313863</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0002200006703761514</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.9953278</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-38.93141712</v>
+      </c>
+      <c r="G4" t="n">
+        <v>220000.6703761514</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.01433121041248653</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1.20709886</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-29.4857379</v>
+      </c>
+      <c r="G5" t="n">
+        <v>14331210.41248653</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>7.282888716064195e-07</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-33.5284048</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-42.86981998</v>
+      </c>
+      <c r="G6" t="n">
+        <v>473971.0042092255</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0009174531789761831</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-2.34961905</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-16.13204981</v>
+      </c>
+      <c r="G7" t="n">
+        <v>474093930.2359426</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0003026741105618699</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-0.5501757</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.21331525</v>
+      </c>
+      <c r="G8" t="n">
+        <v>302674.1105618699</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>8.776180097377979e-07</v>
+      </c>
+      <c r="E9" t="n">
+        <v>90.43450011</v>
+      </c>
+      <c r="F9" t="n">
+        <v>341.46597187</v>
+      </c>
+      <c r="G9" t="n">
+        <v>361820.7337624152</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.006906709711732932</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-13.94771437</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-64.58674212</v>
+      </c>
+      <c r="G10" t="n">
+        <v>6493819.049225112</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0002152914813778749</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.13906295</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-12.16838387</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2152914.813778749</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01155064588959555</v>
+      </c>
+      <c r="E12" t="n">
+        <v>27.77283603</v>
+      </c>
+      <c r="F12" t="n">
+        <v>124.49913512</v>
+      </c>
+      <c r="G12" t="n">
+        <v>11309626.65848795</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0005380745762864847</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-15.74111658</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-39.07219078</v>
+      </c>
+      <c r="G13" t="n">
+        <v>538074.5762864847</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.005107192759242177</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.5204413</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-14.3111087</v>
+      </c>
+      <c r="G14" t="n">
+        <v>4851794.132970544</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>4.448744678682581e-05</v>
+      </c>
+      <c r="E15" t="n">
+        <v>15.4249384</v>
+      </c>
+      <c r="F15" t="n">
+        <v>33.43554369</v>
+      </c>
+      <c r="G15" t="n">
+        <v>300288278.2057566</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.3123541868761538</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-3.66147697</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-8.765895159999999</v>
+      </c>
+      <c r="G16" t="n">
+        <v>311565734.3164321</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>6.453281817970793e-05</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-8.000904329999999</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-22.11666711</v>
+      </c>
+      <c r="G17" t="n">
+        <v>6453281.817970793</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>3.392935538607122e-06</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8.992548790000001</v>
+      </c>
+      <c r="F18" t="n">
+        <v>92.95803191</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1091913.737624796</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.01656059286239183</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-4.10962104</v>
+      </c>
+      <c r="F19" t="n">
+        <v>12.55199864</v>
+      </c>
+      <c r="G19" t="n">
+        <v>16560567.01130637</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32598</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>GODCAT</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Godcat Exploding Kittens</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0001444103492442733</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1.80660253</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-18.9103329</v>
+      </c>
+      <c r="G20" t="n">
+        <v>115084.7139098629</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-08T06:06:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32590</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>DOGY</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Dogy</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1.553447880747774e-07</v>
+      </c>
+      <c r="E21" t="n">
+        <v>34.51662645</v>
+      </c>
+      <c r="F21" t="n">
+        <v>29.92397364</v>
+      </c>
+      <c r="G21" t="n">
+        <v>135130.4370075849</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-07T17:46:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>2.899605688021775e-06</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-10.06344009</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-11.27580869</v>
+      </c>
+      <c r="G22" t="n">
+        <v>20007274.49834415</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0008328635712761528</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2.34283601</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1879.35263458</v>
+      </c>
+      <c r="G23" t="n">
+        <v>349740953.5587537</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>3.629071007607161e-05</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-4.12824193</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-2.80239878</v>
+      </c>
+      <c r="G24" t="n">
+        <v>232824.3940839966</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0009720446583353661</v>
+      </c>
+      <c r="E25" t="n">
+        <v>7.14716655</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-73.89411833</v>
+      </c>
+      <c r="G25" t="n">
+        <v>972044.6282019817</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.001382048342414984</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.56825956</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-27.99319652</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1382045.856110017</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.0865596006093667</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-4.62436273</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-47.95337605</v>
+      </c>
+      <c r="G27" t="n">
+        <v>86559600.6093667</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.01497281131298598</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-10.23374783</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-12.8073303</v>
+      </c>
+      <c r="G28" t="n">
+        <v>14267674.86449182</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.06384730333127277</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-9.350229369999999</v>
+      </c>
+      <c r="F29" t="n">
+        <v>22.92802024</v>
+      </c>
+      <c r="G29" t="n">
+        <v>4471780.33610352</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0005805826810638863</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-6.85566282</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-27.33813777</v>
+      </c>
+      <c r="G30" t="n">
+        <v>537943.5214147829</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.0004735818491482392</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-3.27448304</v>
+      </c>
+      <c r="F31" t="n">
+        <v>33.73179025</v>
+      </c>
+      <c r="G31" t="n">
+        <v>315629.6994971319</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>1.620732579759568e-06</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-9.976767710000001</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-30.78446566</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1440646.161063536</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.002780162268443897</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-1.44276352</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-10.35676369</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1946112.678797666</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0001450533707025335</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.60366308</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-3.75718834</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1450533.707025335</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>2.309771238009569e-06</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-5.08221611</v>
+      </c>
+      <c r="F35" t="n">
+        <v>65.38935407</v>
+      </c>
+      <c r="G35" t="n">
+        <v>6800589.791523218</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0006905372126730031</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1.43977245</v>
+      </c>
+      <c r="F36" t="n">
+        <v>3.9859805</v>
+      </c>
+      <c r="G36" t="n">
+        <v>20716116.38019009</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.0003175865722942854</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-2.57097303</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-10.00152777</v>
+      </c>
+      <c r="G37" t="n">
+        <v>25578908.08497557</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.003836118488037577</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-3.79697189</v>
+      </c>
+      <c r="F38" t="n">
+        <v>11.89616932</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3752634.334154346</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0009507457563944415</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-17.95839284</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-0.25974771</v>
+      </c>
+      <c r="G39" t="n">
+        <v>816424.051761071</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.05363259770729421</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.49551127</v>
+      </c>
+      <c r="F40" t="n">
+        <v>37.4203444</v>
+      </c>
+      <c r="G40" t="n">
+        <v>52327784.45031185</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.0493159797441039</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-7.50320553</v>
+      </c>
+      <c r="F41" t="n">
+        <v>110.74660582</v>
+      </c>
+      <c r="G41" t="n">
+        <v>46166545.73030488</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>1.239282682556597e-05</v>
+      </c>
+      <c r="E42" t="n">
+        <v>4.46772938</v>
+      </c>
+      <c r="F42" t="n">
+        <v>50.74959846</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5184977.830768074</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.001777353042905774</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-4.72712833</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-15.677775</v>
+      </c>
+      <c r="G43" t="n">
+        <v>17773247.6512636</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.07278525989920827</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.16871381</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-1.2224926</v>
+      </c>
+      <c r="G44" t="n">
+        <v>43648470.88659804</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.0001980556620468769</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-8.733706420000001</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-7.73135094</v>
+      </c>
+      <c r="G45" t="n">
+        <v>191039.1167758608</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>2.073476564684544e-09</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-25.42366976</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-24.12211623</v>
+      </c>
+      <c r="G46" t="n">
+        <v>831991.1704501774</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.005898897209588391</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-8.39852436</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-23.2651488</v>
+      </c>
+      <c r="G47" t="n">
+        <v>5898897.209588391</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1.578582086621987e-07</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-7.25788491</v>
+      </c>
+      <c r="F48" t="n">
+        <v>39.89852334</v>
+      </c>
+      <c r="G48" t="n">
+        <v>64904403.89070892</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>2.269121143954215e-06</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-2.78278994</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2.30512983</v>
+      </c>
+      <c r="G49" t="n">
+        <v>954596.5740500989</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.01195184505067535</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.10421616</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-5.00339679</v>
+      </c>
+      <c r="G50" t="n">
+        <v>790721.6864412089</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.05813302165476886</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-21.57193116</v>
+      </c>
+      <c r="F51" t="n">
+        <v>6.61794127</v>
+      </c>
+      <c r="G51" t="n">
+        <v>57327481.3442053</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>1.223068790212721e-08</v>
+      </c>
+      <c r="E52" t="n">
+        <v>37.55400277</v>
+      </c>
+      <c r="F52" t="n">
+        <v>55.48317385</v>
+      </c>
+      <c r="G52" t="n">
+        <v>387777.8147740534</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.009026945773276689</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-8.824020300000001</v>
+      </c>
+      <c r="F53" t="n">
+        <v>10.27554533</v>
+      </c>
+      <c r="G53" t="n">
+        <v>902694.5773276689</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>6.612397352928391e-05</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-6.59548266</v>
+      </c>
+      <c r="F54" t="n">
+        <v>5.06428139</v>
+      </c>
+      <c r="G54" t="n">
+        <v>25805468.89809173</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.01495895342965117</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-8.66022122</v>
+      </c>
+      <c r="F55" t="n">
+        <v>14.41417161</v>
+      </c>
+      <c r="G55" t="n">
+        <v>14089856.93408022</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.001150773742559421</v>
+      </c>
+      <c r="E56" t="n">
+        <v>3.03263374</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-0.68967486</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1150773.742559421</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.09521651775028665</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-1.3614819</v>
+      </c>
+      <c r="F57" t="n">
+        <v>4.69666805</v>
+      </c>
+      <c r="G57" t="n">
+        <v>19351877.90820434</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.006902696754273205</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-5.55561858</v>
+      </c>
+      <c r="F58" t="n">
+        <v>11.00755046</v>
+      </c>
+      <c r="G58" t="n">
+        <v>11700886.56591999</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>5.627818040665032e-05</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-1.3794912</v>
+      </c>
+      <c r="F59" t="n">
+        <v>1.44308424</v>
+      </c>
+      <c r="G59" t="n">
+        <v>53375810.37413085</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1.725315523015887e-05</v>
+      </c>
+      <c r="E60" t="n">
+        <v>5.76970365</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-25.76599978</v>
+      </c>
+      <c r="G60" t="n">
+        <v>149663.5642047895</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.03761102582099914</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-0.1841764</v>
+      </c>
+      <c r="F61" t="n">
+        <v>4.24523837</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3573047.452994918</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.0005387732173913737</v>
+      </c>
+      <c r="E62" t="n">
+        <v>5.60744926</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-5.42680522</v>
+      </c>
+      <c r="G62" t="n">
+        <v>8829297.845477814</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.01447674154571553</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-3.81171637</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-4.97263516</v>
+      </c>
+      <c r="G63" t="n">
+        <v>14474604.73335118</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0004519454942692541</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-5.45418918</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-55.7498403</v>
+      </c>
+      <c r="G64" t="n">
+        <v>418922.6577360173</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Elon MemeLord</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>4.150887613456569e-06</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-18.76102284</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-3.01767978</v>
+      </c>
+      <c r="G65" t="n">
+        <v>2844270.30452413</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>1.166248440543341e-06</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-0.8542047699999999</v>
+      </c>
+      <c r="F66" t="n">
+        <v>5.0042053</v>
+      </c>
+      <c r="G66" t="n">
+        <v>914005.0381692281</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.5333051336673907</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.5301390499999999</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-23.61715435</v>
+      </c>
+      <c r="G67" t="n">
+        <v>46110135.69320643</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.1503487140929211</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-1.31081166</v>
+      </c>
+      <c r="F68" t="n">
+        <v>24.0367356</v>
+      </c>
+      <c r="G68" t="n">
+        <v>83559218.12584391</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.00252675013640109</v>
+      </c>
+      <c r="E69" t="n">
+        <v>2.57379203</v>
+      </c>
+      <c r="F69" t="n">
+        <v>7.02913147</v>
+      </c>
+      <c r="G69" t="n">
+        <v>252675013.6401089</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.00597244746087485</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-3.33364666</v>
+      </c>
+      <c r="F70" t="n">
+        <v>8.3968284</v>
+      </c>
+      <c r="G70" t="n">
+        <v>50305251.34254465</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>2.697080285845089e-07</v>
+      </c>
+      <c r="E71" t="n">
+        <v>3.04611896</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-1.43110349</v>
+      </c>
+      <c r="G71" t="n">
+        <v>113277372.0054938</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>7.232738105902917e-05</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-1.84037694</v>
+      </c>
+      <c r="F72" t="n">
+        <v>15.377346</v>
+      </c>
+      <c r="G72" t="n">
+        <v>30427405.93772298</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0002816150202086012</v>
+      </c>
+      <c r="E73" t="n">
+        <v>4.07331201</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.46542718</v>
+      </c>
+      <c r="G73" t="n">
+        <v>5457042.002132189</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>3.434838885997393e-07</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-2.4122059</v>
+      </c>
+      <c r="F74" t="n">
+        <v>5.75401227</v>
+      </c>
+      <c r="G74" t="n">
+        <v>304362.0474722664</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.01451835379551873</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-4.51001866</v>
+      </c>
+      <c r="F75" t="n">
+        <v>-16.79571364</v>
+      </c>
+      <c r="G75" t="n">
+        <v>1379964.214546566</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.0008898544746290083</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.61201756</v>
+      </c>
+      <c r="F76" t="n">
+        <v>8.52302946</v>
+      </c>
+      <c r="G76" t="n">
+        <v>869903.1466505671</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.007247749553474098</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-8.51501961</v>
+      </c>
+      <c r="F77" t="n">
+        <v>5.57775532</v>
+      </c>
+      <c r="G77" t="n">
+        <v>5049633.039931079</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.002119650282763494</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-13.44763557</v>
+      </c>
+      <c r="F78" t="n">
+        <v>24.02472014</v>
+      </c>
+      <c r="G78" t="n">
+        <v>2039604.735410359</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.01130646016400733</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-9.99735993</v>
+      </c>
+      <c r="F79" t="n">
+        <v>23.60064708</v>
+      </c>
+      <c r="G79" t="n">
+        <v>10741140.01634139</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>2.775018976726927</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-8.71496537</v>
+      </c>
+      <c r="F80" t="n">
+        <v>2.430648</v>
+      </c>
+      <c r="G80" t="n">
+        <v>21561897.44916822</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0001894942556208088</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-3.02617365</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-4.51743541</v>
+      </c>
+      <c r="G81" t="n">
+        <v>121884.871134646</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.002084694022116011</v>
+      </c>
+      <c r="E82" t="n">
+        <v>1.80691039</v>
+      </c>
+      <c r="F82" t="n">
+        <v>16.6770151</v>
+      </c>
+      <c r="G82" t="n">
+        <v>1953658.017266956</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>3.778300430548061e-08</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-0.41557637</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-2.91889364</v>
+      </c>
+      <c r="G83" t="n">
+        <v>29087676.50511553</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.0003668692336241368</v>
+      </c>
+      <c r="E84" t="n">
+        <v>3.21222061</v>
+      </c>
+      <c r="F84" t="n">
+        <v>1.12458912</v>
+      </c>
+      <c r="G84" t="n">
+        <v>183232.8724855446</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.01603694239534597</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-13.43394938</v>
+      </c>
+      <c r="F85" t="n">
+        <v>24.47696058</v>
+      </c>
+      <c r="G85" t="n">
+        <v>15874897.4156141</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>9.583051282155816e-05</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-0.23737573</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-3.90897048</v>
+      </c>
+      <c r="G86" t="n">
+        <v>1006220.384626361</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>3.917032154745979e-05</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-4.4724632</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0.92524474</v>
+      </c>
+      <c r="G87" t="n">
+        <v>89433851.17188293</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>1.09889500826549e-05</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.4439469</v>
+      </c>
+      <c r="F88" t="n">
+        <v>14.88529143</v>
+      </c>
+      <c r="G88" t="n">
+        <v>367729.0011993152</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.0002215538777300108</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-1.86137457</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-9.168529680000001</v>
+      </c>
+      <c r="G89" t="n">
+        <v>204362.684631652</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.02255493801346995</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-1.84550055</v>
+      </c>
+      <c r="F90" t="n">
+        <v>43.28019224</v>
+      </c>
+      <c r="G90" t="n">
+        <v>20796664.88848796</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.0008756932324717792</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-0.8353010199999999</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-1.45873552</v>
+      </c>
+      <c r="G91" t="n">
+        <v>701644.5841119051</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.005122682457250407</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-7.37411387</v>
+      </c>
+      <c r="F92" t="n">
+        <v>15.22712038</v>
+      </c>
+      <c r="G92" t="n">
+        <v>455349551.7510382</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.0004457351803332384</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.91357228</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-0.98140287</v>
+      </c>
+      <c r="G93" t="n">
+        <v>445253.8634506647</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.004515585150257032</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-10.49204357</v>
+      </c>
+      <c r="F94" t="n">
+        <v>38.4179774</v>
+      </c>
+      <c r="G94" t="n">
+        <v>64029231.29046517</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>1.431437167612165e-05</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-5.2880934</v>
+      </c>
+      <c r="F95" t="n">
+        <v>3.09151384</v>
+      </c>
+      <c r="G95" t="n">
+        <v>3578565.650124</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.0198614722366436</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-14.62009027</v>
+      </c>
+      <c r="F96" t="n">
+        <v>9.8995663</v>
+      </c>
+      <c r="G96" t="n">
+        <v>184759595.4473354</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30011</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>SKID</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Success Kid</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.02436727318695634</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-9.08038002</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-7.01026204</v>
+      </c>
+      <c r="G97" t="n">
+        <v>2113683.019139652</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-20T13:27:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30008</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>APU</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Apu Apustaja</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.0002566278036722942</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-8.206473839999999</v>
+      </c>
+      <c r="F98" t="n">
+        <v>16.86104019</v>
+      </c>
+      <c r="G98" t="n">
+        <v>81696566.01420388</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:03:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30007</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.006500326092454685</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-11.57906355</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-6.03144102</v>
+      </c>
+      <c r="G99" t="n">
+        <v>2485250.897232814</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:00:29.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>29999</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>CHKN</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Chickencoin</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>5.568551550225353e-08</v>
+      </c>
+      <c r="E100" t="n">
+        <v>1.50351371</v>
+      </c>
+      <c r="F100" t="n">
+        <v>8.112850509999999</v>
+      </c>
+      <c r="G100" t="n">
+        <v>3577181.830349264</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-20T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>29932</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>BSHIB</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Based Shiba Inu</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>2.632009413796827e-05</v>
+      </c>
+      <c r="E101" t="n">
+        <v>3.99203352</v>
+      </c>
+      <c r="F101" t="n">
+        <v>32.54575366</v>
+      </c>
+      <c r="G101" t="n">
+        <v>237970.2650744291</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-19T05:05:42.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>63065.11</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>146.94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update portfolios at 2024-09-22 12:19:35
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -13,6 +13,7 @@
     <sheet name="Portfolio_4" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Portfolio_5" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Portfolio_6" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Portfolio_7" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16950,4 +16951,3285 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.01851779197428869</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-3.74317771</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-59.93685743</v>
+      </c>
+      <c r="G2" t="n">
+        <v>18517791.97428869</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0003900742959553927</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-10.56918642</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-27.11173234</v>
+      </c>
+      <c r="G3" t="n">
+        <v>370570.5811576231</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.001047680841587692</v>
+      </c>
+      <c r="E4" t="n">
+        <v>376.21711325</v>
+      </c>
+      <c r="F4" t="n">
+        <v>229.76606776</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1047680.841587692</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.01348739245496323</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-5.8879741</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-33.66731132</v>
+      </c>
+      <c r="G5" t="n">
+        <v>13487392.45496323</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>7.566056085515406e-07</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.88811886</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-40.86449129</v>
+      </c>
+      <c r="G6" t="n">
+        <v>492399.560197186</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0009289413608594552</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.25218182</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-13.18313283</v>
+      </c>
+      <c r="G7" t="n">
+        <v>480030448.2241235</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0003026741105618699</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.5336858799999999</v>
+      </c>
+      <c r="G8" t="n">
+        <v>302674.1105618699</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4.791121093538518e-07</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-45.40767121</v>
+      </c>
+      <c r="F9" t="n">
+        <v>153.10774998</v>
+      </c>
+      <c r="G9" t="n">
+        <v>197526.3645884626</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.00835657444745882</v>
+      </c>
+      <c r="E10" t="n">
+        <v>20.9921192</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-54.46388938</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7857009.284897286</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0002067825533768012</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-3.95228271</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-16.44487848</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2067825.533768012</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01490178750487508</v>
+      </c>
+      <c r="E12" t="n">
+        <v>29.0125907</v>
+      </c>
+      <c r="F12" t="n">
+        <v>251.79160023</v>
+      </c>
+      <c r="G12" t="n">
+        <v>14590842.35073535</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0005012468113502368</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-6.84436072</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-44.13014631</v>
+      </c>
+      <c r="G13" t="n">
+        <v>501246.8113502368</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.004421501534039541</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-13.42599071</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-26.246638</v>
+      </c>
+      <c r="G14" t="n">
+        <v>4200392.703594853</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>4.193635761678238e-05</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-5.7344023</v>
+      </c>
+      <c r="F15" t="n">
+        <v>19.78890879</v>
+      </c>
+      <c r="G15" t="n">
+        <v>283068540.2852484</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.288742282169221</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-7.55933671</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-16.0154457</v>
+      </c>
+      <c r="G16" t="n">
+        <v>288011108.7503524</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>5.764519432970598e-05</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-10.67305604</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-22.13256043</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5764519.432970598</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>2.975817246287555e-06</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-12.29372877</v>
+      </c>
+      <c r="F18" t="n">
+        <v>87.42262635</v>
+      </c>
+      <c r="G18" t="n">
+        <v>957676.8243631587</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.01756658990249219</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6.07464388</v>
+      </c>
+      <c r="F19" t="n">
+        <v>32.80759357</v>
+      </c>
+      <c r="G19" t="n">
+        <v>17566562.48104535</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32598</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>GODCAT</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Godcat Exploding Kittens</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.000153378771618434</v>
+      </c>
+      <c r="E20" t="n">
+        <v>6.21037372</v>
+      </c>
+      <c r="F20" t="n">
+        <v>7.34748516</v>
+      </c>
+      <c r="G20" t="n">
+        <v>122231.9047348586</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-08T06:06:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32590</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>DOGY</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Dogy</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1.165627061770847e-07</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-24.96516451</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-1.99394424</v>
+      </c>
+      <c r="G21" t="n">
+        <v>101394.9011080702</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-07T17:46:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>2.627932746486651e-06</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-9.36930641</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-10.4050046</v>
+      </c>
+      <c r="G22" t="n">
+        <v>18132731.64670073</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0008266499268790409</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-0.74605789</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1864.06894655</v>
+      </c>
+      <c r="G23" t="n">
+        <v>347273345.0247428</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>3.614259372308452e-05</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-0.40813848</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-2.08686091</v>
+      </c>
+      <c r="G24" t="n">
+        <v>231874.1481376961</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0009875547916785856</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1.59561942</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-70.58470646000001</v>
+      </c>
+      <c r="G25" t="n">
+        <v>987554.761064387</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.001477457299182054</v>
+      </c>
+      <c r="E26" t="n">
+        <v>6.90344569</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-23.05587874</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1477454.641236373</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.08394381484459855</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-3.02194759</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-37.33108818</v>
+      </c>
+      <c r="G27" t="n">
+        <v>83943814.84459855</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.01347215965944532</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-10.02251095</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-11.74164574</v>
+      </c>
+      <c r="G28" t="n">
+        <v>12837695.58872212</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.05702569517451831</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-10.68425415</v>
+      </c>
+      <c r="F29" t="n">
+        <v>13.60414961</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3994003.959900071</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0006427513270207827</v>
+      </c>
+      <c r="E30" t="n">
+        <v>10.70797459</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-7.91393928</v>
+      </c>
+      <c r="G30" t="n">
+        <v>595546.3769914578</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.0004478300796593132</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-5.43765973</v>
+      </c>
+      <c r="F31" t="n">
+        <v>33.00472368</v>
+      </c>
+      <c r="G31" t="n">
+        <v>298466.8304388524</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>1.522704785157574e-06</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-6.0483633</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-27.68681047</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1353510.647324535</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.002805710777556744</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.91895748</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-8.54769651</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1963996.626822296</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0001465191987598877</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1.01054395</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3.44755759</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1465191.987598876</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>2.262849041208601e-06</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-2.03146511</v>
+      </c>
+      <c r="F35" t="n">
+        <v>37.51618743</v>
+      </c>
+      <c r="G35" t="n">
+        <v>6662438.182693122</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.00066662659791958</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-3.4626106</v>
+      </c>
+      <c r="F36" t="n">
+        <v>4.27469429</v>
+      </c>
+      <c r="G36" t="n">
+        <v>19998797.9375874</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.000310873794007305</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-2.11368454</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-5.40789676</v>
+      </c>
+      <c r="G37" t="n">
+        <v>25038250.65869628</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.00362554814209809</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-5.48915125</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.96731194</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3546646.559691333</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0008794926559883019</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-7.49444317</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-1.15422899</v>
+      </c>
+      <c r="G39" t="n">
+        <v>755237.6151739332</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.04830412226352811</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-9.935143310000001</v>
+      </c>
+      <c r="F40" t="n">
+        <v>20.30771508</v>
+      </c>
+      <c r="G40" t="n">
+        <v>47128944.07357114</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.04313186766852552</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-12.53977333</v>
+      </c>
+      <c r="F41" t="n">
+        <v>111.84102731</v>
+      </c>
+      <c r="G41" t="n">
+        <v>40377365.54124753</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>1.153857184928826e-05</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-6.89314059</v>
+      </c>
+      <c r="F42" t="n">
+        <v>46.04607144</v>
+      </c>
+      <c r="G42" t="n">
+        <v>4827570.01928428</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.001793629284724818</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.91575739</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-10.32965456</v>
+      </c>
+      <c r="G43" t="n">
+        <v>17936006.67390802</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.07264957289328026</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-0.186421</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-3.66101324</v>
+      </c>
+      <c r="G44" t="n">
+        <v>43567100.97274268</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.0002090419493251349</v>
+      </c>
+      <c r="E45" t="n">
+        <v>5.54707054</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-5.65145852</v>
+      </c>
+      <c r="G45" t="n">
+        <v>201636.1913386043</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>2.113820716160617e-09</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1.94572498</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-14.57085633</v>
+      </c>
+      <c r="G46" t="n">
+        <v>848179.4304860481</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.005671388506584539</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-3.8568006</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-20.67028546</v>
+      </c>
+      <c r="G47" t="n">
+        <v>5671388.506584538</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1.4452243509281e-07</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-8.44794432</v>
+      </c>
+      <c r="F48" t="n">
+        <v>29.62567569</v>
+      </c>
+      <c r="G48" t="n">
+        <v>59421315.99000406</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>2.385377848402854e-06</v>
+      </c>
+      <c r="E49" t="n">
+        <v>5.12342432</v>
+      </c>
+      <c r="F49" t="n">
+        <v>6.02720348</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1003504.607044597</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.01086803565322903</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-9.06813461</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-13.4652945</v>
+      </c>
+      <c r="G50" t="n">
+        <v>719017.979532696</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.07286604066601834</v>
+      </c>
+      <c r="E51" t="n">
+        <v>25.34363188</v>
+      </c>
+      <c r="F51" t="n">
+        <v>22.45771092</v>
+      </c>
+      <c r="G51" t="n">
+        <v>71856347.18446806</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>1.184418551187625e-08</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-3.16010345</v>
+      </c>
+      <c r="F52" t="n">
+        <v>45.72810585</v>
+      </c>
+      <c r="G52" t="n">
+        <v>375523.6346743062</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.008874433389000558</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-1.68952366</v>
+      </c>
+      <c r="F53" t="n">
+        <v>10.55487734</v>
+      </c>
+      <c r="G53" t="n">
+        <v>887443.3389000559</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>6.645648745217376e-05</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.5028644</v>
+      </c>
+      <c r="F54" t="n">
+        <v>2.90224644</v>
+      </c>
+      <c r="G54" t="n">
+        <v>25935235.41449015</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.01448537704833377</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-3.165839</v>
+      </c>
+      <c r="F55" t="n">
+        <v>20.3451313</v>
+      </c>
+      <c r="G55" t="n">
+        <v>13643794.74854689</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.001042788267578684</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-9.38372775</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-20.27688088</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1042788.267578684</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.09365068605843783</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-1.64449586</v>
+      </c>
+      <c r="F57" t="n">
+        <v>4.02903148</v>
+      </c>
+      <c r="G57" t="n">
+        <v>19033637.07729174</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.006669303308892886</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-3.38119222</v>
+      </c>
+      <c r="F58" t="n">
+        <v>10.30325763</v>
+      </c>
+      <c r="G58" t="n">
+        <v>11305257.10009799</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>5.698582401539569e-05</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.25740314</v>
+      </c>
+      <c r="F59" t="n">
+        <v>3.73300055</v>
+      </c>
+      <c r="G59" t="n">
+        <v>54046959.49089218</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1.606376440537279e-05</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-6.89375832</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-27.23142503</v>
+      </c>
+      <c r="G60" t="n">
+        <v>139346.1197898227</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.03875940410355447</v>
+      </c>
+      <c r="E61" t="n">
+        <v>3.05330221</v>
+      </c>
+      <c r="F61" t="n">
+        <v>7.90913952</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3682143.389837674</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.0005310383431661138</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-1.43564564</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-2.49943092</v>
+      </c>
+      <c r="G62" t="n">
+        <v>8702540.415584043</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.01398212556484946</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-3.41662507</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-9.567029160000001</v>
+      </c>
+      <c r="G63" t="n">
+        <v>13980061.75935204</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0004619920388751601</v>
+      </c>
+      <c r="E64" t="n">
+        <v>2.22295492</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-52.87620447</v>
+      </c>
+      <c r="G64" t="n">
+        <v>428235.1195720948</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Elon MemeLord</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>4.674047268757558e-06</v>
+      </c>
+      <c r="E65" t="n">
+        <v>12.60356107</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-3.47557486</v>
+      </c>
+      <c r="G65" t="n">
+        <v>3202749.649345171</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>1.178346197981916e-06</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1.0373225</v>
+      </c>
+      <c r="F66" t="n">
+        <v>6.56014791</v>
+      </c>
+      <c r="G66" t="n">
+        <v>923486.2180490962</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.5304282108684756</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-0.53945155</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-23.95962933</v>
+      </c>
+      <c r="G67" t="n">
+        <v>45861393.85244329</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.1425534887353259</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-5.18476357</v>
+      </c>
+      <c r="F68" t="n">
+        <v>20.89833663</v>
+      </c>
+      <c r="G68" t="n">
+        <v>79226869.13686804</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.002529274140123833</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.09989131</v>
+      </c>
+      <c r="F69" t="n">
+        <v>15.58336079</v>
+      </c>
+      <c r="G69" t="n">
+        <v>252927414.0123833</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.005720027392258572</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-4.22640919</v>
+      </c>
+      <c r="F70" t="n">
+        <v>5.45460428</v>
+      </c>
+      <c r="G70" t="n">
+        <v>48179145.57454443</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>2.507206447275316e-07</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-7.03997725</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-6.41032986</v>
+      </c>
+      <c r="G71" t="n">
+        <v>105302670.7855633</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>7.766020667968128e-05</v>
+      </c>
+      <c r="E72" t="n">
+        <v>7.37317672</v>
+      </c>
+      <c r="F72" t="n">
+        <v>35.47012276</v>
+      </c>
+      <c r="G72" t="n">
+        <v>32670872.34807511</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0002896304674464489</v>
+      </c>
+      <c r="E73" t="n">
+        <v>2.8462428</v>
+      </c>
+      <c r="F73" t="n">
+        <v>4.37893357</v>
+      </c>
+      <c r="G73" t="n">
+        <v>5612362.667238792</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>3.438253188154996e-07</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.09940211</v>
+      </c>
+      <c r="F74" t="n">
+        <v>5.50358947</v>
+      </c>
+      <c r="G74" t="n">
+        <v>304664.5897544133</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.01392839660016336</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-4.06352679</v>
+      </c>
+      <c r="F75" t="n">
+        <v>-19.19582992</v>
+      </c>
+      <c r="G75" t="n">
+        <v>1323888.999052372</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.0008719252603461925</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-2.01484791</v>
+      </c>
+      <c r="F76" t="n">
+        <v>5.75431513</v>
+      </c>
+      <c r="G76" t="n">
+        <v>852375.9212825132</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.00572131704858808</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-21.06077885</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-11.05965925</v>
+      </c>
+      <c r="G77" t="n">
+        <v>3986140.99276949</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.002120805309711141</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.05449139</v>
+      </c>
+      <c r="F78" t="n">
+        <v>21.17539588</v>
+      </c>
+      <c r="G78" t="n">
+        <v>2040716.144424904</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.01036765487390738</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-8.30326447</v>
+      </c>
+      <c r="F79" t="n">
+        <v>20.52568824</v>
+      </c>
+      <c r="G79" t="n">
+        <v>9849274.75322869</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>2.762080095986604</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-0.46626278</v>
+      </c>
+      <c r="F80" t="n">
+        <v>1.57586556</v>
+      </c>
+      <c r="G80" t="n">
+        <v>21461362.34581591</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0001841492790116341</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-2.82065363</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-5.05913643</v>
+      </c>
+      <c r="G81" t="n">
+        <v>118446.9210865421</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.002018878945802975</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-3.15706169</v>
+      </c>
+      <c r="F82" t="n">
+        <v>-2.82577761</v>
+      </c>
+      <c r="G82" t="n">
+        <v>1891979.828462304</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>3.732487086039327e-08</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-1.21253842</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-0.91168578</v>
+      </c>
+      <c r="G83" t="n">
+        <v>28734977.25073301</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.0003650620060910666</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-0.49260809</v>
+      </c>
+      <c r="F84" t="n">
+        <v>4.95635478</v>
+      </c>
+      <c r="G84" t="n">
+        <v>182330.2525278878</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.01598801874511589</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-0.30506844</v>
+      </c>
+      <c r="F85" t="n">
+        <v>32.64788548</v>
+      </c>
+      <c r="G85" t="n">
+        <v>15826468.11347822</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>9.264004946905597e-05</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-3.32927714</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-4.21916088</v>
+      </c>
+      <c r="G86" t="n">
+        <v>972720.5194250877</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>3.832560340195786e-05</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-2.15652594</v>
+      </c>
+      <c r="F87" t="n">
+        <v>4.96956685</v>
+      </c>
+      <c r="G87" t="n">
+        <v>87505186.97096553</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>1.071798476099682e-05</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-2.46579809</v>
+      </c>
+      <c r="F88" t="n">
+        <v>13.24996398</v>
+      </c>
+      <c r="G88" t="n">
+        <v>358661.5464976825</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.0002192477792873534</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-1.04087478</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-10.364789</v>
+      </c>
+      <c r="G89" t="n">
+        <v>202235.5249827443</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.02317494806661312</v>
+      </c>
+      <c r="E90" t="n">
+        <v>2.7488883</v>
+      </c>
+      <c r="F90" t="n">
+        <v>49.61484436</v>
+      </c>
+      <c r="G90" t="n">
+        <v>21368341.97733704</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.0008917103341417447</v>
+      </c>
+      <c r="E91" t="n">
+        <v>1.82907679</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-0.23974029</v>
+      </c>
+      <c r="G91" t="n">
+        <v>714478.2023507707</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.004682757486462045</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-8.5877853</v>
+      </c>
+      <c r="F92" t="n">
+        <v>9.53224925</v>
+      </c>
+      <c r="G92" t="n">
+        <v>416245109.9035749</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.0004467828950386281</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.23505318</v>
+      </c>
+      <c r="F93" t="n">
+        <v>4.3136806</v>
+      </c>
+      <c r="G93" t="n">
+        <v>446300.4468054273</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.004254182240780478</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-5.78890444</v>
+      </c>
+      <c r="F94" t="n">
+        <v>31.08925538</v>
+      </c>
+      <c r="G94" t="n">
+        <v>60322640.27425499</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>1.414317497337453e-05</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-1.19597777</v>
+      </c>
+      <c r="F95" t="n">
+        <v>3.13621669</v>
+      </c>
+      <c r="G95" t="n">
+        <v>3535766.800567276</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.01830821447534919</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-7.82045632</v>
+      </c>
+      <c r="F96" t="n">
+        <v>9.11175791</v>
+      </c>
+      <c r="G96" t="n">
+        <v>170310551.983542</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30011</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>SKID</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Success Kid</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.02478645023618547</v>
+      </c>
+      <c r="E97" t="n">
+        <v>1.72024603</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-6.97451449</v>
+      </c>
+      <c r="G97" t="n">
+        <v>2150043.567329464</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-20T13:27:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30008</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>APU</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Apu Apustaja</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.0002617065188377752</v>
+      </c>
+      <c r="E98" t="n">
+        <v>1.97901985</v>
+      </c>
+      <c r="F98" t="n">
+        <v>39.55776898</v>
+      </c>
+      <c r="G98" t="n">
+        <v>83313357.26926947</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:03:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30007</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.006202474770071105</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-4.58209816</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-6.37679256</v>
+      </c>
+      <c r="G99" t="n">
+        <v>2371374.261558335</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:00:29.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>29999</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>CHKN</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Chickencoin</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>6.125997657866488e-08</v>
+      </c>
+      <c r="E100" t="n">
+        <v>10.01061232</v>
+      </c>
+      <c r="F100" t="n">
+        <v>18.67742375</v>
+      </c>
+      <c r="G100" t="n">
+        <v>3935279.635436853</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-20T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>29932</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>BSHIB</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Based Shiba Inu</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>2.874803874428806e-05</v>
+      </c>
+      <c r="E101" t="n">
+        <v>9.224680559999999</v>
+      </c>
+      <c r="F101" t="n">
+        <v>38.4782607</v>
+      </c>
+      <c r="G101" t="n">
+        <v>259922.2618462976</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-19T05:05:42.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>62920.12</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>145.07</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update portfolios at 2024-09-23 12:21:57
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Portfolio_5" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Portfolio_6" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Portfolio_7" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Portfolio_8" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20232,4 +20233,3285 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.01380503620558708</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-24.8893568</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-52.25721989</v>
+      </c>
+      <c r="G2" t="n">
+        <v>13805036.20558708</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.000441950035051499</v>
+      </c>
+      <c r="E3" t="n">
+        <v>13.27589438</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-12.32836953</v>
+      </c>
+      <c r="G3" t="n">
+        <v>419852.533298924</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.000758960655963322</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-26.69983388</v>
+      </c>
+      <c r="F4" t="n">
+        <v>200.50565235</v>
+      </c>
+      <c r="G4" t="n">
+        <v>758960.655963322</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.01411085685669867</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4.69995608</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-27.28914851</v>
+      </c>
+      <c r="G5" t="n">
+        <v>14110856.85669867</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>9.003544827376009e-07</v>
+      </c>
+      <c r="E6" t="n">
+        <v>18.99918168</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-24.78865274</v>
+      </c>
+      <c r="G6" t="n">
+        <v>585951.4472411677</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0008498595598264487</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-8.40598803</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-12.85828107</v>
+      </c>
+      <c r="G7" t="n">
+        <v>439164927.5403174</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0003123088774302989</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.18321473</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-5.96210514</v>
+      </c>
+      <c r="G8" t="n">
+        <v>312308.8774302989</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4.791534612815871e-07</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.26161576</v>
+      </c>
+      <c r="F9" t="n">
+        <v>227.09009244</v>
+      </c>
+      <c r="G9" t="n">
+        <v>197543.4129906942</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.008146658605404661</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-2.22597996</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-46.0567158</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7659642.441529056</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0002141505326283091</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.06227574</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-2.50017979</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2141505.326283091</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01253767374976207</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-16.36148456</v>
+      </c>
+      <c r="F12" t="n">
+        <v>172.20182913</v>
+      </c>
+      <c r="G12" t="n">
+        <v>12276058.90017452</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0005392458282876642</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5.94554368</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-23.77029515</v>
+      </c>
+      <c r="G13" t="n">
+        <v>539245.8282876642</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.004570319739251061</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2.95852117</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-4.05096991</v>
+      </c>
+      <c r="G14" t="n">
+        <v>4341768.862467619</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>4.14159910855606e-05</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-1.00766342</v>
+      </c>
+      <c r="F15" t="n">
+        <v>32.21977714</v>
+      </c>
+      <c r="G15" t="n">
+        <v>279556089.4483808</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.3119326613022866</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8.11853773</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-3.57294488</v>
+      </c>
+      <c r="G16" t="n">
+        <v>311142763.5820506</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>6.882749002353027e-05</v>
+      </c>
+      <c r="E17" t="n">
+        <v>19.01699351</v>
+      </c>
+      <c r="F17" t="n">
+        <v>8.183976489999999</v>
+      </c>
+      <c r="G17" t="n">
+        <v>6882749.002353027</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>2.908425341567609e-06</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-2.49537848</v>
+      </c>
+      <c r="F18" t="n">
+        <v>55.80047002</v>
+      </c>
+      <c r="G18" t="n">
+        <v>935988.7770274229</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.01769786370122913</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.64068318</v>
+      </c>
+      <c r="F19" t="n">
+        <v>35.38477865</v>
+      </c>
+      <c r="G19" t="n">
+        <v>17697836.07486389</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32598</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>GODCAT</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Godcat Exploding Kittens</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0001336845119262673</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-12.84027736</v>
+      </c>
+      <c r="F20" t="n">
+        <v>3.99702988</v>
+      </c>
+      <c r="G20" t="n">
+        <v>106536.9891405081</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-08T06:06:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>2.65924854636789e-06</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1.21568785</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-14.51524525</v>
+      </c>
+      <c r="G21" t="n">
+        <v>18348810.61459192</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.001158350866977658</v>
+      </c>
+      <c r="E22" t="n">
+        <v>40.53677626</v>
+      </c>
+      <c r="F22" t="n">
+        <v>268.23701396</v>
+      </c>
+      <c r="G22" t="n">
+        <v>486655002.2912722</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>3.761327390846022e-05</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.88570776</v>
+      </c>
+      <c r="F23" t="n">
+        <v>4.75766559</v>
+      </c>
+      <c r="G23" t="n">
+        <v>241309.3513159665</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.00342295147575863</v>
+      </c>
+      <c r="E24" t="n">
+        <v>246.5946235</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-20.56917025</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3422951.369647134</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.001325609886608031</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-10.28346436</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-15.04242691</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1325607.501835845</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.08321853719951647</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-0.59973101</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-6.73473312</v>
+      </c>
+      <c r="G26" t="n">
+        <v>83218537.19951648</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.01410986394707475</v>
+      </c>
+      <c r="E27" t="n">
+        <v>4.71659707</v>
+      </c>
+      <c r="F27" t="n">
+        <v>5.52539753</v>
+      </c>
+      <c r="G27" t="n">
+        <v>13445367.53792366</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.05220531174111225</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-8.934960909999999</v>
+      </c>
+      <c r="F28" t="n">
+        <v>16.70414621</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3656390.70569351</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.0005600286248047128</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-12.87725704</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-16.84022688</v>
+      </c>
+      <c r="G29" t="n">
+        <v>518898.9963814902</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0003703337925132588</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-17.30484187</v>
+      </c>
+      <c r="F30" t="n">
+        <v>35.0055903</v>
+      </c>
+      <c r="G30" t="n">
+        <v>246817.6173872006</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>1.489394471818434e-06</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-2.20196832</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-24.77088781</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1323901.582691985</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.002769835478449557</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-1.44019615</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-7.84879186</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1938883.929178488</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.0001500372519619859</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2.40108684</v>
+      </c>
+      <c r="F33" t="n">
+        <v>11.54983412</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1500372.519619859</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>2.447401370203935e-06</v>
+      </c>
+      <c r="E34" t="n">
+        <v>8.16066154</v>
+      </c>
+      <c r="F34" t="n">
+        <v>35.22503808</v>
+      </c>
+      <c r="G34" t="n">
+        <v>7205810.038708199</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.0006721032805790435</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.81330437</v>
+      </c>
+      <c r="F35" t="n">
+        <v>6.35805012</v>
+      </c>
+      <c r="G35" t="n">
+        <v>20163098.4173713</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0003073137582509248</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-1.13215348</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2.05261974</v>
+      </c>
+      <c r="G36" t="n">
+        <v>24751519.93600282</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.003784238417869652</v>
+      </c>
+      <c r="E37" t="n">
+        <v>4.13814557</v>
+      </c>
+      <c r="F37" t="n">
+        <v>14.44442897</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3701883.312469902</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0008664166655516829</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-1.48676516</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-3.9540516</v>
+      </c>
+      <c r="G38" t="n">
+        <v>744009.0053997083</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.04874816396940204</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.66500183</v>
+      </c>
+      <c r="F39" t="n">
+        <v>35.81007117</v>
+      </c>
+      <c r="G39" t="n">
+        <v>47562182.80645391</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.03939640097210115</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-8.40291702</v>
+      </c>
+      <c r="F40" t="n">
+        <v>95.06815971</v>
+      </c>
+      <c r="G40" t="n">
+        <v>36880454.50025529</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>1.042820775160819e-05</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-9.859842779999999</v>
+      </c>
+      <c r="F41" t="n">
+        <v>62.0620411</v>
+      </c>
+      <c r="G41" t="n">
+        <v>4363009.890139649</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.001776097354187369</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-1.54271359</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-1.19375163</v>
+      </c>
+      <c r="G42" t="n">
+        <v>17760690.15687047</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.07584846922044845</v>
+      </c>
+      <c r="E43" t="n">
+        <v>4.32196614</v>
+      </c>
+      <c r="F43" t="n">
+        <v>3.20026314</v>
+      </c>
+      <c r="G43" t="n">
+        <v>45485441.76590601</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.0001613002528656282</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-13.43143071</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-16.17819969</v>
+      </c>
+      <c r="G44" t="n">
+        <v>155585.8465479227</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>2.23135206001566e-09</v>
+      </c>
+      <c r="E45" t="n">
+        <v>5.56013776</v>
+      </c>
+      <c r="F45" t="n">
+        <v>7.85144867</v>
+      </c>
+      <c r="G45" t="n">
+        <v>895339.3752879399</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.005544713384191151</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-1.84626228</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-19.3665793</v>
+      </c>
+      <c r="G46" t="n">
+        <v>5544713.384191151</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1.550225732048578e-07</v>
+      </c>
+      <c r="E47" t="n">
+        <v>7.06155014</v>
+      </c>
+      <c r="F47" t="n">
+        <v>47.87112809</v>
+      </c>
+      <c r="G47" t="n">
+        <v>63738514.38410804</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>2.454472753889007e-06</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2.89660213</v>
+      </c>
+      <c r="F48" t="n">
+        <v>29.17690959</v>
+      </c>
+      <c r="G48" t="n">
+        <v>1032572.142833567</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.01125480747123189</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3.91006128</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-9.527783319999999</v>
+      </c>
+      <c r="G49" t="n">
+        <v>744606.4023161615</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.06998126895687611</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-3.68599695</v>
+      </c>
+      <c r="F50" t="n">
+        <v>28.90729868</v>
+      </c>
+      <c r="G50" t="n">
+        <v>69011549.31175028</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>1.184340185107099e-08</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-0.04953062</v>
+      </c>
+      <c r="F51" t="n">
+        <v>37.1947988</v>
+      </c>
+      <c r="G51" t="n">
+        <v>375498.7884614833</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.009231956793546454</v>
+      </c>
+      <c r="E52" t="n">
+        <v>4.02868993</v>
+      </c>
+      <c r="F52" t="n">
+        <v>26.03344997</v>
+      </c>
+      <c r="G52" t="n">
+        <v>923195.6793546454</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>6.459509859915177e-05</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-2.80005204</v>
+      </c>
+      <c r="F53" t="n">
+        <v>1.32228314</v>
+      </c>
+      <c r="G53" t="n">
+        <v>25208811.8559809</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.01472592790393377</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1.65939385</v>
+      </c>
+      <c r="F54" t="n">
+        <v>30.70453438</v>
+      </c>
+      <c r="G54" t="n">
+        <v>13870369.9001251</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.0009740683204630615</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-6.25158576</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-12.28237889</v>
+      </c>
+      <c r="G55" t="n">
+        <v>974068.3204630614</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.09517418178461992</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.55375411</v>
+      </c>
+      <c r="F56" t="n">
+        <v>11.58837553</v>
+      </c>
+      <c r="G56" t="n">
+        <v>19343273.51415522</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.006573726183322362</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-1.44817305</v>
+      </c>
+      <c r="F57" t="n">
+        <v>10.97934894</v>
+      </c>
+      <c r="G57" t="n">
+        <v>11143242.57962742</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>5.802508701169304e-05</v>
+      </c>
+      <c r="E58" t="n">
+        <v>1.35051342</v>
+      </c>
+      <c r="F58" t="n">
+        <v>3.70180492</v>
+      </c>
+      <c r="G58" t="n">
+        <v>55032625.76898427</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>1.493209045483961e-05</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-6.55105607</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-31.62341633</v>
+      </c>
+      <c r="G59" t="n">
+        <v>129529.3439772196</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.0393595338419323</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1.53567296</v>
+      </c>
+      <c r="F60" t="n">
+        <v>11.54237528</v>
+      </c>
+      <c r="G60" t="n">
+        <v>3739155.714983568</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.0005311247409346452</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-0.00656747</v>
+      </c>
+      <c r="F61" t="n">
+        <v>3.96490725</v>
+      </c>
+      <c r="G61" t="n">
+        <v>8703956.283349782</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.01411647077425225</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.90169739</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-7.62591718</v>
+      </c>
+      <c r="G62" t="n">
+        <v>14114387.13898141</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.0004813787873632426</v>
+      </c>
+      <c r="E63" t="n">
+        <v>4.19633822</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-44.3503204</v>
+      </c>
+      <c r="G63" t="n">
+        <v>446205.3135544883</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Elon MemeLord</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>4.20720659976616e-06</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-9.689269680000001</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-7.25126544</v>
+      </c>
+      <c r="G64" t="n">
+        <v>2882861.188031063</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>1.206198888871024e-06</v>
+      </c>
+      <c r="E65" t="n">
+        <v>2.36371034</v>
+      </c>
+      <c r="F65" t="n">
+        <v>15.72632464</v>
+      </c>
+      <c r="G65" t="n">
+        <v>945314.7572472752</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.5301932676498419</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-0.04438226</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-23.93542851</v>
+      </c>
+      <c r="G66" t="n">
+        <v>45841080.40896132</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.1534337044316229</v>
+      </c>
+      <c r="E67" t="n">
+        <v>7.61380063</v>
+      </c>
+      <c r="F67" t="n">
+        <v>35.862609</v>
+      </c>
+      <c r="G67" t="n">
+        <v>85273760.25176911</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.002507021113253721</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-0.69669339</v>
+      </c>
+      <c r="F68" t="n">
+        <v>17.15663056</v>
+      </c>
+      <c r="G68" t="n">
+        <v>250702111.325372</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.005518202506709662</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-3.59789039</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-2.3431068</v>
+      </c>
+      <c r="G69" t="n">
+        <v>46479197.32699116</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>2.363127761279505e-07</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-5.80745184</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-12.23584653</v>
+      </c>
+      <c r="G70" t="n">
+        <v>99251365.97373921</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>7.721732536027163e-05</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-0.58266023</v>
+      </c>
+      <c r="F71" t="n">
+        <v>43.83915474</v>
+      </c>
+      <c r="G71" t="n">
+        <v>32484556.60581267</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.0002824774454055172</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-2.52603896</v>
+      </c>
+      <c r="F72" t="n">
+        <v>5.54210201</v>
+      </c>
+      <c r="G72" t="n">
+        <v>5473753.790160332</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>3.438253188154996e-07</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" t="n">
+        <v>9.18074365</v>
+      </c>
+      <c r="G73" t="n">
+        <v>304664.5897544133</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.01569254024613258</v>
+      </c>
+      <c r="E74" t="n">
+        <v>12.64807761</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-0.75839489</v>
+      </c>
+      <c r="G74" t="n">
+        <v>1491570.206925171</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.000855265776296268</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-1.93282164</v>
+      </c>
+      <c r="F75" t="n">
+        <v>6.31899061</v>
+      </c>
+      <c r="G75" t="n">
+        <v>836089.8690514211</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.005179910205108802</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-9.481721909999999</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-5.53952633</v>
+      </c>
+      <c r="G76" t="n">
+        <v>3608933.438244737</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.002137412466919821</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.7481288699999999</v>
+      </c>
+      <c r="F77" t="n">
+        <v>31.83820759</v>
+      </c>
+      <c r="G77" t="n">
+        <v>2056696.156203247</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.01198584038239239</v>
+      </c>
+      <c r="E78" t="n">
+        <v>15.56281471</v>
+      </c>
+      <c r="F78" t="n">
+        <v>35.53405752</v>
+      </c>
+      <c r="G78" t="n">
+        <v>11386551.39569039</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>2.828208001227382</v>
+      </c>
+      <c r="E79" t="n">
+        <v>1.48998529</v>
+      </c>
+      <c r="F79" t="n">
+        <v>12.80164039</v>
+      </c>
+      <c r="G79" t="n">
+        <v>21975176.16953676</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.0001813981671585688</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-1.50356279</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-3.61968472</v>
+      </c>
+      <c r="G80" t="n">
+        <v>116677.3744974421</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.002271275792760426</v>
+      </c>
+      <c r="E81" t="n">
+        <v>12.50089054</v>
+      </c>
+      <c r="F81" t="n">
+        <v>29.84540616</v>
+      </c>
+      <c r="G81" t="n">
+        <v>2128511.96140852</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>3.75613184461369e-08</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.7814051400000001</v>
+      </c>
+      <c r="F82" t="n">
+        <v>4.05678301</v>
+      </c>
+      <c r="G82" t="n">
+        <v>28917009.11958385</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.0003679966055885946</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.79744211</v>
+      </c>
+      <c r="F83" t="n">
+        <v>6.62294738</v>
+      </c>
+      <c r="G83" t="n">
+        <v>183795.9385169113</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.01631386993101668</v>
+      </c>
+      <c r="E84" t="n">
+        <v>2.06258714</v>
+      </c>
+      <c r="F84" t="n">
+        <v>40.91190412</v>
+      </c>
+      <c r="G84" t="n">
+        <v>16149026.74226225</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>9.499498167554037e-05</v>
+      </c>
+      <c r="E85" t="n">
+        <v>2.54202391</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-1.08015793</v>
+      </c>
+      <c r="G85" t="n">
+        <v>997447.3075931739</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>5.614046184217572e-05</v>
+      </c>
+      <c r="E86" t="n">
+        <v>46.02417443</v>
+      </c>
+      <c r="F86" t="n">
+        <v>69.52490706</v>
+      </c>
+      <c r="G86" t="n">
+        <v>128180150.4496334</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>1.069083862431442e-05</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-0.30009245</v>
+      </c>
+      <c r="F87" t="n">
+        <v>14.6787296</v>
+      </c>
+      <c r="G87" t="n">
+        <v>357753.1410855589</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.0002251821050079821</v>
+      </c>
+      <c r="E88" t="n">
+        <v>2.70667541</v>
+      </c>
+      <c r="F88" t="n">
+        <v>3.71886669</v>
+      </c>
+      <c r="G88" t="n">
+        <v>207709.3842000685</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.02149968447746158</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-7.55074769</v>
+      </c>
+      <c r="F89" t="n">
+        <v>46.34471801</v>
+      </c>
+      <c r="G89" t="n">
+        <v>19823673.77906208</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.0009073721017763695</v>
+      </c>
+      <c r="E90" t="n">
+        <v>1.75637391</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-7.40166921</v>
+      </c>
+      <c r="G90" t="n">
+        <v>727027.1110678513</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.004948737300466586</v>
+      </c>
+      <c r="E91" t="n">
+        <v>5.64015729</v>
+      </c>
+      <c r="F91" t="n">
+        <v>17.20125946</v>
+      </c>
+      <c r="G91" t="n">
+        <v>439887760.0370754</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.0004438642236002263</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-0.65843376</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-3.27330819</v>
+      </c>
+      <c r="G92" t="n">
+        <v>443384.9270272487</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.005155559731577147</v>
+      </c>
+      <c r="E93" t="n">
+        <v>21.09994247</v>
+      </c>
+      <c r="F93" t="n">
+        <v>74.63824424000001</v>
+      </c>
+      <c r="G93" t="n">
+        <v>73103820.54608618</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>1.391841262117517e-05</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-1.39480366</v>
+      </c>
+      <c r="F94" t="n">
+        <v>4.44680205</v>
+      </c>
+      <c r="G94" t="n">
+        <v>3479576.640690164</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.02053275806738718</v>
+      </c>
+      <c r="E95" t="n">
+        <v>11.91879336</v>
+      </c>
+      <c r="F95" t="n">
+        <v>24.72009903</v>
+      </c>
+      <c r="G95" t="n">
+        <v>191004172.7394904</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30011</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>SKID</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Success Kid</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.02531521059644578</v>
+      </c>
+      <c r="E96" t="n">
+        <v>2.14118994</v>
+      </c>
+      <c r="F96" t="n">
+        <v>-0.06322074</v>
+      </c>
+      <c r="G96" t="n">
+        <v>2195909.667573896</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-20T13:27:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30008</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>APU</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Apu Apustaja</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.0002701867732515241</v>
+      </c>
+      <c r="E97" t="n">
+        <v>3.10566591</v>
+      </c>
+      <c r="F97" t="n">
+        <v>44.86668432</v>
+      </c>
+      <c r="G97" t="n">
+        <v>86013016.6772375</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:03:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30007</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.005989427430464509</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-3.46056273</v>
+      </c>
+      <c r="F98" t="n">
+        <v>-4.60894287</v>
+      </c>
+      <c r="G98" t="n">
+        <v>2290519.430386108</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:00:29.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>29999</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>CHKN</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Chickencoin</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>6.370541512102691e-08</v>
+      </c>
+      <c r="E99" t="n">
+        <v>3.88844278</v>
+      </c>
+      <c r="F99" t="n">
+        <v>31.77081272</v>
+      </c>
+      <c r="G99" t="n">
+        <v>4092372.161959648</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-20T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>29932</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>BSHIB</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Based Shiba Inu</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>2.857795423257404e-05</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-0.59163605</v>
+      </c>
+      <c r="F100" t="n">
+        <v>40.627717</v>
+      </c>
+      <c r="G100" t="n">
+        <v>258384.461254648</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-19T05:05:42.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>29920</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>SLERF</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>SLERF</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.1502355006553216</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-1.74318457</v>
+      </c>
+      <c r="F101" t="n">
+        <v>11.18675019</v>
+      </c>
+      <c r="G101" t="n">
+        <v>75117412.29778434</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-18T09:28:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>63368.53</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>143.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update portfolios at 2024-09-24 12:21:52
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Portfolio_6" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Portfolio_7" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Portfolio_8" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Portfolio_9" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -23514,4 +23515,3285 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.002970622883078241</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-18.4137299</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-31.77673223</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2173795.923130875</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.01233252816959264</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-10.72163817</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-64.29856469000001</v>
+      </c>
+      <c r="G3" t="n">
+        <v>12332528.16959264</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0004371234906703855</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1.09210182</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-23.32797083</v>
+      </c>
+      <c r="G4" t="n">
+        <v>415267.3161368662</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0007875189623261228</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8.149855069999999</v>
+      </c>
+      <c r="F5" t="n">
+        <v>177.02834396</v>
+      </c>
+      <c r="G5" t="n">
+        <v>787518.9623261228</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.01343959723955784</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-4.78084003</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-26.78179278</v>
+      </c>
+      <c r="G6" t="n">
+        <v>13439597.23955784</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>9.147591055171223e-07</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.5998835</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-21.61173178</v>
+      </c>
+      <c r="G7" t="n">
+        <v>595325.9877432152</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0008591242560308368</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.0963272</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-10.22662874</v>
+      </c>
+      <c r="G8" t="n">
+        <v>443952459.3039349</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0003085108831268974</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-1.21610194</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-8.01438557</v>
+      </c>
+      <c r="G9" t="n">
+        <v>308510.8831268974</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>5.071802188839374e-07</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5.84922366</v>
+      </c>
+      <c r="F10" t="n">
+        <v>203.50160393</v>
+      </c>
+      <c r="G10" t="n">
+        <v>209098.169032783</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.008034251126944284</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-1.31357524</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-51.7950913</v>
+      </c>
+      <c r="G11" t="n">
+        <v>7553954.805104822</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0001847806463669999</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-13.71459872</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-3.34233502</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1847806.463669999</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.009263433221667165</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-26.11521558</v>
+      </c>
+      <c r="F13" t="n">
+        <v>51.10063399</v>
+      </c>
+      <c r="G13" t="n">
+        <v>9070139.654030923</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.000486035014730927</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-9.867648409999999</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-39.19715322</v>
+      </c>
+      <c r="G14" t="n">
+        <v>486035.0147309271</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.004032367395931403</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-12.25270507</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-24.13833719</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3830718.243042133</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>4.016693282859956e-05</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-2.94493834</v>
+      </c>
+      <c r="F16" t="n">
+        <v>20.52021862</v>
+      </c>
+      <c r="G16" t="n">
+        <v>271125002.019183</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.3147677455303911</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.87671676</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-3.35375602</v>
+      </c>
+      <c r="G17" t="n">
+        <v>313970667.3523458</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>6.047496743714919e-05</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-12.13220359</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-20.96341061</v>
+      </c>
+      <c r="G18" t="n">
+        <v>6047496.743714919</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2.501824770597703e-06</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-13.98009312</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-9.39923866</v>
+      </c>
+      <c r="G19" t="n">
+        <v>805136.6744406504</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.02017636284661766</v>
+      </c>
+      <c r="E20" t="n">
+        <v>14.27220351</v>
+      </c>
+      <c r="F20" t="n">
+        <v>39.08531606</v>
+      </c>
+      <c r="G20" t="n">
+        <v>20176331.35131526</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32598</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>GODCAT</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Godcat Exploding Kittens</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0001276419659726884</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-4.5200045</v>
+      </c>
+      <c r="F21" t="n">
+        <v>15.26729105</v>
+      </c>
+      <c r="G21" t="n">
+        <v>101721.5124382217</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-08T06:06:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>2.758856698873923e-06</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.7855803</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-3.34227981</v>
+      </c>
+      <c r="G22" t="n">
+        <v>19036106.70374422</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.001214023456040383</v>
+      </c>
+      <c r="E23" t="n">
+        <v>4.64899811</v>
+      </c>
+      <c r="F23" t="n">
+        <v>217.56195711</v>
+      </c>
+      <c r="G23" t="n">
+        <v>510353913.3924764</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>3.677087099798862e-05</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-2.23964261</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.75445137</v>
+      </c>
+      <c r="G24" t="n">
+        <v>235904.884255553</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.003673950948208162</v>
+      </c>
+      <c r="E25" t="n">
+        <v>7.33338213</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-7.97351334</v>
+      </c>
+      <c r="G25" t="n">
+        <v>3673950.834315683</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.001166772477926582</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-12.32469316</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-10.82569562</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1166770.378902894</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.09549375665383134</v>
+      </c>
+      <c r="E27" t="n">
+        <v>14.68986969</v>
+      </c>
+      <c r="F27" t="n">
+        <v>23.69131955</v>
+      </c>
+      <c r="G27" t="n">
+        <v>95493756.65383133</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.01527165995824703</v>
+      </c>
+      <c r="E28" t="n">
+        <v>8.23422746</v>
+      </c>
+      <c r="F28" t="n">
+        <v>13.29934789</v>
+      </c>
+      <c r="G28" t="n">
+        <v>14552449.39448142</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.04446446472916364</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-14.65864178</v>
+      </c>
+      <c r="F29" t="n">
+        <v>12.75744701</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3114232.060821461</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0004717724085413006</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-15.75923307</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-9.89566844</v>
+      </c>
+      <c r="G30" t="n">
+        <v>437124.4941237139</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.0003677204100274048</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-0.70568296</v>
+      </c>
+      <c r="F31" t="n">
+        <v>29.21909362</v>
+      </c>
+      <c r="G31" t="n">
+        <v>245075.8675077136</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>1.250754420201082e-06</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-16.02262236</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-40.73944068</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1111777.830869908</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.002476279332834932</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-10.73465154</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-17.50007528</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1733394.72324111</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0001527008358128977</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1.78505819</v>
+      </c>
+      <c r="F34" t="n">
+        <v>17.30846165</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1527008.358128977</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>2.3709890012699e-06</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-3.12218379</v>
+      </c>
+      <c r="F35" t="n">
+        <v>3.89094219</v>
+      </c>
+      <c r="G35" t="n">
+        <v>6980831.405513897</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.000560736648137447</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-16.5698689</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-9.39902227</v>
+      </c>
+      <c r="G36" t="n">
+        <v>16822099.44412341</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.0002991625198705563</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-2.6524157</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-5.24761026</v>
+      </c>
+      <c r="G37" t="n">
+        <v>24095006.73456631</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.003673295956811062</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-2.9316985</v>
+      </c>
+      <c r="F38" t="n">
+        <v>10.92099166</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3593355.25480372</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0008562552620711267</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-1.17280794</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-8.52877271</v>
+      </c>
+      <c r="G39" t="n">
+        <v>735283.2086813131</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.05869505107598397</v>
+      </c>
+      <c r="E40" t="n">
+        <v>20.40463947</v>
+      </c>
+      <c r="F40" t="n">
+        <v>67.23985862000001</v>
+      </c>
+      <c r="G40" t="n">
+        <v>57267074.73254489</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.04539025275108423</v>
+      </c>
+      <c r="E41" t="n">
+        <v>15.21421153</v>
+      </c>
+      <c r="F41" t="n">
+        <v>116.82915409</v>
+      </c>
+      <c r="G41" t="n">
+        <v>42491524.86103779</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>4.472462934061109e-05</v>
+      </c>
+      <c r="E42" t="n">
+        <v>328.88126518</v>
+      </c>
+      <c r="F42" t="n">
+        <v>477.18502592</v>
+      </c>
+      <c r="G42" t="n">
+        <v>18712132.01672391</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.001764989241800357</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-0.6254225</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-2.53927648</v>
+      </c>
+      <c r="G43" t="n">
+        <v>17649610.77939001</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.07654122653300498</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.91334383</v>
+      </c>
+      <c r="F44" t="n">
+        <v>8.34966739</v>
+      </c>
+      <c r="G44" t="n">
+        <v>45900880.24109279</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.0002304603917946002</v>
+      </c>
+      <c r="E45" t="n">
+        <v>42.87664632</v>
+      </c>
+      <c r="F45" t="n">
+        <v>29.85370759</v>
+      </c>
+      <c r="G45" t="n">
+        <v>222295.8396909588</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>2.781278653177749e-09</v>
+      </c>
+      <c r="E46" t="n">
+        <v>24.64544269</v>
+      </c>
+      <c r="F46" t="n">
+        <v>43.92122783</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1115999.72790505</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.0055740787100534</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.52960945</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-23.95228343</v>
+      </c>
+      <c r="G47" t="n">
+        <v>5574078.7100534</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1.605615826781196e-07</v>
+      </c>
+      <c r="E48" t="n">
+        <v>3.57303415</v>
+      </c>
+      <c r="F48" t="n">
+        <v>48.18507697</v>
+      </c>
+      <c r="G48" t="n">
+        <v>66015913.26664797</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>2.375339212307671e-06</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-3.22405459</v>
+      </c>
+      <c r="F49" t="n">
+        <v>29.44340229</v>
+      </c>
+      <c r="G49" t="n">
+        <v>999281.4532257142</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.01125656584828579</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.01562334</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-12.50426442</v>
+      </c>
+      <c r="G50" t="n">
+        <v>744722.7347203693</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.08942553324023035</v>
+      </c>
+      <c r="E51" t="n">
+        <v>27.78495528</v>
+      </c>
+      <c r="F51" t="n">
+        <v>62.11947199</v>
+      </c>
+      <c r="G51" t="n">
+        <v>88186377.42537451</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>1.171328934990031e-08</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-1.0986075</v>
+      </c>
+      <c r="F52" t="n">
+        <v>34.63553902</v>
+      </c>
+      <c r="G52" t="n">
+        <v>371373.5306033398</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.008023377100409294</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-13.09126245</v>
+      </c>
+      <c r="F53" t="n">
+        <v>7.51037504</v>
+      </c>
+      <c r="G53" t="n">
+        <v>802337.7100409294</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>6.010639889292331e-05</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-6.9489788</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-15.20636807</v>
+      </c>
+      <c r="G54" t="n">
+        <v>23457056.86487085</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.01436982855187953</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-2.41817938</v>
+      </c>
+      <c r="F55" t="n">
+        <v>5.67728405</v>
+      </c>
+      <c r="G55" t="n">
+        <v>13534959.47530102</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.00103312816849763</v>
+      </c>
+      <c r="E56" t="n">
+        <v>6.06321413</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-0.8985370499999999</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1033128.16849763</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.09354665399574628</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-1.71005178</v>
+      </c>
+      <c r="F57" t="n">
+        <v>8.64512167</v>
+      </c>
+      <c r="G57" t="n">
+        <v>19012493.52128578</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.006804537801116508</v>
+      </c>
+      <c r="E58" t="n">
+        <v>3.62904328</v>
+      </c>
+      <c r="F58" t="n">
+        <v>11.99054885</v>
+      </c>
+      <c r="G58" t="n">
+        <v>11534495.54264276</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>5.871755592118516e-05</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.19339573</v>
+      </c>
+      <c r="F59" t="n">
+        <v>16.2948924</v>
+      </c>
+      <c r="G59" t="n">
+        <v>55689382.77384765</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1.482593074401177e-05</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-0.71095009</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-30.31553806</v>
+      </c>
+      <c r="G60" t="n">
+        <v>128608.4549870324</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.03864803281286845</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-1.80794765</v>
+      </c>
+      <c r="F61" t="n">
+        <v>11.97960655</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3671563.117222503</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.0005672488987399845</v>
+      </c>
+      <c r="E62" t="n">
+        <v>6.86391924</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-0.70221897</v>
+      </c>
+      <c r="G62" t="n">
+        <v>9295951.093753826</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.01521521076650088</v>
+      </c>
+      <c r="E63" t="n">
+        <v>7.78339013</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-0.25850904</v>
+      </c>
+      <c r="G63" t="n">
+        <v>15212964.95376814</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0005092397386643659</v>
+      </c>
+      <c r="E64" t="n">
+        <v>5.78773972</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-41.28319868</v>
+      </c>
+      <c r="G64" t="n">
+        <v>472030.5157395261</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>4.376658717361872e-06</v>
+      </c>
+      <c r="E65" t="n">
+        <v>4.02766333</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-0.62490508</v>
+      </c>
+      <c r="G65" t="n">
+        <v>2998973.131065547</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>1.22988421115892e-06</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1.96363324</v>
+      </c>
+      <c r="F66" t="n">
+        <v>17.96526426</v>
+      </c>
+      <c r="G66" t="n">
+        <v>963877.2720161802</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.5303530457526978</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.01601355</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-23.75463973</v>
+      </c>
+      <c r="G67" t="n">
+        <v>45854894.99565548</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.1850995611374242</v>
+      </c>
+      <c r="E68" t="n">
+        <v>20.56974986</v>
+      </c>
+      <c r="F68" t="n">
+        <v>74.81356719999999</v>
+      </c>
+      <c r="G68" t="n">
+        <v>102872674.9275318</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.002640765064895556</v>
+      </c>
+      <c r="E69" t="n">
+        <v>5.09130668</v>
+      </c>
+      <c r="F69" t="n">
+        <v>12.36368615</v>
+      </c>
+      <c r="G69" t="n">
+        <v>264076506.4895556</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.005686782412026734</v>
+      </c>
+      <c r="E70" t="n">
+        <v>3.02413106</v>
+      </c>
+      <c r="F70" t="n">
+        <v>6.69204476</v>
+      </c>
+      <c r="G70" t="n">
+        <v>47899126.85568649</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>2.366680029632562e-07</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.20507467</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-11.55287419</v>
+      </c>
+      <c r="G71" t="n">
+        <v>99400561.24456759</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>8.42699180317991e-05</v>
+      </c>
+      <c r="E72" t="n">
+        <v>9.133432989999999</v>
+      </c>
+      <c r="F72" t="n">
+        <v>52.48848922</v>
+      </c>
+      <c r="G72" t="n">
+        <v>35451511.81679756</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0002837663373373113</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.45628136</v>
+      </c>
+      <c r="F73" t="n">
+        <v>12.69237237</v>
+      </c>
+      <c r="G73" t="n">
+        <v>5498729.508439847</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>3.382680023340938e-07</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-1.61631973</v>
+      </c>
+      <c r="F74" t="n">
+        <v>5.58955777</v>
+      </c>
+      <c r="G74" t="n">
+        <v>299740.2358651308</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.01666433095187371</v>
+      </c>
+      <c r="E75" t="n">
+        <v>6.19269214</v>
+      </c>
+      <c r="F75" t="n">
+        <v>5.8669694</v>
+      </c>
+      <c r="G75" t="n">
+        <v>1583938.557830468</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.0008707219875124023</v>
+      </c>
+      <c r="E76" t="n">
+        <v>1.80718224</v>
+      </c>
+      <c r="F76" t="n">
+        <v>8.672761850000001</v>
+      </c>
+      <c r="G76" t="n">
+        <v>851199.5366774204</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.005133163003874935</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-0.90247127</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-8.966678229999999</v>
+      </c>
+      <c r="G77" t="n">
+        <v>3576363.850935894</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.002334242417037081</v>
+      </c>
+      <c r="E78" t="n">
+        <v>9.20879583</v>
+      </c>
+      <c r="F78" t="n">
+        <v>38.20912914</v>
+      </c>
+      <c r="G78" t="n">
+        <v>2246093.10606535</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.01357387682032658</v>
+      </c>
+      <c r="E79" t="n">
+        <v>13.24432585</v>
+      </c>
+      <c r="F79" t="n">
+        <v>43.0714618</v>
+      </c>
+      <c r="G79" t="n">
+        <v>12895186.41350109</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>3.832497553288913</v>
+      </c>
+      <c r="E80" t="n">
+        <v>35.51453189</v>
+      </c>
+      <c r="F80" t="n">
+        <v>40.95480873</v>
+      </c>
+      <c r="G80" t="n">
+        <v>29778505.98905485</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0001827035684807738</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.71963314</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-1.82048752</v>
+      </c>
+      <c r="G81" t="n">
+        <v>117517.0235486214</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.00236408935081011</v>
+      </c>
+      <c r="E82" t="n">
+        <v>4.08583698</v>
+      </c>
+      <c r="F82" t="n">
+        <v>44.9895461</v>
+      </c>
+      <c r="G82" t="n">
+        <v>2215491.609199129</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>3.640892781936487e-08</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-3.06809169</v>
+      </c>
+      <c r="F83" t="n">
+        <v>2.12220027</v>
+      </c>
+      <c r="G83" t="n">
+        <v>28029828.06092437</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.0003872583436237654</v>
+      </c>
+      <c r="E84" t="n">
+        <v>5.23308307</v>
+      </c>
+      <c r="F84" t="n">
+        <v>14.17841707</v>
+      </c>
+      <c r="G84" t="n">
+        <v>193416.2153506573</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.02036141505773391</v>
+      </c>
+      <c r="E85" t="n">
+        <v>24.77163141</v>
+      </c>
+      <c r="F85" t="n">
+        <v>75.03847609</v>
+      </c>
+      <c r="G85" t="n">
+        <v>20155673.52614992</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>9.287815339352854e-05</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-2.22835801</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-3.43702729</v>
+      </c>
+      <c r="G86" t="n">
+        <v>975220.6106320496</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>5.246693147480315e-05</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-6.51026534</v>
+      </c>
+      <c r="F87" t="n">
+        <v>54.13633582</v>
+      </c>
+      <c r="G87" t="n">
+        <v>119792729.6889199</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>9.566071415857839e-06</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-10.52085106</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-11.43439165</v>
+      </c>
+      <c r="G88" t="n">
+        <v>320114.4659585942</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.0002396716749563462</v>
+      </c>
+      <c r="E89" t="n">
+        <v>6.43460099</v>
+      </c>
+      <c r="F89" t="n">
+        <v>13.30725996</v>
+      </c>
+      <c r="G89" t="n">
+        <v>221074.6542831056</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.02238286355031725</v>
+      </c>
+      <c r="E90" t="n">
+        <v>4.10786993</v>
+      </c>
+      <c r="F90" t="n">
+        <v>38.66516124</v>
+      </c>
+      <c r="G90" t="n">
+        <v>20638004.51248001</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.0008981648033935318</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-1.01472134</v>
+      </c>
+      <c r="F91" t="n">
+        <v>12.04741898</v>
+      </c>
+      <c r="G91" t="n">
+        <v>719649.8117978943</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.005473758809448844</v>
+      </c>
+      <c r="E92" t="n">
+        <v>10.56507821</v>
+      </c>
+      <c r="F92" t="n">
+        <v>33.76038725</v>
+      </c>
+      <c r="G92" t="n">
+        <v>486556338.6128095</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.0004832093078341875</v>
+      </c>
+      <c r="E93" t="n">
+        <v>8.86421616</v>
+      </c>
+      <c r="F93" t="n">
+        <v>10.91986445</v>
+      </c>
+      <c r="G93" t="n">
+        <v>482687.5253769368</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.005550815938971094</v>
+      </c>
+      <c r="E94" t="n">
+        <v>7.66660126</v>
+      </c>
+      <c r="F94" t="n">
+        <v>87.24472905</v>
+      </c>
+      <c r="G94" t="n">
+        <v>78708398.97392926</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>1.421031921934505e-05</v>
+      </c>
+      <c r="E95" t="n">
+        <v>2.09726925</v>
+      </c>
+      <c r="F95" t="n">
+        <v>4.9499764</v>
+      </c>
+      <c r="G95" t="n">
+        <v>3552552.734149985</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.0220467599755166</v>
+      </c>
+      <c r="E96" t="n">
+        <v>7.48317458</v>
+      </c>
+      <c r="F96" t="n">
+        <v>38.68840064</v>
+      </c>
+      <c r="G96" t="n">
+        <v>205088042.0881282</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30011</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>SKID</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Success Kid</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.02294731897426381</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-9.353631930000001</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-4.62010408</v>
+      </c>
+      <c r="G97" t="n">
+        <v>1990512.359694236</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-20T13:27:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30008</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>APU</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Apu Apustaja</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.0002476134392367748</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-8.354714680000001</v>
+      </c>
+      <c r="F98" t="n">
+        <v>7.22574234</v>
+      </c>
+      <c r="G98" t="n">
+        <v>78826874.54412873</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:03:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30007</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.006101059698026575</v>
+      </c>
+      <c r="E99" t="n">
+        <v>1.86382202</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-4.36755178</v>
+      </c>
+      <c r="G99" t="n">
+        <v>2333210.635994244</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:00:29.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>29999</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>CHKN</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Chickencoin</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>7.154172708049658e-08</v>
+      </c>
+      <c r="E100" t="n">
+        <v>12.30085691</v>
+      </c>
+      <c r="F100" t="n">
+        <v>50.94728412</v>
+      </c>
+      <c r="G100" t="n">
+        <v>4595769.00592402</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-20T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>29932</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>BSHIB</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Based Shiba Inu</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>2.824291938335478e-05</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-1.17235421</v>
+      </c>
+      <c r="F101" t="n">
+        <v>42.40104109</v>
+      </c>
+      <c r="G101" t="n">
+        <v>255355.2801483818</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-19T05:05:42.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>63590.34</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>147.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update portfolios at 2024-09-25 12:21:55
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Portfolio_7" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Portfolio_8" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Portfolio_9" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Portfolio_10" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -550,6 +551,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.002704847806387689</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-8.94677942</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-37.52130922</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1979311.196890213</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.008568017914404365</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-30.52504891</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-72.67494342000001</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8568017.914404366</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0004080284091883962</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-6.65603247</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-32.16857262</v>
+      </c>
+      <c r="G4" t="n">
+        <v>387626.9887289764</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0006722011667048397</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-14.64317701</v>
+      </c>
+      <c r="F5" t="n">
+        <v>132.83828812</v>
+      </c>
+      <c r="G5" t="n">
+        <v>672201.1667048397</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.01065709523064798</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-20.70376038</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-31.93101974</v>
+      </c>
+      <c r="G6" t="n">
+        <v>10657095.23064798</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>9.147591055171223e-07</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-21.79310835</v>
+      </c>
+      <c r="G7" t="n">
+        <v>595325.9877432152</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0008656700088784723</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.76190991</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-7.85421033</v>
+      </c>
+      <c r="G8" t="n">
+        <v>447334977.0879506</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0003042254149311844</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-1.38908169</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-8.839105760000001</v>
+      </c>
+      <c r="G9" t="n">
+        <v>304225.4149311844</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>4.129126872340216e-07</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-18.58659469</v>
+      </c>
+      <c r="F10" t="n">
+        <v>111.5939569</v>
+      </c>
+      <c r="G10" t="n">
+        <v>170233.9398429848</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.007277902949556759</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-9.414047</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-56.88438263</v>
+      </c>
+      <c r="G11" t="n">
+        <v>6842821.949206429</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0001685386623809436</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-8.78987291</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-25.41153739</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1685386.623809436</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.01139410892411404</v>
+      </c>
+      <c r="E13" t="n">
+        <v>23.00092905</v>
+      </c>
+      <c r="F13" t="n">
+        <v>159.77483556</v>
+      </c>
+      <c r="G13" t="n">
+        <v>11156356.04013723</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0004406867589434575</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-9.330244609999999</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-37.78910075</v>
+      </c>
+      <c r="G14" t="n">
+        <v>440686.7589434575</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.00398933119452439</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-1.06726886</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-24.96320903</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3789834.180243832</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>3.834384532251995e-05</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-4.53877699</v>
+      </c>
+      <c r="F16" t="n">
+        <v>12.93320967</v>
+      </c>
+      <c r="G16" t="n">
+        <v>258819242.7203798</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.3340016079026149</v>
+      </c>
+      <c r="E17" t="n">
+        <v>6.11049342</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2.608921</v>
+      </c>
+      <c r="G17" t="n">
+        <v>333151904.138093</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>5.813453340343969e-05</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-3.8700873</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-16.35587602</v>
+      </c>
+      <c r="G18" t="n">
+        <v>5813453.340343969</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2.013499993233641e-06</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-19.5187442</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-53.37610903</v>
+      </c>
+      <c r="G19" t="n">
+        <v>647984.1064772508</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.02200091358854646</v>
+      </c>
+      <c r="E20" t="n">
+        <v>9.04301115</v>
+      </c>
+      <c r="F20" t="n">
+        <v>49.85682636</v>
+      </c>
+      <c r="G20" t="n">
+        <v>22000879.24512035</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32598</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>GODCAT</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Godcat Exploding Kittens</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.000143432536973569</v>
+      </c>
+      <c r="E21" t="n">
+        <v>12.37098699</v>
+      </c>
+      <c r="F21" t="n">
+        <v>33.11285049</v>
+      </c>
+      <c r="G21" t="n">
+        <v>114305.4675052911</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-08T06:06:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>3.133505970777622e-06</v>
+      </c>
+      <c r="E22" t="n">
+        <v>13.5798743</v>
+      </c>
+      <c r="F22" t="n">
+        <v>12.25301216</v>
+      </c>
+      <c r="G22" t="n">
+        <v>21621186.06627505</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.001196599586471208</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-1.43521688</v>
+      </c>
+      <c r="F23" t="n">
+        <v>48.50002903</v>
+      </c>
+      <c r="G23" t="n">
+        <v>502837617.4079964</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>3.676849122950013e-05</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-0.00647189</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.84630341</v>
+      </c>
+      <c r="G24" t="n">
+        <v>235889.6167627089</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.00362838327705554</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-1.24029068</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-14.07926051</v>
+      </c>
+      <c r="G25" t="n">
+        <v>3628383.164575659</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.002487728576009428</v>
+      </c>
+      <c r="E26" t="n">
+        <v>113.21454037</v>
+      </c>
+      <c r="F26" t="n">
+        <v>94.49400042000001</v>
+      </c>
+      <c r="G26" t="n">
+        <v>2487724.10058572</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.09173216920544866</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-3.93909254</v>
+      </c>
+      <c r="F27" t="n">
+        <v>17.91482763</v>
+      </c>
+      <c r="G27" t="n">
+        <v>91732169.20544866</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.01684104604555013</v>
+      </c>
+      <c r="E28" t="n">
+        <v>10.2764604</v>
+      </c>
+      <c r="F28" t="n">
+        <v>37.19349239</v>
+      </c>
+      <c r="G28" t="n">
+        <v>16047926.09304086</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.06290337413840959</v>
+      </c>
+      <c r="E29" t="n">
+        <v>41.46886625</v>
+      </c>
+      <c r="F29" t="n">
+        <v>16.49678011</v>
+      </c>
+      <c r="G29" t="n">
+        <v>4405668.788973352</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0006680258020436667</v>
+      </c>
+      <c r="E30" t="n">
+        <v>41.5991673</v>
+      </c>
+      <c r="F30" t="n">
+        <v>6.20794133</v>
+      </c>
+      <c r="G30" t="n">
+        <v>618964.6437416918</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.0002922812334851252</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-20.51536289</v>
+      </c>
+      <c r="F31" t="n">
+        <v>2.6627881</v>
+      </c>
+      <c r="G31" t="n">
+        <v>194797.6639296504</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>1.420694869570915e-06</v>
+      </c>
+      <c r="E32" t="n">
+        <v>13.58703568</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-28.16675266</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1262835.481457364</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.003032837459599066</v>
+      </c>
+      <c r="E33" t="n">
+        <v>22.47557937</v>
+      </c>
+      <c r="F33" t="n">
+        <v>2.48008521</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2122985.229981497</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0001514945232037559</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-0.78998429</v>
+      </c>
+      <c r="F34" t="n">
+        <v>16.05602948</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1514945.232037559</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>2.371200920679468e-06</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.00893802</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-5.18559046</v>
+      </c>
+      <c r="G35" t="n">
+        <v>6981455.353439829</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0005652820440863182</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.81061153</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-9.745731230000001</v>
+      </c>
+      <c r="G36" t="n">
+        <v>16958461.32258955</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.000292049278443914</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-2.37771811</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-7.29645065</v>
+      </c>
+      <c r="G37" t="n">
+        <v>23522095.39475776</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.003633013949862818</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-1.09661752</v>
+      </c>
+      <c r="F38" t="n">
+        <v>23.14829337</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3553949.891597654</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0008390634686186863</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-2.00778836</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-16.01361609</v>
+      </c>
+      <c r="G39" t="n">
+        <v>720520.2780312627</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.05688203251254626</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-3.08887807</v>
+      </c>
+      <c r="F40" t="n">
+        <v>53.96821951</v>
+      </c>
+      <c r="G40" t="n">
+        <v>55498164.61728714</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.04805753465915372</v>
+      </c>
+      <c r="E41" t="n">
+        <v>5.87633191</v>
+      </c>
+      <c r="F41" t="n">
+        <v>46.09289645</v>
+      </c>
+      <c r="G41" t="n">
+        <v>44988467.89701646</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>8.848462002670772e-06</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-80.21568399</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-1.80033892</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3702067.330239353</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.001698053451408228</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-3.79241917</v>
+      </c>
+      <c r="F43" t="n">
+        <v>3.86476365</v>
+      </c>
+      <c r="G43" t="n">
+        <v>16980263.54763158</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.08579002854256056</v>
+      </c>
+      <c r="E44" t="n">
+        <v>12.0834254</v>
+      </c>
+      <c r="F44" t="n">
+        <v>17.12574807</v>
+      </c>
+      <c r="G44" t="n">
+        <v>51447278.86368516</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.000188329645937475</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-18.2811222</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-7.75823309</v>
+      </c>
+      <c r="G45" t="n">
+        <v>181657.665581357</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>3.068210407642013e-09</v>
+      </c>
+      <c r="E46" t="n">
+        <v>10.31654107</v>
+      </c>
+      <c r="F46" t="n">
+        <v>69.86668274</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1231132.2981506</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.004943938388955823</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-11.30483357</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-24.67209687</v>
+      </c>
+      <c r="G47" t="n">
+        <v>4943938.388955823</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1.569970224810299e-07</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-2.22005796</v>
+      </c>
+      <c r="F48" t="n">
+        <v>43.99247901</v>
+      </c>
+      <c r="G48" t="n">
+        <v>64550321.7292466</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>2.132505272941356e-06</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-10.22312679</v>
+      </c>
+      <c r="F49" t="n">
+        <v>12.00206556</v>
+      </c>
+      <c r="G49" t="n">
+        <v>897123.6432736992</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.01230426737080755</v>
+      </c>
+      <c r="E50" t="n">
+        <v>9.307470289999999</v>
+      </c>
+      <c r="F50" t="n">
+        <v>3.30781167</v>
+      </c>
+      <c r="G50" t="n">
+        <v>814037.5820316314</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.09846702125275726</v>
+      </c>
+      <c r="E51" t="n">
+        <v>10.1106336</v>
+      </c>
+      <c r="F51" t="n">
+        <v>97.89766713</v>
+      </c>
+      <c r="G51" t="n">
+        <v>97102578.93370385</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>1.179056529564701e-08</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.65972882</v>
+      </c>
+      <c r="F52" t="n">
+        <v>31.39055793</v>
+      </c>
+      <c r="G52" t="n">
+        <v>373823.588818875</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.007993812187023875</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-0.36848465</v>
+      </c>
+      <c r="F53" t="n">
+        <v>6.53282987</v>
+      </c>
+      <c r="G53" t="n">
+        <v>799381.2187023875</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>6.147903016396804e-05</v>
+      </c>
+      <c r="E54" t="n">
+        <v>2.28366912</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-13.65539972</v>
+      </c>
+      <c r="G54" t="n">
+        <v>23992738.42910422</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.0151411204509939</v>
+      </c>
+      <c r="E55" t="n">
+        <v>5.36743982</v>
+      </c>
+      <c r="F55" t="n">
+        <v>2.60056506</v>
+      </c>
+      <c r="G55" t="n">
+        <v>14261440.27919172</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.001018851276243828</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-1.38190911</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-2.30905431</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1018851.276243828</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.09548054712606092</v>
+      </c>
+      <c r="E57" t="n">
+        <v>2.06730337</v>
+      </c>
+      <c r="F57" t="n">
+        <v>8.367270169999999</v>
+      </c>
+      <c r="G57" t="n">
+        <v>19405539.44051917</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.006742672146112932</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-0.90918233</v>
+      </c>
+      <c r="F58" t="n">
+        <v>13.0829857</v>
+      </c>
+      <c r="G58" t="n">
+        <v>11429625.94786083</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>5.662929113118119e-05</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-3.55645728</v>
+      </c>
+      <c r="F59" t="n">
+        <v>12.45867548</v>
+      </c>
+      <c r="G59" t="n">
+        <v>53708813.66808007</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1.577133597034594e-05</v>
+      </c>
+      <c r="E60" t="n">
+        <v>6.37670068</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-11.86101194</v>
+      </c>
+      <c r="G60" t="n">
+        <v>136809.4312086846</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.03791441695849889</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-1.89819714</v>
+      </c>
+      <c r="F61" t="n">
+        <v>9.87569364</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3601869.611057395</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.0005913516130147355</v>
+      </c>
+      <c r="E62" t="n">
+        <v>4.2490544</v>
+      </c>
+      <c r="F62" t="n">
+        <v>5.24845459</v>
+      </c>
+      <c r="G62" t="n">
+        <v>9690941.112460783</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.01507912450336849</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-0.89440932</v>
+      </c>
+      <c r="F63" t="n">
+        <v>9.7926626</v>
+      </c>
+      <c r="G63" t="n">
+        <v>15076898.77739413</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0004697355521598344</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-7.75748307</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-49.87459366</v>
+      </c>
+      <c r="G64" t="n">
+        <v>435412.828403278</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>3.927991554477563e-06</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-10.25136278</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-0.57622283</v>
+      </c>
+      <c r="G65" t="n">
+        <v>2691537.515639607</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>1.197964351111679e-06</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-2.59535489</v>
+      </c>
+      <c r="F66" t="n">
+        <v>12.85472834</v>
+      </c>
+      <c r="G66" t="n">
+        <v>938861.2360785522</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.5748513924662344</v>
+      </c>
+      <c r="E67" t="n">
+        <v>8.39032548</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-17.55318571</v>
+      </c>
+      <c r="G67" t="n">
+        <v>49702269.93272892</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.207352401998236</v>
+      </c>
+      <c r="E68" t="n">
+        <v>12.02209272</v>
+      </c>
+      <c r="F68" t="n">
+        <v>91.36491098</v>
+      </c>
+      <c r="G68" t="n">
+        <v>115240123.2862941</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.003108647947968113</v>
+      </c>
+      <c r="E69" t="n">
+        <v>17.71770194</v>
+      </c>
+      <c r="F69" t="n">
+        <v>38.21092412</v>
+      </c>
+      <c r="G69" t="n">
+        <v>310864794.7968113</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.005767324337502817</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1.41630046</v>
+      </c>
+      <c r="F70" t="n">
+        <v>5.8953121</v>
+      </c>
+      <c r="G70" t="n">
+        <v>48577522.40980885</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>2.266311233799594e-07</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-4.24091109</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-21.71705673</v>
+      </c>
+      <c r="G71" t="n">
+        <v>95185071.81958295</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.0001056842679482847</v>
+      </c>
+      <c r="E72" t="n">
+        <v>25.41161831</v>
+      </c>
+      <c r="F72" t="n">
+        <v>65.93959150000001</v>
+      </c>
+      <c r="G72" t="n">
+        <v>44460314.68316388</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0002843993637129242</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.22308015</v>
+      </c>
+      <c r="F73" t="n">
+        <v>13.28893764</v>
+      </c>
+      <c r="G73" t="n">
+        <v>5510996.082565112</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>3.464428512013895e-07</v>
+      </c>
+      <c r="E74" t="n">
+        <v>2.41667814</v>
+      </c>
+      <c r="F74" t="n">
+        <v>9.463789390000001</v>
+      </c>
+      <c r="G74" t="n">
+        <v>306983.9926223097</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.01531444708514809</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-8.10043842</v>
+      </c>
+      <c r="F75" t="n">
+        <v>3.57787608</v>
+      </c>
+      <c r="G75" t="n">
+        <v>1455632.590355693</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.0008902716778346834</v>
+      </c>
+      <c r="E76" t="n">
+        <v>2.24522759</v>
+      </c>
+      <c r="F76" t="n">
+        <v>11.20515056</v>
+      </c>
+      <c r="G76" t="n">
+        <v>872934.2545153912</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.005892984211986351</v>
+      </c>
+      <c r="E77" t="n">
+        <v>14.802203</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-0.26590256</v>
+      </c>
+      <c r="G77" t="n">
+        <v>4105743.206325449</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.002763865484679367</v>
+      </c>
+      <c r="E78" t="n">
+        <v>18.40524637</v>
+      </c>
+      <c r="F78" t="n">
+        <v>65.50267239999999</v>
+      </c>
+      <c r="G78" t="n">
+        <v>2659492.075853095</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.01640546654783168</v>
+      </c>
+      <c r="E79" t="n">
+        <v>20.86058217</v>
+      </c>
+      <c r="F79" t="n">
+        <v>75.77308291999999</v>
+      </c>
+      <c r="G79" t="n">
+        <v>15585197.37102313</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>4.158983726051213</v>
+      </c>
+      <c r="E80" t="n">
+        <v>8.518887960000001</v>
+      </c>
+      <c r="F80" t="n">
+        <v>56.57222181</v>
+      </c>
+      <c r="G80" t="n">
+        <v>32315303.55141792</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0001848168135234323</v>
+      </c>
+      <c r="E81" t="n">
+        <v>1.15665231</v>
+      </c>
+      <c r="F81" t="n">
+        <v>1.6648907</v>
+      </c>
+      <c r="G81" t="n">
+        <v>118876.2869144502</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.002516491082288342</v>
+      </c>
+      <c r="E82" t="n">
+        <v>6.4465301</v>
+      </c>
+      <c r="F82" t="n">
+        <v>43.7014714</v>
+      </c>
+      <c r="G82" t="n">
+        <v>2358313.942543569</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>3.57375311635284e-08</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-1.84404402</v>
+      </c>
+      <c r="F83" t="n">
+        <v>3.97512212</v>
+      </c>
+      <c r="G83" t="n">
+        <v>27512945.6930298</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.0003726794572446383</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-3.764641</v>
+      </c>
+      <c r="F84" t="n">
+        <v>11.39671415</v>
+      </c>
+      <c r="G84" t="n">
+        <v>186134.7892073446</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.02595512003223477</v>
+      </c>
+      <c r="E85" t="n">
+        <v>27.47208364</v>
+      </c>
+      <c r="F85" t="n">
+        <v>126.6274303</v>
+      </c>
+      <c r="G85" t="n">
+        <v>25692857.01501633</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>9.081625697837684e-05</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-2.22000152</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-5.3865479</v>
+      </c>
+      <c r="G86" t="n">
+        <v>953570.6982729569</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>5.427689699751444e-05</v>
+      </c>
+      <c r="E87" t="n">
+        <v>3.44972628</v>
+      </c>
+      <c r="F87" t="n">
+        <v>68.64874911</v>
+      </c>
+      <c r="G87" t="n">
+        <v>123925250.9649649</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>9.828661537656138e-06</v>
+      </c>
+      <c r="E88" t="n">
+        <v>2.74501528</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-9.100888619999999</v>
+      </c>
+      <c r="G88" t="n">
+        <v>328901.6569538568</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.0002423859535094743</v>
+      </c>
+      <c r="E89" t="n">
+        <v>1.13249868</v>
+      </c>
+      <c r="F89" t="n">
+        <v>14.47141715</v>
+      </c>
+      <c r="G89" t="n">
+        <v>223578.3218227519</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.02787361043976213</v>
+      </c>
+      <c r="E90" t="n">
+        <v>24.53102963</v>
+      </c>
+      <c r="F90" t="n">
+        <v>68.03182524</v>
+      </c>
+      <c r="G90" t="n">
+        <v>25700719.51436111</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.0009083191239788502</v>
+      </c>
+      <c r="E91" t="n">
+        <v>1.13056318</v>
+      </c>
+      <c r="F91" t="n">
+        <v>11.1437202</v>
+      </c>
+      <c r="G91" t="n">
+        <v>727785.9076129938</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.006034658066206676</v>
+      </c>
+      <c r="E92" t="n">
+        <v>10.24705831</v>
+      </c>
+      <c r="F92" t="n">
+        <v>43.84697884</v>
+      </c>
+      <c r="G92" t="n">
+        <v>536414050.3241181</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.000505059597491424</v>
+      </c>
+      <c r="E93" t="n">
+        <v>4.52190993</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0.9518023</v>
+      </c>
+      <c r="G93" t="n">
+        <v>504514.2205014437</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.005331992879867511</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-3.94217826</v>
+      </c>
+      <c r="F94" t="n">
+        <v>82.09595619</v>
+      </c>
+      <c r="G94" t="n">
+        <v>75605573.58213414</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30089</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>KOKO</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Koala AI</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>2.853920928887545e-06</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-4.83272048</v>
+      </c>
+      <c r="F95" t="n">
+        <v>-21.28314461</v>
+      </c>
+      <c r="G95" t="n">
+        <v>26000314.84746402</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-25T05:26:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>1.456117052711724e-05</v>
+      </c>
+      <c r="E96" t="n">
+        <v>2.46898963</v>
+      </c>
+      <c r="F96" t="n">
+        <v>12.86475389</v>
+      </c>
+      <c r="G96" t="n">
+        <v>3640264.892720596</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.021163865059335</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-4.00464702</v>
+      </c>
+      <c r="F97" t="n">
+        <v>51.87726419</v>
+      </c>
+      <c r="G97" t="n">
+        <v>196874989.9239857</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30011</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>SKID</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Success Kid</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.02456577685165207</v>
+      </c>
+      <c r="E98" t="n">
+        <v>7.05292797</v>
+      </c>
+      <c r="F98" t="n">
+        <v>8.299706690000001</v>
+      </c>
+      <c r="G98" t="n">
+        <v>2130901.762578246</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-20T13:27:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30008</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>APU</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Apu Apustaja</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.0002556887345395912</v>
+      </c>
+      <c r="E99" t="n">
+        <v>3.26125081</v>
+      </c>
+      <c r="F99" t="n">
+        <v>5.34257043</v>
+      </c>
+      <c r="G99" t="n">
+        <v>81397616.63189244</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:03:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30007</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>HUND</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.006134319964585441</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0.54515557</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-0.65019415</v>
+      </c>
+      <c r="G100" t="n">
+        <v>2345930.263654379</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:00:29.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>29999</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>CHKN</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Chickencoin</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>6.838792781322726e-08</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-4.40833538</v>
+      </c>
+      <c r="F101" t="n">
+        <v>44.47847171</v>
+      </c>
+      <c r="G101" t="n">
+        <v>4393172.094793906</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-20T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>63758.4</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>150.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-09-26 12:21:59
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -17,6 +17,7 @@
     <sheet name="Portfolio_8" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Portfolio_9" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Portfolio_10" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Portfolio_11" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3832,6 +3833,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1257032183067232</v>
+      </c>
+      <c r="E2" t="n">
+        <v>39.21753757</v>
+      </c>
+      <c r="F2" t="n">
+        <v>263.27566258</v>
+      </c>
+      <c r="G2" t="n">
+        <v>124442640.1829403</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.002597523569609299</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-3.96784753</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-34.95644418</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1900775.146524829</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.01203273941607049</v>
+      </c>
+      <c r="E4" t="n">
+        <v>40.43784147</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-50.13951456</v>
+      </c>
+      <c r="G4" t="n">
+        <v>12032739.41607049</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0003165984829075004</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-22.4077354</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-38.10287519</v>
+      </c>
+      <c r="G5" t="n">
+        <v>300768.5587621253</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0004606750880184539</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-31.46767503</v>
+      </c>
+      <c r="F6" t="n">
+        <v>65.00291467</v>
+      </c>
+      <c r="G6" t="n">
+        <v>460675.0880184539</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.01072135916940863</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.60301553</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-33.4799032</v>
+      </c>
+      <c r="G7" t="n">
+        <v>10721359.16940862</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>9.164530104478733e-07</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.18517497</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-22.33854335</v>
+      </c>
+      <c r="G8" t="n">
+        <v>596428.3824829453</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0008447199357618783</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-2.42009922</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-14.31159395</v>
+      </c>
+      <c r="G9" t="n">
+        <v>436509026.8049506</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0003051451719496002</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.30232748</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-8.5161675</v>
+      </c>
+      <c r="G10" t="n">
+        <v>305145.1719496002</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4.214556830384805e-07</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2.06895939</v>
+      </c>
+      <c r="F11" t="n">
+        <v>95.93980345999999</v>
+      </c>
+      <c r="G11" t="n">
+        <v>173756.0109219752</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.00657090041294131</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-9.714371590000001</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-58.56170262</v>
+      </c>
+      <c r="G12" t="n">
+        <v>6178084.797690626</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0001386859173691264</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-17.71269843</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-32.34562593</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1386859.173691264</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.01165138881720668</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2.25800802</v>
+      </c>
+      <c r="F14" t="n">
+        <v>184.98234801</v>
+      </c>
+      <c r="G14" t="n">
+        <v>11408267.45404652</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0003761930058317112</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-14.63482889</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-47.28530258</v>
+      </c>
+      <c r="G15" t="n">
+        <v>376193.0058317112</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.003759163059612968</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-5.76959204</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-37.72816359</v>
+      </c>
+      <c r="G16" t="n">
+        <v>3571176.209181522</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>4.227588182467852e-05</v>
+      </c>
+      <c r="E17" t="n">
+        <v>10.25467443</v>
+      </c>
+      <c r="F17" t="n">
+        <v>23.04177394</v>
+      </c>
+      <c r="G17" t="n">
+        <v>285360310.8713253</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.3387331056285746</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.41660927</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-0.85365963</v>
+      </c>
+      <c r="G18" t="n">
+        <v>337870563.4392635</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>5.490787951996041e-05</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-5.55032215</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-32.55371155</v>
+      </c>
+      <c r="G19" t="n">
+        <v>5490787.951996041</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>2.381215859220631e-06</v>
+      </c>
+      <c r="E20" t="n">
+        <v>18.26252134</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-20.33896938</v>
+      </c>
+      <c r="G20" t="n">
+        <v>766322.3422159184</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.019789941679118</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-10.04945499</v>
+      </c>
+      <c r="F21" t="n">
+        <v>10.94308965</v>
+      </c>
+      <c r="G21" t="n">
+        <v>19789910.78701904</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32598</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>GODCAT</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Godcat Exploding Kittens</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0001280663736567868</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-10.71316428</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-1.42970646</v>
+      </c>
+      <c r="G22" t="n">
+        <v>102059.7349905611</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-08T06:06:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>4.092135691678503e-06</v>
+      </c>
+      <c r="E23" t="n">
+        <v>30.59287998</v>
+      </c>
+      <c r="F23" t="n">
+        <v>27.22717401</v>
+      </c>
+      <c r="G23" t="n">
+        <v>28235729.57043682</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.001013024230542687</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-15.34141897</v>
+      </c>
+      <c r="F24" t="n">
+        <v>15.68388513</v>
+      </c>
+      <c r="G24" t="n">
+        <v>425680334.4855781</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>3.686645730203501e-05</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.26644028</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.31388505</v>
+      </c>
+      <c r="G25" t="n">
+        <v>236518.1217280543</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.00350833033738326</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-3.30871715</v>
+      </c>
+      <c r="F26" t="n">
+        <v>123.03555848</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3508330.22862502</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.002156219068814631</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-13.32579086</v>
+      </c>
+      <c r="F27" t="n">
+        <v>51.97802161</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2156215.189776526</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.09011185988028278</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-1.76634799</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-23.42966413</v>
+      </c>
+      <c r="G28" t="n">
+        <v>90111859.88028277</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.01533792743004233</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-8.9253281</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-2.10736203</v>
+      </c>
+      <c r="G29" t="n">
+        <v>14615596.03554322</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.06449933798709807</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2.53716732</v>
+      </c>
+      <c r="F30" t="n">
+        <v>12.14500394</v>
+      </c>
+      <c r="G30" t="n">
+        <v>4517447.977495503</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.000838609977413669</v>
+      </c>
+      <c r="E31" t="n">
+        <v>25.53556687</v>
+      </c>
+      <c r="F31" t="n">
+        <v>31.47092557</v>
+      </c>
+      <c r="G31" t="n">
+        <v>777020.7742277446</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.0002652370526049117</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-9.25279415</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-3.13243815</v>
+      </c>
+      <c r="G32" t="n">
+        <v>176773.4370727298</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>1.48987810027319e-06</v>
+      </c>
+      <c r="E33" t="n">
+        <v>4.86967555</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-16.28724372</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1324330.879744888</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.002776205675260263</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-8.461771779999999</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-11.46869152</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1943343.064862929</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.0001404634868200291</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-7.28147536</v>
+      </c>
+      <c r="F35" t="n">
+        <v>2.4186144</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1404634.868200291</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>2.270491139855503e-06</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-4.24720571</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-2.01742639</v>
+      </c>
+      <c r="G36" t="n">
+        <v>6684938.583247386</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.0004889308414642734</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-13.50674472</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-23.26575906</v>
+      </c>
+      <c r="G37" t="n">
+        <v>14667925.2439282</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0002900376214113215</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-0.6888074</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-9.02024404</v>
+      </c>
+      <c r="G38" t="n">
+        <v>23360073.46176653</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.00379515023290657</v>
+      </c>
+      <c r="E39" t="n">
+        <v>4.46285881</v>
+      </c>
+      <c r="F39" t="n">
+        <v>15.94596483</v>
+      </c>
+      <c r="G39" t="n">
+        <v>3712557.657353452</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.0009501714861258692</v>
+      </c>
+      <c r="E40" t="n">
+        <v>13.24190859</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-20.5139009</v>
+      </c>
+      <c r="G40" t="n">
+        <v>815930.9146039285</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.06076730465823912</v>
+      </c>
+      <c r="E41" t="n">
+        <v>6.83040316</v>
+      </c>
+      <c r="F41" t="n">
+        <v>40.19880248</v>
+      </c>
+      <c r="G41" t="n">
+        <v>59288913.00654456</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.06317624083442268</v>
+      </c>
+      <c r="E42" t="n">
+        <v>31.45959584</v>
+      </c>
+      <c r="F42" t="n">
+        <v>33.40244642</v>
+      </c>
+      <c r="G42" t="n">
+        <v>59141658.07280417</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>1.031254898556439e-05</v>
+      </c>
+      <c r="E43" t="n">
+        <v>16.54623123</v>
+      </c>
+      <c r="F43" t="n">
+        <v>6.29778053</v>
+      </c>
+      <c r="G43" t="n">
+        <v>4314619.950837507</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.00166232492189826</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-2.10408745</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-20.10689366</v>
+      </c>
+      <c r="G44" t="n">
+        <v>16622983.94392902</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.1022723559551646</v>
+      </c>
+      <c r="E45" t="n">
+        <v>19.21240463</v>
+      </c>
+      <c r="F45" t="n">
+        <v>37.01232523</v>
+      </c>
+      <c r="G45" t="n">
+        <v>61331538.24819069</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.0001460256130991643</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-22.46275812</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-27.02020492</v>
+      </c>
+      <c r="G46" t="n">
+        <v>140852.3435523656</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>2.967338404792195e-09</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-3.28764946</v>
+      </c>
+      <c r="F47" t="n">
+        <v>25.75167559</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1190656.983818103</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.004889679775035227</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-1.09747755</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-30.72124983</v>
+      </c>
+      <c r="G48" t="n">
+        <v>4889679.775035227</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>1.762165873543477e-07</v>
+      </c>
+      <c r="E49" t="n">
+        <v>12.24199324</v>
+      </c>
+      <c r="F49" t="n">
+        <v>13.52833765</v>
+      </c>
+      <c r="G49" t="n">
+        <v>72452567.74934994</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>2.258697393393587e-06</v>
+      </c>
+      <c r="E50" t="n">
+        <v>5.91755256</v>
+      </c>
+      <c r="F50" t="n">
+        <v>11.81258966</v>
+      </c>
+      <c r="G50" t="n">
+        <v>950211.406426748</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.01597013005022112</v>
+      </c>
+      <c r="E51" t="n">
+        <v>29.79342507</v>
+      </c>
+      <c r="F51" t="n">
+        <v>31.80723633</v>
+      </c>
+      <c r="G51" t="n">
+        <v>1056567.259067898</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.003230697741859466</v>
+      </c>
+      <c r="E52" t="n">
+        <v>4.32833356</v>
+      </c>
+      <c r="F52" t="n">
+        <v>22.9246926</v>
+      </c>
+      <c r="G52" t="n">
+        <v>3230184.862131551</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.1351511057732246</v>
+      </c>
+      <c r="E53" t="n">
+        <v>37.2551988</v>
+      </c>
+      <c r="F53" t="n">
+        <v>127.68622922</v>
+      </c>
+      <c r="G53" t="n">
+        <v>133278337.7556922</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1.293418816109637e-08</v>
+      </c>
+      <c r="E54" t="n">
+        <v>9.69947443</v>
+      </c>
+      <c r="F54" t="n">
+        <v>51.04016355</v>
+      </c>
+      <c r="G54" t="n">
+        <v>410082.5122120933</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.008010638097723058</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.21048669</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-7.52268909</v>
+      </c>
+      <c r="G55" t="n">
+        <v>801063.8097723058</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>7.046226408565416e-05</v>
+      </c>
+      <c r="E56" t="n">
+        <v>14.61186668</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-3.22762529</v>
+      </c>
+      <c r="G56" t="n">
+        <v>27498525.38045388</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.01663391605347477</v>
+      </c>
+      <c r="E57" t="n">
+        <v>9.859214890000001</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-4.40917576</v>
+      </c>
+      <c r="G57" t="n">
+        <v>15667506.32316295</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.001181972593572147</v>
+      </c>
+      <c r="E58" t="n">
+        <v>16.01031683</v>
+      </c>
+      <c r="F58" t="n">
+        <v>2.93764956</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1181972.593572147</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.0968889683600533</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.4750871</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.95073436</v>
+      </c>
+      <c r="G59" t="n">
+        <v>19691788.04955803</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.006830112302086106</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1.37976757</v>
+      </c>
+      <c r="F60" t="n">
+        <v>5.05427594</v>
+      </c>
+      <c r="G60" t="n">
+        <v>11577847.34346467</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>5.862091421706208e-05</v>
+      </c>
+      <c r="E61" t="n">
+        <v>3.51694864</v>
+      </c>
+      <c r="F61" t="n">
+        <v>6.95772706</v>
+      </c>
+      <c r="G61" t="n">
+        <v>55597725.06145833</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>2.081857995060057e-05</v>
+      </c>
+      <c r="E62" t="n">
+        <v>32.00264068</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-2.96640778</v>
+      </c>
+      <c r="G62" t="n">
+        <v>180592.0618880656</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.03560700719704924</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-6.08583738</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-13.57599276</v>
+      </c>
+      <c r="G63" t="n">
+        <v>3382665.683719678</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0006584258500580371</v>
+      </c>
+      <c r="E64" t="n">
+        <v>11.3425305</v>
+      </c>
+      <c r="F64" t="n">
+        <v>6.27171958</v>
+      </c>
+      <c r="G64" t="n">
+        <v>10790139.06346675</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.015069791025612</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-0.06189668</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-0.25934022</v>
+      </c>
+      <c r="G65" t="n">
+        <v>15067566.67728817</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.0004753642870748806</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1.19827739</v>
+      </c>
+      <c r="F66" t="n">
+        <v>43.24033759</v>
+      </c>
+      <c r="G66" t="n">
+        <v>440630.2818798643</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>4.400282021712681e-06</v>
+      </c>
+      <c r="E67" t="n">
+        <v>12.02371392</v>
+      </c>
+      <c r="F67" t="n">
+        <v>6.41857258</v>
+      </c>
+      <c r="G67" t="n">
+        <v>3015160.286516809</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1.34976392548139e-06</v>
+      </c>
+      <c r="E68" t="n">
+        <v>12.67146007</v>
+      </c>
+      <c r="F68" t="n">
+        <v>19.55914147</v>
+      </c>
+      <c r="G68" t="n">
+        <v>1057828.66269412</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.5725539961357518</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-0.39965048</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-17.6872915</v>
+      </c>
+      <c r="G69" t="n">
+        <v>49503634.57399694</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.242255207855035</v>
+      </c>
+      <c r="E70" t="n">
+        <v>16.83260262</v>
+      </c>
+      <c r="F70" t="n">
+        <v>60.76104122</v>
+      </c>
+      <c r="G70" t="n">
+        <v>134638035.227056</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.003445302385575316</v>
+      </c>
+      <c r="E71" t="n">
+        <v>10.82960963</v>
+      </c>
+      <c r="F71" t="n">
+        <v>33.85006307</v>
+      </c>
+      <c r="G71" t="n">
+        <v>344530238.5575316</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.006624935244743597</v>
+      </c>
+      <c r="E72" t="n">
+        <v>14.87016955</v>
+      </c>
+      <c r="F72" t="n">
+        <v>12.34873138</v>
+      </c>
+      <c r="G72" t="n">
+        <v>55801082.35327893</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>2.363345922576993e-07</v>
+      </c>
+      <c r="E73" t="n">
+        <v>4.28161355</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-19.1759023</v>
+      </c>
+      <c r="G73" t="n">
+        <v>99260528.74823369</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.0001252333486282636</v>
+      </c>
+      <c r="E74" t="n">
+        <v>18.49762605</v>
+      </c>
+      <c r="F74" t="n">
+        <v>83.36504408</v>
+      </c>
+      <c r="G74" t="n">
+        <v>52684417.43442422</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.0002986405352246416</v>
+      </c>
+      <c r="E75" t="n">
+        <v>5.00745548</v>
+      </c>
+      <c r="F75" t="n">
+        <v>16.96707743</v>
+      </c>
+      <c r="G75" t="n">
+        <v>5786956.75767912</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>3.484551141089124e-07</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.58083545</v>
+      </c>
+      <c r="F76" t="n">
+        <v>6.23040081</v>
+      </c>
+      <c r="G76" t="n">
+        <v>308767.0644894733</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.01507868501367803</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-1.53947492</v>
+      </c>
+      <c r="F77" t="n">
+        <v>3.50938472</v>
+      </c>
+      <c r="G77" t="n">
+        <v>1433223.491751381</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.0008844817624051283</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-0.6503537700000001</v>
+      </c>
+      <c r="F78" t="n">
+        <v>4.15766864</v>
+      </c>
+      <c r="G78" t="n">
+        <v>871679.3614250054</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.00576544443761278</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-2.16426465</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-20.56419241</v>
+      </c>
+      <c r="G79" t="n">
+        <v>4016883.99736092</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.002490054775682085</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-9.906803010000001</v>
+      </c>
+      <c r="F80" t="n">
+        <v>15.04521482</v>
+      </c>
+      <c r="G80" t="n">
+        <v>2396021.434861872</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0149698376185981</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-8.750918029999999</v>
+      </c>
+      <c r="F81" t="n">
+        <v>23.71367465</v>
+      </c>
+      <c r="G81" t="n">
+        <v>14221349.52503711</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>4.565686117629194</v>
+      </c>
+      <c r="E82" t="n">
+        <v>9.77888875</v>
+      </c>
+      <c r="F82" t="n">
+        <v>66.38952107999999</v>
+      </c>
+      <c r="G82" t="n">
+        <v>35475381.13397884</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.0001828514831907147</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-1.06339369</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-3.24630512</v>
+      </c>
+      <c r="G83" t="n">
+        <v>117612.1639807206</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.003439066150160824</v>
+      </c>
+      <c r="E84" t="n">
+        <v>36.66116977</v>
+      </c>
+      <c r="F84" t="n">
+        <v>78.20814018999999</v>
+      </c>
+      <c r="G84" t="n">
+        <v>3222899.420680167</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>3.547896041095407e-08</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-0.72352718</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-1.62705858</v>
+      </c>
+      <c r="G85" t="n">
+        <v>27313882.05204042</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.0003778780873056329</v>
+      </c>
+      <c r="E86" t="n">
+        <v>1.39493336</v>
+      </c>
+      <c r="F86" t="n">
+        <v>3.72095725</v>
+      </c>
+      <c r="G86" t="n">
+        <v>188731.2454695824</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.02707369618033705</v>
+      </c>
+      <c r="E87" t="n">
+        <v>4.30965508</v>
+      </c>
+      <c r="F87" t="n">
+        <v>82.45503918999999</v>
+      </c>
+      <c r="G87" t="n">
+        <v>26800130.53168306</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>9.074312947538836e-05</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-0.08052247999999999</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-1.83497074</v>
+      </c>
+      <c r="G88" t="n">
+        <v>952802.8594915777</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>5.546034073346929e-05</v>
+      </c>
+      <c r="E89" t="n">
+        <v>2.18038208</v>
+      </c>
+      <c r="F89" t="n">
+        <v>35.49251601</v>
+      </c>
+      <c r="G89" t="n">
+        <v>126627294.9301502</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>9.873551764811638e-06</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.45672778</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-9.41880534</v>
+      </c>
+      <c r="G90" t="n">
+        <v>330403.8421736766</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.0001983400970486615</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-18.17178587</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-14.72753655</v>
+      </c>
+      <c r="G91" t="n">
+        <v>182950.1479200533</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.02664825209608226</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-4.39612352</v>
+      </c>
+      <c r="F92" t="n">
+        <v>11.5704808</v>
+      </c>
+      <c r="G92" t="n">
+        <v>24570884.1396594</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.0008854018503021599</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-2.52304208</v>
+      </c>
+      <c r="F93" t="n">
+        <v>1.25832312</v>
+      </c>
+      <c r="G93" t="n">
+        <v>709423.5629452472</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.006430337439471716</v>
+      </c>
+      <c r="E94" t="n">
+        <v>6.55678199</v>
+      </c>
+      <c r="F94" t="n">
+        <v>22.01898353</v>
+      </c>
+      <c r="G94" t="n">
+        <v>571585550.1695478</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.0004454162887250192</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-11.80916254</v>
+      </c>
+      <c r="F95" t="n">
+        <v>-8.653721620000001</v>
+      </c>
+      <c r="G95" t="n">
+        <v>444935.3161902141</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.005173838276600813</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-2.96614431</v>
+      </c>
+      <c r="F96" t="n">
+        <v>51.70211371</v>
+      </c>
+      <c r="G96" t="n">
+        <v>73363003.16539894</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30089</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>KOKO</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Koala AI</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>3.011379765905054e-06</v>
+      </c>
+      <c r="E97" t="n">
+        <v>5.51728099</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-19.54147106</v>
+      </c>
+      <c r="G97" t="n">
+        <v>27434825.27714386</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-25T05:26:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>1.481679752125882e-05</v>
+      </c>
+      <c r="E98" t="n">
+        <v>1.75553877</v>
+      </c>
+      <c r="F98" t="n">
+        <v>2.32697443</v>
+      </c>
+      <c r="G98" t="n">
+        <v>3704171.154286062</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.02084771043519136</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-1.49384162</v>
+      </c>
+      <c r="F99" t="n">
+        <v>17.69043325</v>
+      </c>
+      <c r="G99" t="n">
+        <v>193933989.3899057</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30011</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>SKID</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Success Kid</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.02597514812385736</v>
+      </c>
+      <c r="E100" t="n">
+        <v>5.73713293</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-0.07367993</v>
+      </c>
+      <c r="G100" t="n">
+        <v>2253154.429213026</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-20T13:27:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30008</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>APU</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Apu Apustaja</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.0003039300660564612</v>
+      </c>
+      <c r="E101" t="n">
+        <v>18.8672104</v>
+      </c>
+      <c r="F101" t="n">
+        <v>-1.47290745</v>
+      </c>
+      <c r="G101" t="n">
+        <v>96755076.22311349</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-20T12:03:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>64397</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>152.94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-09-27 12:21:52
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -18,6 +18,7 @@
     <sheet name="Portfolio_9" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Portfolio_10" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Portfolio_11" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Portfolio_12" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -7114,6 +7115,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.01922429057355912</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-14.36801626</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-14.36801626</v>
+      </c>
+      <c r="G2" t="n">
+        <v>19224290.57355912</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.02025016093641847</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-6.97175124</v>
+      </c>
+      <c r="F3" t="n">
+        <v>29.52281769</v>
+      </c>
+      <c r="G3" t="n">
+        <v>12382209.27279696</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.183441008529114</v>
+      </c>
+      <c r="E4" t="n">
+        <v>45.93183134</v>
+      </c>
+      <c r="F4" t="n">
+        <v>430.13482722</v>
+      </c>
+      <c r="G4" t="n">
+        <v>181601423.7875983</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.001311235924210212</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-49.519768</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-64.85310593</v>
+      </c>
+      <c r="G5" t="n">
+        <v>959515.7037763351</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.01073902133226073</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-10.75165047</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-53.27696892</v>
+      </c>
+      <c r="G6" t="n">
+        <v>10739021.33226073</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0003451135278705224</v>
+      </c>
+      <c r="E7" t="n">
+        <v>9.00669034</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-25.32358245</v>
+      </c>
+      <c r="G7" t="n">
+        <v>327857.8514769963</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0006575275989588826</v>
+      </c>
+      <c r="E8" t="n">
+        <v>42.73131238</v>
+      </c>
+      <c r="F8" t="n">
+        <v>192.515892</v>
+      </c>
+      <c r="G8" t="n">
+        <v>657527.5989588826</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.009892212887703072</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-7.733593</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-31.03117734</v>
+      </c>
+      <c r="G9" t="n">
+        <v>9892212.887703072</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>9.009072944650895e-07</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-1.69629166</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-17.77336257</v>
+      </c>
+      <c r="G10" t="n">
+        <v>586311.2175738359</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0008683392004512142</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2.79610599</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-7.59603304</v>
+      </c>
+      <c r="G11" t="n">
+        <v>448714281.8331649</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0003133457911230112</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2.68744844</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2.95622515</v>
+      </c>
+      <c r="G12" t="n">
+        <v>313345.7911230112</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>4.21857719667053e-07</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.09539238999999999</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-8.950400910000001</v>
+      </c>
+      <c r="G13" t="n">
+        <v>173921.760925206</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.004958847026708187</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-24.53321896</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-38.86107607</v>
+      </c>
+      <c r="G14" t="n">
+        <v>4662401.726472924</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0001376551312728215</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-0.74325217</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-36.09875913</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1376551.312728215</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.01672857168689157</v>
+      </c>
+      <c r="E16" t="n">
+        <v>43.57577409</v>
+      </c>
+      <c r="F16" t="n">
+        <v>82.26951384</v>
+      </c>
+      <c r="G16" t="n">
+        <v>16379508.30774887</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0003542584468863677</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-5.83066633</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-44.23773617</v>
+      </c>
+      <c r="G17" t="n">
+        <v>354258.4468863677</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.003749434512648617</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-0.25879556</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-23.73534679</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3561934.163833117</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>4.167408523979216e-05</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-1.4234986</v>
+      </c>
+      <c r="F19" t="n">
+        <v>8.18298723</v>
+      </c>
+      <c r="G19" t="n">
+        <v>281298210.8480391</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.3515592775927126</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.78651267</v>
+      </c>
+      <c r="F20" t="n">
+        <v>8.364362420000001</v>
+      </c>
+      <c r="G20" t="n">
+        <v>350664074.0794361</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>4.910925990268005e-05</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-10.56063295</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-29.40465151</v>
+      </c>
+      <c r="G21" t="n">
+        <v>4910925.990268005</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>2.032606414710454e-06</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-14.6399766</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-32.29858995</v>
+      </c>
+      <c r="G22" t="n">
+        <v>654132.930659141</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.01574165815644653</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-20.45626808</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-9.671246780000001</v>
+      </c>
+      <c r="G23" t="n">
+        <v>15741633.58371815</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32598</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>GODCAT</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Godcat Exploding Kittens</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0001394609072304512</v>
+      </c>
+      <c r="E24" t="n">
+        <v>8.89736568</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-1.68266177</v>
+      </c>
+      <c r="G24" t="n">
+        <v>111140.3628217655</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-08T06:06:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>3.58765953251946e-06</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-12.32794309</v>
+      </c>
+      <c r="F25" t="n">
+        <v>11.32697293</v>
+      </c>
+      <c r="G25" t="n">
+        <v>24754844.89847602</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.001105610538739647</v>
+      </c>
+      <c r="E26" t="n">
+        <v>9.139594629999999</v>
+      </c>
+      <c r="F26" t="n">
+        <v>36.59927131</v>
+      </c>
+      <c r="G26" t="n">
+        <v>464626664.3600332</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>3.624333239258288e-05</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-1.69022183</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-4.29662071</v>
+      </c>
+      <c r="G27" t="n">
+        <v>232520.4408015107</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.003206091299808995</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-8.61489679</v>
+      </c>
+      <c r="F28" t="n">
+        <v>253.50786193</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3206091.200420165</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.002180914819650806</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1.14532661</v>
+      </c>
+      <c r="F29" t="n">
+        <v>58.72753818</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2180910.896185046</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0906220362710584</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.56615898</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-0.53307107</v>
+      </c>
+      <c r="G30" t="n">
+        <v>90622036.2710584</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.01479812430827209</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-3.51940068</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-11.0239296</v>
+      </c>
+      <c r="G31" t="n">
+        <v>14101214.64975927</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.11073884032494</v>
+      </c>
+      <c r="E32" t="n">
+        <v>71.68988672</v>
+      </c>
+      <c r="F32" t="n">
+        <v>57.31951628</v>
+      </c>
+      <c r="G32" t="n">
+        <v>7756001.315178845</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.0006201890444715286</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-26.04559197</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-0.46919143</v>
+      </c>
+      <c r="G33" t="n">
+        <v>574641.1138453712</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.000282187685586427</v>
+      </c>
+      <c r="E34" t="n">
+        <v>6.39074851</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-42.36529585</v>
+      </c>
+      <c r="G34" t="n">
+        <v>188070.5828646648</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1.361908292190658e-06</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-8.589280430000001</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-23.94723421</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1210580.33963516</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.002653311984314675</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-4.42667818</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-5.92208713</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1857317.521387253</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.0001427928459880224</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.65833785</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-0.95364399</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1427928.459880224</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2.502512432709983e-06</v>
+      </c>
+      <c r="E38" t="n">
+        <v>10.21899134</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2.45318983</v>
+      </c>
+      <c r="G38" t="n">
+        <v>7368071.877851021</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0005979683880989433</v>
+      </c>
+      <c r="E39" t="n">
+        <v>22.30122082</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-12.16211811</v>
+      </c>
+      <c r="G39" t="n">
+        <v>17939051.6429683</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.0003036331501066676</v>
+      </c>
+      <c r="E40" t="n">
+        <v>4.68750524</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-6.87145345</v>
+      </c>
+      <c r="G40" t="n">
+        <v>24455078.12884881</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.003973148767358751</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4.69015779</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-0.3604742</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3886682.469685858</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.000784417018149249</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-17.44468976</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-32.31120253</v>
+      </c>
+      <c r="G42" t="n">
+        <v>673594.2978661625</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.05839904601381438</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-3.897258</v>
+      </c>
+      <c r="F43" t="n">
+        <v>9.45187636</v>
+      </c>
+      <c r="G43" t="n">
+        <v>56978271.09909149</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.06029314666133929</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-4.56357348</v>
+      </c>
+      <c r="F44" t="n">
+        <v>13.28352399</v>
+      </c>
+      <c r="G44" t="n">
+        <v>56442685.04870354</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>1.248040105589145e-05</v>
+      </c>
+      <c r="E45" t="n">
+        <v>21.02149598</v>
+      </c>
+      <c r="F45" t="n">
+        <v>5.28562018</v>
+      </c>
+      <c r="G45" t="n">
+        <v>5222865.650415123</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.003370953554298459</v>
+      </c>
+      <c r="E46" t="n">
+        <v>102.78547893</v>
+      </c>
+      <c r="F46" t="n">
+        <v>80.92442843000001</v>
+      </c>
+      <c r="G46" t="n">
+        <v>33708997.54936217</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.1174923285394645</v>
+      </c>
+      <c r="E47" t="n">
+        <v>14.881805</v>
+      </c>
+      <c r="F47" t="n">
+        <v>61.39073827</v>
+      </c>
+      <c r="G47" t="n">
+        <v>70458778.17507404</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.0001943827239397655</v>
+      </c>
+      <c r="E48" t="n">
+        <v>33.11549927</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-10.52007529</v>
+      </c>
+      <c r="G48" t="n">
+        <v>187496.3003539355</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>5.606944990303377e-09</v>
+      </c>
+      <c r="E49" t="n">
+        <v>88.95536085000001</v>
+      </c>
+      <c r="F49" t="n">
+        <v>101.66390512</v>
+      </c>
+      <c r="G49" t="n">
+        <v>2249810.200214142</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.005116632851761146</v>
+      </c>
+      <c r="E50" t="n">
+        <v>4.64147116</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-19.49580932</v>
+      </c>
+      <c r="G50" t="n">
+        <v>5116632.851761146</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>2.089051023644835e-07</v>
+      </c>
+      <c r="E51" t="n">
+        <v>18.55019184</v>
+      </c>
+      <c r="F51" t="n">
+        <v>22.72180709</v>
+      </c>
+      <c r="G51" t="n">
+        <v>85892658.06068392</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>2.765732311831614e-06</v>
+      </c>
+      <c r="E52" t="n">
+        <v>22.4481119</v>
+      </c>
+      <c r="F52" t="n">
+        <v>18.23724615</v>
+      </c>
+      <c r="G52" t="n">
+        <v>1163515.926264442</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.01422851912956959</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-10.90542729</v>
+      </c>
+      <c r="F53" t="n">
+        <v>17.88676906</v>
+      </c>
+      <c r="G53" t="n">
+        <v>941344.0848665057</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.004419176848970646</v>
+      </c>
+      <c r="E54" t="n">
+        <v>36.78707208</v>
+      </c>
+      <c r="F54" t="n">
+        <v>38.37626799</v>
+      </c>
+      <c r="G54" t="n">
+        <v>4418475.295807518</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.124360179122185</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-7.98434211</v>
+      </c>
+      <c r="F55" t="n">
+        <v>68.20990440999999</v>
+      </c>
+      <c r="G55" t="n">
+        <v>122636939.3101081</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>1.220001126652141e-08</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-5.6762503</v>
+      </c>
+      <c r="F56" t="n">
+        <v>37.21282963</v>
+      </c>
+      <c r="G56" t="n">
+        <v>386805.2023735876</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.009599200290082713</v>
+      </c>
+      <c r="E57" t="n">
+        <v>19.83065735</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-3.04400705</v>
+      </c>
+      <c r="G57" t="n">
+        <v>959920.0290082714</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>7.381624699146511e-05</v>
+      </c>
+      <c r="E58" t="n">
+        <v>4.75997039</v>
+      </c>
+      <c r="F58" t="n">
+        <v>4.55796732</v>
+      </c>
+      <c r="G58" t="n">
+        <v>28807447.0459419</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.01439154897577744</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-13.48069252</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-12.29746771</v>
+      </c>
+      <c r="G59" t="n">
+        <v>13555417.96972099</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.00141533698206841</v>
+      </c>
+      <c r="E60" t="n">
+        <v>19.74363786</v>
+      </c>
+      <c r="F60" t="n">
+        <v>26.61433352</v>
+      </c>
+      <c r="G60" t="n">
+        <v>1415336.98206841</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.09827222442762501</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1.42767138</v>
+      </c>
+      <c r="F61" t="n">
+        <v>1.8911477</v>
+      </c>
+      <c r="G61" t="n">
+        <v>19972922.0709222</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.006824696513267945</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-0.09841577999999999</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-6.41112984</v>
+      </c>
+      <c r="G62" t="n">
+        <v>11568666.9415316</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>5.839375439120126e-05</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-0.38750645</v>
+      </c>
+      <c r="F63" t="n">
+        <v>2.49813099</v>
+      </c>
+      <c r="G63" t="n">
+        <v>55382280.28868572</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>1.856089856000747e-05</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-10.84455038</v>
+      </c>
+      <c r="F64" t="n">
+        <v>13.85629808</v>
+      </c>
+      <c r="G64" t="n">
+        <v>161007.6647591077</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.03495047141300782</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-1.84383872</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-7.24244171</v>
+      </c>
+      <c r="G65" t="n">
+        <v>3320294.784235743</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.0009790833256696021</v>
+      </c>
+      <c r="E66" t="n">
+        <v>48.70062067</v>
+      </c>
+      <c r="F66" t="n">
+        <v>93.20758239</v>
+      </c>
+      <c r="G66" t="n">
+        <v>16045003.75822928</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.01478951686892456</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-1.85984103</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-1.64205984</v>
+      </c>
+      <c r="G67" t="n">
+        <v>14787333.88994352</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.0006631139694819526</v>
+      </c>
+      <c r="E68" t="n">
+        <v>39.49595868</v>
+      </c>
+      <c r="F68" t="n">
+        <v>38.72170142</v>
+      </c>
+      <c r="G68" t="n">
+        <v>614661.4359468749</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>5.687967239815501e-06</v>
+      </c>
+      <c r="E69" t="n">
+        <v>29.26369746</v>
+      </c>
+      <c r="F69" t="n">
+        <v>11.24990496</v>
+      </c>
+      <c r="G69" t="n">
+        <v>3897507.670616336</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1.409658951345602e-06</v>
+      </c>
+      <c r="E70" t="n">
+        <v>4.43744456</v>
+      </c>
+      <c r="F70" t="n">
+        <v>19.84623928</v>
+      </c>
+      <c r="G70" t="n">
+        <v>1104769.223125362</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.418459175098039</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-26.91358755</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-21.12524376</v>
+      </c>
+      <c r="G71" t="n">
+        <v>36180430.54104885</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.2081372469209708</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-14.08347884</v>
+      </c>
+      <c r="F72" t="n">
+        <v>35.30250088</v>
+      </c>
+      <c r="G72" t="n">
+        <v>115676315.7339846</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.004297741590755248</v>
+      </c>
+      <c r="E73" t="n">
+        <v>24.74207224</v>
+      </c>
+      <c r="F73" t="n">
+        <v>74.22811079</v>
+      </c>
+      <c r="G73" t="n">
+        <v>429774159.0755247</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.006443938680213594</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-2.73205032</v>
+      </c>
+      <c r="F74" t="n">
+        <v>4.36935085</v>
+      </c>
+      <c r="G74" t="n">
+        <v>54276568.70448323</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>2.698193499453035e-07</v>
+      </c>
+      <c r="E75" t="n">
+        <v>14.16836925</v>
+      </c>
+      <c r="F75" t="n">
+        <v>2.98560309</v>
+      </c>
+      <c r="G75" t="n">
+        <v>113324126.9770275</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.0001124202840889473</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-10.23135186</v>
+      </c>
+      <c r="F76" t="n">
+        <v>52.5745476</v>
+      </c>
+      <c r="G76" t="n">
+        <v>47294089.31337924</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.000299533430799633</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.29898673</v>
+      </c>
+      <c r="F77" t="n">
+        <v>10.51715469</v>
+      </c>
+      <c r="G77" t="n">
+        <v>5804258.990538138</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>3.666284073727295e-07</v>
+      </c>
+      <c r="E78" t="n">
+        <v>5.21539003</v>
+      </c>
+      <c r="F78" t="n">
+        <v>4.16342285</v>
+      </c>
+      <c r="G78" t="n">
+        <v>324870.4711722097</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.01487451946121576</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-1.35400104</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-2.13588779</v>
+      </c>
+      <c r="G79" t="n">
+        <v>1413817.630714435</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.0009001657068367899</v>
+      </c>
+      <c r="E80" t="n">
+        <v>1.77323548</v>
+      </c>
+      <c r="F80" t="n">
+        <v>1.8167671</v>
+      </c>
+      <c r="G80" t="n">
+        <v>893437.4490879581</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.005234645975560537</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-9.20654891</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-33.88265076</v>
+      </c>
+      <c r="G81" t="n">
+        <v>3647067.607468821</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.002402392770689188</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-3.520485</v>
+      </c>
+      <c r="F82" t="n">
+        <v>-2.22083122</v>
+      </c>
+      <c r="G82" t="n">
+        <v>2311669.859532203</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.01323869225366162</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-11.56422273</v>
+      </c>
+      <c r="F83" t="n">
+        <v>4.89638159</v>
+      </c>
+      <c r="G83" t="n">
+        <v>12576760.99036768</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>6.636912806814102</v>
+      </c>
+      <c r="E84" t="n">
+        <v>45.36506969</v>
+      </c>
+      <c r="F84" t="n">
+        <v>116.5938234</v>
+      </c>
+      <c r="G84" t="n">
+        <v>51568812.50894558</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.0001848918430864088</v>
+      </c>
+      <c r="E85" t="n">
+        <v>1.11585636</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-5.35362753</v>
+      </c>
+      <c r="G85" t="n">
+        <v>118924.5467869446</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.004145733015957523</v>
+      </c>
+      <c r="E86" t="n">
+        <v>20.54821963</v>
+      </c>
+      <c r="F86" t="n">
+        <v>103.07696404</v>
+      </c>
+      <c r="G86" t="n">
+        <v>3885147.872133636</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>3.60075095539323e-08</v>
+      </c>
+      <c r="E87" t="n">
+        <v>1.48975375</v>
+      </c>
+      <c r="F87" t="n">
+        <v>-5.18333802</v>
+      </c>
+      <c r="G87" t="n">
+        <v>27720791.63402347</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.0003134928277675131</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-17.03863275</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-12.78523756</v>
+      </c>
+      <c r="G88" t="n">
+        <v>156574.0216698245</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.03376845100264025</v>
+      </c>
+      <c r="E89" t="n">
+        <v>24.72789374</v>
+      </c>
+      <c r="F89" t="n">
+        <v>82.28678703999999</v>
+      </c>
+      <c r="G89" t="n">
+        <v>33427238.33108465</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>9.056087640485017e-05</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-0.20084504</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-5.72478077</v>
+      </c>
+      <c r="G90" t="n">
+        <v>950889.2022509268</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>5.532077116017575e-05</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-0.25165654</v>
+      </c>
+      <c r="F91" t="n">
+        <v>34.90056727</v>
+      </c>
+      <c r="G91" t="n">
+        <v>126308629.0639297</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>1.001930842876432e-05</v>
+      </c>
+      <c r="E92" t="n">
+        <v>1.47623335</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-8.378587230000001</v>
+      </c>
+      <c r="G92" t="n">
+        <v>335281.373880556</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.0002048102821001787</v>
+      </c>
+      <c r="E93" t="n">
+        <v>3.26216693</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-9.278051169999999</v>
+      </c>
+      <c r="G93" t="n">
+        <v>188918.2871408119</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.03488953993813326</v>
+      </c>
+      <c r="E94" t="n">
+        <v>30.92618537</v>
+      </c>
+      <c r="F94" t="n">
+        <v>51.4957811</v>
+      </c>
+      <c r="G94" t="n">
+        <v>32169721.31661589</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.001064732838738235</v>
+      </c>
+      <c r="E95" t="n">
+        <v>20.25419174</v>
+      </c>
+      <c r="F95" t="n">
+        <v>20.57180247</v>
+      </c>
+      <c r="G95" t="n">
+        <v>853111.5716380189</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.006303110320150174</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-1.97854499</v>
+      </c>
+      <c r="F96" t="n">
+        <v>14.24649999</v>
+      </c>
+      <c r="G96" t="n">
+        <v>560276472.8966349</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.0005046918965562042</v>
+      </c>
+      <c r="E97" t="n">
+        <v>13.30791202</v>
+      </c>
+      <c r="F97" t="n">
+        <v>14.26562377</v>
+      </c>
+      <c r="G97" t="n">
+        <v>504146.9166196216</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.005096257655981713</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-1.49947904</v>
+      </c>
+      <c r="F98" t="n">
+        <v>1.08398773</v>
+      </c>
+      <c r="G98" t="n">
+        <v>72262940.30843003</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30089</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>KOKO</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Koala AI</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>2.958266789763607e-06</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-1.76374221</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-6.63978224</v>
+      </c>
+      <c r="G99" t="n">
+        <v>26950945.68251832</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-25T05:26:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>1.511546192792971e-05</v>
+      </c>
+      <c r="E100" t="n">
+        <v>2.01571498</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-0.04897397</v>
+      </c>
+      <c r="G100" t="n">
+        <v>3778836.686997496</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.02081806491951036</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-0.14220034</v>
+      </c>
+      <c r="F101" t="n">
+        <v>-10.52641338</v>
+      </c>
+      <c r="G101" t="n">
+        <v>193658214.592409</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>65355.91</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>155.64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-09-28 12:19:40
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -19,6 +19,7 @@
     <sheet name="Portfolio_10" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Portfolio_11" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Portfolio_12" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Portfolio_13" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -10396,6 +10397,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.01791600907824786</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-7.37843123</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-20.19557798</v>
+      </c>
+      <c r="G2" t="n">
+        <v>17916009.07824786</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.01829154434615698</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-9.67210382</v>
+      </c>
+      <c r="F3" t="n">
+        <v>16.99523628</v>
+      </c>
+      <c r="G3" t="n">
+        <v>11184589.13624909</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.3035437358627666</v>
+      </c>
+      <c r="E4" t="n">
+        <v>61.02835356</v>
+      </c>
+      <c r="F4" t="n">
+        <v>734.80882151</v>
+      </c>
+      <c r="G4" t="n">
+        <v>300499735.8904964</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.00126613729871839</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-3.4338164</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-58.54793026</v>
+      </c>
+      <c r="G5" t="n">
+        <v>926514.1374074186</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.01000302610512045</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-7.23011986</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-48.00354667</v>
+      </c>
+      <c r="G6" t="n">
+        <v>10003026.10512045</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0003042480205822212</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-11.83234734</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-30.24624208</v>
+      </c>
+      <c r="G7" t="n">
+        <v>289035.6195531102</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0218462740771731</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5.18384082</v>
+      </c>
+      <c r="F8" t="n">
+        <v>14.08168245</v>
+      </c>
+      <c r="G8" t="n">
+        <v>21846274.0771731</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0005885704003256729</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-9.29004321</v>
+      </c>
+      <c r="F9" t="n">
+        <v>167.53118494</v>
+      </c>
+      <c r="G9" t="n">
+        <v>588570.4003256728</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.008632111738062127</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-13.12621775</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-39.76704347</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8632111.738062127</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>8.252758292012198e-07</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-8.39503307</v>
+      </c>
+      <c r="F11" t="n">
+        <v>13.31710004</v>
+      </c>
+      <c r="G11" t="n">
+        <v>537090.1969891579</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0008724014075128601</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.02241562</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-4.91052541</v>
+      </c>
+      <c r="G12" t="n">
+        <v>450813427.3322704</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0004680907560577386</v>
+      </c>
+      <c r="E13" t="n">
+        <v>49.38472745</v>
+      </c>
+      <c r="F13" t="n">
+        <v>54.65173258</v>
+      </c>
+      <c r="G13" t="n">
+        <v>468090.7560577386</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>4.210661287215662e-07</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.50100277</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-52.0217083</v>
+      </c>
+      <c r="G14" t="n">
+        <v>173595.4070747178</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.00560541146363258</v>
+      </c>
+      <c r="E15" t="n">
+        <v>17.88772243</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-18.84107343</v>
+      </c>
+      <c r="G15" t="n">
+        <v>5270313.834016482</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0001091743806052702</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-16.91186729</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-49.2899673</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1091743.806052702</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.01951009832508904</v>
+      </c>
+      <c r="E17" t="n">
+        <v>16.4762053</v>
+      </c>
+      <c r="F17" t="n">
+        <v>68.90915462</v>
+      </c>
+      <c r="G17" t="n">
+        <v>19102994.77935725</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0003630511130310689</v>
+      </c>
+      <c r="E18" t="n">
+        <v>4.60836011</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-32.52773332</v>
+      </c>
+      <c r="G18" t="n">
+        <v>363051.1130310689</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.003712302959877632</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-1.05646714</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-27.31226067</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3526659.472162955</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>3.807210661827294e-05</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-8.70667956</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-14.42056272</v>
+      </c>
+      <c r="G20" t="n">
+        <v>256985016.307208</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.3304365617546082</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-6.41423257</v>
+      </c>
+      <c r="F21" t="n">
+        <v>5.78906115</v>
+      </c>
+      <c r="G21" t="n">
+        <v>329593741.9992828</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>4.654082738652662e-05</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-5.17770429</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-27.88037358</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4654082.738652662</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2.629117660430573e-06</v>
+      </c>
+      <c r="E23" t="n">
+        <v>29.21825431</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-22.51200677</v>
+      </c>
+      <c r="G23" t="n">
+        <v>846102.043080554</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.01325490922930736</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-17.87397935</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-19.96114306</v>
+      </c>
+      <c r="G24" t="n">
+        <v>13254888.53839405</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32598</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>GODCAT</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Godcat Exploding Kittens</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0001344836604896484</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-3.56891895</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-6.87394554</v>
+      </c>
+      <c r="G25" t="n">
+        <v>107173.8533560541</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-08T06:06:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2.859546248012099e-06</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-20.53453294</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-1.38154785</v>
+      </c>
+      <c r="G26" t="n">
+        <v>19730864.42788718</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.001201488863948448</v>
+      </c>
+      <c r="E27" t="n">
+        <v>8.43109054</v>
+      </c>
+      <c r="F27" t="n">
+        <v>44.25998511</v>
+      </c>
+      <c r="G27" t="n">
+        <v>504822360.1068751</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>3.655331002999358e-05</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.69898912</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.72360104</v>
+      </c>
+      <c r="G28" t="n">
+        <v>234509.1138106211</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.003081650813003331</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-3.84185439</v>
+      </c>
+      <c r="F29" t="n">
+        <v>217.02769894</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3081650.717472156</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.001456729747992036</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-33.21736402</v>
+      </c>
+      <c r="F30" t="n">
+        <v>5.40367535</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1456727.12733522</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.09400182512856957</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2.9926378</v>
+      </c>
+      <c r="F31" t="n">
+        <v>8.597803669999999</v>
+      </c>
+      <c r="G31" t="n">
+        <v>94001825.12856957</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.01633793860927922</v>
+      </c>
+      <c r="E32" t="n">
+        <v>11.0158367</v>
+      </c>
+      <c r="F32" t="n">
+        <v>9.1173746</v>
+      </c>
+      <c r="G32" t="n">
+        <v>15568512.2293</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.1635177318034099</v>
+      </c>
+      <c r="E33" t="n">
+        <v>47.57124912</v>
+      </c>
+      <c r="F33" t="n">
+        <v>156.1074991</v>
+      </c>
+      <c r="G33" t="n">
+        <v>11452564.78396299</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0005493139487277638</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-11.48644258</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-5.3857501</v>
+      </c>
+      <c r="G34" t="n">
+        <v>508971.227662846</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.0003567642587772045</v>
+      </c>
+      <c r="E35" t="n">
+        <v>39.3744087</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-24.66682171</v>
+      </c>
+      <c r="G35" t="n">
+        <v>237773.8842645522</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1.470540837580637e-06</v>
+      </c>
+      <c r="E36" t="n">
+        <v>7.24197819</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-9.266904609999999</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1307142.218593556</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.002687831141432551</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.54251393</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-3.32106971</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1881480.920082002</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0001662426929880256</v>
+      </c>
+      <c r="E38" t="n">
+        <v>16.39696021</v>
+      </c>
+      <c r="F38" t="n">
+        <v>14.60794891</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1662426.929880256</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>2.522646661379249e-06</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.93578679</v>
+      </c>
+      <c r="F39" t="n">
+        <v>9.21629899</v>
+      </c>
+      <c r="G39" t="n">
+        <v>7427352.480057499</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.0005835873160038652</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-2.40375202</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-15.4879266</v>
+      </c>
+      <c r="G40" t="n">
+        <v>17507619.48011596</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.0003166000016194732</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4.29159471</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-0.31064622</v>
+      </c>
+      <c r="G41" t="n">
+        <v>25499448.17447605</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.005363666931617021</v>
+      </c>
+      <c r="E42" t="n">
+        <v>34.99789571</v>
+      </c>
+      <c r="F42" t="n">
+        <v>39.82015802</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5246939.255739995</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.0008982715465234485</v>
+      </c>
+      <c r="E43" t="n">
+        <v>13.81222319</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-5.51926838</v>
+      </c>
+      <c r="G43" t="n">
+        <v>771363.4172563159</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.05876949736187929</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.8515382500000001</v>
+      </c>
+      <c r="F44" t="n">
+        <v>9.57794303</v>
+      </c>
+      <c r="G44" t="n">
+        <v>57339709.83447894</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.05310123553015365</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-12.75136883</v>
+      </c>
+      <c r="F45" t="n">
+        <v>7.67551574</v>
+      </c>
+      <c r="G45" t="n">
+        <v>49710066.2130032</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>1.269906081805019e-05</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1.50974847</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2.47105843</v>
+      </c>
+      <c r="G46" t="n">
+        <v>5314371.568838132</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.002723414351175088</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-19.47499536</v>
+      </c>
+      <c r="F47" t="n">
+        <v>53.22866563</v>
+      </c>
+      <c r="G47" t="n">
+        <v>27233708.85660413</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.1417235489142476</v>
+      </c>
+      <c r="E48" t="n">
+        <v>20.36919011</v>
+      </c>
+      <c r="F48" t="n">
+        <v>94.71462919</v>
+      </c>
+      <c r="G48" t="n">
+        <v>84989958.23186141</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.0001400234444774581</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-29.39033652</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-29.30096366</v>
+      </c>
+      <c r="G49" t="n">
+        <v>135062.8145867198</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>6.363265265176841e-09</v>
+      </c>
+      <c r="E50" t="n">
+        <v>13.81436078</v>
+      </c>
+      <c r="F50" t="n">
+        <v>206.88869957</v>
+      </c>
+      <c r="G50" t="n">
+        <v>2553286.883502774</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.005088690910490775</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-0.9253475799999999</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-13.73487739</v>
+      </c>
+      <c r="G51" t="n">
+        <v>5088690.910490775</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>2.01051992019711e-07</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-4.18132065</v>
+      </c>
+      <c r="F52" t="n">
+        <v>27.36239295</v>
+      </c>
+      <c r="G52" t="n">
+        <v>82663801.92494674</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>3.138043600563903e-06</v>
+      </c>
+      <c r="E53" t="n">
+        <v>13.46158076</v>
+      </c>
+      <c r="F53" t="n">
+        <v>38.29334802</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1320143.562321228</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.01299060398369034</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-8.752626940000001</v>
+      </c>
+      <c r="F54" t="n">
+        <v>8.691201469999999</v>
+      </c>
+      <c r="G54" t="n">
+        <v>859444.901295226</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.004570139949571769</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2.75682644</v>
+      </c>
+      <c r="F55" t="n">
+        <v>44.45052153</v>
+      </c>
+      <c r="G55" t="n">
+        <v>4569414.430714495</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.1141889375753751</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-7.7239122</v>
+      </c>
+      <c r="F56" t="n">
+        <v>96.42697785999999</v>
+      </c>
+      <c r="G56" t="n">
+        <v>112606639.087888</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>1.197044165169014e-08</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-2.05983587</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-2.12781368</v>
+      </c>
+      <c r="G57" t="n">
+        <v>379526.6253801948</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.009360118245553465</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-2.49064544</v>
+      </c>
+      <c r="F58" t="n">
+        <v>3.690866</v>
+      </c>
+      <c r="G58" t="n">
+        <v>936011.8245553465</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>7.105252800767907e-05</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-3.84308182</v>
+      </c>
+      <c r="F59" t="n">
+        <v>7.45350622</v>
+      </c>
+      <c r="G59" t="n">
+        <v>27728881.12691751</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.01176639930565385</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-18.30164004</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-21.34209548</v>
+      </c>
+      <c r="G60" t="n">
+        <v>11082786.21399449</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.001465359004464173</v>
+      </c>
+      <c r="E61" t="n">
+        <v>3.54057181</v>
+      </c>
+      <c r="F61" t="n">
+        <v>27.3368474</v>
+      </c>
+      <c r="G61" t="n">
+        <v>1465359.004464173</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.09602512340000938</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-2.32144725</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.84922834</v>
+      </c>
+      <c r="G62" t="n">
+        <v>19516219.53903731</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.006896122433286455</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.66026505</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-0.09524278999999999</v>
+      </c>
+      <c r="G63" t="n">
+        <v>11689742.31507828</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>5.650154972143398e-05</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-3.37216526</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.39690216</v>
+      </c>
+      <c r="G64" t="n">
+        <v>53587660.1195054</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>1.917217799060795e-05</v>
+      </c>
+      <c r="E65" t="n">
+        <v>3.28725646</v>
+      </c>
+      <c r="F65" t="n">
+        <v>11.12273515</v>
+      </c>
+      <c r="G65" t="n">
+        <v>166310.2460602265</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.03315531973922037</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-5.20848761</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-11.84680818</v>
+      </c>
+      <c r="G66" t="n">
+        <v>3149755.375225935</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.0008953690625594235</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-8.75519993</v>
+      </c>
+      <c r="F67" t="n">
+        <v>66.18663171</v>
+      </c>
+      <c r="G67" t="n">
+        <v>14673112.69338902</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.01381716838386933</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-6.54797729</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-4.55608854</v>
+      </c>
+      <c r="G68" t="n">
+        <v>13815128.92656813</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.0008130424879925737</v>
+      </c>
+      <c r="E69" t="n">
+        <v>22.60246954</v>
+      </c>
+      <c r="F69" t="n">
+        <v>79.8983502</v>
+      </c>
+      <c r="G69" t="n">
+        <v>753634.9498801145</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>4.788331576095808e-06</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-15.81646006</v>
+      </c>
+      <c r="F70" t="n">
+        <v>15.35681093</v>
+      </c>
+      <c r="G70" t="n">
+        <v>3281059.517475908</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1.412749504055322e-06</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.21924117</v>
+      </c>
+      <c r="F71" t="n">
+        <v>21.1362395</v>
+      </c>
+      <c r="G71" t="n">
+        <v>1107191.332042477</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.5332528180491652</v>
+      </c>
+      <c r="E72" t="n">
+        <v>27.44606383</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-0.009809699999999999</v>
+      </c>
+      <c r="G72" t="n">
+        <v>46105612.42856305</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.1905793301015024</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-9.22889155</v>
+      </c>
+      <c r="F73" t="n">
+        <v>26.75820425</v>
+      </c>
+      <c r="G73" t="n">
+        <v>105918158.5489165</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.004131510595536956</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-3.32249977</v>
+      </c>
+      <c r="F74" t="n">
+        <v>63.51084882</v>
+      </c>
+      <c r="G74" t="n">
+        <v>413151059.5536956</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.006639725440302194</v>
+      </c>
+      <c r="E75" t="n">
+        <v>2.91549828</v>
+      </c>
+      <c r="F75" t="n">
+        <v>11.17260526</v>
+      </c>
+      <c r="G75" t="n">
+        <v>55925658.50231242</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>2.447201003033214e-07</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-9.24954046</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-9.26480699</v>
+      </c>
+      <c r="G76" t="n">
+        <v>102782442.127395</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.0001211175644108144</v>
+      </c>
+      <c r="E77" t="n">
+        <v>7.02165722</v>
+      </c>
+      <c r="F77" t="n">
+        <v>67.45741742</v>
+      </c>
+      <c r="G77" t="n">
+        <v>50952948.1719855</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.0002750532153598538</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-8.440119510000001</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-2.3300621</v>
+      </c>
+      <c r="G78" t="n">
+        <v>5329889.534757101</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>3.612540499939913e-07</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-1.46588679</v>
+      </c>
+      <c r="F79" t="n">
+        <v>5.17350653</v>
+      </c>
+      <c r="G79" t="n">
+        <v>320108.2378624937</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.01506353351415327</v>
+      </c>
+      <c r="E80" t="n">
+        <v>1.24471682</v>
+      </c>
+      <c r="F80" t="n">
+        <v>3.75510699</v>
+      </c>
+      <c r="G80" t="n">
+        <v>1431783.347267002</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0008862043990389871</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-1.57904824</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-0.41018792</v>
+      </c>
+      <c r="G81" t="n">
+        <v>879580.494607173</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.00541924970338972</v>
+      </c>
+      <c r="E82" t="n">
+        <v>3.29386118</v>
+      </c>
+      <c r="F82" t="n">
+        <v>-25.22851868</v>
+      </c>
+      <c r="G82" t="n">
+        <v>3775684.175972998</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.002333080860177129</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-2.93313269</v>
+      </c>
+      <c r="F83" t="n">
+        <v>10.06914108</v>
+      </c>
+      <c r="G83" t="n">
+        <v>2244975.413731255</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.01243983788115172</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-6.21559475</v>
+      </c>
+      <c r="F84" t="n">
+        <v>10.02416053</v>
+      </c>
+      <c r="G84" t="n">
+        <v>11817849.13437312</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>6.46895845081794</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-2.81875464</v>
+      </c>
+      <c r="F85" t="n">
+        <v>133.11402571</v>
+      </c>
+      <c r="G85" t="n">
+        <v>50263807.16285539</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.0001827614000102058</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-1.2070649</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-3.55306581</v>
+      </c>
+      <c r="G86" t="n">
+        <v>117554.2214493665</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.00376496088325578</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-9.415924950000001</v>
+      </c>
+      <c r="F87" t="n">
+        <v>80.6001669</v>
+      </c>
+      <c r="G87" t="n">
+        <v>3528309.639801812</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>3.688259660188771e-08</v>
+      </c>
+      <c r="E88" t="n">
+        <v>2.41649458</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-2.38310246</v>
+      </c>
+      <c r="G88" t="n">
+        <v>28394487.37189922</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.0003134943032534697</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-0.00408401</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-14.54876165</v>
+      </c>
+      <c r="G89" t="n">
+        <v>156574.7586014213</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.02955405398686858</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-13.43695007</v>
+      </c>
+      <c r="F90" t="n">
+        <v>84.28733644</v>
+      </c>
+      <c r="G90" t="n">
+        <v>29255425.60988529</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>8.682823259005978e-05</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-4.12169577</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-9.3939602</v>
+      </c>
+      <c r="G91" t="n">
+        <v>911696.4421956276</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>5.085946376740764e-05</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-7.75182158</v>
+      </c>
+      <c r="F92" t="n">
+        <v>29.84183371</v>
+      </c>
+      <c r="G92" t="n">
+        <v>116122552.3192337</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>1.047874043299189e-05</v>
+      </c>
+      <c r="E93" t="n">
+        <v>1.12282648</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-4.64293355</v>
+      </c>
+      <c r="G93" t="n">
+        <v>350655.5880468639</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.0002066922977243896</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.91890681</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-6.7078853</v>
+      </c>
+      <c r="G94" t="n">
+        <v>190654.27014153</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.03127558786731869</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-10.32666185</v>
+      </c>
+      <c r="F95" t="n">
+        <v>38.66403822</v>
+      </c>
+      <c r="G95" t="n">
+        <v>28837495.34929544</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.001415209567052089</v>
+      </c>
+      <c r="E96" t="n">
+        <v>32.91687037</v>
+      </c>
+      <c r="F96" t="n">
+        <v>61.61019802</v>
+      </c>
+      <c r="G96" t="n">
+        <v>1133929.20178523</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.00588828159803752</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-7.624061</v>
+      </c>
+      <c r="F97" t="n">
+        <v>14.94527813</v>
+      </c>
+      <c r="G97" t="n">
+        <v>523402808.7092122</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.0005137549417599755</v>
+      </c>
+      <c r="E98" t="n">
+        <v>1.79612161</v>
+      </c>
+      <c r="F98" t="n">
+        <v>15.26012853</v>
+      </c>
+      <c r="G98" t="n">
+        <v>513200.1753024796</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.004859012359023802</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-4.83719484</v>
+      </c>
+      <c r="F99" t="n">
+        <v>7.60537555</v>
+      </c>
+      <c r="G99" t="n">
+        <v>68898894.78918464</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30089</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>KOKO</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Koala AI</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>2.900060225918946e-06</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-2.08145942</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-3.10659422</v>
+      </c>
+      <c r="G100" t="n">
+        <v>26420661.54926445</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-25T05:26:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>1.526167404648692e-05</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.71236172</v>
+      </c>
+      <c r="F101" t="n">
+        <v>6.61784109</v>
+      </c>
+      <c r="G101" t="n">
+        <v>3815389.438102424</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>65667.3</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>156.51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-09-29 12:20:11
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -20,6 +20,7 @@
     <sheet name="Portfolio_11" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Portfolio_12" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="Portfolio_13" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Portfolio_14" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -13678,6 +13679,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.009854378874898031</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-44.94880588</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-56.10501161</v>
+      </c>
+      <c r="G2" t="n">
+        <v>9854378.874898031</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.01653255181123346</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-9.61642441</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5.74447783</v>
+      </c>
+      <c r="G3" t="n">
+        <v>10109031.57672667</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2831534142467664</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-6.88055294</v>
+      </c>
+      <c r="F4" t="n">
+        <v>488.34065559</v>
+      </c>
+      <c r="G4" t="n">
+        <v>280313892.6777723</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.001264066607151696</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-0.163544</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-58.02804801</v>
+      </c>
+      <c r="G5" t="n">
+        <v>924998.8791390664</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.009820595160847221</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-1.70362013</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-46.80438545</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9820595.160847221</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0002946004558106231</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-3.17910638</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-24.49116988</v>
+      </c>
+      <c r="G7" t="n">
+        <v>279870.433020092</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.02138748351250649</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-2.08774148</v>
+      </c>
+      <c r="F8" t="n">
+        <v>9.39576372</v>
+      </c>
+      <c r="G8" t="n">
+        <v>21387483.51250649</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0004976505783487579</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-15.45451038</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-51.69757366</v>
+      </c>
+      <c r="G9" t="n">
+        <v>497650.5783487579</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.008290400677496845</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-3.73159765</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-38.58581658</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8290400.677496845</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>7.609781042866549e-07</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-7.79105878</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.57790951</v>
+      </c>
+      <c r="G11" t="n">
+        <v>495245.1840633058</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0008479616544912699</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-2.88886103</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-8.68370328</v>
+      </c>
+      <c r="G12" t="n">
+        <v>438184184.9583637</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0004955063631161489</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5.85689991</v>
+      </c>
+      <c r="F13" t="n">
+        <v>63.70952976</v>
+      </c>
+      <c r="G13" t="n">
+        <v>495506.3631161489</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>3.619011791704317e-07</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-11.68031255</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-24.27311936</v>
+      </c>
+      <c r="G14" t="n">
+        <v>149203.1256697322</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.007891066793932621</v>
+      </c>
+      <c r="E15" t="n">
+        <v>41.43574805</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-5.46280717</v>
+      </c>
+      <c r="G15" t="n">
+        <v>7419330.188164257</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0001135874948667834</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4.0356434</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-46.39560047</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1135874.948667834</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0223103127886146</v>
+      </c>
+      <c r="E17" t="n">
+        <v>12.47215961</v>
+      </c>
+      <c r="F17" t="n">
+        <v>49.32608369</v>
+      </c>
+      <c r="G17" t="n">
+        <v>21844779.13054224</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.000340516488954806</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-6.20701143</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-32.06610371</v>
+      </c>
+      <c r="G18" t="n">
+        <v>340516.488954806</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.003628121947544316</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-2.26709508</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-17.94670877</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3446688.153084153</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>3.548975158883721e-05</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-6.84417428</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-15.32277186</v>
+      </c>
+      <c r="G20" t="n">
+        <v>239554235.3944431</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.3234519190949197</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-2.14378873</v>
+      </c>
+      <c r="F21" t="n">
+        <v>12.04364095</v>
+      </c>
+      <c r="G21" t="n">
+        <v>322626914.5437782</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>4.864744067256559e-05</v>
+      </c>
+      <c r="E22" t="n">
+        <v>4.52876937</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-15.62931703</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4864744.067256559</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2.492509613224495e-06</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-5.19596552</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-16.2411732</v>
+      </c>
+      <c r="G23" t="n">
+        <v>802138.8726291494</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.01427862547156183</v>
+      </c>
+      <c r="E24" t="n">
+        <v>7.71065066</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-18.95076589</v>
+      </c>
+      <c r="G24" t="n">
+        <v>14278603.18262746</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32598</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>GODCAT</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Godcat Exploding Kittens</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0001327064802613445</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-1.32148413</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-13.47793514</v>
+      </c>
+      <c r="G25" t="n">
+        <v>105757.5678944447</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-08T06:06:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2.754593439756976e-06</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-3.4515224</v>
+      </c>
+      <c r="F26" t="n">
+        <v>4.84461544</v>
+      </c>
+      <c r="G26" t="n">
+        <v>19006690.2228197</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.001099154997377902</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-8.705455860000001</v>
+      </c>
+      <c r="F27" t="n">
+        <v>33.00236143</v>
+      </c>
+      <c r="G27" t="n">
+        <v>461778026.1259238</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>3.621189750682257e-05</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-0.9340126</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.191751</v>
+      </c>
+      <c r="G28" t="n">
+        <v>232318.7691281016</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.002928047035897361</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-5.10910155</v>
+      </c>
+      <c r="F29" t="n">
+        <v>196.45058766</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2928046.945127903</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.001606921918976972</v>
+      </c>
+      <c r="E30" t="n">
+        <v>10.29909257</v>
+      </c>
+      <c r="F30" t="n">
+        <v>8.762664060000001</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1606919.02812444</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.08362956078906192</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-10.9912565</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-0.3065855</v>
+      </c>
+      <c r="G31" t="n">
+        <v>83629560.78906192</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.01870704956625557</v>
+      </c>
+      <c r="E32" t="n">
+        <v>14.52099818</v>
+      </c>
+      <c r="F32" t="n">
+        <v>38.85734867</v>
+      </c>
+      <c r="G32" t="n">
+        <v>17826051.18744658</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.1454796595263247</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-11.01000169</v>
+      </c>
+      <c r="F33" t="n">
+        <v>153.83314647</v>
+      </c>
+      <c r="G33" t="n">
+        <v>10189202.15623593</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0009788661790548917</v>
+      </c>
+      <c r="E34" t="n">
+        <v>78.19794697</v>
+      </c>
+      <c r="F34" t="n">
+        <v>52.29314012</v>
+      </c>
+      <c r="G34" t="n">
+        <v>906976.2783652144</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.0002834783702702428</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-20.54182467</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-36.69956907</v>
+      </c>
+      <c r="G35" t="n">
+        <v>248806.4908200196</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1.708585646847998e-06</v>
+      </c>
+      <c r="E36" t="n">
+        <v>16.18753839</v>
+      </c>
+      <c r="F36" t="n">
+        <v>12.19662244</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1518736.762723864</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.002627934719728907</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-2.22842949</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-6.45030409</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1839553.444475581</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0001106835045629459</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-33.4205296</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-24.4580195</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1106835.045629459</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>2.43636981257062e-06</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-3.38444574</v>
+      </c>
+      <c r="F39" t="n">
+        <v>7.66824336</v>
+      </c>
+      <c r="G39" t="n">
+        <v>7173330.156289034</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.000589811855639746</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.06659954</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-11.5229039</v>
+      </c>
+      <c r="G40" t="n">
+        <v>17694355.66919238</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.0003358972928025847</v>
+      </c>
+      <c r="E41" t="n">
+        <v>6.09525118</v>
+      </c>
+      <c r="F41" t="n">
+        <v>8.04996379</v>
+      </c>
+      <c r="G41" t="n">
+        <v>27053681.50964499</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.007530726861256077</v>
+      </c>
+      <c r="E42" t="n">
+        <v>39.95338773</v>
+      </c>
+      <c r="F42" t="n">
+        <v>107.23716103</v>
+      </c>
+      <c r="G42" t="n">
+        <v>7366838.190429512</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.0009282961918303585</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3.68941087</v>
+      </c>
+      <c r="F43" t="n">
+        <v>5.54905553</v>
+      </c>
+      <c r="G43" t="n">
+        <v>797146.169805344</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.06732639271461593</v>
+      </c>
+      <c r="E44" t="n">
+        <v>14.54146273</v>
+      </c>
+      <c r="F44" t="n">
+        <v>39.37752183</v>
+      </c>
+      <c r="G44" t="n">
+        <v>65688426.74775612</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.05079020376142505</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-4.26641915</v>
+      </c>
+      <c r="F45" t="n">
+        <v>17.77082468</v>
+      </c>
+      <c r="G45" t="n">
+        <v>47546622.34777304</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>1.188174980945055e-05</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-6.4359957</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2.97418055</v>
+      </c>
+      <c r="G46" t="n">
+        <v>4972338.843014296</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.002863197161539527</v>
+      </c>
+      <c r="E47" t="n">
+        <v>5.13263104</v>
+      </c>
+      <c r="F47" t="n">
+        <v>59.63149052</v>
+      </c>
+      <c r="G47" t="n">
+        <v>28631514.64675697</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.1389507093081125</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-1.77315237</v>
+      </c>
+      <c r="F48" t="n">
+        <v>91.2609119</v>
+      </c>
+      <c r="G48" t="n">
+        <v>83327118.68180427</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.0001358534272439102</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-3.45307785</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-35.01363019</v>
+      </c>
+      <c r="G49" t="n">
+        <v>131040.5291291672</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>1.254327491680687e-08</v>
+      </c>
+      <c r="E50" t="n">
+        <v>97.12010099</v>
+      </c>
+      <c r="F50" t="n">
+        <v>493.39350877</v>
+      </c>
+      <c r="G50" t="n">
+        <v>5033041.683256355</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.005316209211015248</v>
+      </c>
+      <c r="E51" t="n">
+        <v>4.47105758</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-6.26265147</v>
+      </c>
+      <c r="G51" t="n">
+        <v>5316209.211015248</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>2.088529325515833e-07</v>
+      </c>
+      <c r="E52" t="n">
+        <v>3.89042742</v>
+      </c>
+      <c r="F52" t="n">
+        <v>44.45243037</v>
+      </c>
+      <c r="G52" t="n">
+        <v>85871208.11116232</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>3.135726881681332e-06</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-0.07382685</v>
+      </c>
+      <c r="F53" t="n">
+        <v>31.45619189</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1319168.94185452</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.01186070842269006</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-8.69610084</v>
+      </c>
+      <c r="F54" t="n">
+        <v>9.133874799999999</v>
+      </c>
+      <c r="G54" t="n">
+        <v>784692.1815512482</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.006552210891232533</v>
+      </c>
+      <c r="E55" t="n">
+        <v>43.15390037</v>
+      </c>
+      <c r="F55" t="n">
+        <v>108.90468287</v>
+      </c>
+      <c r="G55" t="n">
+        <v>6551170.714649129</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.1168771846241621</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2.36371738</v>
+      </c>
+      <c r="F56" t="n">
+        <v>60.50084616</v>
+      </c>
+      <c r="G56" t="n">
+        <v>115257635.5121434</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>1.194148801623239e-08</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-0.24178751</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.82152128</v>
+      </c>
+      <c r="G57" t="n">
+        <v>378608.6412424736</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.009638957360851618</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.97901274</v>
+      </c>
+      <c r="F58" t="n">
+        <v>8.614904620000001</v>
+      </c>
+      <c r="G58" t="n">
+        <v>963895.7360851618</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>7.010230032858354e-05</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-1.32132107</v>
+      </c>
+      <c r="F59" t="n">
+        <v>5.53761588</v>
+      </c>
+      <c r="G59" t="n">
+        <v>27358046.32207708</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.01104787924812614</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-6.04776554</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-23.73136042</v>
+      </c>
+      <c r="G60" t="n">
+        <v>10406011.27365907</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.001293763637187249</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-11.71012474</v>
+      </c>
+      <c r="F61" t="n">
+        <v>24.06772088</v>
+      </c>
+      <c r="G61" t="n">
+        <v>1293763.637187249</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.09304750383779464</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-3.04001336</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-0.72572347</v>
+      </c>
+      <c r="G62" t="n">
+        <v>18911045.86133382</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.006204485561207304</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-9.62140621</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-7.06304014</v>
+      </c>
+      <c r="G63" t="n">
+        <v>10517336.09862441</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>5.378480426492115e-05</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-4.84711951</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-6.05523953</v>
+      </c>
+      <c r="G64" t="n">
+        <v>51011022.25961334</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>1.849936371652294e-05</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-3.50932625</v>
+      </c>
+      <c r="F65" t="n">
+        <v>15.16207067</v>
+      </c>
+      <c r="G65" t="n">
+        <v>160473.8769460484</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.03137506461814214</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-5.37280007</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-19.06616236</v>
+      </c>
+      <c r="G66" t="n">
+        <v>2980631.138723503</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.0009194868216190926</v>
+      </c>
+      <c r="E67" t="n">
+        <v>2.64301819</v>
+      </c>
+      <c r="F67" t="n">
+        <v>73.11142618</v>
+      </c>
+      <c r="G67" t="n">
+        <v>15068349.26274619</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.01234362489655479</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-10.64191455</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-11.77024882</v>
+      </c>
+      <c r="G68" t="n">
+        <v>12341802.93888452</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.0008514059887134103</v>
+      </c>
+      <c r="E69" t="n">
+        <v>4.72164611</v>
+      </c>
+      <c r="F69" t="n">
+        <v>84.29018621</v>
+      </c>
+      <c r="G69" t="n">
+        <v>789195.2992713968</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>5.11447911929996e-06</v>
+      </c>
+      <c r="E70" t="n">
+        <v>6.81128379</v>
+      </c>
+      <c r="F70" t="n">
+        <v>9.422882939999999</v>
+      </c>
+      <c r="G70" t="n">
+        <v>3504542.265845621</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1.392017579563617e-06</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-1.46748765</v>
+      </c>
+      <c r="F71" t="n">
+        <v>18.13315832</v>
+      </c>
+      <c r="G71" t="n">
+        <v>1090943.435987384</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.4265057446515975</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-20.0222235</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-19.59225479</v>
+      </c>
+      <c r="G72" t="n">
+        <v>36876145.60275836</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.2133402659322273</v>
+      </c>
+      <c r="E73" t="n">
+        <v>11.80731572</v>
+      </c>
+      <c r="F73" t="n">
+        <v>49.61769855</v>
+      </c>
+      <c r="G73" t="n">
+        <v>118567990.0307337</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.004294421799384785</v>
+      </c>
+      <c r="E74" t="n">
+        <v>3.94313896</v>
+      </c>
+      <c r="F74" t="n">
+        <v>69.78870464000001</v>
+      </c>
+      <c r="G74" t="n">
+        <v>429442179.9384785</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.006344380403978737</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-4.5215036</v>
+      </c>
+      <c r="F75" t="n">
+        <v>10.89912122</v>
+      </c>
+      <c r="G75" t="n">
+        <v>53438000.5727359</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>2.507121672629878e-07</v>
+      </c>
+      <c r="E76" t="n">
+        <v>2.47564493</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-0.07674516000000001</v>
+      </c>
+      <c r="G76" t="n">
+        <v>105299110.2504549</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.0001187416477906485</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-1.91016093</v>
+      </c>
+      <c r="F77" t="n">
+        <v>52.87830554</v>
+      </c>
+      <c r="G77" t="n">
+        <v>49953423.80904792</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.0002730731980112245</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-0.71717587</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-5.77114849</v>
+      </c>
+      <c r="G78" t="n">
+        <v>5291521.418495343</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>3.649916907666628e-07</v>
+      </c>
+      <c r="E79" t="n">
+        <v>1.03462945</v>
+      </c>
+      <c r="F79" t="n">
+        <v>6.15614115</v>
+      </c>
+      <c r="G79" t="n">
+        <v>323420.171947448</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.01456283900686444</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-3.47248886</v>
+      </c>
+      <c r="F80" t="n">
+        <v>4.5550283</v>
+      </c>
+      <c r="G80" t="n">
+        <v>1384192.517603388</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0008860655891907268</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-0.01566341</v>
+      </c>
+      <c r="F81" t="n">
+        <v>1.62173634</v>
+      </c>
+      <c r="G81" t="n">
+        <v>879442.7222883699</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.005035847491240755</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-7.07482093</v>
+      </c>
+      <c r="F82" t="n">
+        <v>-11.98097486</v>
+      </c>
+      <c r="G82" t="n">
+        <v>3508561.27287379</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.002275732830453624</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-2.45803867</v>
+      </c>
+      <c r="F83" t="n">
+        <v>7.30512697</v>
+      </c>
+      <c r="G83" t="n">
+        <v>2189793.049950934</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.01072773322740219</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-13.76294808</v>
+      </c>
+      <c r="F84" t="n">
+        <v>3.47340156</v>
+      </c>
+      <c r="G84" t="n">
+        <v>10191349.28014859</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>7.107253163186583</v>
+      </c>
+      <c r="E85" t="n">
+        <v>10.0214082</v>
+      </c>
+      <c r="F85" t="n">
+        <v>157.31094104</v>
+      </c>
+      <c r="G85" t="n">
+        <v>55223357.07795975</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.0001781110920544334</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-2.54446943</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-3.27896313</v>
+      </c>
+      <c r="G86" t="n">
+        <v>114563.0902191937</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.003670510398012323</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-2.50879141</v>
+      </c>
+      <c r="F87" t="n">
+        <v>81.8131741</v>
+      </c>
+      <c r="G87" t="n">
+        <v>3439795.955887979</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>3.644660862946112e-08</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-1.24376214</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-2.35302149</v>
+      </c>
+      <c r="G88" t="n">
+        <v>28058837.06205273</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.0003273892445940203</v>
+      </c>
+      <c r="E89" t="n">
+        <v>4.43230636</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-10.31839801</v>
+      </c>
+      <c r="G89" t="n">
+        <v>163514.5883322939</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.02440344001335342</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-17.39522537</v>
+      </c>
+      <c r="F90" t="n">
+        <v>52.63579811</v>
+      </c>
+      <c r="G90" t="n">
+        <v>24156855.91740385</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>8.358272624662851e-05</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-3.73784683</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-9.77689808</v>
+      </c>
+      <c r="G91" t="n">
+        <v>877618.6255895994</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>5.14842905859121e-05</v>
+      </c>
+      <c r="E92" t="n">
+        <v>1.22849737</v>
+      </c>
+      <c r="F92" t="n">
+        <v>34.3279809</v>
+      </c>
+      <c r="G92" t="n">
+        <v>117549159.6710938</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>1.068908410046789e-05</v>
+      </c>
+      <c r="E93" t="n">
+        <v>2.00733732</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-0.2696464</v>
+      </c>
+      <c r="G93" t="n">
+        <v>357694.4285336945</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.0001981763753227177</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-4.12009663</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-9.6107719</v>
+      </c>
+      <c r="G94" t="n">
+        <v>182799.1299744898</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.02811122465940877</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-10.11766185</v>
+      </c>
+      <c r="F95" t="n">
+        <v>21.30115581</v>
+      </c>
+      <c r="G95" t="n">
+        <v>25919810.48662536</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.001841187164122919</v>
+      </c>
+      <c r="E96" t="n">
+        <v>30.0999659</v>
+      </c>
+      <c r="F96" t="n">
+        <v>106.47816826</v>
+      </c>
+      <c r="G96" t="n">
+        <v>1475241.504832385</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.006121879879594188</v>
+      </c>
+      <c r="E97" t="n">
+        <v>3.9591739</v>
+      </c>
+      <c r="F97" t="n">
+        <v>30.70524002</v>
+      </c>
+      <c r="G97" t="n">
+        <v>544167100.4029306</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.0004692662020925978</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-8.6595254</v>
+      </c>
+      <c r="F98" t="n">
+        <v>5.03226675</v>
+      </c>
+      <c r="G98" t="n">
+        <v>468759.4757773908</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.004572246949042317</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-5.82666615</v>
+      </c>
+      <c r="F99" t="n">
+        <v>7.49906787</v>
+      </c>
+      <c r="G99" t="n">
+        <v>64832673.43562111</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30089</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>KOKO</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Koala AI</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>2.721075853606717e-06</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-6.15887945</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-1.33800146</v>
+      </c>
+      <c r="G100" t="n">
+        <v>24790045.23267727</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-25T05:26:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>1.517076437959438e-05</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-0.59567282</v>
+      </c>
+      <c r="F101" t="n">
+        <v>7.26562546</v>
+      </c>
+      <c r="G101" t="n">
+        <v>3792662.194562384</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>65748.78999999999</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>157.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-09-30 12:24:03
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -21,6 +21,7 @@
     <sheet name="Portfolio_12" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="Portfolio_13" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="Portfolio_14" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Portfolio_15" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16960,6 +16961,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.006573305335696168</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-34.87895182</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-70.72010675999999</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6573305.335696167</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.01647249948825986</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.30013857</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5.3603749</v>
+      </c>
+      <c r="G3" t="n">
+        <v>10072311.84730272</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2184247629742642</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-22.74728086</v>
+      </c>
+      <c r="F4" t="n">
+        <v>397.97740735</v>
+      </c>
+      <c r="G4" t="n">
+        <v>216234353.837515</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.001186010794423342</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-6.25622082</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-67.44188658</v>
+      </c>
+      <c r="G5" t="n">
+        <v>867880.4180741807</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.01010783884400932</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.75376385</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-27.45792859</v>
+      </c>
+      <c r="G6" t="n">
+        <v>10107838.84400932</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0003029852559690895</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.82707644</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-31.43825505</v>
+      </c>
+      <c r="G7" t="n">
+        <v>287835.9931706351</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.02124648684937575</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-0.61195584</v>
+      </c>
+      <c r="F8" t="n">
+        <v>7.4526693</v>
+      </c>
+      <c r="G8" t="n">
+        <v>21246486.84937574</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0004942955685395164</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-2.46954265</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-34.75397381</v>
+      </c>
+      <c r="G9" t="n">
+        <v>494295.5685395164</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.008151190351452923</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-1.17772164</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-42.11078756</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8151190.351452923</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>7.934686972499654e-07</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4.26958316</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-11.87152255</v>
+      </c>
+      <c r="G11" t="n">
+        <v>516390.0890241709</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0008042678451164653</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-5.17783124</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-5.49119418</v>
+      </c>
+      <c r="G12" t="n">
+        <v>415605408.9639335</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0005541090156686663</v>
+      </c>
+      <c r="E13" t="n">
+        <v>11.82682139</v>
+      </c>
+      <c r="F13" t="n">
+        <v>77.42339578000001</v>
+      </c>
+      <c r="G13" t="n">
+        <v>554109.0156686663</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>3.646961498380052e-07</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2.24454854</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-24.19414965</v>
+      </c>
+      <c r="G14" t="n">
+        <v>150355.4246501143</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.007553354143664367</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-4.41012398</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-7.20548564</v>
+      </c>
+      <c r="G15" t="n">
+        <v>7101806.369586678</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0001000206679043097</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-11.24447381</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-53.29878592</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1000206.679043097</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.02079289680558158</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-6.87077907</v>
+      </c>
+      <c r="F17" t="n">
+        <v>65.47969845</v>
+      </c>
+      <c r="G17" t="n">
+        <v>20359026.0031622</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0003240061600354477</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-3.94007298</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-39.12987188</v>
+      </c>
+      <c r="G18" t="n">
+        <v>324006.1600354477</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.003154649372582377</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-13.06700578</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-31.26198176</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2996892.821359947</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>3.795418013714693e-05</v>
+      </c>
+      <c r="E20" t="n">
+        <v>7.07818417</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-8.37946659</v>
+      </c>
+      <c r="G20" t="n">
+        <v>256189017.5587496</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.3262925046069349</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.72963585</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3.41419013</v>
+      </c>
+      <c r="G21" t="n">
+        <v>325460254.7873719</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>4.564521867991922e-05</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-5.55147468</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-34.14440337</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4564521.867991921</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2.43012415865072e-06</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-2.5171715</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-15.25497242</v>
+      </c>
+      <c r="G23" t="n">
+        <v>782061.9999323466</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0142362414056516</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-0.30641027</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-19.34527156</v>
+      </c>
+      <c r="G24" t="n">
+        <v>14236219.18287877</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>2.332976173302038e-06</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-15.01907053</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-12.22911554</v>
+      </c>
+      <c r="G25" t="n">
+        <v>16097531.77481002</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.001053583528415712</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-3.96792017</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-9.743742709999999</v>
+      </c>
+      <c r="G26" t="n">
+        <v>442960676.4211671</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>3.621678190497714e-05</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-0.01644039</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-3.72638475</v>
+      </c>
+      <c r="G27" t="n">
+        <v>232350.1051652973</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.002940281170604531</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.21955891</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-13.79852953</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2940281.079455815</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.001479259680819875</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-7.87079171</v>
+      </c>
+      <c r="F29" t="n">
+        <v>11.00976305</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1479257.019631709</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.07281861390124056</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-12.98819279</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-12.84280367</v>
+      </c>
+      <c r="G30" t="n">
+        <v>72818613.90124056</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.01818785083073298</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-2.79011937</v>
+      </c>
+      <c r="F31" t="n">
+        <v>29.0820568</v>
+      </c>
+      <c r="G31" t="n">
+        <v>17331303.83548691</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.1465282437995563</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-0.7628476199999999</v>
+      </c>
+      <c r="F32" t="n">
+        <v>180.07303948</v>
+      </c>
+      <c r="G32" t="n">
+        <v>10262643.60621315</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.001064587834882402</v>
+      </c>
+      <c r="E33" t="n">
+        <v>8.76186087</v>
+      </c>
+      <c r="F33" t="n">
+        <v>89.88085847000001</v>
+      </c>
+      <c r="G33" t="n">
+        <v>986402.3634025025</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.000285462755926751</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.70001307</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-22.91744321</v>
+      </c>
+      <c r="G34" t="n">
+        <v>250548.1687870501</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1.420332673139028e-06</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-16.89685896</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-5.26106752</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1262512.282725299</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.002702823675755156</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.88212931</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-2.58036153</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1891975.689205267</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>9.361904141745453e-05</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-16.41477274</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-37.59680835</v>
+      </c>
+      <c r="G37" t="n">
+        <v>936190.4141745453</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2.317026494008421e-06</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-4.94449758</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-6.1755032</v>
+      </c>
+      <c r="G38" t="n">
+        <v>6821951.222936314</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0006398595946724623</v>
+      </c>
+      <c r="E39" t="n">
+        <v>8.47876649</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-4.79714992</v>
+      </c>
+      <c r="G39" t="n">
+        <v>19195787.84017387</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.0003347252279287269</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-0.54044117</v>
+      </c>
+      <c r="F40" t="n">
+        <v>8.900934469999999</v>
+      </c>
+      <c r="G40" t="n">
+        <v>26959281.61275559</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.01025476006944977</v>
+      </c>
+      <c r="E41" t="n">
+        <v>35.61904717</v>
+      </c>
+      <c r="F41" t="n">
+        <v>170.98609911</v>
+      </c>
+      <c r="G41" t="n">
+        <v>10031589.18191248</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.0008219623415365953</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-11.45473884</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-5.13082513</v>
+      </c>
+      <c r="G42" t="n">
+        <v>705835.2043739374</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.07709146010577425</v>
+      </c>
+      <c r="E43" t="n">
+        <v>13.33054697</v>
+      </c>
+      <c r="F43" t="n">
+        <v>57.94987797</v>
+      </c>
+      <c r="G43" t="n">
+        <v>75215922.40209779</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.05138035986180139</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1.48496237</v>
+      </c>
+      <c r="F44" t="n">
+        <v>29.64288089</v>
+      </c>
+      <c r="G44" t="n">
+        <v>48099089.69684359</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>1.116130205727634e-05</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-5.92994576</v>
+      </c>
+      <c r="F45" t="n">
+        <v>7.16582739</v>
+      </c>
+      <c r="G45" t="n">
+        <v>4670841.975974657</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.002806480836153721</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-1.89509661</v>
+      </c>
+      <c r="F46" t="n">
+        <v>57.75202424</v>
+      </c>
+      <c r="G46" t="n">
+        <v>28064360.38448615</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.1540004629354584</v>
+      </c>
+      <c r="E47" t="n">
+        <v>10.55371646</v>
+      </c>
+      <c r="F47" t="n">
+        <v>102.87377927</v>
+      </c>
+      <c r="G47" t="n">
+        <v>92352280.28682348</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.0002241179007192419</v>
+      </c>
+      <c r="E48" t="n">
+        <v>64.96519433</v>
+      </c>
+      <c r="F48" t="n">
+        <v>9.651470399999999</v>
+      </c>
+      <c r="G48" t="n">
+        <v>216178.044922191</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>1.051371537147821e-08</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-12.22745985</v>
+      </c>
+      <c r="F49" t="n">
+        <v>371.18137742</v>
+      </c>
+      <c r="G49" t="n">
+        <v>4218672.401068097</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.006056005997043592</v>
+      </c>
+      <c r="E50" t="n">
+        <v>12.35429329</v>
+      </c>
+      <c r="F50" t="n">
+        <v>7.8948394</v>
+      </c>
+      <c r="G50" t="n">
+        <v>6056005.997043592</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>2.001668233059353e-07</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-4.49553381</v>
+      </c>
+      <c r="F51" t="n">
+        <v>28.88555092</v>
+      </c>
+      <c r="G51" t="n">
+        <v>82299859.19306605</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>3.580931554445864e-06</v>
+      </c>
+      <c r="E52" t="n">
+        <v>14.19781408</v>
+      </c>
+      <c r="F52" t="n">
+        <v>45.89406491</v>
+      </c>
+      <c r="G52" t="n">
+        <v>1506462.09563983</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.01179672326732591</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-0.39063648</v>
+      </c>
+      <c r="F53" t="n">
+        <v>4.81495548</v>
+      </c>
+      <c r="G53" t="n">
+        <v>780458.9899609773</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.005915336501947463</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-9.19966941</v>
+      </c>
+      <c r="F54" t="n">
+        <v>84.88100125</v>
+      </c>
+      <c r="G54" t="n">
+        <v>5914397.430447106</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.1120495205018507</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-3.87541788</v>
+      </c>
+      <c r="F55" t="n">
+        <v>59.76157612</v>
+      </c>
+      <c r="G55" t="n">
+        <v>110496867.5866181</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>1.232899925724523e-08</v>
+      </c>
+      <c r="E56" t="n">
+        <v>3.0721272</v>
+      </c>
+      <c r="F56" t="n">
+        <v>3.68288173</v>
+      </c>
+      <c r="G56" t="n">
+        <v>390894.8072735934</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.009277228129179107</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-3.75278381</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.49037638</v>
+      </c>
+      <c r="G57" t="n">
+        <v>927722.8129179106</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>7.189092455419945e-05</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.0144885</v>
+      </c>
+      <c r="F58" t="n">
+        <v>11.44963871</v>
+      </c>
+      <c r="G58" t="n">
+        <v>28056072.83743862</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.01157771334021902</v>
+      </c>
+      <c r="E59" t="n">
+        <v>4.73446872</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-21.45411822</v>
+      </c>
+      <c r="G59" t="n">
+        <v>10905062.66729398</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.00113756062063323</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-12.08008503</v>
+      </c>
+      <c r="F60" t="n">
+        <v>16.67167579</v>
+      </c>
+      <c r="G60" t="n">
+        <v>1137560.620633231</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.09264019269427358</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-0.51399208</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-2.69016075</v>
+      </c>
+      <c r="G61" t="n">
+        <v>18828263.63293158</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.005895188688282762</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-5.13348925</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-10.31634266</v>
+      </c>
+      <c r="G62" t="n">
+        <v>9993041.354973178</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>5.726412484674585e-05</v>
+      </c>
+      <c r="E63" t="n">
+        <v>6.3873695</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-1.40800927</v>
+      </c>
+      <c r="G63" t="n">
+        <v>54310907.83274997</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>1.754506894402803e-05</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-5.40139652</v>
+      </c>
+      <c r="F64" t="n">
+        <v>17.26080521</v>
+      </c>
+      <c r="G64" t="n">
+        <v>152195.7878053486</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.03033171163252148</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-3.37783103</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-22.89814589</v>
+      </c>
+      <c r="G65" t="n">
+        <v>2881512.605089541</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.0008641313382276943</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-6.31669514</v>
+      </c>
+      <c r="F66" t="n">
+        <v>62.80015369</v>
+      </c>
+      <c r="G66" t="n">
+        <v>14161195.68779775</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.01170666045153327</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-4.96098764</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-17.27385858</v>
+      </c>
+      <c r="G67" t="n">
+        <v>11704932.51180878</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.0007112371096664592</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-16.46322447</v>
+      </c>
+      <c r="F68" t="n">
+        <v>47.74998989</v>
+      </c>
+      <c r="G68" t="n">
+        <v>659268.3056697221</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>4.602904715865019e-06</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-10.01217355</v>
+      </c>
+      <c r="F69" t="n">
+        <v>9.404422629999999</v>
+      </c>
+      <c r="G69" t="n">
+        <v>3154001.364779648</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1.380344621993518e-06</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-0.8385639499999999</v>
+      </c>
+      <c r="F70" t="n">
+        <v>14.43756372</v>
+      </c>
+      <c r="G70" t="n">
+        <v>1081795.177641645</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.5097933021160899</v>
+      </c>
+      <c r="E71" t="n">
+        <v>19.51907459</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-3.84111033</v>
+      </c>
+      <c r="G71" t="n">
+        <v>44077277.4385502</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.2121941800121103</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-0.23761426</v>
+      </c>
+      <c r="F72" t="n">
+        <v>38.28979563</v>
+      </c>
+      <c r="G72" t="n">
+        <v>117931030.5549544</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.004020919029054429</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-6.44772248</v>
+      </c>
+      <c r="F73" t="n">
+        <v>59.58152057</v>
+      </c>
+      <c r="G73" t="n">
+        <v>402091902.905443</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.006251984214673542</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-1.31880807</v>
+      </c>
+      <c r="F74" t="n">
+        <v>13.17127684</v>
+      </c>
+      <c r="G74" t="n">
+        <v>52659757.89139964</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>2.420924031299737e-07</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-3.43381754</v>
+      </c>
+      <c r="F75" t="n">
+        <v>2.3520247</v>
+      </c>
+      <c r="G75" t="n">
+        <v>101678809.3145889</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.0001173138479760083</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-1.20793492</v>
+      </c>
+      <c r="F76" t="n">
+        <v>51.9257111</v>
+      </c>
+      <c r="G76" t="n">
+        <v>49352762.70502694</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.0002744911848602391</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.40907259</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-3.17489219</v>
+      </c>
+      <c r="G77" t="n">
+        <v>5318998.695054712</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>3.656264970097206e-07</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.17392348</v>
+      </c>
+      <c r="F78" t="n">
+        <v>6.34077161</v>
+      </c>
+      <c r="G78" t="n">
+        <v>323982.6755591106</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.01370609455369618</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-5.87266099</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-12.74372792</v>
+      </c>
+      <c r="G79" t="n">
+        <v>1302759.270898215</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.0008755073330432828</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-1.19053593</v>
+      </c>
+      <c r="F80" t="n">
+        <v>2.31395278</v>
+      </c>
+      <c r="G80" t="n">
+        <v>868963.3834649237</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.009513530541176485</v>
+      </c>
+      <c r="E81" t="n">
+        <v>88.65157986</v>
+      </c>
+      <c r="F81" t="n">
+        <v>83.97348119</v>
+      </c>
+      <c r="G81" t="n">
+        <v>6628239.545555269</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.002219605325632304</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-2.4576409</v>
+      </c>
+      <c r="F82" t="n">
+        <v>4.53343234</v>
+      </c>
+      <c r="G82" t="n">
+        <v>2135785.119703553</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.01043324320915572</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-2.958493</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-12.90821732</v>
+      </c>
+      <c r="G83" t="n">
+        <v>9911583.68830847</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>7.183858312883421</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.82776936</v>
+      </c>
+      <c r="F84" t="n">
+        <v>151.31359779</v>
+      </c>
+      <c r="G84" t="n">
+        <v>55818579.09110418</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.0001755369322327058</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-1.4369275</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-3.23114341</v>
+      </c>
+      <c r="G85" t="n">
+        <v>112907.3611992118</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.003557393955430651</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-3.04905798</v>
+      </c>
+      <c r="F86" t="n">
+        <v>56.6108893</v>
+      </c>
+      <c r="G86" t="n">
+        <v>3333789.586324886</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>3.550996376451524e-08</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-2.58870406</v>
+      </c>
+      <c r="F87" t="n">
+        <v>-5.46143444</v>
+      </c>
+      <c r="G87" t="n">
+        <v>27337750.33714739</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.0002851433130319582</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-11.594648</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-22.52410981</v>
+      </c>
+      <c r="G88" t="n">
+        <v>142414.8539269963</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.02295291324656934</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-5.93610102</v>
+      </c>
+      <c r="F89" t="n">
+        <v>40.62530876</v>
+      </c>
+      <c r="G89" t="n">
+        <v>22720985.97077474</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>8.394669987670464e-05</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.43546513</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-11.63038468</v>
+      </c>
+      <c r="G90" t="n">
+        <v>881440.3487053987</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>4.838918990721183e-05</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-6.06549641</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-12.84064916</v>
+      </c>
+      <c r="G91" t="n">
+        <v>110482412.130472</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>1.050959389558806e-05</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-1.7175064</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-1.64858126</v>
+      </c>
+      <c r="G92" t="n">
+        <v>351688.0536508291</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.0001968225203871829</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-0.68315657</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-12.59406675</v>
+      </c>
+      <c r="G93" t="n">
+        <v>181550.3257014052</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.0236867801973088</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-15.93841218</v>
+      </c>
+      <c r="F94" t="n">
+        <v>10.14536405</v>
+      </c>
+      <c r="G94" t="n">
+        <v>21840274.16774617</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.001504152795520892</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-18.30527611</v>
+      </c>
+      <c r="F95" t="n">
+        <v>65.77022728999999</v>
+      </c>
+      <c r="G95" t="n">
+        <v>1205194.494509271</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.005969749416495933</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-2.44925844</v>
+      </c>
+      <c r="F96" t="n">
+        <v>20.29000878</v>
+      </c>
+      <c r="G96" t="n">
+        <v>530644392.5721098</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.0004889928684601666</v>
+      </c>
+      <c r="E97" t="n">
+        <v>4.19792009</v>
+      </c>
+      <c r="F97" t="n">
+        <v>10.16835188</v>
+      </c>
+      <c r="G97" t="n">
+        <v>488464.8407579958</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.004570814037118655</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-0.0801934</v>
+      </c>
+      <c r="F98" t="n">
+        <v>-11.55386558</v>
+      </c>
+      <c r="G98" t="n">
+        <v>64812355.30498552</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30089</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>KOKO</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Koala AI</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>2.362819953735406e-06</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-13.37360928</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-9.253804499999999</v>
+      </c>
+      <c r="G99" t="n">
+        <v>21526196.50500894</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-25T05:26:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>1.506930495453988e-05</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-1.07750302</v>
+      </c>
+      <c r="F100" t="n">
+        <v>8.65004613</v>
+      </c>
+      <c r="G100" t="n">
+        <v>3767297.480201629</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.0274441304488502</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-3.12601535</v>
+      </c>
+      <c r="F101" t="n">
+        <v>34.05649981</v>
+      </c>
+      <c r="G101" t="n">
+        <v>255296605.3432069</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>63859.28</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>155.86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-01 12:22:35
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -22,6 +22,7 @@
     <sheet name="Portfolio_13" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="Portfolio_14" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="Portfolio_15" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Portfolio_16" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20242,6 +20243,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.01011006086047036</v>
+      </c>
+      <c r="E2" t="n">
+        <v>49.28248719</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-54.96611103</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10110060.86047036</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.01535294310892741</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-6.62033659</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-10.73126088</v>
+      </c>
+      <c r="G3" t="n">
+        <v>9387745.367800897</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2244589002554722</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.19396402</v>
+      </c>
+      <c r="F4" t="n">
+        <v>243.48424507</v>
+      </c>
+      <c r="G4" t="n">
+        <v>222207979.5299581</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.001172867995009846</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1.10815175</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-60.51777552</v>
+      </c>
+      <c r="G5" t="n">
+        <v>858262.9860041831</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.009942668415805407</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.6535328500000001</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-19.37850634</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9942668.415805407</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0003069616738577323</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.97437243</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-29.7768982</v>
+      </c>
+      <c r="G7" t="n">
+        <v>291613.5901648457</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.02075914043278144</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-2.78768813</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2.37306372</v>
+      </c>
+      <c r="G8" t="n">
+        <v>20759140.43278144</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0004614916602886421</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-5.93134943</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-41.39929546</v>
+      </c>
+      <c r="G9" t="n">
+        <v>461491.6602886421</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.008557794550575351</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5.72195024</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-36.32402521</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8557794.550575351</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>7.810479392289119e-07</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-1.56537467</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-14.6170905</v>
+      </c>
+      <c r="G11" t="n">
+        <v>508306.6493592298</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0007750923625983742</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-3.70003014</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-9.781110569999999</v>
+      </c>
+      <c r="G12" t="n">
+        <v>400528978.3727099</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.000460623746180008</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-16.87127746</v>
+      </c>
+      <c r="F13" t="n">
+        <v>49.30550959</v>
+      </c>
+      <c r="G13" t="n">
+        <v>460623.746180008</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>2.868168370935666e-07</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-20.1788309</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-43.44873352</v>
+      </c>
+      <c r="G14" t="n">
+        <v>118247.6627657335</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.007271441132957792</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-3.91233665</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-9.494475359999999</v>
+      </c>
+      <c r="G15" t="n">
+        <v>6836746.427072976</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0001000157002027803</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-1.90635551</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-45.87328155</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1000157.002027803</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.01738441248049573</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-16.43557534</v>
+      </c>
+      <c r="F17" t="n">
+        <v>87.66705674000001</v>
+      </c>
+      <c r="G17" t="n">
+        <v>17021664.13123843</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0003298493506600999</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-2.39737472</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-32.13465272</v>
+      </c>
+      <c r="G18" t="n">
+        <v>329849.3506600999</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.003198514297386968</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1.38560486</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-20.67899615</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3038564.165059474</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>3.657304637653743e-05</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-3.81079907</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-8.947375859999999</v>
+      </c>
+      <c r="G20" t="n">
+        <v>246866426.445222</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.3145996631527912</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-3.60110073</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-0.05339886</v>
+      </c>
+      <c r="G21" t="n">
+        <v>313797237.3869621</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>4.324676218391841e-05</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-5.19767107</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-28.48815962</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4324676.218391841</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2.073592419910117e-06</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-14.67239922</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-17.11680033</v>
+      </c>
+      <c r="G23" t="n">
+        <v>667323.0374615371</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.01526851116584397</v>
+      </c>
+      <c r="E24" t="n">
+        <v>7.58890436</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-24.32475921</v>
+      </c>
+      <c r="G24" t="n">
+        <v>15268487.33169804</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>2.459337826904174e-06</v>
+      </c>
+      <c r="E25" t="n">
+        <v>5.04730719</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-10.85663029</v>
+      </c>
+      <c r="G25" t="n">
+        <v>16969426.97770825</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.001151833182777624</v>
+      </c>
+      <c r="E26" t="n">
+        <v>9.418801330000001</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-5.12265829</v>
+      </c>
+      <c r="G26" t="n">
+        <v>484300313.7588367</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>3.646581276656307e-05</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.56609857</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-0.82961927</v>
+      </c>
+      <c r="G27" t="n">
+        <v>233947.7718776714</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.002904501397350561</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-1.4238362</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-20.94338116</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2904501.307311018</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.001567267341592897</v>
+      </c>
+      <c r="E29" t="n">
+        <v>5.83353494</v>
+      </c>
+      <c r="F29" t="n">
+        <v>34.32501805</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1567264.52207895</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.07381336168221292</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2.08065061</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-22.70346851</v>
+      </c>
+      <c r="G30" t="n">
+        <v>73813361.68221292</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.01768980969737625</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-2.83394928</v>
+      </c>
+      <c r="F31" t="n">
+        <v>15.83422985</v>
+      </c>
+      <c r="G31" t="n">
+        <v>16856717.67986536</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.1365476019534494</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-6.64331923</v>
+      </c>
+      <c r="F32" t="n">
+        <v>207.09377204</v>
+      </c>
+      <c r="G32" t="n">
+        <v>9563612.705604199</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.0007438643503145769</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-29.37403741</v>
+      </c>
+      <c r="F33" t="n">
+        <v>57.67440758</v>
+      </c>
+      <c r="G33" t="n">
+        <v>689233.4565162659</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0002654859542783359</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-6.99804133</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-27.802225</v>
+      </c>
+      <c r="G34" t="n">
+        <v>233014.7043777145</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1.391070830026572e-06</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-2.0717474</v>
+      </c>
+      <c r="F35" t="n">
+        <v>11.21854199</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1236501.774885105</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.002741685581421271</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1.51174733</v>
+      </c>
+      <c r="F36" t="n">
+        <v>10.71794466</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1919179.010463705</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>3.059918852185937e-06</v>
+      </c>
+      <c r="E37" t="n">
+        <v>31.95232326</v>
+      </c>
+      <c r="F37" t="n">
+        <v>29.05664474</v>
+      </c>
+      <c r="G37" t="n">
+        <v>9009226.786890538</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0006159606669109042</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-3.7414011</v>
+      </c>
+      <c r="F38" t="n">
+        <v>9.848476809999999</v>
+      </c>
+      <c r="G38" t="n">
+        <v>18478820.00732713</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0003499934233973338</v>
+      </c>
+      <c r="E39" t="n">
+        <v>4.60905849</v>
+      </c>
+      <c r="F39" t="n">
+        <v>16.99106678</v>
+      </c>
+      <c r="G39" t="n">
+        <v>28189005.41906642</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.01027768950495259</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.2341653</v>
+      </c>
+      <c r="F40" t="n">
+        <v>179.79475724</v>
+      </c>
+      <c r="G40" t="n">
+        <v>10054019.61183767</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.0008522212129192065</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.68129656</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-0.47112693</v>
+      </c>
+      <c r="G41" t="n">
+        <v>731819.091453902</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.07526737377393371</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-2.27634639</v>
+      </c>
+      <c r="F42" t="n">
+        <v>28.23461671</v>
+      </c>
+      <c r="G42" t="n">
+        <v>73436213.78324172</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.05448923006999708</v>
+      </c>
+      <c r="E43" t="n">
+        <v>6.11708367</v>
+      </c>
+      <c r="F43" t="n">
+        <v>20.0461041</v>
+      </c>
+      <c r="G43" t="n">
+        <v>51009420.16946102</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>1.271081186935266e-05</v>
+      </c>
+      <c r="E44" t="n">
+        <v>13.88282309</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-71.57983854</v>
+      </c>
+      <c r="G44" t="n">
+        <v>5319289.212263938</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.002630553772622499</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-6.053571</v>
+      </c>
+      <c r="F45" t="n">
+        <v>49.04078225</v>
+      </c>
+      <c r="G45" t="n">
+        <v>26305117.82770522</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.1596477383738961</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3.73052851</v>
+      </c>
+      <c r="F46" t="n">
+        <v>108.57744983</v>
+      </c>
+      <c r="G46" t="n">
+        <v>95738885.45804347</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.0001448861905473509</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-35.36765162</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-37.13184751</v>
+      </c>
+      <c r="G47" t="n">
+        <v>139753.2874805356</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1.100143931071516e-08</v>
+      </c>
+      <c r="E48" t="n">
+        <v>3.84072828</v>
+      </c>
+      <c r="F48" t="n">
+        <v>295.55329338</v>
+      </c>
+      <c r="G48" t="n">
+        <v>4414373.677838525</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.007535642850083501</v>
+      </c>
+      <c r="E49" t="n">
+        <v>24.09713052</v>
+      </c>
+      <c r="F49" t="n">
+        <v>35.19082241</v>
+      </c>
+      <c r="G49" t="n">
+        <v>7535642.850083501</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>1.925817740042586e-07</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-3.96745442</v>
+      </c>
+      <c r="F50" t="n">
+        <v>19.94262313</v>
+      </c>
+      <c r="G50" t="n">
+        <v>79181218.05568659</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>4.89933735617959e-06</v>
+      </c>
+      <c r="E51" t="n">
+        <v>36.81739742</v>
+      </c>
+      <c r="F51" t="n">
+        <v>106.25842957</v>
+      </c>
+      <c r="G51" t="n">
+        <v>2061102.232371192</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.01177621088103144</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.71963641</v>
+      </c>
+      <c r="F52" t="n">
+        <v>4.6163727</v>
+      </c>
+      <c r="G52" t="n">
+        <v>779101.9117345673</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.005439632976794602</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-8.114489839999999</v>
+      </c>
+      <c r="F53" t="n">
+        <v>73.47058018</v>
+      </c>
+      <c r="G53" t="n">
+        <v>5438769.42418027</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.1104141757699597</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-0.88871818</v>
+      </c>
+      <c r="F54" t="n">
+        <v>23.47052544</v>
+      </c>
+      <c r="G54" t="n">
+        <v>108884183.5743269</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>1.180730092089101e-08</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-4.26381293</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.8026060699999999</v>
+      </c>
+      <c r="G55" t="n">
+        <v>374354.1970919278</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.01060836754409811</v>
+      </c>
+      <c r="E56" t="n">
+        <v>14.34846051</v>
+      </c>
+      <c r="F56" t="n">
+        <v>32.21823443</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1060836.754409811</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>8.886115300944871e-05</v>
+      </c>
+      <c r="E57" t="n">
+        <v>23.72299798</v>
+      </c>
+      <c r="F57" t="n">
+        <v>47.83975524</v>
+      </c>
+      <c r="G57" t="n">
+        <v>34678855.45653675</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.01575107257033179</v>
+      </c>
+      <c r="E58" t="n">
+        <v>36.09223906</v>
+      </c>
+      <c r="F58" t="n">
+        <v>9.61211203</v>
+      </c>
+      <c r="G58" t="n">
+        <v>14835954.94283622</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.001043618570692904</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-8.25820165</v>
+      </c>
+      <c r="F59" t="n">
+        <v>1.01540182</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1043618.570692904</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.09115299934859303</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-1.54279589</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-2.55878168</v>
+      </c>
+      <c r="G60" t="n">
+        <v>18526005.31965255</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.005799433406539535</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-1.4729322</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-14.77108988</v>
+      </c>
+      <c r="G61" t="n">
+        <v>9830724.838740362</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>5.765215356247945e-05</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.67761223</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-1.81546185</v>
+      </c>
+      <c r="G62" t="n">
+        <v>54678925.18869609</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>1.679715221818468e-05</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-4.1942939</v>
+      </c>
+      <c r="F63" t="n">
+        <v>13.2957688</v>
+      </c>
+      <c r="G63" t="n">
+        <v>145707.9378193688</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.03166473878093291</v>
+      </c>
+      <c r="E64" t="n">
+        <v>4.39962595</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-18.06895079</v>
+      </c>
+      <c r="G64" t="n">
+        <v>3008150.184188627</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.0008886967491637132</v>
+      </c>
+      <c r="E65" t="n">
+        <v>2.76223899</v>
+      </c>
+      <c r="F65" t="n">
+        <v>56.66786681</v>
+      </c>
+      <c r="G65" t="n">
+        <v>14563768.27835975</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.01297326562236421</v>
+      </c>
+      <c r="E66" t="n">
+        <v>10.84936046</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-14.73489378</v>
+      </c>
+      <c r="G66" t="n">
+        <v>12971350.72775202</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.0006866282995945531</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-3.46000085</v>
+      </c>
+      <c r="F67" t="n">
+        <v>34.83399811</v>
+      </c>
+      <c r="G67" t="n">
+        <v>636457.6166601711</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>7.543996091127702e-06</v>
+      </c>
+      <c r="E68" t="n">
+        <v>63.89643244</v>
+      </c>
+      <c r="F68" t="n">
+        <v>72.36884524</v>
+      </c>
+      <c r="G68" t="n">
+        <v>5169295.35501748</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1.357361674839747e-06</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-1.66501516</v>
+      </c>
+      <c r="F69" t="n">
+        <v>10.36499717</v>
+      </c>
+      <c r="G69" t="n">
+        <v>1063783.123982874</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.5200531658199158</v>
+      </c>
+      <c r="E70" t="n">
+        <v>2.01255365</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-1.94207991</v>
+      </c>
+      <c r="G70" t="n">
+        <v>44964356.29399634</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.235993886652698</v>
+      </c>
+      <c r="E71" t="n">
+        <v>11.50874037</v>
+      </c>
+      <c r="F71" t="n">
+        <v>27.49564894</v>
+      </c>
+      <c r="G71" t="n">
+        <v>131158179.0117751</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.004108247453261901</v>
+      </c>
+      <c r="E72" t="n">
+        <v>2.24406767</v>
+      </c>
+      <c r="F72" t="n">
+        <v>55.57034997</v>
+      </c>
+      <c r="G72" t="n">
+        <v>410824745.3261901</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.006154101313682305</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-1.87419666</v>
+      </c>
+      <c r="F73" t="n">
+        <v>8.217632890000001</v>
+      </c>
+      <c r="G73" t="n">
+        <v>51835301.25636709</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>2.384290384735916e-07</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-1.61502512</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.74409531</v>
+      </c>
+      <c r="G74" t="n">
+        <v>100140196.1589085</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.0001482414239639182</v>
+      </c>
+      <c r="E75" t="n">
+        <v>26.6005167</v>
+      </c>
+      <c r="F75" t="n">
+        <v>75.9126239</v>
+      </c>
+      <c r="G75" t="n">
+        <v>62363684.64738077</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.0002722529064596173</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-1.26030258</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-4.05736318</v>
+      </c>
+      <c r="G76" t="n">
+        <v>5275626.08220327</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>3.623041720915336e-07</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-0.90866634</v>
+      </c>
+      <c r="F77" t="n">
+        <v>7.10565871</v>
+      </c>
+      <c r="G77" t="n">
+        <v>321038.7540302442</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.0130887064365256</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-4.0328732</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-21.4567541</v>
+      </c>
+      <c r="G78" t="n">
+        <v>1244076.756325203</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.0008840408022855906</v>
+      </c>
+      <c r="E79" t="n">
+        <v>1.02558627</v>
+      </c>
+      <c r="F79" t="n">
+        <v>1.52962886</v>
+      </c>
+      <c r="G79" t="n">
+        <v>877433.0695836152</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.009102336963118081</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-5.37577824</v>
+      </c>
+      <c r="F80" t="n">
+        <v>77.32413633</v>
+      </c>
+      <c r="G80" t="n">
+        <v>6341753.300833509</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.002659299296393508</v>
+      </c>
+      <c r="E81" t="n">
+        <v>19.52158258</v>
+      </c>
+      <c r="F81" t="n">
+        <v>13.92558361</v>
+      </c>
+      <c r="G81" t="n">
+        <v>2558874.679424098</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.01848307217888838</v>
+      </c>
+      <c r="E82" t="n">
+        <v>75.8724577</v>
+      </c>
+      <c r="F82" t="n">
+        <v>36.16649409</v>
+      </c>
+      <c r="G82" t="n">
+        <v>17558923.24616122</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>8.709422944456117</v>
+      </c>
+      <c r="E83" t="n">
+        <v>21.0230692</v>
+      </c>
+      <c r="F83" t="n">
+        <v>127.25188531</v>
+      </c>
+      <c r="G83" t="n">
+        <v>67672216.27842402</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.0001752569965713989</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-0.14131961</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-4.07576709</v>
+      </c>
+      <c r="G84" t="n">
+        <v>112727.3033821946</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.003140931692852572</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-11.70780807</v>
+      </c>
+      <c r="F85" t="n">
+        <v>32.86010919</v>
+      </c>
+      <c r="G85" t="n">
+        <v>2943504.571093273</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>3.583798786066799e-08</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.89620233</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-1.56813175</v>
+      </c>
+      <c r="G86" t="n">
+        <v>27590283.42630118</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.0002650172669805114</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-7.00092084</v>
+      </c>
+      <c r="F87" t="n">
+        <v>-31.56576964</v>
+      </c>
+      <c r="G87" t="n">
+        <v>132362.898375005</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.02492568842606686</v>
+      </c>
+      <c r="E88" t="n">
+        <v>8.55691494</v>
+      </c>
+      <c r="F88" t="n">
+        <v>22.41628765</v>
+      </c>
+      <c r="G88" t="n">
+        <v>24673827.28095375</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>8.662014597044911e-05</v>
+      </c>
+      <c r="E89" t="n">
+        <v>3.18469469</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-6.73786805</v>
+      </c>
+      <c r="G89" t="n">
+        <v>909511.5326897157</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>5.245256623699324e-05</v>
+      </c>
+      <c r="E90" t="n">
+        <v>8.516292310000001</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-0.0273796</v>
+      </c>
+      <c r="G90" t="n">
+        <v>119759930.9145012</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>1.039024676062587e-05</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-1.13560178</v>
+      </c>
+      <c r="F91" t="n">
+        <v>8.61560937</v>
+      </c>
+      <c r="G91" t="n">
+        <v>347694.2778664691</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.0002092017404741994</v>
+      </c>
+      <c r="E92" t="n">
+        <v>6.28953438</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-12.71319796</v>
+      </c>
+      <c r="G92" t="n">
+        <v>192968.9958531039</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.03000951211686791</v>
+      </c>
+      <c r="E93" t="n">
+        <v>26.6310719</v>
+      </c>
+      <c r="F93" t="n">
+        <v>34.07360524</v>
+      </c>
+      <c r="G93" t="n">
+        <v>27670116.6985609</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.001483511622699751</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-1.37227899</v>
+      </c>
+      <c r="F94" t="n">
+        <v>65.17142701</v>
+      </c>
+      <c r="G94" t="n">
+        <v>1188655.863647878</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.005990992049819912</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.49425033</v>
+      </c>
+      <c r="F95" t="n">
+        <v>9.449324649999999</v>
+      </c>
+      <c r="G95" t="n">
+        <v>532532626.6453335</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.0004669174442798682</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-4.51446751</v>
+      </c>
+      <c r="F96" t="n">
+        <v>-3.37159556</v>
+      </c>
+      <c r="G96" t="n">
+        <v>466413.2542167638</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.004510539640693044</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-1.42167417</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-18.74096186</v>
+      </c>
+      <c r="G97" t="n">
+        <v>63957687.93825255</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30089</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>KOKO</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Koala AI</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>2.307006423573886e-06</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-2.56885941</v>
+      </c>
+      <c r="F98" t="n">
+        <v>-23.07021441</v>
+      </c>
+      <c r="G98" t="n">
+        <v>21017713.82692941</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-25T05:26:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>1.512830871420816e-05</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.85421254</v>
+      </c>
+      <c r="F99" t="n">
+        <v>6.46002022</v>
+      </c>
+      <c r="G99" t="n">
+        <v>3782048.307515251</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.02745189735394497</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0.16133992</v>
+      </c>
+      <c r="F100" t="n">
+        <v>24.51669717</v>
+      </c>
+      <c r="G100" t="n">
+        <v>255368856.2934934</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30011</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>SKID</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Success Kid</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.02545798316244776</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-8.853710810000001</v>
+      </c>
+      <c r="F101" t="n">
+        <v>10.94099137</v>
+      </c>
+      <c r="G101" t="n">
+        <v>2208294.145149291</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-20T13:27:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>63776.62</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>156.33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-02 12:22:14
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -23,6 +23,7 @@
     <sheet name="Portfolio_14" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="Portfolio_15" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="Portfolio_16" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Portfolio_17" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -23524,6 +23525,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0123138498590983</v>
+      </c>
+      <c r="E2" t="n">
+        <v>21.79797955</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-45.14963312</v>
+      </c>
+      <c r="G2" t="n">
+        <v>12313849.8590983</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.01429835215578575</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-6.86898236</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-16.7439633</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8742902.794944389</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.213536265837916</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-4.86620687</v>
+      </c>
+      <c r="F4" t="n">
+        <v>136.49349247</v>
+      </c>
+      <c r="G4" t="n">
+        <v>211394879.571315</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.001094763568077331</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-6.65926833</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-59.52587183</v>
+      </c>
+      <c r="G5" t="n">
+        <v>801108.9507977888</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.00639018811984565</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-35.72964668</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-25.4181284</v>
+      </c>
+      <c r="G6" t="n">
+        <v>6390188.119845649</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0002623060562315769</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-14.54761992</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-35.71377622</v>
+      </c>
+      <c r="G7" t="n">
+        <v>249190.7534199981</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.01874435887871093</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-9.70551532</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-5.27176428</v>
+      </c>
+      <c r="G8" t="n">
+        <v>18744358.87871093</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0004767746722667138</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.31165507</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-29.07262054</v>
+      </c>
+      <c r="G9" t="n">
+        <v>476774.6722667138</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.007960850212453083</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-6.97544601</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-25.29999929</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7960850.212453083</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>7.454880020099965e-07</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-4.5528495</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-18.50444587</v>
+      </c>
+      <c r="G11" t="n">
+        <v>485164.2126004614</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0006454965037975766</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-16.72005364</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-25.43388391</v>
+      </c>
+      <c r="G12" t="n">
+        <v>333560318.3373978</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0003781830484446997</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-17.89762217</v>
+      </c>
+      <c r="F13" t="n">
+        <v>24.31014303</v>
+      </c>
+      <c r="G13" t="n">
+        <v>378183.0484446997</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.006121138757672206</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-15.81945524</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-15.89419645</v>
+      </c>
+      <c r="G14" t="n">
+        <v>5755210.386212761</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>8.540324839055022e-05</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-14.61015799</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-49.32720648</v>
+      </c>
+      <c r="G15" t="n">
+        <v>854032.4839055021</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.01399113185079543</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-19.5190987</v>
+      </c>
+      <c r="F16" t="n">
+        <v>22.79268124</v>
+      </c>
+      <c r="G16" t="n">
+        <v>13699188.70984595</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0002982739855181531</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-9.572662510000001</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-32.31609994</v>
+      </c>
+      <c r="G17" t="n">
+        <v>298273.9855181531</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.003568794382408867</v>
+      </c>
+      <c r="E18" t="n">
+        <v>11.57662748</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-10.5415367</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3390327.419112108</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2.899307515140503e-05</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-20.72556698</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-24.38662605</v>
+      </c>
+      <c r="G19" t="n">
+        <v>195701959.8694627</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.2408384051322486</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-23.44607025</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-27.8930402</v>
+      </c>
+      <c r="G20" t="n">
+        <v>240224116.6751581</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>4.076526097612464e-05</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-5.73800461</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-29.87771882</v>
+      </c>
+      <c r="G21" t="n">
+        <v>4076526.097612464</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1.863383976780116e-06</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-10.13740411</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-7.45547638</v>
+      </c>
+      <c r="G22" t="n">
+        <v>599673.8044576599</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.01373625015591701</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-10.0354317</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-37.56509201</v>
+      </c>
+      <c r="G23" t="n">
+        <v>13736228.71363051</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>2.107437562623136e-06</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-14.30874036</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-32.74505993</v>
+      </c>
+      <c r="G24" t="n">
+        <v>14541315.73051522</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0009873734069584207</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-14.27808977</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-17.48506199</v>
+      </c>
+      <c r="G25" t="n">
+        <v>415229356.2713232</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>3.621202877750718e-05</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-0.69595045</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-1.51342205</v>
+      </c>
+      <c r="G26" t="n">
+        <v>232319.6113000387</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.002478330758241838</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-14.67276413</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-31.69600428</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2478330.681413584</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.001293877352367513</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-17.44373675</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-47.98960928</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1293875.024682156</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.06183697195327367</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-16.22523274</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-32.58965476</v>
+      </c>
+      <c r="G29" t="n">
+        <v>61836971.95327368</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.01559382262470001</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-11.84855636</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-7.40585482</v>
+      </c>
+      <c r="G30" t="n">
+        <v>14859439.9844478</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.1257968097149915</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-7.8732926</v>
+      </c>
+      <c r="F31" t="n">
+        <v>99.98420027</v>
+      </c>
+      <c r="G31" t="n">
+        <v>8810641.4942747</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.0006558036643491392</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-11.83827212</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-1.82959066</v>
+      </c>
+      <c r="G32" t="n">
+        <v>607640.1244181695</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.000215319811011067</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-18.89596887</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-26.33129112</v>
+      </c>
+      <c r="G33" t="n">
+        <v>188984.3183824633</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>1.228758023778634e-06</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-11.66819135</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-13.5100682</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1092224.381757449</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.002442583329699211</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-10.90942936</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-19.46210892</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1709807.532064699</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>2.773181537818392e-06</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-9.370748969999999</v>
+      </c>
+      <c r="F36" t="n">
+        <v>16.95261728</v>
+      </c>
+      <c r="G36" t="n">
+        <v>8164994.760424967</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.0006619354280805553</v>
+      </c>
+      <c r="E37" t="n">
+        <v>7.46391184</v>
+      </c>
+      <c r="F37" t="n">
+        <v>17.0982583</v>
+      </c>
+      <c r="G37" t="n">
+        <v>19858062.84241666</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0003348661248048968</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-4.32216653</v>
+      </c>
+      <c r="F38" t="n">
+        <v>14.66082936</v>
+      </c>
+      <c r="G38" t="n">
+        <v>26970629.66257701</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.008622960271945685</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-16.10020649</v>
+      </c>
+      <c r="F39" t="n">
+        <v>137.35004575</v>
+      </c>
+      <c r="G39" t="n">
+        <v>8435301.693484943</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.0007280896528862972</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-14.56565011</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-13.22591435</v>
+      </c>
+      <c r="G40" t="n">
+        <v>625224.8831580668</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.06633240815905936</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-11.87096768</v>
+      </c>
+      <c r="F41" t="n">
+        <v>16.6139908</v>
+      </c>
+      <c r="G41" t="n">
+        <v>64718624.57904577</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.04214354368754732</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-22.65711291</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-12.306064</v>
+      </c>
+      <c r="G42" t="n">
+        <v>39452158.24533769</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>1.105640837045478e-05</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-13.01571855</v>
+      </c>
+      <c r="F43" t="n">
+        <v>24.95288297</v>
+      </c>
+      <c r="G43" t="n">
+        <v>4626945.499299564</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.04021714166144226</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-19.3522833</v>
+      </c>
+      <c r="F44" t="n">
+        <v>34.55415649</v>
+      </c>
+      <c r="G44" t="n">
+        <v>40217141.66144226</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.002336096792446569</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-11.19372595</v>
+      </c>
+      <c r="F45" t="n">
+        <v>37.57498567</v>
+      </c>
+      <c r="G45" t="n">
+        <v>23360594.99474027</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.148356433035096</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-7.0726372</v>
+      </c>
+      <c r="F46" t="n">
+        <v>72.92969306000001</v>
+      </c>
+      <c r="G46" t="n">
+        <v>88967621.42690869</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.0001423297157667682</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-1.76447098</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-24.42521991</v>
+      </c>
+      <c r="G47" t="n">
+        <v>137287.3812847981</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1.082324254562332e-08</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-1.61975865</v>
+      </c>
+      <c r="F48" t="n">
+        <v>252.75424784</v>
+      </c>
+      <c r="G48" t="n">
+        <v>4342871.478255306</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.00682109062584335</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-9.4822995</v>
+      </c>
+      <c r="F49" t="n">
+        <v>37.96876274</v>
+      </c>
+      <c r="G49" t="n">
+        <v>6821090.625843351</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>1.722537497117852e-07</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-10.55552863</v>
+      </c>
+      <c r="F50" t="n">
+        <v>9.717844960000001</v>
+      </c>
+      <c r="G50" t="n">
+        <v>70823221.91370465</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>3.148797822575999e-06</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-35.73012851</v>
+      </c>
+      <c r="F51" t="n">
+        <v>47.65721157</v>
+      </c>
+      <c r="G51" t="n">
+        <v>1324667.755979497</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.01164824834206664</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-1.08661895</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-5.33163828</v>
+      </c>
+      <c r="G52" t="n">
+        <v>770636.0427258466</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.004827215256107817</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-11.25843827</v>
+      </c>
+      <c r="F53" t="n">
+        <v>55.88438277</v>
+      </c>
+      <c r="G53" t="n">
+        <v>4826448.92603148</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.09709072305297221</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-12.06679543</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-1.39772503</v>
+      </c>
+      <c r="G54" t="n">
+        <v>95745351.88569665</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>9.967135525737579e-09</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-15.58497922</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-15.46515985</v>
+      </c>
+      <c r="G55" t="n">
+        <v>316011.1732599385</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.008636900022972639</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-18.58408009</v>
+      </c>
+      <c r="F56" t="n">
+        <v>8.04482043</v>
+      </c>
+      <c r="G56" t="n">
+        <v>863690.0022972639</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>8.231829986590845e-05</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-7.36300726</v>
+      </c>
+      <c r="F57" t="n">
+        <v>33.89654919</v>
+      </c>
+      <c r="G57" t="n">
+        <v>32125448.81309545</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.0135064258316084</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-14.25075485</v>
+      </c>
+      <c r="F58" t="n">
+        <v>-10.79639135</v>
+      </c>
+      <c r="G58" t="n">
+        <v>12721719.37382424</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.0009926582216509563</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-4.88304353</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-2.57084181</v>
+      </c>
+      <c r="G59" t="n">
+        <v>992658.2216509563</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.08046634333618943</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-11.72386656</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-15.72488244</v>
+      </c>
+      <c r="G60" t="n">
+        <v>16354041.17639979</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.005360506971197263</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-7.56843651</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-20.49877474</v>
+      </c>
+      <c r="G61" t="n">
+        <v>9086692.670799023</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>4.94864406854408e-05</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-14.1634019</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-12.61334956</v>
+      </c>
+      <c r="G62" t="n">
+        <v>46934333.25368553</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>1.758239932562695e-05</v>
+      </c>
+      <c r="E63" t="n">
+        <v>4.67488237</v>
+      </c>
+      <c r="F63" t="n">
+        <v>11.48325899</v>
+      </c>
+      <c r="G63" t="n">
+        <v>152519.6125138548</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.02840179450913327</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-10.3046619</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-25.08972368</v>
+      </c>
+      <c r="G64" t="n">
+        <v>2698170.478367661</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.0008063459974253387</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-9.266462580000001</v>
+      </c>
+      <c r="F65" t="n">
+        <v>36.35643832</v>
+      </c>
+      <c r="G65" t="n">
+        <v>13214222.14015791</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.01185605639214786</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-8.61162689</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-21.37437164</v>
+      </c>
+      <c r="G66" t="n">
+        <v>11854306.40111492</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.0005904715502273874</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-14.00419258</v>
+      </c>
+      <c r="F67" t="n">
+        <v>25.70297213</v>
+      </c>
+      <c r="G67" t="n">
+        <v>547326.8663486073</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>6.23226603634112e-06</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-17.38773508</v>
+      </c>
+      <c r="F68" t="n">
+        <v>58.66291844</v>
+      </c>
+      <c r="G68" t="n">
+        <v>4270471.973173509</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1.271483341984596e-06</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-6.32685705</v>
+      </c>
+      <c r="F69" t="n">
+        <v>6.13699321</v>
+      </c>
+      <c r="G69" t="n">
+        <v>996479.0863778051</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.5041707511625931</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-3.05399826</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-12.29546318</v>
+      </c>
+      <c r="G70" t="n">
+        <v>43591145.63324606</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.187792022679608</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-20.42504772</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-9.433398950000001</v>
+      </c>
+      <c r="G71" t="n">
+        <v>104369058.3554944</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.003543526017542622</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-13.74604237</v>
+      </c>
+      <c r="F72" t="n">
+        <v>13.98929943</v>
+      </c>
+      <c r="G72" t="n">
+        <v>354352601.7542622</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.005053436968188039</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-17.88505404</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-12.37813807</v>
+      </c>
+      <c r="G73" t="n">
+        <v>42564529.61599909</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>2.240114922334288e-07</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-6.04689191</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-1.15590088</v>
+      </c>
+      <c r="G74" t="n">
+        <v>94084826.7380401</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.0001303906529307774</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-12.04168886</v>
+      </c>
+      <c r="F75" t="n">
+        <v>23.37754281</v>
+      </c>
+      <c r="G75" t="n">
+        <v>54854043.78144874</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.0002578626555316</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-5.28561884</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-9.33079028</v>
+      </c>
+      <c r="G76" t="n">
+        <v>4996776.595846883</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>3.420032637663216e-07</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-5.60327755</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-1.28147757</v>
+      </c>
+      <c r="G77" t="n">
+        <v>303050.0616097724</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.01251139537641968</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-4.41075719</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-18.30331642</v>
+      </c>
+      <c r="G78" t="n">
+        <v>1189203.551357983</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.0008196558034898667</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-7.28303475</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-7.93194663</v>
+      </c>
+      <c r="G79" t="n">
+        <v>813529.3142564724</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.008442865140885259</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-7.2450825</v>
+      </c>
+      <c r="F80" t="n">
+        <v>43.26977364</v>
+      </c>
+      <c r="G80" t="n">
+        <v>5882288.042287465</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.002262677835507319</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-14.91451005</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-18.13357604</v>
+      </c>
+      <c r="G81" t="n">
+        <v>2177231.058130979</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.01834113539710244</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-0.76792852</v>
+      </c>
+      <c r="F82" t="n">
+        <v>11.79892595</v>
+      </c>
+      <c r="G82" t="n">
+        <v>17424083.26755457</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>5.875469398854041</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-32.53893586</v>
+      </c>
+      <c r="F83" t="n">
+        <v>41.27175738</v>
+      </c>
+      <c r="G83" t="n">
+        <v>45652397.2290959</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.0001582068477852518</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-9.72865513</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-14.39802214</v>
+      </c>
+      <c r="G84" t="n">
+        <v>101760.4527997441</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.003217996701672718</v>
+      </c>
+      <c r="E85" t="n">
+        <v>2.45357163</v>
+      </c>
+      <c r="F85" t="n">
+        <v>27.87634037</v>
+      </c>
+      <c r="G85" t="n">
+        <v>3015725.564071133</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>3.336514638759932e-08</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-6.90005667</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-6.63835665</v>
+      </c>
+      <c r="G86" t="n">
+        <v>25686538.23347592</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.0002597259602227903</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-1.99658944</v>
+      </c>
+      <c r="F87" t="n">
+        <v>-30.3084849</v>
+      </c>
+      <c r="G87" t="n">
+        <v>129720.154728061</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.0181662068750626</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-27.11853504</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-30.00915868</v>
+      </c>
+      <c r="G88" t="n">
+        <v>17982646.78285147</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>8.391222005285845e-05</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-3.12620798</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-7.60220379</v>
+      </c>
+      <c r="G89" t="n">
+        <v>881078.3105550138</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>4.654071605660354e-05</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-11.27085023</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-14.25317468</v>
+      </c>
+      <c r="G90" t="n">
+        <v>106261968.4700819</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>1.027811339943037e-05</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-1.0792175</v>
+      </c>
+      <c r="F91" t="n">
+        <v>4.57286946</v>
+      </c>
+      <c r="G91" t="n">
+        <v>343941.9003778656</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.0001948998474670379</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-6.83641206</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-19.591113</v>
+      </c>
+      <c r="G92" t="n">
+        <v>179776.8401562403</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.02923876482553197</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-2.56834329</v>
+      </c>
+      <c r="F93" t="n">
+        <v>4.89765898</v>
+      </c>
+      <c r="G93" t="n">
+        <v>26959453.1125182</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.001446927478139359</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-2.46605042</v>
+      </c>
+      <c r="F94" t="n">
+        <v>59.29726017</v>
+      </c>
+      <c r="G94" t="n">
+        <v>1159343.010763642</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.005046275433438492</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-15.76895126</v>
+      </c>
+      <c r="F95" t="n">
+        <v>-16.37843639</v>
+      </c>
+      <c r="G95" t="n">
+        <v>448557816.3011581</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.000456987317678938</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-2.1267414</v>
+      </c>
+      <c r="F96" t="n">
+        <v>-9.51814005</v>
+      </c>
+      <c r="G96" t="n">
+        <v>456493.8504346507</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.01012739996451446</v>
+      </c>
+      <c r="E97" t="n">
+        <v>124.52745727</v>
+      </c>
+      <c r="F97" t="n">
+        <v>89.93648703</v>
+      </c>
+      <c r="G97" t="n">
+        <v>143602570.4580135</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30089</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>KOKO</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Koala AI</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>2.405193771862471e-06</v>
+      </c>
+      <c r="E98" t="n">
+        <v>4.25605006</v>
+      </c>
+      <c r="F98" t="n">
+        <v>-15.72318113</v>
+      </c>
+      <c r="G98" t="n">
+        <v>21912238.24899738</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-25T05:26:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>1.415727974474023e-05</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-6.41862212</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-2.77375216</v>
+      </c>
+      <c r="G99" t="n">
+        <v>3539292.918271024</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.02591931626567445</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-5.58278748</v>
+      </c>
+      <c r="F100" t="n">
+        <v>22.46967269</v>
+      </c>
+      <c r="G100" t="n">
+        <v>241112155.7586417</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30011</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>SKID</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Success Kid</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.02448687919127496</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-3.81453615</v>
+      </c>
+      <c r="F101" t="n">
+        <v>-0.321169</v>
+      </c>
+      <c r="G101" t="n">
+        <v>2124057.966651248</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-20T13:27:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>60942.07</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>145.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-03 12:21:51
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -24,6 +24,7 @@
     <sheet name="Portfolio_15" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="Portfolio_16" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="Portfolio_17" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Portfolio_18" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -26806,6 +26807,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.007909974190574492</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-35.76359724</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-64.76609741999999</v>
+      </c>
+      <c r="G2" t="n">
+        <v>7909974.190574492</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.815474977005101</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-0.6719293</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-6.64770289</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2486790.942377056</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.01318647235230595</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-7.77627933</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-39.42199106</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8063030.251900874</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1890704836227439</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-11.45743657</v>
+      </c>
+      <c r="F5" t="n">
+        <v>50.41021715</v>
+      </c>
+      <c r="G5" t="n">
+        <v>187174445.3293859</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.001101361238227794</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.60265708</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-57.5995671</v>
+      </c>
+      <c r="G6" t="n">
+        <v>805936.8906069569</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.005254455123088323</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-17.77307609</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-56.33201267</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5254455.123088324</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0002510664411826375</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-4.28492396</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-20.69878577</v>
+      </c>
+      <c r="G8" t="n">
+        <v>238513.1191235056</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.01832800225303504</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-2.22123695</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-3.32732275</v>
+      </c>
+      <c r="G9" t="n">
+        <v>18328002.25303504</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0005004836130249274</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4.9727769</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8.64134529</v>
+      </c>
+      <c r="G10" t="n">
+        <v>500483.6130249274</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.008200189408946698</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.0064527</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-23.51539316</v>
+      </c>
+      <c r="G11" t="n">
+        <v>8200189.408946698</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>6.663285661621343e-07</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-10.61847215</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-27.29266437</v>
+      </c>
+      <c r="G12" t="n">
+        <v>433647.1858213909</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0006615265707350083</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.48337006</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-21.686876</v>
+      </c>
+      <c r="G13" t="n">
+        <v>341843855.4273155</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0003768917976759188</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.34143539</v>
+      </c>
+      <c r="F14" t="n">
+        <v>23.51229261</v>
+      </c>
+      <c r="G14" t="n">
+        <v>376891.7976759188</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.005681227590047988</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-7.18675372</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-13.53958768</v>
+      </c>
+      <c r="G15" t="n">
+        <v>5341597.589451935</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>7.133829639110883e-05</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-16.4688724</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-48.56125428</v>
+      </c>
+      <c r="G16" t="n">
+        <v>713382.9639110883</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.01456519136595923</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4.10302412</v>
+      </c>
+      <c r="F17" t="n">
+        <v>25.0081994</v>
+      </c>
+      <c r="G17" t="n">
+        <v>14261269.72750604</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0002542090483899094</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-14.77330886</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-32.42589723</v>
+      </c>
+      <c r="G18" t="n">
+        <v>254209.0483899094</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.002867799103611568</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-19.64235548</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-23.71176621</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2724387.255652633</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>2.86070719025401e-05</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-1.3313636</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-32.3324064</v>
+      </c>
+      <c r="G20" t="n">
+        <v>193096455.2127693</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.237836035372752</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-1.24663247</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-29.78659853</v>
+      </c>
+      <c r="G21" t="n">
+        <v>237229404.8350294</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>3.744817609047298e-05</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-8.13703827</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-31.79817466</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3744817.609047298</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1.824392621911899e-06</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-2.09250242</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-23.38398827</v>
+      </c>
+      <c r="G23" t="n">
+        <v>587125.6155679034</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.00996441250717069</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-27.45900523</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-49.64910625</v>
+      </c>
+      <c r="G24" t="n">
+        <v>9964396.952722766</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1.670289036062e-06</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-20.74313063</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-59.18295086</v>
+      </c>
+      <c r="G25" t="n">
+        <v>11524991.61321004</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.000896763507319441</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-9.17686247</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-11.47659846</v>
+      </c>
+      <c r="G26" t="n">
+        <v>377113877.9637083</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>3.626095400814803e-05</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.13510768</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-1.64242333</v>
+      </c>
+      <c r="G27" t="n">
+        <v>232633.4929285739</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.00222129633070909</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-10.37127214</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-36.68508615</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2221296.261848903</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.001269927194407524</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-1.85103773</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-41.10398091</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1269924.909808501</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.06010105605830661</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-2.80724596</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-33.30394452</v>
+      </c>
+      <c r="G30" t="n">
+        <v>60101056.05830661</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.01221316079626825</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-21.67949392</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-20.37280883</v>
+      </c>
+      <c r="G31" t="n">
+        <v>11637988.59588799</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.1054861479447766</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-16.14560959</v>
+      </c>
+      <c r="F32" t="n">
+        <v>63.54609402</v>
+      </c>
+      <c r="G32" t="n">
+        <v>7388109.716447685</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.0005723300930926867</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-12.72843929</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-31.75252996</v>
+      </c>
+      <c r="G33" t="n">
+        <v>530297.0201001426</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0002207240669407246</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2.50987399</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-16.78234064</v>
+      </c>
+      <c r="G34" t="n">
+        <v>193727.5866327696</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1.16037673010171e-06</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-5.56507403</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-22.11599527</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1031441.286335312</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.002207098753425549</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-9.640800110000001</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-20.49945099</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1544968.405676592</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>2.416052697926165e-06</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-12.87794668</v>
+      </c>
+      <c r="F37" t="n">
+        <v>6.41101634</v>
+      </c>
+      <c r="G37" t="n">
+        <v>7113511.088421796</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0006012486434620652</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-9.168082269999999</v>
+      </c>
+      <c r="F38" t="n">
+        <v>22.97212458</v>
+      </c>
+      <c r="G38" t="n">
+        <v>18037459.30386196</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.000335480494819436</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.18346735</v>
+      </c>
+      <c r="F39" t="n">
+        <v>15.66792376</v>
+      </c>
+      <c r="G39" t="n">
+        <v>27020111.96284726</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.009411304777964443</v>
+      </c>
+      <c r="E40" t="n">
+        <v>9.142388240000001</v>
+      </c>
+      <c r="F40" t="n">
+        <v>147.98240387</v>
+      </c>
+      <c r="G40" t="n">
+        <v>9206489.723691313</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.0006119198318728683</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-15.95542809</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-35.59901125</v>
+      </c>
+      <c r="G41" t="n">
+        <v>525467.5765108903</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.05794345028472017</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-12.64684655</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-4.64699626</v>
+      </c>
+      <c r="G42" t="n">
+        <v>56533759.43775754</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.0387863625733607</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-7.9660627</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-38.60609295</v>
+      </c>
+      <c r="G43" t="n">
+        <v>36309374.58297838</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>1.062066331904766e-05</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-3.94110851</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2.98776116</v>
+      </c>
+      <c r="G44" t="n">
+        <v>4444592.556382056</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>8.862978974427277e-07</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-4.27995313</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-15.9942305</v>
+      </c>
+      <c r="G45" t="n">
+        <v>18612255.84629728</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.03992895035876039</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-0.71658823</v>
+      </c>
+      <c r="F46" t="n">
+        <v>39.50536546</v>
+      </c>
+      <c r="G46" t="n">
+        <v>39928950.35876039</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.00212247239742496</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-9.14450102</v>
+      </c>
+      <c r="F47" t="n">
+        <v>27.68095873</v>
+      </c>
+      <c r="G47" t="n">
+        <v>21224385.10856466</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.1340838337151878</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-9.620478889999999</v>
+      </c>
+      <c r="F48" t="n">
+        <v>31.10466896</v>
+      </c>
+      <c r="G48" t="n">
+        <v>80408510.18991123</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.0001373748618367356</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-3.48125049</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-5.92413281</v>
+      </c>
+      <c r="G49" t="n">
+        <v>132508.0636487146</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>8.439012281570304e-09</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-22.02879825</v>
+      </c>
+      <c r="F50" t="n">
+        <v>184.3966926</v>
+      </c>
+      <c r="G50" t="n">
+        <v>3386189.082226397</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.00660741124119094</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-3.13262785</v>
+      </c>
+      <c r="F51" t="n">
+        <v>35.12973334</v>
+      </c>
+      <c r="G51" t="n">
+        <v>6607411.24119094</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>1.537314214299344e-07</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-10.75293183</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-12.75995992</v>
+      </c>
+      <c r="G52" t="n">
+        <v>63207649.14121681</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>3.401234083274242e-06</v>
+      </c>
+      <c r="E53" t="n">
+        <v>8.01690915</v>
+      </c>
+      <c r="F53" t="n">
+        <v>50.58387605</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1430865.166492641</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.01053726465070538</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-9.53777477</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-34.01891771</v>
+      </c>
+      <c r="G54" t="n">
+        <v>697134.5126844898</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.004330128396835236</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-10.29759049</v>
+      </c>
+      <c r="F55" t="n">
+        <v>34.03074948</v>
+      </c>
+      <c r="G55" t="n">
+        <v>4329440.980291981</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.08160562567378826</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-15.94910089</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-39.618973</v>
+      </c>
+      <c r="G56" t="n">
+        <v>80474829.11139067</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>8.201346139808467e-09</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-17.71611695</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-36.59172081</v>
+      </c>
+      <c r="G57" t="n">
+        <v>260026.2642420478</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.00861180137389329</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-0.29059789</v>
+      </c>
+      <c r="F58" t="n">
+        <v>7.50456167</v>
+      </c>
+      <c r="G58" t="n">
+        <v>861180.137389329</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>8.160530523303779e-05</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-0.86614354</v>
+      </c>
+      <c r="F59" t="n">
+        <v>15.81419685</v>
+      </c>
+      <c r="G59" t="n">
+        <v>31847196.3149315</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.01217762188873915</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-9.838309260000001</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-26.79040913</v>
+      </c>
+      <c r="G60" t="n">
+        <v>11470117.27903077</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.0008970961315854547</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-9.626887480000001</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-24.10178235</v>
+      </c>
+      <c r="G61" t="n">
+        <v>897096.1315854547</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.0769126750033523</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-4.41634127</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-20.61771706</v>
+      </c>
+      <c r="G62" t="n">
+        <v>15631790.9058777</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.00517369686608064</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-3.48493354</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-24.26615422</v>
+      </c>
+      <c r="G63" t="n">
+        <v>8770027.470638806</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>4.649442152892912e-05</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-6.04918878</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-20.68629064</v>
+      </c>
+      <c r="G64" t="n">
+        <v>44096618.06851472</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>1.580445850908571e-05</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-10.11204889</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-24.0848389</v>
+      </c>
+      <c r="G65" t="n">
+        <v>137096.7547235533</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.02735486996146747</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-3.68612113</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-23.17559909</v>
+      </c>
+      <c r="G66" t="n">
+        <v>2598712.64633941</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.0007779867791732284</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-3.51700366</v>
+      </c>
+      <c r="F67" t="n">
+        <v>18.15860193</v>
+      </c>
+      <c r="G67" t="n">
+        <v>12749477.46367763</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.01063376595398148</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-10.30941822</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-29.43654006</v>
+      </c>
+      <c r="G68" t="n">
+        <v>10632196.37684298</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.0005263131308765828</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-10.86562415</v>
+      </c>
+      <c r="F69" t="n">
+        <v>10.71785264</v>
+      </c>
+      <c r="G69" t="n">
+        <v>487856.3861880766</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>5.20862516171076e-06</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-16.42485845</v>
+      </c>
+      <c r="F70" t="n">
+        <v>18.37025754</v>
+      </c>
+      <c r="G70" t="n">
+        <v>3569052.996478128</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1.17965598962549e-06</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-7.22206492</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-12.60279169</v>
+      </c>
+      <c r="G71" t="n">
+        <v>924512.7198814339</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.5701464550642659</v>
+      </c>
+      <c r="E72" t="n">
+        <v>13.08598401</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-0.42049153</v>
+      </c>
+      <c r="G72" t="n">
+        <v>49295475.98244207</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.1731908613843876</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-7.77517654</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-28.50892127</v>
+      </c>
+      <c r="G73" t="n">
+        <v>96254165.5408694</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.003143864517146522</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-11.2786388</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-8.749242730000001</v>
+      </c>
+      <c r="G74" t="n">
+        <v>314386451.7146522</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.00453846853104596</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-10.19045929</v>
+      </c>
+      <c r="F75" t="n">
+        <v>-31.49414502</v>
+      </c>
+      <c r="G75" t="n">
+        <v>38227008.55221144</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>2.248884498856378e-07</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.39147887</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-4.84319382</v>
+      </c>
+      <c r="G76" t="n">
+        <v>94453148.9519679</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.0001367893113906995</v>
+      </c>
+      <c r="E77" t="n">
+        <v>4.90729843</v>
+      </c>
+      <c r="F77" t="n">
+        <v>9.227544330000001</v>
+      </c>
+      <c r="G77" t="n">
+        <v>57545895.40895338</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.0002513170868700311</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-2.53839341</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-15.84629103</v>
+      </c>
+      <c r="G78" t="n">
+        <v>4869938.74789558</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>3.193451543112841e-07</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-6.62511498</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-8.35400561</v>
+      </c>
+      <c r="G79" t="n">
+        <v>282972.6465854475</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.01144622074436705</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-8.51363577</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-24.09006002</v>
+      </c>
+      <c r="G80" t="n">
+        <v>1087959.092435295</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0007534862204317228</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-8.072849939999999</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-14.81042883</v>
+      </c>
+      <c r="G81" t="n">
+        <v>747854.3134808645</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.006146663858201458</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-27.19694374</v>
+      </c>
+      <c r="F82" t="n">
+        <v>6.61214282</v>
+      </c>
+      <c r="G82" t="n">
+        <v>4282485.465920846</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.00217489635160183</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-3.87953966</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-12.6566864</v>
+      </c>
+      <c r="G83" t="n">
+        <v>2092764.51583818</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.01480106430944309</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-19.30126468</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-1.12742244</v>
+      </c>
+      <c r="G84" t="n">
+        <v>14061014.83864021</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>6.185006702008145</v>
+      </c>
+      <c r="E85" t="n">
+        <v>5.26829913</v>
+      </c>
+      <c r="F85" t="n">
+        <v>35.46719031</v>
+      </c>
+      <c r="G85" t="n">
+        <v>48057502.07460329</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.003098378023709529</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-3.71717839</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-9.906413880000001</v>
+      </c>
+      <c r="G86" t="n">
+        <v>2903625.665122676</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>3.064529089279659e-08</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-8.151786489999999</v>
+      </c>
+      <c r="F87" t="n">
+        <v>-13.62404496</v>
+      </c>
+      <c r="G87" t="n">
+        <v>23592626.48061918</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.0002588149090800924</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-0.350774</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-31.50835738</v>
+      </c>
+      <c r="G88" t="n">
+        <v>129265.1301510238</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.01716578237330972</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-5.50706324</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-36.59608847</v>
+      </c>
+      <c r="G89" t="n">
+        <v>16992331.05146848</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>7.82642064960136e-05</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-6.73085941</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-13.75192045</v>
+      </c>
+      <c r="G90" t="n">
+        <v>821774.1682081429</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>4.204862392373784e-05</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-9.65196179</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-24.1825359</v>
+      </c>
+      <c r="G91" t="n">
+        <v>96005603.87081939</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>9.747594814352781e-06</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-5.1616339</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-1.27570051</v>
+      </c>
+      <c r="G92" t="n">
+        <v>326188.8786659748</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.0001927826634090478</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-1.08629334</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-2.80197183</v>
+      </c>
+      <c r="G93" t="n">
+        <v>177823.9363191093</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.02560621913357276</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-12.42373169</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-3.91032387</v>
+      </c>
+      <c r="G94" t="n">
+        <v>23610082.99220661</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.001422134746474983</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-1.71347438</v>
+      </c>
+      <c r="F95" t="n">
+        <v>60.62025915</v>
+      </c>
+      <c r="G95" t="n">
+        <v>1139477.965274427</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.004816073139818355</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-4.56182578</v>
+      </c>
+      <c r="F96" t="n">
+        <v>-25.10388164</v>
+      </c>
+      <c r="G96" t="n">
+        <v>428095390.201795</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.0004313450095111967</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-5.61116407</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-3.15912991</v>
+      </c>
+      <c r="G97" t="n">
+        <v>430879.2315236112</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.007212734409171637</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-28.77999847</v>
+      </c>
+      <c r="F98" t="n">
+        <v>39.40780565</v>
+      </c>
+      <c r="G98" t="n">
+        <v>102273752.870159</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30089</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>KOKO</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Koala AI</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>2.205369575473094e-06</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-8.30802901</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-26.76547806</v>
+      </c>
+      <c r="G99" t="n">
+        <v>20091763.13783497</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-25T05:26:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30071</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>LADYF</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Milady Wif Hat</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>1.303052860493739e-05</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-7.95881102</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-12.05570174</v>
+      </c>
+      <c r="G100" t="n">
+        <v>3257607.28362503</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-22T09:31:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30063</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>GIGA</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Gigachad</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.02610008554308928</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.69743073</v>
+      </c>
+      <c r="F101" t="n">
+        <v>25.19401411</v>
+      </c>
+      <c r="G101" t="n">
+        <v>242793746.0338507</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-21T16:22:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>60545.16</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>135.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-04 12:21:33
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -25,6 +25,7 @@
     <sheet name="Portfolio_16" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="Portfolio_17" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="Portfolio_18" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Portfolio_19" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -30088,6 +30089,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33287</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MANYU</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>littlemanyu</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.02470340315102647</v>
+      </c>
+      <c r="E2" t="n">
+        <v>48.82261635</v>
+      </c>
+      <c r="F2" t="n">
+        <v>47.17547182</v>
+      </c>
+      <c r="G2" t="n">
+        <v>24686553.13142581</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-10-03T09:11:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.006551706891568292</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-15.43415046</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-65.81578035</v>
+      </c>
+      <c r="G3" t="n">
+        <v>6551706.891568292</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.836572647515511</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.58716345</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-4.88422403</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2551128.28859855</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.014307359860125</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8.5002833</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-29.34693257</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8748410.666242117</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.15994033591637</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-15.03962385</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-13.84187934</v>
+      </c>
+      <c r="G6" t="n">
+        <v>158336420.8274603</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.001124750630833959</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.12368039</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-14.22210069</v>
+      </c>
+      <c r="G7" t="n">
+        <v>823052.4142843016</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.003717588723660549</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-29.31066205</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-65.43288705000001</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3717588.72366055</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0001573483471705551</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-37.32800512</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-54.40678662</v>
+      </c>
+      <c r="G9" t="n">
+        <v>149480.9298120273</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.01912688623215535</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4.36623779</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-7.90903414</v>
+      </c>
+      <c r="G10" t="n">
+        <v>19126886.23215535</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0004995589255969943</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.18475878</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-24.02464529</v>
+      </c>
+      <c r="G11" t="n">
+        <v>499558.9255969943</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.008120244552396431</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-0.94724463</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-17.91459582</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8120244.552396432</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>6.546449851674903e-07</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-1.7534264</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-27.33492234</v>
+      </c>
+      <c r="G13" t="n">
+        <v>426043.5015792075</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0006668733939684064</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.9483497400000001</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-23.18687814</v>
+      </c>
+      <c r="G14" t="n">
+        <v>344606826.333174</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0003855370421472952</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.29382664</v>
+      </c>
+      <c r="F15" t="n">
+        <v>23.03884497</v>
+      </c>
+      <c r="G15" t="n">
+        <v>385537.0421472952</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>2.460690346230302e-07</v>
+      </c>
+      <c r="E16" t="n">
+        <v>7.29343391</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-41.67013589</v>
+      </c>
+      <c r="G16" t="n">
+        <v>101448.3268069144</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.005773444819580117</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.16272356</v>
+      </c>
+      <c r="F17" t="n">
+        <v>20.18729427</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5428301.972116985</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>7.090661177359881e-05</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-0.60512325</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-48.48967091</v>
+      </c>
+      <c r="G18" t="n">
+        <v>709066.1177359881</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.01419105611704784</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-2.56869436</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-15.16326025</v>
+      </c>
+      <c r="G19" t="n">
+        <v>13894941.29657563</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0002205554713523362</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-13.23854412</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-37.74164786</v>
+      </c>
+      <c r="G20" t="n">
+        <v>220555.4713523362</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.002234019868605398</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-21.84762881</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-40.43955079</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2122301.820667451</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>2.941622269671281e-05</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2.86154987</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-29.40909583</v>
+      </c>
+      <c r="G22" t="n">
+        <v>198558186.7626397</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.2413338785491054</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1.58157238</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-31.4272446</v>
+      </c>
+      <c r="G23" t="n">
+        <v>240718326.3251311</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>3.342276046405964e-05</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-10.7476837</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-32.00824268</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3342276.046405965</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1.972452910192758e-06</v>
+      </c>
+      <c r="E25" t="n">
+        <v>8.115593459999999</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-2.95942707</v>
+      </c>
+      <c r="G25" t="n">
+        <v>634774.3436179879</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.01170961613261389</v>
+      </c>
+      <c r="E26" t="n">
+        <v>17.59495776</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-26.09204973</v>
+      </c>
+      <c r="G26" t="n">
+        <v>11709597.85390311</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1.804226307325879e-06</v>
+      </c>
+      <c r="E27" t="n">
+        <v>8.0186773</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-49.89422755</v>
+      </c>
+      <c r="G27" t="n">
+        <v>12449158.56556687</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.0009888127175633177</v>
+      </c>
+      <c r="E28" t="n">
+        <v>10.2688194</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-10.53140705</v>
+      </c>
+      <c r="G28" t="n">
+        <v>415840163.7279929</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>3.623204276248921e-05</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-0.07973107</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-0.03114954</v>
+      </c>
+      <c r="G29" t="n">
+        <v>232448.0117616687</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.002400682438139767</v>
+      </c>
+      <c r="E30" t="n">
+        <v>7.65762583</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-25.04697016</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2400682.363718612</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.001284971180172487</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1.18463372</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-41.08109273</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1284968.868509333</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.06246442108188475</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3.98990561</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-31.06848476</v>
+      </c>
+      <c r="G32" t="n">
+        <v>62464421.08188475</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.01470696683070678</v>
+      </c>
+      <c r="E33" t="n">
+        <v>20.41920952</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-0.66828582</v>
+      </c>
+      <c r="G33" t="n">
+        <v>14014350.1842837</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.1279731109339474</v>
+      </c>
+      <c r="E34" t="n">
+        <v>21.31745582</v>
+      </c>
+      <c r="F34" t="n">
+        <v>15.56298635</v>
+      </c>
+      <c r="G34" t="n">
+        <v>8963066.741522355</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.000698496727149438</v>
+      </c>
+      <c r="E35" t="n">
+        <v>22.04438236</v>
+      </c>
+      <c r="F35" t="n">
+        <v>12.62642147</v>
+      </c>
+      <c r="G35" t="n">
+        <v>647197.7228306651</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0002114047386777101</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-4.22216226</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-17.41210134</v>
+      </c>
+      <c r="G36" t="n">
+        <v>185548.0935740575</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>1.048793410674114e-06</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-9.616048429999999</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-22.99089324</v>
+      </c>
+      <c r="G37" t="n">
+        <v>932256.5643498139</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.002313008902592921</v>
+      </c>
+      <c r="E38" t="n">
+        <v>4.79861397</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-12.82559623</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1619105.475461134</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0001351421036015336</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1275.63992312</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-5.36645884</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1351421.036015336</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>2.220417232167947e-06</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-8.09494849</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-11.29141375</v>
+      </c>
+      <c r="G40" t="n">
+        <v>6537507.487112031</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.0005056952030157025</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-19.47173271</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-15.43111424</v>
+      </c>
+      <c r="G41" t="n">
+        <v>15170856.09047107</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.0003482331715288463</v>
+      </c>
+      <c r="E42" t="n">
+        <v>3.80246415</v>
+      </c>
+      <c r="F42" t="n">
+        <v>14.70416246</v>
+      </c>
+      <c r="G42" t="n">
+        <v>28047232.04236104</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.007912746247480815</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-15.9229625</v>
+      </c>
+      <c r="F43" t="n">
+        <v>99.15554917999999</v>
+      </c>
+      <c r="G43" t="n">
+        <v>7740543.817492376</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.0006238852337106229</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1.95538716</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-20.9872806</v>
+      </c>
+      <c r="G44" t="n">
+        <v>535742.5020455315</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.06202225907903707</v>
+      </c>
+      <c r="E45" t="n">
+        <v>6.70968885</v>
+      </c>
+      <c r="F45" t="n">
+        <v>6.18582984</v>
+      </c>
+      <c r="G45" t="n">
+        <v>60513335.97380184</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.04496387099063005</v>
+      </c>
+      <c r="E46" t="n">
+        <v>15.96602915</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-25.44881268</v>
+      </c>
+      <c r="G46" t="n">
+        <v>42092372.83881868</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1.363977949293652e-05</v>
+      </c>
+      <c r="E47" t="n">
+        <v>28.42681369</v>
+      </c>
+      <c r="F47" t="n">
+        <v>9.28959279</v>
+      </c>
+      <c r="G47" t="n">
+        <v>5710776.557370896</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>8.910419168305559e-07</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.5352624</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-21.85851748</v>
+      </c>
+      <c r="G48" t="n">
+        <v>18711880.25344167</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.04088702741817437</v>
+      </c>
+      <c r="E49" t="n">
+        <v>2.40140373</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-10.7293139</v>
+      </c>
+      <c r="G49" t="n">
+        <v>40887027.41817437</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.002341602716782486</v>
+      </c>
+      <c r="E50" t="n">
+        <v>10.32429537</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-30.53589499</v>
+      </c>
+      <c r="G50" t="n">
+        <v>23415653.17834655</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.1319077279808699</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-1.40994899</v>
+      </c>
+      <c r="F51" t="n">
+        <v>12.0504947</v>
+      </c>
+      <c r="G51" t="n">
+        <v>79103524.97831665</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.0002179212333836037</v>
+      </c>
+      <c r="E52" t="n">
+        <v>58.64969174</v>
+      </c>
+      <c r="F52" t="n">
+        <v>12.10936289</v>
+      </c>
+      <c r="G52" t="n">
+        <v>210200.9077753926</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>7.62528439699326e-09</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-9.379229690000001</v>
+      </c>
+      <c r="F53" t="n">
+        <v>35.99713231</v>
+      </c>
+      <c r="G53" t="n">
+        <v>3067302.639098656</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.006098348653075832</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-7.70441811</v>
+      </c>
+      <c r="F54" t="n">
+        <v>19.18675484</v>
+      </c>
+      <c r="G54" t="n">
+        <v>6098348.653075832</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>1.611393413688418e-07</v>
+      </c>
+      <c r="E55" t="n">
+        <v>4.93015133</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-22.94899401</v>
+      </c>
+      <c r="G55" t="n">
+        <v>66253462.41744473</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>3.537244622187246e-06</v>
+      </c>
+      <c r="E56" t="n">
+        <v>3.99885852</v>
+      </c>
+      <c r="F56" t="n">
+        <v>27.89540792</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1488083.440107953</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.01135732080649057</v>
+      </c>
+      <c r="E57" t="n">
+        <v>7.78243864</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-20.25839809</v>
+      </c>
+      <c r="G57" t="n">
+        <v>751388.5783730606</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.004393218250891839</v>
+      </c>
+      <c r="E58" t="n">
+        <v>1.45699731</v>
+      </c>
+      <c r="F58" t="n">
+        <v>-0.58740799</v>
+      </c>
+      <c r="G58" t="n">
+        <v>4392520.818708073</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.09206753637930863</v>
+      </c>
+      <c r="E59" t="n">
+        <v>12.8092576</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-26.00413515</v>
+      </c>
+      <c r="G59" t="n">
+        <v>90791770.73464209</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>8.16699818051124e-09</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-0.4188088</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-33.05745378</v>
+      </c>
+      <c r="G60" t="n">
+        <v>258937.2513668267</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.008824923301394151</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2.47476594</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-8.06605723</v>
+      </c>
+      <c r="G61" t="n">
+        <v>882492.3301394151</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>9.841343155320437e-05</v>
+      </c>
+      <c r="E62" t="n">
+        <v>20.5858072</v>
+      </c>
+      <c r="F62" t="n">
+        <v>33.23784649</v>
+      </c>
+      <c r="G62" t="n">
+        <v>38406717.13377895</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.01286405088275085</v>
+      </c>
+      <c r="E63" t="n">
+        <v>5.63669332</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-10.61385467</v>
+      </c>
+      <c r="G63" t="n">
+        <v>12116665.60652663</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0009459927584504606</v>
+      </c>
+      <c r="E64" t="n">
+        <v>5.45054483</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-33.16130572</v>
+      </c>
+      <c r="G64" t="n">
+        <v>945992.7584504606</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.07655968659119293</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-0.4580869</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-22.12160721</v>
+      </c>
+      <c r="G65" t="n">
+        <v>15560049.27095429</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.005184732672646127</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.21330601</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-24.02984275</v>
+      </c>
+      <c r="G66" t="n">
+        <v>8788734.466669925</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>5.122939397781215e-05</v>
+      </c>
+      <c r="E67" t="n">
+        <v>9.9417642</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-12.26905255</v>
+      </c>
+      <c r="G67" t="n">
+        <v>48587399.21552652</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1.666624434488951e-05</v>
+      </c>
+      <c r="E68" t="n">
+        <v>5.45280204</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-10.20777205</v>
+      </c>
+      <c r="G68" t="n">
+        <v>144572.3693602399</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.02736304054357589</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.02506699</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-21.70909451</v>
+      </c>
+      <c r="G69" t="n">
+        <v>2599488.851639709</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.0008471622298040202</v>
+      </c>
+      <c r="E70" t="n">
+        <v>8.89350404</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-13.47528269</v>
+      </c>
+      <c r="G70" t="n">
+        <v>13883109.6441554</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.01152147754366368</v>
+      </c>
+      <c r="E71" t="n">
+        <v>8.34804521</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-22.10151455</v>
+      </c>
+      <c r="G71" t="n">
+        <v>11519776.93751601</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.00058629211958756</v>
+      </c>
+      <c r="E72" t="n">
+        <v>11.39606542</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-11.58501456</v>
+      </c>
+      <c r="G72" t="n">
+        <v>543452.8191157861</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>6.040280945578369e-06</v>
+      </c>
+      <c r="E73" t="n">
+        <v>15.96689641</v>
+      </c>
+      <c r="F73" t="n">
+        <v>6.19401784</v>
+      </c>
+      <c r="G73" t="n">
+        <v>4138919.991183531</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>1.206539972752483e-06</v>
+      </c>
+      <c r="E74" t="n">
+        <v>2.27896805</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-14.40908657</v>
+      </c>
+      <c r="G74" t="n">
+        <v>945582.0694041485</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.5743785413660081</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.74228056</v>
+      </c>
+      <c r="F75" t="n">
+        <v>37.26035311</v>
+      </c>
+      <c r="G75" t="n">
+        <v>49661386.71781557</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.1992113646018788</v>
+      </c>
+      <c r="E76" t="n">
+        <v>15.04336361</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-4.41156168</v>
+      </c>
+      <c r="G76" t="n">
+        <v>110715562.6609184</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.003343614042376892</v>
+      </c>
+      <c r="E77" t="n">
+        <v>6.32339878</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-21.82747806</v>
+      </c>
+      <c r="G77" t="n">
+        <v>334361404.2376893</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.004690435183506652</v>
+      </c>
+      <c r="E78" t="n">
+        <v>3.35258045</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-27.21647949</v>
+      </c>
+      <c r="G78" t="n">
+        <v>39507006.52587306</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>2.632275008323521e-07</v>
+      </c>
+      <c r="E79" t="n">
+        <v>17.10858375</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-2.45678424</v>
+      </c>
+      <c r="G79" t="n">
+        <v>110555550.3495879</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.0001583509850544022</v>
+      </c>
+      <c r="E80" t="n">
+        <v>15.69271714</v>
+      </c>
+      <c r="F80" t="n">
+        <v>40.97202867</v>
+      </c>
+      <c r="G80" t="n">
+        <v>66616675.90253647</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0002530171593211036</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.67646513</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-15.54801075</v>
+      </c>
+      <c r="G81" t="n">
+        <v>4902882.185235316</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>3.274171788833967e-07</v>
+      </c>
+      <c r="E82" t="n">
+        <v>2.52768031</v>
+      </c>
+      <c r="F82" t="n">
+        <v>-10.69508737</v>
+      </c>
+      <c r="G82" t="n">
+        <v>290125.2904431557</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.01133744790188965</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-0.95029482</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-23.77940053</v>
+      </c>
+      <c r="G83" t="n">
+        <v>1077620.273568679</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.0007663118628750041</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1.70217346</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-14.8699115</v>
+      </c>
+      <c r="G84" t="n">
+        <v>760584.0910989282</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.005818990769296669</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-5.22407936</v>
+      </c>
+      <c r="F85" t="n">
+        <v>11.11199144</v>
+      </c>
+      <c r="G85" t="n">
+        <v>4054189.105649745</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.002260357359045224</v>
+      </c>
+      <c r="E86" t="n">
+        <v>3.92942898</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-5.91224771</v>
+      </c>
+      <c r="G86" t="n">
+        <v>2174998.211128346</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.0166302571298907</v>
+      </c>
+      <c r="E87" t="n">
+        <v>12.38425533</v>
+      </c>
+      <c r="F87" t="n">
+        <v>25.61570405</v>
+      </c>
+      <c r="G87" t="n">
+        <v>15798748.48085122</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>6.463910377401948</v>
+      </c>
+      <c r="E88" t="n">
+        <v>4.50935122</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-2.60667022</v>
+      </c>
+      <c r="G88" t="n">
+        <v>50224583.63241313</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.003688210859409003</v>
+      </c>
+      <c r="E89" t="n">
+        <v>19.03947312</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-11.04217794</v>
+      </c>
+      <c r="G89" t="n">
+        <v>3456383.833029704</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>3.110416500991274e-08</v>
+      </c>
+      <c r="E90" t="n">
+        <v>1.48360099</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-13.69753398</v>
+      </c>
+      <c r="G90" t="n">
+        <v>23945895.94980507</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.0002359606609602159</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-8.830120429999999</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-24.73393676</v>
+      </c>
+      <c r="G91" t="n">
+        <v>117850.5738249606</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.0210168656502691</v>
+      </c>
+      <c r="E92" t="n">
+        <v>22.76360169</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-37.75043545</v>
+      </c>
+      <c r="G92" t="n">
+        <v>20804501.1306264</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>7.415320173919942e-05</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-5.25271985</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-18.11783997</v>
+      </c>
+      <c r="G93" t="n">
+        <v>778608.618261594</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>4.303236477369847e-05</v>
+      </c>
+      <c r="E94" t="n">
+        <v>2.34115054</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-22.21233884</v>
+      </c>
+      <c r="G94" t="n">
+        <v>98251685.32461806</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>9.881860742078313e-06</v>
+      </c>
+      <c r="E95" t="n">
+        <v>1.33867162</v>
+      </c>
+      <c r="F95" t="n">
+        <v>-1.37182808</v>
+      </c>
+      <c r="G95" t="n">
+        <v>330681.8898386746</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.000194228918110362</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.75019956</v>
+      </c>
+      <c r="F96" t="n">
+        <v>-5.16642225</v>
+      </c>
+      <c r="G96" t="n">
+        <v>179157.970714941</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.02876818550823859</v>
+      </c>
+      <c r="E97" t="n">
+        <v>12.30028521</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-17.54634605</v>
+      </c>
+      <c r="G97" t="n">
+        <v>26525557.86707973</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.001489930134864796</v>
+      </c>
+      <c r="E98" t="n">
+        <v>4.76715646</v>
+      </c>
+      <c r="F98" t="n">
+        <v>39.93464658</v>
+      </c>
+      <c r="G98" t="n">
+        <v>1193798.662668887</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.005200826542367564</v>
+      </c>
+      <c r="E99" t="n">
+        <v>8.04425382</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-17.50853018</v>
+      </c>
+      <c r="G99" t="n">
+        <v>462295692.6502717</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.0004230721608073575</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-1.91791919</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-16.17219066</v>
+      </c>
+      <c r="G100" t="n">
+        <v>422615.3160651693</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.008162080001542763</v>
+      </c>
+      <c r="E101" t="n">
+        <v>13.12461234</v>
+      </c>
+      <c r="F101" t="n">
+        <v>60.00813736</v>
+      </c>
+      <c r="G101" t="n">
+        <v>115735102.0609841</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>61475.12</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>139.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-05 12:20:19
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -26,6 +26,7 @@
     <sheet name="Portfolio_17" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="Portfolio_18" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="Portfolio_19" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Portfolio_20" sheetId="20" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -36651,6 +36652,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33287</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MANYU</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>littlemanyu</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.01988468575245944</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-18.72783961</v>
+      </c>
+      <c r="F2" t="n">
+        <v>18.46699784</v>
+      </c>
+      <c r="G2" t="n">
+        <v>19871122.54650626</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-10-03T09:11:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.00408002895501584</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-38.12938175</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-77.25275144</v>
+      </c>
+      <c r="G3" t="n">
+        <v>4080028.95501584</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.8353472013182026</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.14648413</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-3.05871829</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2547391.290419859</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.01408533513638685</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1.55182176</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-22.99537497</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8612650.925779186</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.154491307972043</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-3.48571739</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-49.19310716</v>
+      </c>
+      <c r="G6" t="n">
+        <v>152942036.8732795</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.001287137518324028</v>
+      </c>
+      <c r="E7" t="n">
+        <v>14.43759026</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.72956624</v>
+      </c>
+      <c r="G7" t="n">
+        <v>941881.3494569955</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.004989274107378729</v>
+      </c>
+      <c r="E8" t="n">
+        <v>34.46422408</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-50.06131758</v>
+      </c>
+      <c r="G8" t="n">
+        <v>4989274.10737873</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0001346544015576741</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-14.42274166</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-55.7456235</v>
+      </c>
+      <c r="G9" t="n">
+        <v>127921.6814797904</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.01899121786302015</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-0.68938345</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-13.05788585</v>
+      </c>
+      <c r="G10" t="n">
+        <v>18991217.86302015</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0004754717699272826</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-4.82168458</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-19.22245178</v>
+      </c>
+      <c r="G11" t="n">
+        <v>475471.7699272826</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.006627160507433174</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-18.38202182</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-23.04519661</v>
+      </c>
+      <c r="G12" t="n">
+        <v>6627160.507433173</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>6.678582667292424e-07</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.01838888</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-19.07453931</v>
+      </c>
+      <c r="G13" t="n">
+        <v>434642.716224502</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0007039733217414568</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5.66252594</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-19.37884134</v>
+      </c>
+      <c r="G14" t="n">
+        <v>363778214.0098978</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0003816580684846553</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-1.00612217</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-18.46494221</v>
+      </c>
+      <c r="G15" t="n">
+        <v>381658.0684846553</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>2.459292327778804e-07</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.05681407</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-39.98253053</v>
+      </c>
+      <c r="G16" t="n">
+        <v>101390.6898787382</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.00722811416683604</v>
+      </c>
+      <c r="E17" t="n">
+        <v>25.18447775</v>
+      </c>
+      <c r="F17" t="n">
+        <v>29.55329879</v>
+      </c>
+      <c r="G17" t="n">
+        <v>6796009.594385683</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>6.14304442614686e-05</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-13.36429322</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-43.7353927</v>
+      </c>
+      <c r="G18" t="n">
+        <v>614304.442614686</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.01640368463361745</v>
+      </c>
+      <c r="E19" t="n">
+        <v>15.59171142</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-17.30470775</v>
+      </c>
+      <c r="G19" t="n">
+        <v>16061400.44487894</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0002706394294867468</v>
+      </c>
+      <c r="E20" t="n">
+        <v>21.81443947</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-25.45417993</v>
+      </c>
+      <c r="G20" t="n">
+        <v>270639.4294867468</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.002007663444869042</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-11.49451318</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-45.91836124</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1907264.946122852</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>3.250806251037919e-05</v>
+      </c>
+      <c r="E22" t="n">
+        <v>10.6525382</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-14.67070718</v>
+      </c>
+      <c r="G22" t="n">
+        <v>219427967.1383076</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.2429184015355451</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.79900143</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-26.508167</v>
+      </c>
+      <c r="G23" t="n">
+        <v>242294669.1868216</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>3.418133106903834e-05</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.49584078</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-26.55456438</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3418133.106903834</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>2.242703525293083e-06</v>
+      </c>
+      <c r="E25" t="n">
+        <v>13.82086441</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-14.69748353</v>
+      </c>
+      <c r="G25" t="n">
+        <v>721746.3346481321</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.009542653179618518</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-18.27660388</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-28.01510306</v>
+      </c>
+      <c r="G26" t="n">
+        <v>9542638.283536904</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1.867703432525815e-06</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3.56287101</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-34.53700992</v>
+      </c>
+      <c r="G27" t="n">
+        <v>12887150.6254829</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.001028265282638033</v>
+      </c>
+      <c r="E28" t="n">
+        <v>4.03679253</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-14.59347366</v>
+      </c>
+      <c r="G28" t="n">
+        <v>432435528.7484751</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>3.624133145013892e-05</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.01838509</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-0.85348927</v>
+      </c>
+      <c r="G29" t="n">
+        <v>232507.6036811805</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.002454040082900841</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1.80925199</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-20.47051654</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2454040.006825599</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.001410575801466553</v>
+      </c>
+      <c r="E31" t="n">
+        <v>9.77811466</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-3.17810152</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1410573.263840686</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.06274347708308088</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.51954217</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-33.22076541</v>
+      </c>
+      <c r="G32" t="n">
+        <v>62743477.08308088</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.01590355504828692</v>
+      </c>
+      <c r="E33" t="n">
+        <v>8.55007144</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-2.64146185</v>
+      </c>
+      <c r="G33" t="n">
+        <v>15154585.72711113</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.1360396730070987</v>
+      </c>
+      <c r="E34" t="n">
+        <v>5.99626872</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-16.78444732</v>
+      </c>
+      <c r="G34" t="n">
+        <v>9528038.036731441</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.000659859151192868</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-5.51540829</v>
+      </c>
+      <c r="F35" t="n">
+        <v>20.12423</v>
+      </c>
+      <c r="G35" t="n">
+        <v>611397.7681525106</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0002095665522689795</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-0.8695105</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-41.25909558</v>
+      </c>
+      <c r="G36" t="n">
+        <v>183934.733410482</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>7.125803133883235e-07</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-31.43064583</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-51.54298956</v>
+      </c>
+      <c r="G37" t="n">
+        <v>633401.8387431772</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.00233563382746976</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.97850684</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-13.10340179</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1634942.915476571</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0001646936029752074</v>
+      </c>
+      <c r="E39" t="n">
+        <v>21.86704295</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-0.93182442</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1646936.029752074</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>2.258620399539667e-06</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.72369418</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-10.43319424</v>
+      </c>
+      <c r="G40" t="n">
+        <v>6649987.920566496</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.0005402706501566506</v>
+      </c>
+      <c r="E41" t="n">
+        <v>6.81356826</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-7.4224824</v>
+      </c>
+      <c r="G41" t="n">
+        <v>16208119.50469952</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.0003720337411342747</v>
+      </c>
+      <c r="E42" t="n">
+        <v>6.84106221</v>
+      </c>
+      <c r="F42" t="n">
+        <v>17.50917337</v>
+      </c>
+      <c r="G42" t="n">
+        <v>29964166.3066447</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.009049990862900962</v>
+      </c>
+      <c r="E43" t="n">
+        <v>14.37232203</v>
+      </c>
+      <c r="F43" t="n">
+        <v>68.187866</v>
+      </c>
+      <c r="G43" t="n">
+        <v>8853038.96159857</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.0005473126399895287</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-12.27350634</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-38.86592911</v>
+      </c>
+      <c r="G44" t="n">
+        <v>469988.1120846324</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.07984661141443709</v>
+      </c>
+      <c r="E45" t="n">
+        <v>28.77959138</v>
+      </c>
+      <c r="F45" t="n">
+        <v>35.84193801</v>
+      </c>
+      <c r="G45" t="n">
+        <v>77904044.36468728</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.04331645796628184</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-3.49390269</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-18.35355396</v>
+      </c>
+      <c r="G46" t="n">
+        <v>40550167.47009407</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1.672804593028388e-05</v>
+      </c>
+      <c r="E47" t="n">
+        <v>22.70015991</v>
+      </c>
+      <c r="F47" t="n">
+        <v>31.72663845</v>
+      </c>
+      <c r="G47" t="n">
+        <v>7003788.631536158</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>8.849257882590145e-07</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-1.1852722</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-13.90396387</v>
+      </c>
+      <c r="G48" t="n">
+        <v>18583441.5534393</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.04581496090969454</v>
+      </c>
+      <c r="E49" t="n">
+        <v>12.05964475</v>
+      </c>
+      <c r="F49" t="n">
+        <v>26.13538246</v>
+      </c>
+      <c r="G49" t="n">
+        <v>45814960.90969454</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.002152416727073575</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-8.26229036</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-20.96624129</v>
+      </c>
+      <c r="G50" t="n">
+        <v>21523823.49493661</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.1363809022213305</v>
+      </c>
+      <c r="E51" t="n">
+        <v>3.25846455</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-3.58979692</v>
+      </c>
+      <c r="G51" t="n">
+        <v>81786035.36401565</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.0002382180405239826</v>
+      </c>
+      <c r="E52" t="n">
+        <v>9.326562920000001</v>
+      </c>
+      <c r="F52" t="n">
+        <v>69.29435700000001</v>
+      </c>
+      <c r="G52" t="n">
+        <v>229778.6571282499</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>8.072749842799518e-09</v>
+      </c>
+      <c r="E53" t="n">
+        <v>5.86817676</v>
+      </c>
+      <c r="F53" t="n">
+        <v>26.86489572</v>
+      </c>
+      <c r="G53" t="n">
+        <v>3247297.491929088</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.005990770141706759</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-2.4756273</v>
+      </c>
+      <c r="F54" t="n">
+        <v>17.72713743</v>
+      </c>
+      <c r="G54" t="n">
+        <v>5990770.141706758</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>1.733666666474928e-07</v>
+      </c>
+      <c r="E55" t="n">
+        <v>7.84301891</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-13.761627</v>
+      </c>
+      <c r="G55" t="n">
+        <v>71280804.77179056</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>3.619754535087956e-06</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2.33260409</v>
+      </c>
+      <c r="F56" t="n">
+        <v>15.35067691</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1522794.535366152</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.01198978674976755</v>
+      </c>
+      <c r="E57" t="n">
+        <v>5.61570604</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-7.70245408</v>
+      </c>
+      <c r="G57" t="n">
+        <v>793231.8699455481</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.004917395291153545</v>
+      </c>
+      <c r="E58" t="n">
+        <v>11.95415706</v>
+      </c>
+      <c r="F58" t="n">
+        <v>7.43615052</v>
+      </c>
+      <c r="G58" t="n">
+        <v>4916614.644816283</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.1075568972260401</v>
+      </c>
+      <c r="E59" t="n">
+        <v>16.83742986</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-5.79920397</v>
+      </c>
+      <c r="G59" t="n">
+        <v>106066497.8982837</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>8.739173754720266e-09</v>
+      </c>
+      <c r="E60" t="n">
+        <v>7.01179542</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-26.99365847</v>
+      </c>
+      <c r="G60" t="n">
+        <v>277078.2582839663</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.009289180693862002</v>
+      </c>
+      <c r="E61" t="n">
+        <v>5.26075272</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-0.75787025</v>
+      </c>
+      <c r="G61" t="n">
+        <v>928918.0693862002</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.0001124771370818696</v>
+      </c>
+      <c r="E62" t="n">
+        <v>14.32968586</v>
+      </c>
+      <c r="F62" t="n">
+        <v>58.32711973</v>
+      </c>
+      <c r="G62" t="n">
+        <v>43895203.32481476</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.01348527390007695</v>
+      </c>
+      <c r="E63" t="n">
+        <v>5.58505102</v>
+      </c>
+      <c r="F63" t="n">
+        <v>14.6800745</v>
+      </c>
+      <c r="G63" t="n">
+        <v>12701796.34307485</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0009388751605462348</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-0.8509071499999999</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-35.92865928</v>
+      </c>
+      <c r="G64" t="n">
+        <v>938875.1605462348</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.07899880471612578</v>
+      </c>
+      <c r="E65" t="n">
+        <v>3.2141915</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-17.67943541</v>
+      </c>
+      <c r="G65" t="n">
+        <v>16055777.50459101</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.005234063456121809</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.98126608</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-23.75720915</v>
+      </c>
+      <c r="G66" t="n">
+        <v>8872355.973191934</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>4.975173665392455e-05</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-2.88412786</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-11.94411712</v>
+      </c>
+      <c r="G67" t="n">
+        <v>47185947.41754959</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1.635257851737348e-05</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-1.86027288</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-14.70672489</v>
+      </c>
+      <c r="G68" t="n">
+        <v>141851.4557018944</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.02694072713398491</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-1.54342938</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-18.74676263</v>
+      </c>
+      <c r="G69" t="n">
+        <v>2559369.077728567</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.0009197273379503412</v>
+      </c>
+      <c r="E70" t="n">
+        <v>9.52191882</v>
+      </c>
+      <c r="F70" t="n">
+        <v>2.66986721</v>
+      </c>
+      <c r="G70" t="n">
+        <v>15072290.79186595</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.01137492169732125</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-1.36716306</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-17.65455986</v>
+      </c>
+      <c r="G71" t="n">
+        <v>11373242.72327522</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.0006621280670566761</v>
+      </c>
+      <c r="E72" t="n">
+        <v>12.93483998</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-18.55925136</v>
+      </c>
+      <c r="G72" t="n">
+        <v>613747.5716214145</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>6.31560546675248e-06</v>
+      </c>
+      <c r="E73" t="n">
+        <v>4.55814098</v>
+      </c>
+      <c r="F73" t="n">
+        <v>31.89572429</v>
+      </c>
+      <c r="G73" t="n">
+        <v>4327577.799490401</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>1.254407354596733e-06</v>
+      </c>
+      <c r="E74" t="n">
+        <v>3.96732665</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-11.20808388</v>
+      </c>
+      <c r="G74" t="n">
+        <v>983096.3988117245</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.574836767559044</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.07977774</v>
+      </c>
+      <c r="F75" t="n">
+        <v>7.79260795</v>
+      </c>
+      <c r="G75" t="n">
+        <v>49701005.44751684</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.2548782630131634</v>
+      </c>
+      <c r="E76" t="n">
+        <v>28.03328947</v>
+      </c>
+      <c r="F76" t="n">
+        <v>33.57653932</v>
+      </c>
+      <c r="G76" t="n">
+        <v>141653516.3768698</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.003802029943925529</v>
+      </c>
+      <c r="E77" t="n">
+        <v>13.87032201</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-8.07274673</v>
+      </c>
+      <c r="G77" t="n">
+        <v>380202994.3925529</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.00482575508947409</v>
+      </c>
+      <c r="E78" t="n">
+        <v>2.76299048</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-27.31996025</v>
+      </c>
+      <c r="G78" t="n">
+        <v>40646790.83137523</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>2.641839090637252e-07</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.31823523</v>
+      </c>
+      <c r="F79" t="n">
+        <v>7.98206069</v>
+      </c>
+      <c r="G79" t="n">
+        <v>110957241.8067646</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.0001537071445279637</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-2.93262497</v>
+      </c>
+      <c r="F80" t="n">
+        <v>26.97405966</v>
+      </c>
+      <c r="G80" t="n">
+        <v>64663058.63146904</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0002618158109426705</v>
+      </c>
+      <c r="E81" t="n">
+        <v>3.47749206</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-4.81009011</v>
+      </c>
+      <c r="G81" t="n">
+        <v>5073379.52385544</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>3.365642498056021e-07</v>
+      </c>
+      <c r="E82" t="n">
+        <v>3.46677249</v>
+      </c>
+      <c r="F82" t="n">
+        <v>-6.83447014</v>
+      </c>
+      <c r="G82" t="n">
+        <v>298230.5359194601</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.01067235087605884</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-5.89764638</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-29.25998375</v>
+      </c>
+      <c r="G83" t="n">
+        <v>1014403.044688972</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.0007835116931004227</v>
+      </c>
+      <c r="E84" t="n">
+        <v>2.08484877</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-11.58792555</v>
+      </c>
+      <c r="G84" t="n">
+        <v>777655.3617823494</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.006007907685321754</v>
+      </c>
+      <c r="E85" t="n">
+        <v>3.21090493</v>
+      </c>
+      <c r="F85" t="n">
+        <v>10.86235206</v>
+      </c>
+      <c r="G85" t="n">
+        <v>4185810.670984538</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.00220225065210481</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-2.54549869</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-5.60761568</v>
+      </c>
+      <c r="G86" t="n">
+        <v>2119085.820485903</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.01770588275035984</v>
+      </c>
+      <c r="E87" t="n">
+        <v>6.42512347</v>
+      </c>
+      <c r="F87" t="n">
+        <v>42.33231734</v>
+      </c>
+      <c r="G87" t="n">
+        <v>16820593.09243018</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>8.285233949732042</v>
+      </c>
+      <c r="E88" t="n">
+        <v>28.78036662</v>
+      </c>
+      <c r="F88" t="n">
+        <v>28.25673794</v>
+      </c>
+      <c r="G88" t="n">
+        <v>64376267.78941797</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.003078719276073189</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-16.52467853</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-18.22715901</v>
+      </c>
+      <c r="G89" t="n">
+        <v>2885202.592229619</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>3.224457751087146e-08</v>
+      </c>
+      <c r="E90" t="n">
+        <v>3.66946898</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-12.62964412</v>
+      </c>
+      <c r="G90" t="n">
+        <v>24823855.51178371</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.000246346265708074</v>
+      </c>
+      <c r="E91" t="n">
+        <v>4.40214911</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-21.41920019</v>
+      </c>
+      <c r="G91" t="n">
+        <v>123037.665071754</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.01863408045842193</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-10.76438731</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-36.92430183</v>
+      </c>
+      <c r="G92" t="n">
+        <v>18445792.74647734</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>7.323007658248603e-05</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-1.24372282</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-15.66098445</v>
+      </c>
+      <c r="G93" t="n">
+        <v>768915.8041161033</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>4.744704306584803e-05</v>
+      </c>
+      <c r="E94" t="n">
+        <v>10.40810768</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-6.70954538</v>
+      </c>
+      <c r="G94" t="n">
+        <v>108331298.3008217</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>9.959972808185136e-06</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.3130428</v>
+      </c>
+      <c r="F95" t="n">
+        <v>-4.95066777</v>
+      </c>
+      <c r="G95" t="n">
+        <v>333295.7948828349</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.0001981008861718842</v>
+      </c>
+      <c r="E96" t="n">
+        <v>1.99350751</v>
+      </c>
+      <c r="F96" t="n">
+        <v>-4.15661911</v>
+      </c>
+      <c r="G96" t="n">
+        <v>182729.4983088969</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.02911649848889436</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.1734784</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-6.90341689</v>
+      </c>
+      <c r="G97" t="n">
+        <v>26846718.06404779</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.001668704860096158</v>
+      </c>
+      <c r="E98" t="n">
+        <v>11.99886633</v>
+      </c>
+      <c r="F98" t="n">
+        <v>17.91220883</v>
+      </c>
+      <c r="G98" t="n">
+        <v>1337040.968402614</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30126</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>MEW</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>cat in a dogs world</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.005693667046527279</v>
+      </c>
+      <c r="E99" t="n">
+        <v>9.58765446</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-3.31255525</v>
+      </c>
+      <c r="G99" t="n">
+        <v>506103737.4640304</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-26T06:41:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30119</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>WIF</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>DOGWIFHOOD</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.0004528005782712833</v>
+      </c>
+      <c r="E100" t="n">
+        <v>7.03162941</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-11.86448218</v>
+      </c>
+      <c r="G100" t="n">
+        <v>452311.6319812504</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-26T05:42:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30096</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>DEGEN</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Degen</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.007605652946501881</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-7.07075578</v>
+      </c>
+      <c r="F101" t="n">
+        <v>56.6515768</v>
+      </c>
+      <c r="G101" t="n">
+        <v>107845184.0508106</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-25T10:09:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>62197.64</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>143.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-06 12:20:06
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -27,6 +27,7 @@
     <sheet name="Portfolio_18" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="Portfolio_19" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="Portfolio_20" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Portfolio_21" sheetId="21" state="visible" r:id="rId21"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -39933,6 +39934,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33287</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MANYU</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>littlemanyu</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0166364640701559</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-16.33529301</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-0.88493338</v>
+      </c>
+      <c r="G2" t="n">
+        <v>16625116.45363707</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-10-03T09:11:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.002721080339534742</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-33.19529947</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-72.38709437</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2721080.339534742</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.8383659291715601</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.36137403</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-1.66498243</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2556596.901008673</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33145</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CHEEMS</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cheems</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>3.263232351135636e-09</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-11.1487013</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-9.256840390000001</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1372809.217799251</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-24T07:29:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.01333872556322139</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-5.30061632</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-19.31841064</v>
+      </c>
+      <c r="G6" t="n">
+        <v>8156127.345100749</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1322518187179665</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-14.39530129</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-53.29322831</v>
+      </c>
+      <c r="G7" t="n">
+        <v>130925569.8617154</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.00126190351868972</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-1.95657195</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-0.1711214</v>
+      </c>
+      <c r="G8" t="n">
+        <v>923416.0081166957</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.004605736701531392</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-7.68723862</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-53.10124665</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4605736.701531392</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0001350121424379169</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.26567337</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-54.17110199</v>
+      </c>
+      <c r="G10" t="n">
+        <v>128261.5353160211</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.01880905040622035</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.95921946</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-12.05580406</v>
+      </c>
+      <c r="G11" t="n">
+        <v>18809050.40622035</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0004373922068602991</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-8.00879578</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-12.10857057</v>
+      </c>
+      <c r="G12" t="n">
+        <v>437392.2068602991</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.006267981672530418</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-5.50598552</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-24.17434364</v>
+      </c>
+      <c r="G13" t="n">
+        <v>6267981.672530418</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>6.466803662213858e-07</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-3.1710172</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-15.01984583</v>
+      </c>
+      <c r="G14" t="n">
+        <v>420860.1209356145</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0006731868774091474</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-4.3732402</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-20.61116516</v>
+      </c>
+      <c r="G15" t="n">
+        <v>347869318.9011769</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0003793115226291002</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.61482936</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-23.44971712</v>
+      </c>
+      <c r="G16" t="n">
+        <v>379311.5226291002</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>2.434104743481714e-07</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-1.02418017</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-32.74117677</v>
+      </c>
+      <c r="G17" t="n">
+        <v>100352.2665406849</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.00717932778371665</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-0.67495313</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-9.019553739999999</v>
+      </c>
+      <c r="G18" t="n">
+        <v>6750139.714621473</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>8.569376790811989e-05</v>
+      </c>
+      <c r="E19" t="n">
+        <v>39.51134013</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-24.55211689</v>
+      </c>
+      <c r="G19" t="n">
+        <v>856937.6790811989</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.01086187550495225</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-33.78392875</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-51.31455301</v>
+      </c>
+      <c r="G20" t="n">
+        <v>10635228.36265277</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0003932460728155134</v>
+      </c>
+      <c r="E21" t="n">
+        <v>45.30257973</v>
+      </c>
+      <c r="F21" t="n">
+        <v>15.48517783</v>
+      </c>
+      <c r="G21" t="n">
+        <v>393246.0728155134</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.001919698794991407</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-4.38144402</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-47.08836079</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1823699.200261236</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>3.088998605846915e-05</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-4.97746198</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-12.96082763</v>
+      </c>
+      <c r="G23" t="n">
+        <v>208506023.5003678</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.227300332719237</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-6.42934776</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-29.72670147</v>
+      </c>
+      <c r="G24" t="n">
+        <v>226716702.2923265</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>3.861977180705318e-05</v>
+      </c>
+      <c r="E25" t="n">
+        <v>12.98498508</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-20.61294228</v>
+      </c>
+      <c r="G25" t="n">
+        <v>3861977.180705318</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2.007309743065427e-06</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-10.49598307</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-19.46631891</v>
+      </c>
+      <c r="G26" t="n">
+        <v>645991.9615864634</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.01044955765318991</v>
+      </c>
+      <c r="E27" t="n">
+        <v>9.503693119999999</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-26.81678167</v>
+      </c>
+      <c r="G27" t="n">
+        <v>10449541.34143041</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32538</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ONI</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Onigiri</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2.182213664994582e-06</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-15.64500947</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-44.89927718</v>
+      </c>
+      <c r="G28" t="n">
+        <v>890306.2959046687</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-08-02T11:10:58.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>1.720455980031819e-06</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-7.8838776</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-37.54229008</v>
+      </c>
+      <c r="G29" t="n">
+        <v>11871143.44443783</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0009784409586948105</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-4.84547371</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-10.98244005</v>
+      </c>
+      <c r="G30" t="n">
+        <v>411475006.6732446</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>3.626824931525523e-05</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.07427394</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.15561683</v>
+      </c>
+      <c r="G31" t="n">
+        <v>232680.2962414144</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.002574769687921617</v>
+      </c>
+      <c r="E32" t="n">
+        <v>4.91962645</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-12.06528938</v>
+      </c>
+      <c r="G32" t="n">
+        <v>2574769.608103757</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.001267213110874424</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-10.16341628</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-21.14034317</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1267210.831158037</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.06029825331700921</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-3.89717606</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-27.89839771</v>
+      </c>
+      <c r="G34" t="n">
+        <v>60298253.31700921</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.01421420678564266</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-10.62245679</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-24.0168433</v>
+      </c>
+      <c r="G35" t="n">
+        <v>13544796.40695869</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.1260836200260966</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-7.31849229</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-13.33247518</v>
+      </c>
+      <c r="G36" t="n">
+        <v>8830729.30758041</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.0006181866109500727</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-6.31536899</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-36.84666769</v>
+      </c>
+      <c r="G37" t="n">
+        <v>572785.7430686248</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0001889862698621247</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-9.820404160000001</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-33.33309004</v>
+      </c>
+      <c r="G38" t="n">
+        <v>165871.599207851</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>8.186775166946855e-07</v>
+      </c>
+      <c r="E39" t="n">
+        <v>14.88915724</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-52.08449057</v>
+      </c>
+      <c r="G39" t="n">
+        <v>727710.034461091</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.002347981514407124</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.52866536</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-10.65297411</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1643586.292295032</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.0001669580156785452</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1.3749245</v>
+      </c>
+      <c r="F41" t="n">
+        <v>50.84272615</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1669580.156785452</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>2.151300580104471e-06</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-4.75156513</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-11.70057316</v>
+      </c>
+      <c r="G42" t="n">
+        <v>6334009.413055056</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.0005404482899396063</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.03287978</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-8.369374949999999</v>
+      </c>
+      <c r="G43" t="n">
+        <v>16213448.69818819</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.0003778321445164957</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1.55856922</v>
+      </c>
+      <c r="F44" t="n">
+        <v>12.48442682</v>
+      </c>
+      <c r="G44" t="n">
+        <v>30431178.58012334</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.007530082332304328</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-16.79458636</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-0.008558659999999999</v>
+      </c>
+      <c r="G45" t="n">
+        <v>7366207.688144134</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.0005598141512953238</v>
+      </c>
+      <c r="E46" t="n">
+        <v>2.28416272</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-39.69444707</v>
+      </c>
+      <c r="G46" t="n">
+        <v>480723.4053475977</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.09309037491914118</v>
+      </c>
+      <c r="E47" t="n">
+        <v>16.58650664</v>
+      </c>
+      <c r="F47" t="n">
+        <v>38.26728444</v>
+      </c>
+      <c r="G47" t="n">
+        <v>90825603.85668275</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.04037669348011594</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-6.78671485</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-20.50298977</v>
+      </c>
+      <c r="G48" t="n">
+        <v>37798143.23188291</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>1.694872632989789e-05</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1.31922402</v>
+      </c>
+      <c r="F49" t="n">
+        <v>42.64503631</v>
+      </c>
+      <c r="G49" t="n">
+        <v>7096184.293316435</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>8.578883626351663e-07</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-3.05533255</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-11.60033433</v>
+      </c>
+      <c r="G50" t="n">
+        <v>18015655.61533849</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.0470160597686912</v>
+      </c>
+      <c r="E51" t="n">
+        <v>2.62163022</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.1625489</v>
+      </c>
+      <c r="G51" t="n">
+        <v>47016059.7686912</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.002311072761616396</v>
+      </c>
+      <c r="E52" t="n">
+        <v>7.37106493</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-19.28349215</v>
+      </c>
+      <c r="G52" t="n">
+        <v>23110358.48140844</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.1308604894713065</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-4.04779017</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-5.82236671</v>
+      </c>
+      <c r="G53" t="n">
+        <v>78475508.26642607</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.0002304563062061432</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-3.25824791</v>
+      </c>
+      <c r="F54" t="n">
+        <v>69.63598996</v>
+      </c>
+      <c r="G54" t="n">
+        <v>222291.8988432079</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>1.13414520763612e-08</v>
+      </c>
+      <c r="E55" t="n">
+        <v>40.49056762</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-9.581411940000001</v>
+      </c>
+      <c r="G55" t="n">
+        <v>4562146.678588255</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.00637430044941951</v>
+      </c>
+      <c r="E56" t="n">
+        <v>6.40202008</v>
+      </c>
+      <c r="F56" t="n">
+        <v>19.9031151</v>
+      </c>
+      <c r="G56" t="n">
+        <v>6374300.44941951</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>1.729155245044147e-07</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-0.26022427</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-17.20704019</v>
+      </c>
+      <c r="G57" t="n">
+        <v>71095314.81777041</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>3.8654942829292e-06</v>
+      </c>
+      <c r="E58" t="n">
+        <v>6.78885116</v>
+      </c>
+      <c r="F58" t="n">
+        <v>23.27267102</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1626174.789885485</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.01187811803769481</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-0.93136529</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.14678394</v>
+      </c>
+      <c r="G59" t="n">
+        <v>785843.9836436014</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.004921101034223069</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.07535988</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-24.89403782</v>
+      </c>
+      <c r="G60" t="n">
+        <v>4920319.799591685</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.09914954606090629</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-7.81665461</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-15.16774948</v>
+      </c>
+      <c r="G61" t="n">
+        <v>97775646.10090676</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>8.859575124532966e-09</v>
+      </c>
+      <c r="E62" t="n">
+        <v>1.37772029</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-25.8084494</v>
+      </c>
+      <c r="G62" t="n">
+        <v>280895.6216616755</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.008327763735701734</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-10.34985743</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-13.6030649</v>
+      </c>
+      <c r="G63" t="n">
+        <v>832776.3735701734</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.000112392216118313</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-0.07550063999999999</v>
+      </c>
+      <c r="F64" t="n">
+        <v>60.32600299</v>
+      </c>
+      <c r="G64" t="n">
+        <v>43862062.16334347</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.01299417680599039</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-3.64172873</v>
+      </c>
+      <c r="F65" t="n">
+        <v>17.61693366</v>
+      </c>
+      <c r="G65" t="n">
+        <v>12239231.37628335</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.0008273112446787703</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-11.882721</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-36.05391117</v>
+      </c>
+      <c r="G66" t="n">
+        <v>827311.2446787703</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.07900850489281985</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.01227889</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-15.08799094</v>
+      </c>
+      <c r="G67" t="n">
+        <v>16057748.97592295</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.005129393314233382</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-1.99978741</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-17.32766136</v>
+      </c>
+      <c r="G68" t="n">
+        <v>8694927.715704445</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>4.658730209571316e-05</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-6.36045045</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-13.46538583</v>
+      </c>
+      <c r="G69" t="n">
+        <v>44184708.61238597</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1.590004353359947e-05</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-2.76783051</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-14.05513833</v>
+      </c>
+      <c r="G70" t="n">
+        <v>137925.9129420063</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.02544346867202194</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-5.55760227</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-18.90544615</v>
+      </c>
+      <c r="G71" t="n">
+        <v>2417129.523842085</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.0008209288566070711</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-10.74214903</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-10.71880126</v>
+      </c>
+      <c r="G72" t="n">
+        <v>13453202.85226084</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.01111631411919972</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-2.27348886</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-9.942871630000001</v>
+      </c>
+      <c r="G73" t="n">
+        <v>11114673.31644166</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.0008298925512626722</v>
+      </c>
+      <c r="E74" t="n">
+        <v>25.33716551</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-2.52681303</v>
+      </c>
+      <c r="G74" t="n">
+        <v>769253.8096267818</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>9.051579423337407e-06</v>
+      </c>
+      <c r="E75" t="n">
+        <v>43.32084977</v>
+      </c>
+      <c r="F75" t="n">
+        <v>76.97949706999999</v>
+      </c>
+      <c r="G75" t="n">
+        <v>6202321.276870584</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>1.238024365583208e-06</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-1.3060342</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-11.06259118</v>
+      </c>
+      <c r="G76" t="n">
+        <v>970256.8236594034</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.5781093106904285</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.56929955</v>
+      </c>
+      <c r="F77" t="n">
+        <v>35.54549216</v>
+      </c>
+      <c r="G77" t="n">
+        <v>49983953.04791275</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.2444038239140388</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-4.10958509</v>
+      </c>
+      <c r="F78" t="n">
+        <v>14.56056964</v>
+      </c>
+      <c r="G78" t="n">
+        <v>135832144.5769714</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.003711911259025654</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-2.37027815</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-13.57412742</v>
+      </c>
+      <c r="G79" t="n">
+        <v>371191125.9025654</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.004565050997963678</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-5.3488861</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-28.04575534</v>
+      </c>
+      <c r="G80" t="n">
+        <v>38450909.6728761</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>2.591967813531651e-07</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-1.88774847</v>
+      </c>
+      <c r="F81" t="n">
+        <v>3.38420516</v>
+      </c>
+      <c r="G81" t="n">
+        <v>108862648.1683293</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.0001529201559327432</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-0.58863827</v>
+      </c>
+      <c r="F82" t="n">
+        <v>28.75331079</v>
+      </c>
+      <c r="G82" t="n">
+        <v>64331980.39934575</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.0002593135938887178</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-0.95571656</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-5.038797</v>
+      </c>
+      <c r="G83" t="n">
+        <v>5024892.395747866</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>3.32789962686203e-07</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-1.12141653</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-8.8225921</v>
+      </c>
+      <c r="G84" t="n">
+        <v>294886.1294027773</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.01017593972110969</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-4.65137588</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-30.12392902</v>
+      </c>
+      <c r="G85" t="n">
+        <v>967219.3460975386</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.0007801923201398036</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-0.42365328</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-11.94869436</v>
+      </c>
+      <c r="G86" t="n">
+        <v>774360.7993612498</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.007344554293203369</v>
+      </c>
+      <c r="E87" t="n">
+        <v>22.24812161</v>
+      </c>
+      <c r="F87" t="n">
+        <v>45.84544719</v>
+      </c>
+      <c r="G87" t="n">
+        <v>5117074.919314364</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.002197686367207499</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-0.20725547</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-3.42950904</v>
+      </c>
+      <c r="G88" t="n">
+        <v>2114693.899249642</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.01772511524422665</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.10862206</v>
+      </c>
+      <c r="F89" t="n">
+        <v>65.2270323</v>
+      </c>
+      <c r="G89" t="n">
+        <v>16838863.96646947</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals)</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>9.386940316263386</v>
+      </c>
+      <c r="E90" t="n">
+        <v>13.29722701</v>
+      </c>
+      <c r="F90" t="n">
+        <v>32.07550232</v>
+      </c>
+      <c r="G90" t="n">
+        <v>72936526.25736651</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.0001706075752889285</v>
+      </c>
+      <c r="E91" t="n">
+        <v>11.51448401</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-4.21282958</v>
+      </c>
+      <c r="G91" t="n">
+        <v>109736.7424704244</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.002510591182693232</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-18.4533906</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-31.60103336</v>
+      </c>
+      <c r="G92" t="n">
+        <v>2352784.888388486</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>3.128825105898995e-08</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-2.96585202</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-14.15318946</v>
+      </c>
+      <c r="G93" t="n">
+        <v>24087616.69285053</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.0002592174988818273</v>
+      </c>
+      <c r="E94" t="n">
+        <v>5.22485419</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-20.82284218</v>
+      </c>
+      <c r="G94" t="n">
+        <v>129466.2036645385</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.02028417421653705</v>
+      </c>
+      <c r="E95" t="n">
+        <v>8.8552465</v>
+      </c>
+      <c r="F95" t="n">
+        <v>-16.87985708</v>
+      </c>
+      <c r="G95" t="n">
+        <v>20079213.16356536</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>7.19968949097669e-05</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-1.6839825</v>
+      </c>
+      <c r="F96" t="n">
+        <v>-13.86151404</v>
+      </c>
+      <c r="G96" t="n">
+        <v>755967.3965525525</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>4.48663921569923e-05</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-5.43901314</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-12.85420922</v>
+      </c>
+      <c r="G97" t="n">
+        <v>102439144.747026</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>1.025443272252209e-05</v>
+      </c>
+      <c r="E98" t="n">
+        <v>2.95643291</v>
+      </c>
+      <c r="F98" t="n">
+        <v>-4.06631077</v>
+      </c>
+      <c r="G98" t="n">
+        <v>343149.4614640741</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.001153828299894308</v>
+      </c>
+      <c r="E99" t="n">
+        <v>482.44479477</v>
+      </c>
+      <c r="F99" t="n">
+        <v>482.22293047</v>
+      </c>
+      <c r="G99" t="n">
+        <v>1064298.45140298</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.02910694133700653</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-0.03282384</v>
+      </c>
+      <c r="F100" t="n">
+        <v>3.54206083</v>
+      </c>
+      <c r="G100" t="n">
+        <v>26837905.94117781</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.001708043615350154</v>
+      </c>
+      <c r="E101" t="n">
+        <v>2.35744236</v>
+      </c>
+      <c r="F101" t="n">
+        <v>-7.23139675</v>
+      </c>
+      <c r="G101" t="n">
+        <v>1368560.938577283</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>62085.98</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>144.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-07 12:22:58
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -28,6 +28,7 @@
     <sheet name="Portfolio_19" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="Portfolio_20" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="Portfolio_21" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Portfolio_22" sheetId="22" state="visible" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -43215,6 +43216,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33287</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MANYU</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>littlemanyu</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.02384419310761754</v>
+      </c>
+      <c r="E2" t="n">
+        <v>44.76940954</v>
+      </c>
+      <c r="F2" t="n">
+        <v>42.05655591</v>
+      </c>
+      <c r="G2" t="n">
+        <v>23827929.14921598</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-10-03T09:11:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.00398776437523811</v>
+      </c>
+      <c r="E3" t="n">
+        <v>47.41409097</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-41.11772496</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3987764.37523811</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.8325485313477771</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.69389721</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-3.43032782</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2538856.746345046</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33145</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CHEEMS</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cheems</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4.346754062264006e-09</v>
+      </c>
+      <c r="E5" t="n">
+        <v>33.20393998</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5.38822521</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1828635.966453845</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-24T07:29:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.01559732008431601</v>
+      </c>
+      <c r="E6" t="n">
+        <v>17.65640956</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-5.13398706</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9537172.666685855</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.116995952266189</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-10.54451861</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-46.73287572</v>
+      </c>
+      <c r="G7" t="n">
+        <v>115822692.424599</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.001051714656242995</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-16.65744004</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-11.32334873</v>
+      </c>
+      <c r="G8" t="n">
+        <v>769607.2918111286</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.00461505054025181</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.23498949</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-53.97612563</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4615050.54025181</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0001538838438886445</v>
+      </c>
+      <c r="E10" t="n">
+        <v>13.9775963</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-49.21078143</v>
+      </c>
+      <c r="G10" t="n">
+        <v>146189.6516942123</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.01860124805512178</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-1.04023832</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-12.89281303</v>
+      </c>
+      <c r="G11" t="n">
+        <v>18601248.05512178</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0005343999087600548</v>
+      </c>
+      <c r="E12" t="n">
+        <v>22.1788111</v>
+      </c>
+      <c r="F12" t="n">
+        <v>8.113433089999999</v>
+      </c>
+      <c r="G12" t="n">
+        <v>534399.9087600549</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.00676329432254165</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7.95082378</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-16.33991748</v>
+      </c>
+      <c r="G13" t="n">
+        <v>6763294.32254165</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>6.528163320768632e-07</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.9488406</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-17.72626515</v>
+      </c>
+      <c r="G14" t="n">
+        <v>424853.4126248026</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0007089492440844218</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5.26075197</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-11.91469264</v>
+      </c>
+      <c r="G15" t="n">
+        <v>366349521.8806249</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0003775625050970519</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.46110319</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-31.86133154</v>
+      </c>
+      <c r="G16" t="n">
+        <v>377562.5050970519</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.007490229284107056</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.36171775</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-0.89616619</v>
+      </c>
+      <c r="G17" t="n">
+        <v>7042455.183192299</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.00134105345148106</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1362.06347056</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1240.77634111</v>
+      </c>
+      <c r="G18" t="n">
+        <v>13410534.5148106</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0115884962346265</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6.6801105</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-44.2957292</v>
+      </c>
+      <c r="G19" t="n">
+        <v>11346687.20690114</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.000341071784727244</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-12.65384503</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.92335041</v>
+      </c>
+      <c r="G20" t="n">
+        <v>341071.784727244</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.002130417085344916</v>
+      </c>
+      <c r="E21" t="n">
+        <v>10.97141712</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-32.46724006</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2023879.967473641</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>3.113573536832029e-05</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1.11603093</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-18.4644798</v>
+      </c>
+      <c r="G22" t="n">
+        <v>210164820.344045</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.2393341531584591</v>
+      </c>
+      <c r="E23" t="n">
+        <v>5.19461092</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-26.59742788</v>
+      </c>
+      <c r="G23" t="n">
+        <v>238719623.9480919</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>4.266528248746651e-05</v>
+      </c>
+      <c r="E24" t="n">
+        <v>10.60346707</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-6.47136055</v>
+      </c>
+      <c r="G24" t="n">
+        <v>4266528.248746651</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1.933243057583434e-06</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-3.27498344</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-20.44772625</v>
+      </c>
+      <c r="G25" t="n">
+        <v>622155.8378352519</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.01196194126633692</v>
+      </c>
+      <c r="E26" t="n">
+        <v>14.4571702</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-15.86675383</v>
+      </c>
+      <c r="G26" t="n">
+        <v>11961922.5937466</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32538</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ONI</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Onigiri</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>3.756344529305765e-06</v>
+      </c>
+      <c r="E27" t="n">
+        <v>72.13465229000001</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1.79061752</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1532525.085730451</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-02T11:10:58.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>1.808143832998879e-06</v>
+      </c>
+      <c r="E28" t="n">
+        <v>4.27988756</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-22.44573557</v>
+      </c>
+      <c r="G28" t="n">
+        <v>12476189.48629441</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.001481961844725461</v>
+      </c>
+      <c r="E29" t="n">
+        <v>51.72642822</v>
+      </c>
+      <c r="F29" t="n">
+        <v>40.77519095</v>
+      </c>
+      <c r="G29" t="n">
+        <v>623331076.9852492</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>3.63866549401881e-05</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.21217874</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.34779564</v>
+      </c>
+      <c r="G30" t="n">
+        <v>233439.9319119026</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.002786020215852126</v>
+      </c>
+      <c r="E31" t="n">
+        <v>8.223883669999999</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-5.37428776</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2786020.1294855</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.001183485335424507</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-6.89749682</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-19.84310438</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1183483.206334389</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.06840696893094132</v>
+      </c>
+      <c r="E33" t="n">
+        <v>13.29899104</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-5.42590389</v>
+      </c>
+      <c r="G33" t="n">
+        <v>68406968.93094133</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.02190610100036218</v>
+      </c>
+      <c r="E34" t="n">
+        <v>53.95003862</v>
+      </c>
+      <c r="F34" t="n">
+        <v>20.32516784</v>
+      </c>
+      <c r="G34" t="n">
+        <v>20874445.02495077</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.1726943661691577</v>
+      </c>
+      <c r="E35" t="n">
+        <v>36.3553522</v>
+      </c>
+      <c r="F35" t="n">
+        <v>18.06998133</v>
+      </c>
+      <c r="G35" t="n">
+        <v>12095284.06836954</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0009801682427456574</v>
+      </c>
+      <c r="E36" t="n">
+        <v>58.53550759</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-6.93824</v>
+      </c>
+      <c r="G36" t="n">
+        <v>908182.7158800801</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.0001870112157544581</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-1.04507809</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-34.48840107</v>
+      </c>
+      <c r="G37" t="n">
+        <v>164138.1114597743</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>1.029854293105609e-06</v>
+      </c>
+      <c r="E38" t="n">
+        <v>25.79407898</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-27.50057784</v>
+      </c>
+      <c r="G38" t="n">
+        <v>915421.869819497</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.002350096525721056</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-0.00713685</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-13.04928947</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1645066.799523175</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.0001599482101519383</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-4.11580631</v>
+      </c>
+      <c r="F40" t="n">
+        <v>71.05013657000001</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1599482.101519383</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>2.086524198621077e-06</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-2.98794825</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-9.948193180000001</v>
+      </c>
+      <c r="G41" t="n">
+        <v>6143290.266760988</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.0006057656706051277</v>
+      </c>
+      <c r="E42" t="n">
+        <v>12.09021946</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-5.33461331</v>
+      </c>
+      <c r="G42" t="n">
+        <v>18172970.11815383</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.0003977260785355366</v>
+      </c>
+      <c r="E43" t="n">
+        <v>5.25876827</v>
+      </c>
+      <c r="F43" t="n">
+        <v>18.87644835</v>
+      </c>
+      <c r="G43" t="n">
+        <v>32033466.44149452</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.008470384759530105</v>
+      </c>
+      <c r="E44" t="n">
+        <v>12.48768065</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-17.40048826</v>
+      </c>
+      <c r="G44" t="n">
+        <v>8286046.630528115</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.0006300086012657198</v>
+      </c>
+      <c r="E45" t="n">
+        <v>12.53888604</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-23.35310641</v>
+      </c>
+      <c r="G45" t="n">
+        <v>541000.7580157852</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.08791520655705783</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-6.04293944</v>
+      </c>
+      <c r="F46" t="n">
+        <v>14.19338832</v>
+      </c>
+      <c r="G46" t="n">
+        <v>85776340.7942609</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.04637751807751814</v>
+      </c>
+      <c r="E47" t="n">
+        <v>14.75824765</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-9.42128883</v>
+      </c>
+      <c r="G47" t="n">
+        <v>43415741.11056298</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>2.074746192648019e-05</v>
+      </c>
+      <c r="E48" t="n">
+        <v>22.40981884</v>
+      </c>
+      <c r="F48" t="n">
+        <v>85.88738158</v>
+      </c>
+      <c r="G48" t="n">
+        <v>8686659.432877662</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>8.491888796726001e-07</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-0.9141555099999999</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-7.11931872</v>
+      </c>
+      <c r="G49" t="n">
+        <v>17832966.4731246</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.05790124124583166</v>
+      </c>
+      <c r="E50" t="n">
+        <v>23.8723618</v>
+      </c>
+      <c r="F50" t="n">
+        <v>44.83054016</v>
+      </c>
+      <c r="G50" t="n">
+        <v>57901241.24583166</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.002511887842852969</v>
+      </c>
+      <c r="E51" t="n">
+        <v>8.626607809999999</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-10.2915533</v>
+      </c>
+      <c r="G51" t="n">
+        <v>25118477.12769087</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.1435566997792201</v>
+      </c>
+      <c r="E52" t="n">
+        <v>9.581514739999999</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-6.88552273</v>
+      </c>
+      <c r="G52" t="n">
+        <v>86089277.41092727</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.0002227507560180187</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-0.29873953</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-0.63301126</v>
+      </c>
+      <c r="G53" t="n">
+        <v>214859.3342449641</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1.211985466383785e-08</v>
+      </c>
+      <c r="E54" t="n">
+        <v>6.8633415</v>
+      </c>
+      <c r="F54" t="n">
+        <v>14.39726198</v>
+      </c>
+      <c r="G54" t="n">
+        <v>4875262.385038469</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.006208017339241103</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-2.48880823</v>
+      </c>
+      <c r="F55" t="n">
+        <v>2.23376471</v>
+      </c>
+      <c r="G55" t="n">
+        <v>6208017.339241102</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31670</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Doug The Duck</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.001498118537575227</v>
+      </c>
+      <c r="E56" t="n">
+        <v>33.96218953</v>
+      </c>
+      <c r="F56" t="n">
+        <v>34.25444968</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1498059.977619711</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-06-06T17:28:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>1.732856284012647e-07</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.31879152</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-13.51905511</v>
+      </c>
+      <c r="G57" t="n">
+        <v>71247485.38277458</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>3.704668095377202e-06</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-4.14875756</v>
+      </c>
+      <c r="F58" t="n">
+        <v>3.45542882</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1558516.821044235</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.01241061671570965</v>
+      </c>
+      <c r="E59" t="n">
+        <v>4.47212384</v>
+      </c>
+      <c r="F59" t="n">
+        <v>6.22910249</v>
+      </c>
+      <c r="G59" t="n">
+        <v>821073.5445124329</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.005564389089847623</v>
+      </c>
+      <c r="E60" t="n">
+        <v>13.0571787</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-6.02236385</v>
+      </c>
+      <c r="G60" t="n">
+        <v>5563505.731950832</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.09075627414742171</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-8.325521139999999</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-18.54316143</v>
+      </c>
+      <c r="G61" t="n">
+        <v>89498678.46116155</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>8.354041068814667e-09</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-5.70628005</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-32.2133695</v>
+      </c>
+      <c r="G62" t="n">
+        <v>264867.5050921888</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.00780373954934522</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-6.29249584</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-15.88285379</v>
+      </c>
+      <c r="G63" t="n">
+        <v>780373.954934522</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0001551073683018468</v>
+      </c>
+      <c r="E64" t="n">
+        <v>38.2242357</v>
+      </c>
+      <c r="F64" t="n">
+        <v>115.97338338</v>
+      </c>
+      <c r="G64" t="n">
+        <v>60532030.29012696</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.01916200792741914</v>
+      </c>
+      <c r="E65" t="n">
+        <v>47.25088931</v>
+      </c>
+      <c r="F65" t="n">
+        <v>65.56336415</v>
+      </c>
+      <c r="G65" t="n">
+        <v>18048719.219346</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.0008147593828772225</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-1.51821558</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-28.37661852</v>
+      </c>
+      <c r="G66" t="n">
+        <v>814759.3828772225</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.07938724732509307</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.48734832</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-14.24894017</v>
+      </c>
+      <c r="G67" t="n">
+        <v>16134724.87759612</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.00511680889494955</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-0.21687651</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-13.17929953</v>
+      </c>
+      <c r="G68" t="n">
+        <v>8673595.638144042</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>4.576655834054513e-05</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-1.65757402</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-20.07813188</v>
+      </c>
+      <c r="G69" t="n">
+        <v>43406292.13329839</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1.725287908967707e-05</v>
+      </c>
+      <c r="E70" t="n">
+        <v>8.50837643</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-1.59497027</v>
+      </c>
+      <c r="G70" t="n">
+        <v>149661.1688070681</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.02662623731531675</v>
+      </c>
+      <c r="E71" t="n">
+        <v>4.64861399</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-12.21246967</v>
+      </c>
+      <c r="G71" t="n">
+        <v>2529492.544955091</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.0008677538197169714</v>
+      </c>
+      <c r="E72" t="n">
+        <v>5.64785178</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.36322393</v>
+      </c>
+      <c r="G72" t="n">
+        <v>14220560.12347519</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0115522872208299</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3.92192139</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-1.29211199</v>
+      </c>
+      <c r="G73" t="n">
+        <v>11550582.06707745</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.001208661612918101</v>
+      </c>
+      <c r="E74" t="n">
+        <v>45.6381425</v>
+      </c>
+      <c r="F74" t="n">
+        <v>69.93792879</v>
+      </c>
+      <c r="G74" t="n">
+        <v>1120346.903791665</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>8.889454466352906e-06</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.9382967800000001</v>
+      </c>
+      <c r="F75" t="n">
+        <v>93.12705812999999</v>
+      </c>
+      <c r="G75" t="n">
+        <v>6091230.049230896</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>1.265129491060164e-06</v>
+      </c>
+      <c r="E76" t="n">
+        <v>2.14175867</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-8.34683811</v>
+      </c>
+      <c r="G76" t="n">
+        <v>991499.4855013393</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.5665051913841878</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-2.00725349</v>
+      </c>
+      <c r="F77" t="n">
+        <v>11.12448693</v>
+      </c>
+      <c r="G77" t="n">
+        <v>48980648.4066628</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.2813471470321864</v>
+      </c>
+      <c r="E78" t="n">
+        <v>15.07316134</v>
+      </c>
+      <c r="F78" t="n">
+        <v>32.93846895</v>
+      </c>
+      <c r="G78" t="n">
+        <v>156364109.7430265</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.003924832624223211</v>
+      </c>
+      <c r="E79" t="n">
+        <v>5.75994399</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-2.22059325</v>
+      </c>
+      <c r="G79" t="n">
+        <v>392483262.4223211</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.004858540733633464</v>
+      </c>
+      <c r="E80" t="n">
+        <v>6.48069008</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-22.32285434</v>
+      </c>
+      <c r="G80" t="n">
+        <v>40922940.6143024</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>2.666511321903073e-07</v>
+      </c>
+      <c r="E81" t="n">
+        <v>2.80017372</v>
+      </c>
+      <c r="F81" t="n">
+        <v>10.04597822</v>
+      </c>
+      <c r="G81" t="n">
+        <v>111993475.5199291</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.0001836511930275832</v>
+      </c>
+      <c r="E82" t="n">
+        <v>20.179405</v>
+      </c>
+      <c r="F82" t="n">
+        <v>56.58117382</v>
+      </c>
+      <c r="G82" t="n">
+        <v>77260220.39477399</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.0002638752002759973</v>
+      </c>
+      <c r="E83" t="n">
+        <v>1.50545927</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-3.86751385</v>
+      </c>
+      <c r="G83" t="n">
+        <v>5113285.683982776</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>3.487793930209236e-07</v>
+      </c>
+      <c r="E84" t="n">
+        <v>4.80466124</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-4.60773607</v>
+      </c>
+      <c r="G84" t="n">
+        <v>309054.408952744</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.01004647362994723</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-1.28387121</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-26.67615515</v>
+      </c>
+      <c r="G85" t="n">
+        <v>954913.641517136</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.0007963507187999074</v>
+      </c>
+      <c r="E86" t="n">
+        <v>2.04828981</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-8.995378909999999</v>
+      </c>
+      <c r="G86" t="n">
+        <v>790398.4226239262</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.00826772190666062</v>
+      </c>
+      <c r="E87" t="n">
+        <v>12.69174605</v>
+      </c>
+      <c r="F87" t="n">
+        <v>-13.15524802</v>
+      </c>
+      <c r="G87" t="n">
+        <v>5760261.290017138</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.00251164177307755</v>
+      </c>
+      <c r="E88" t="n">
+        <v>13.86733484</v>
+      </c>
+      <c r="F88" t="n">
+        <v>13.2673539</v>
+      </c>
+      <c r="G88" t="n">
+        <v>2416793.230188571</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.02249564659910263</v>
+      </c>
+      <c r="E89" t="n">
+        <v>26.73163856</v>
+      </c>
+      <c r="F89" t="n">
+        <v>114.78526767</v>
+      </c>
+      <c r="G89" t="n">
+        <v>21370869.96054609</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals) [Old]</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.2862809881526748</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-96.94963796</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-96.02194037</v>
+      </c>
+      <c r="G90" t="n">
+        <v>2224403.277946284</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.000169983376892421</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-0.38403998</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-3.14614517</v>
+      </c>
+      <c r="G91" t="n">
+        <v>109335.250927203</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.003186640798084369</v>
+      </c>
+      <c r="E92" t="n">
+        <v>27.04559436</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-10.42236354</v>
+      </c>
+      <c r="G92" t="n">
+        <v>2986340.574339235</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>3.063856105134715e-08</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-2.03859401</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-13.74658929</v>
+      </c>
+      <c r="G93" t="n">
+        <v>23587445.43547441</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.0002657776120936663</v>
+      </c>
+      <c r="E94" t="n">
+        <v>2.53055173</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-6.73286101</v>
+      </c>
+      <c r="G94" t="n">
+        <v>132742.652811722</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.02639575211489916</v>
+      </c>
+      <c r="E95" t="n">
+        <v>29.99693448</v>
+      </c>
+      <c r="F95" t="n">
+        <v>14.98539574</v>
+      </c>
+      <c r="G95" t="n">
+        <v>26129036.73917345</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30303</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Gary Banking</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>7.036938329050921e-05</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-2.26053029</v>
+      </c>
+      <c r="F96" t="n">
+        <v>-16.17373477</v>
+      </c>
+      <c r="G96" t="n">
+        <v>738878.5245503468</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-04-02T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30285</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>MUMU</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Mumu the Bull</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>5.2144729935246e-05</v>
+      </c>
+      <c r="E97" t="n">
+        <v>16.39801661</v>
+      </c>
+      <c r="F97" t="n">
+        <v>7.87572022</v>
+      </c>
+      <c r="G97" t="n">
+        <v>119057077.7106436</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-04-01T12:34:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30270</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>FOMO</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>FOMO BULL CLUB</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>1.001918793192557e-05</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-2.27700893</v>
+      </c>
+      <c r="F98" t="n">
+        <v>-4.6662694</v>
+      </c>
+      <c r="G98" t="n">
+        <v>335277.3416316307</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-04-01T09:50:22.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30218</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>MABA</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Make America Based Again</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.002914535348958225</v>
+      </c>
+      <c r="E99" t="n">
+        <v>148.02502841</v>
+      </c>
+      <c r="F99" t="n">
+        <v>1380.79363237</v>
+      </c>
+      <c r="G99" t="n">
+        <v>2688385.662528493</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-03-29T08:51:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30193</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>BENJI</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Basenji</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.03279374769727426</v>
+      </c>
+      <c r="E100" t="n">
+        <v>12.76088653</v>
+      </c>
+      <c r="F100" t="n">
+        <v>38.3800182</v>
+      </c>
+      <c r="G100" t="n">
+        <v>30237306.83234605</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-03-29T04:50:27.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30133</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>COINYE</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Coinye West</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.002820571787236935</v>
+      </c>
+      <c r="E101" t="n">
+        <v>65.13464655999999</v>
+      </c>
+      <c r="F101" t="n">
+        <v>87.51896720000001</v>
+      </c>
+      <c r="G101" t="n">
+        <v>2259968.268827988</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-03-26T11:50:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>62988.23</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>146.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-08 12:21:57
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -29,6 +29,7 @@
     <sheet name="Portfolio_20" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="Portfolio_21" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="Portfolio_22" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Portfolio_23" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -46497,6 +46498,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33287</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MANYU</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>littlemanyu</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.02979007252984982</v>
+      </c>
+      <c r="E2" t="n">
+        <v>25.08648165</v>
+      </c>
+      <c r="F2" t="n">
+        <v>77.4803234</v>
+      </c>
+      <c r="G2" t="n">
+        <v>29769752.92841821</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-10-03T09:11:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33211</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BABYBNB</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Baby BNB</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.08258082275170829</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-18.86195431</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-31.06444422</v>
+      </c>
+      <c r="G3" t="n">
+        <v>45819037.13965751</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-29T01:27:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33210</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>HANA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Hana</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0006551883548715381</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-14.00417213</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-64.43650955</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5710098.379844886</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-28T04:03:56.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.004582162580457017</v>
+      </c>
+      <c r="E5" t="n">
+        <v>17.21220958</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-54.082405</v>
+      </c>
+      <c r="G5" t="n">
+        <v>4582162.580457017</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33180</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>LAIKA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>laikaCTO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0001798773409322981</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-9.38683545</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-95.83686118</v>
+      </c>
+      <c r="G6" t="n">
+        <v>287283.9539395849</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-26T07:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.8854568618247916</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6.35498454</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2.24537564</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2700200.700134702</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33145</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CHEEMS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Cheems</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4.628695926286507e-09</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6.48626216</v>
+      </c>
+      <c r="F8" t="n">
+        <v>6.17579387</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1947246.089229471</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-24T07:29:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.01466757974512668</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-5.96089799</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-4.47750724</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8968671.533023279</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.152482099101342</v>
+      </c>
+      <c r="E10" t="n">
+        <v>28.12176707</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-32.48178979</v>
+      </c>
+      <c r="G10" t="n">
+        <v>150952976.768717</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0008466275840731655</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-19.55707151</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-27.81561201</v>
+      </c>
+      <c r="G11" t="n">
+        <v>619531.8837513702</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.005184730783813916</v>
+      </c>
+      <c r="E12" t="n">
+        <v>12.03697826</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-47.85308736</v>
+      </c>
+      <c r="G12" t="n">
+        <v>5184730.783813916</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0002249124303686838</v>
+      </c>
+      <c r="E13" t="n">
+        <v>46.17154153</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-26.72947487</v>
+      </c>
+      <c r="G13" t="n">
+        <v>213666.8088502496</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.01794781555808855</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-3.54616105</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-13.56350864</v>
+      </c>
+      <c r="G14" t="n">
+        <v>17947815.55808854</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0005388974577324554</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.18378532</v>
+      </c>
+      <c r="F15" t="n">
+        <v>16.77295694</v>
+      </c>
+      <c r="G15" t="n">
+        <v>538897.4577324555</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.006896750350858607</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2.16047962</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-19.47425331</v>
+      </c>
+      <c r="G16" t="n">
+        <v>6896750.350858607</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>6.465105625855984e-07</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.96593317</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-17.22523931</v>
+      </c>
+      <c r="G17" t="n">
+        <v>420749.6125880202</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0007361427522782842</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.73622473</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-5.04249945</v>
+      </c>
+      <c r="G18" t="n">
+        <v>380401767.2398034</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0003775625050970519</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-18.03234023</v>
+      </c>
+      <c r="G19" t="n">
+        <v>377562.5050970519</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.007639668578023672</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1.81885173</v>
+      </c>
+      <c r="F20" t="n">
+        <v>4.98656934</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7182960.832631992</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0009014153487953934</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-41.71724284</v>
+      </c>
+      <c r="F21" t="n">
+        <v>801.27384697</v>
+      </c>
+      <c r="G21" t="n">
+        <v>9014153.487953935</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.01146020751736105</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-1.10703507</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-34.09351595</v>
+      </c>
+      <c r="G22" t="n">
+        <v>11221075.40037217</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0003852892131020421</v>
+      </c>
+      <c r="E23" t="n">
+        <v>12.96425866</v>
+      </c>
+      <c r="F23" t="n">
+        <v>16.80763122</v>
+      </c>
+      <c r="G23" t="n">
+        <v>385289.2131020421</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.001858871690761738</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-12.72748324</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-41.88405137</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1765913.915597164</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>2.932728247443335e-05</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-5.97753569</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-19.75448828</v>
+      </c>
+      <c r="G25" t="n">
+        <v>197957844.1745627</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.2598025293060439</v>
+      </c>
+      <c r="E26" t="n">
+        <v>8.15921541</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-17.37141472</v>
+      </c>
+      <c r="G26" t="n">
+        <v>259135444.2240409</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>3.69099304360325e-05</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-13.53984</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-14.7275916</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3690993.04360325</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2.201535285607708e-06</v>
+      </c>
+      <c r="E28" t="n">
+        <v>13.87783222</v>
+      </c>
+      <c r="F28" t="n">
+        <v>6.17010674</v>
+      </c>
+      <c r="G28" t="n">
+        <v>708497.5811852989</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.01079901767768962</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-9.03168009</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-29.0628684</v>
+      </c>
+      <c r="G29" t="n">
+        <v>10799000.82042302</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32576</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>JHH</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Jen-Hsun Huang</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>4.385233891623918e-06</v>
+      </c>
+      <c r="E30" t="n">
+        <v>70.27521901999999</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-52.56449578</v>
+      </c>
+      <c r="G30" t="n">
+        <v>42343286.3950972</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-08-06T06:01:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32538</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ONI</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Onigiri</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>3.977450141272579e-06</v>
+      </c>
+      <c r="E31" t="n">
+        <v>5.88619096</v>
+      </c>
+      <c r="F31" t="n">
+        <v>56.48619811</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1622732.438727847</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-08-02T11:10:58.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>1.746220243114205e-06</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-3.14433534</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-29.08247034</v>
+      </c>
+      <c r="G32" t="n">
+        <v>12048916.81750929</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.001702880337534754</v>
+      </c>
+      <c r="E33" t="n">
+        <v>15.01626558</v>
+      </c>
+      <c r="F33" t="n">
+        <v>48.13343415</v>
+      </c>
+      <c r="G33" t="n">
+        <v>716274124.8526422</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>3.666648016659265e-05</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.76903257</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.55028912</v>
+      </c>
+      <c r="G34" t="n">
+        <v>235235.1610118703</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.002777428688688654</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-0.3979678</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-4.28031058</v>
+      </c>
+      <c r="G35" t="n">
+        <v>2777428.602588365</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.0009208183173565566</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-22.34515089</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-41.35031918</v>
+      </c>
+      <c r="G36" t="n">
+        <v>920816.6608044037</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.06263433889419981</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-8.537315039999999</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-15.09322678</v>
+      </c>
+      <c r="G37" t="n">
+        <v>62634338.89419981</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.0292376869163648</v>
+      </c>
+      <c r="E38" t="n">
+        <v>33.47070312</v>
+      </c>
+      <c r="F38" t="n">
+        <v>65.24145125</v>
+      </c>
+      <c r="G38" t="n">
+        <v>27860753.86862722</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.2453913164022526</v>
+      </c>
+      <c r="E39" t="n">
+        <v>42.08649232</v>
+      </c>
+      <c r="F39" t="n">
+        <v>79.71118708</v>
+      </c>
+      <c r="G39" t="n">
+        <v>17186881.92114559</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.0009287606347751982</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-5.24477388</v>
+      </c>
+      <c r="F40" t="n">
+        <v>24.85618304</v>
+      </c>
+      <c r="G40" t="n">
+        <v>860550.5860196711</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.0003553195930017739</v>
+      </c>
+      <c r="E41" t="n">
+        <v>89.99908191</v>
+      </c>
+      <c r="F41" t="n">
+        <v>33.83743557</v>
+      </c>
+      <c r="G41" t="n">
+        <v>311860.90483761</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>9.295703066817252e-07</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-9.737030470000001</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-33.17591438</v>
+      </c>
+      <c r="G42" t="n">
+        <v>826280.9544689694</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>32289</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>MIGGLES</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Mr Miggles</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.03254948723146085</v>
+      </c>
+      <c r="E43" t="n">
+        <v>2.83467644</v>
+      </c>
+      <c r="F43" t="n">
+        <v>26.35362684</v>
+      </c>
+      <c r="G43" t="n">
+        <v>31161938.10227424</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-07-18T13:00:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.002306581188881668</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-1.93026632</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-15.86995954</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1614606.077965119</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.0001584283917210649</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-0.9501940800000001</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1512.67595219</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1584283.917210649</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>2.051266266287949e-06</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-2.6108595</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-32.97436165</v>
+      </c>
+      <c r="G46" t="n">
+        <v>6039481.400000003</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.0006264249226971126</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.41043626</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1.6988513</v>
+      </c>
+      <c r="G47" t="n">
+        <v>18792747.68091338</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.0003829359543311896</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-3.71474207</v>
+      </c>
+      <c r="F48" t="n">
+        <v>9.435232040000001</v>
+      </c>
+      <c r="G48" t="n">
+        <v>30842247.22572174</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.007065503617497421</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-16.79495243</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-31.24184094</v>
+      </c>
+      <c r="G49" t="n">
+        <v>6911739.443344544</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.0006308697582694058</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.13668972</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-25.97347394</v>
+      </c>
+      <c r="G50" t="n">
+        <v>541740.2504462516</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.08269390036934698</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-5.78295376</v>
+      </c>
+      <c r="F51" t="n">
+        <v>9.79191099</v>
+      </c>
+      <c r="G51" t="n">
+        <v>80682062.38114473</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.04321844241465798</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-6.93572925</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-20.69212986</v>
+      </c>
+      <c r="G52" t="n">
+        <v>40458411.42124735</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>1.690704577138907e-05</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-18.51029378</v>
+      </c>
+      <c r="F53" t="n">
+        <v>33.01310684</v>
+      </c>
+      <c r="G53" t="n">
+        <v>7080423.956507343</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>8.638719793776491e-07</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1.71724023</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-1.57443091</v>
+      </c>
+      <c r="G54" t="n">
+        <v>18141311.56693063</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.05960903694347176</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2.9378982</v>
+      </c>
+      <c r="F55" t="n">
+        <v>19.52837252</v>
+      </c>
+      <c r="G55" t="n">
+        <v>59609036.94347176</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.002331154801164373</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-7.19510794</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-11.3815948</v>
+      </c>
+      <c r="G56" t="n">
+        <v>23311172.66148926</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.1470796360426131</v>
+      </c>
+      <c r="E57" t="n">
+        <v>2.52073913</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-7.75086865</v>
+      </c>
+      <c r="G57" t="n">
+        <v>88201941.17198265</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.0002275163001130455</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.14151889</v>
+      </c>
+      <c r="F58" t="n">
+        <v>57.03175565</v>
+      </c>
+      <c r="G58" t="n">
+        <v>219456.0487516913</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>1.056132644985415e-08</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-12.85929788</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-4.00050256</v>
+      </c>
+      <c r="G59" t="n">
+        <v>4248337.872459383</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.005755107901423183</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-7.29555691</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-23.62817591</v>
+      </c>
+      <c r="G60" t="n">
+        <v>5755107.901423183</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31670</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Doug The Duck</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.001973765907619947</v>
+      </c>
+      <c r="E61" t="n">
+        <v>31.74964852</v>
+      </c>
+      <c r="F61" t="n">
+        <v>63.43869744</v>
+      </c>
+      <c r="G61" t="n">
+        <v>1973688.755084384</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-06-06T17:28:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>1.581685082202559e-07</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-8.91214036</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-17.80968667</v>
+      </c>
+      <c r="G62" t="n">
+        <v>65031985.52243989</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31601</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>SELFIE</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>SelfieDogCoin</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.02842426489064933</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.64989653</v>
+      </c>
+      <c r="F63" t="n">
+        <v>24.47429284</v>
+      </c>
+      <c r="G63" t="n">
+        <v>27961459.07684977</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-06-03T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>3.575528196539708e-06</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-3.4858696</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-27.02016749</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1504188.95700229</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.01150919236971876</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-7.25969782</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-1.90124426</v>
+      </c>
+      <c r="G65" t="n">
+        <v>761436.2436572979</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.005409175230853828</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-2.79047913</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-1.0867647</v>
+      </c>
+      <c r="G66" t="n">
+        <v>5408316.513467579</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.08517576081659253</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-6.41997871</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-22.85878349</v>
+      </c>
+      <c r="G67" t="n">
+        <v>83995493.44242866</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>8.295072537078966e-09</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-0.70586835</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-29.74624266</v>
+      </c>
+      <c r="G68" t="n">
+        <v>262997.8892079565</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.007397343702903931</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-5.20770643</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-30.26878384</v>
+      </c>
+      <c r="G69" t="n">
+        <v>739734.3702903931</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.0001793980871996027</v>
+      </c>
+      <c r="E70" t="n">
+        <v>15.38206324</v>
+      </c>
+      <c r="F70" t="n">
+        <v>102.61421025</v>
+      </c>
+      <c r="G70" t="n">
+        <v>70011699.42632498</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.01817865701055461</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-5.21823346</v>
+      </c>
+      <c r="F71" t="n">
+        <v>15.41113708</v>
+      </c>
+      <c r="G71" t="n">
+        <v>17122499.76156265</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.000706104278822116</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-13.33309467</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-32.41277372</v>
+      </c>
+      <c r="G72" t="n">
+        <v>706104.2788221161</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.07861332698997453</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-0.96676169</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-13.82325793</v>
+      </c>
+      <c r="G73" t="n">
+        <v>15977432.71663757</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.0048313257604733</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-5.67590589</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-16.36517953</v>
+      </c>
+      <c r="G74" t="n">
+        <v>8189667.994803495</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>4.712693763692348e-05</v>
+      </c>
+      <c r="E75" t="n">
+        <v>2.97388874</v>
+      </c>
+      <c r="F75" t="n">
+        <v>-18.25641279</v>
+      </c>
+      <c r="G75" t="n">
+        <v>44696514.14893065</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>1.627791966373556e-05</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-5.65099553</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-3.09119396</v>
+      </c>
+      <c r="G76" t="n">
+        <v>141203.8228494778</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.02589973055315481</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-2.72513395</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-18.19833859</v>
+      </c>
+      <c r="G77" t="n">
+        <v>2460474.402549707</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.0008121500420205024</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-6.38057945</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-8.65808855</v>
+      </c>
+      <c r="G78" t="n">
+        <v>13309337.55567032</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.01109860204765315</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-3.92723246</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-14.45020575</v>
+      </c>
+      <c r="G79" t="n">
+        <v>11096963.85925229</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.001160715995469233</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-3.96683252</v>
+      </c>
+      <c r="F80" t="n">
+        <v>68.63759406</v>
+      </c>
+      <c r="G80" t="n">
+        <v>1075904.585540544</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>6.649294178162574e-06</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-25.20015561</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-11.8597876</v>
+      </c>
+      <c r="G81" t="n">
+        <v>4556227.905492261</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>1.258653882959897e-06</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-0.51185338</v>
+      </c>
+      <c r="F82" t="n">
+        <v>-7.27203322</v>
+      </c>
+      <c r="G82" t="n">
+        <v>986424.4618416323</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.5495585189179945</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-2.97028505</v>
+      </c>
+      <c r="F83" t="n">
+        <v>5.67352629</v>
+      </c>
+      <c r="G83" t="n">
+        <v>47515420.87061615</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.2388637118892773</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-15.1106285</v>
+      </c>
+      <c r="F84" t="n">
+        <v>1.56704017</v>
+      </c>
+      <c r="G84" t="n">
+        <v>132753120.3122837</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.003785961056933137</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-3.77425191</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-7.80400237</v>
+      </c>
+      <c r="G85" t="n">
+        <v>378596105.6933137</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.004925262400082914</v>
+      </c>
+      <c r="E86" t="n">
+        <v>1.12695993</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-19.99325726</v>
+      </c>
+      <c r="G86" t="n">
+        <v>41484929.6854028</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>2.704043389390019e-07</v>
+      </c>
+      <c r="E87" t="n">
+        <v>1.57020383</v>
+      </c>
+      <c r="F87" t="n">
+        <v>13.388306</v>
+      </c>
+      <c r="G87" t="n">
+        <v>113569822.3543808</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.0001615772213734809</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-11.83116732</v>
+      </c>
+      <c r="F88" t="n">
+        <v>8.9954418</v>
+      </c>
+      <c r="G88" t="n">
+        <v>67973921.25960968</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.0002640143366697459</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-0.02280624</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-3.0260723</v>
+      </c>
+      <c r="G89" t="n">
+        <v>5115981.822648067</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>3.321369200206203e-07</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-4.77163311</v>
+      </c>
+      <c r="F90" t="n">
+        <v>-8.326498669999999</v>
+      </c>
+      <c r="G90" t="n">
+        <v>294307.4664454148</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.009955451971118669</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-0.90600605</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-23.93861059</v>
+      </c>
+      <c r="G91" t="n">
+        <v>946262.0661594081</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.0007664156483990073</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-3.759031</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-13.30539875</v>
+      </c>
+      <c r="G92" t="n">
+        <v>760687.1008815863</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.007157550298594581</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-13.46885211</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-21.36947592</v>
+      </c>
+      <c r="G93" t="n">
+        <v>4986786.00694351</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.002453901634592378</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-2.29890023</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-7.72375122</v>
+      </c>
+      <c r="G94" t="n">
+        <v>2361232.901905559</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.02067032233108945</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-8.34496805</v>
+      </c>
+      <c r="F95" t="n">
+        <v>12.07866094</v>
+      </c>
+      <c r="G95" t="n">
+        <v>19636811.44412653</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals) [Old]</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.2051037114474794</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-28.41308318</v>
+      </c>
+      <c r="F96" t="n">
+        <v>-97.6498986</v>
+      </c>
+      <c r="G96" t="n">
+        <v>1593655.837946915</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.000163397681505746</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-3.87431731</v>
+      </c>
+      <c r="F97" t="n">
+        <v>-6.76681405</v>
+      </c>
+      <c r="G97" t="n">
+        <v>105099.2563799954</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.002841949117372705</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-10.789466</v>
+      </c>
+      <c r="F98" t="n">
+        <v>-9.52343606</v>
+      </c>
+      <c r="G98" t="n">
+        <v>2663314.912844778</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>2.937014109224345e-08</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-4.12529286</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-18.04983263</v>
+      </c>
+      <c r="G99" t="n">
+        <v>22610937.8728482</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30361</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>DOGEMOB</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.0002404679190754572</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-9.51753079</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-9.26362342</v>
+      </c>
+      <c r="G100" t="n">
+        <v>120101.7243052857</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-04-03T15:27:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30309</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Shark Cat</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.0250078064086408</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-5.30158613</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0.23941603</v>
+      </c>
+      <c r="G101" t="n">
+        <v>24755115.50393301</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-04-02T07:00:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>62513.96</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>143.92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-09 12:21:47
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -30,6 +30,7 @@
     <sheet name="Portfolio_21" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="Portfolio_22" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="Portfolio_23" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="Portfolio_24" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -49779,6 +49780,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33287</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MANYU</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>littlemanyu</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.02311848263602614</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-22.39534626</v>
+      </c>
+      <c r="F2" t="n">
+        <v>37.73299043</v>
+      </c>
+      <c r="G2" t="n">
+        <v>23102713.67969356</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-10-03T09:11:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33211</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BABYBNB</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Baby BNB</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.08210630868598545</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-0.57460564</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-10.96311236</v>
+      </c>
+      <c r="G3" t="n">
+        <v>45555758.36770806</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-09-29T01:27:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33210</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>HANA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Hana</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.000526367768388494</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-19.66161113</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-74.72348655</v>
+      </c>
+      <c r="G4" t="n">
+        <v>4587401.041440998</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-28T04:03:56.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.005247612670405813</v>
+      </c>
+      <c r="E5" t="n">
+        <v>14.52262067</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-58.48044083</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5247612.670405813</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33180</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>LAIKA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>laikaCTO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0001958773449076299</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8.89495247</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-32.76201305</v>
+      </c>
+      <c r="G6" t="n">
+        <v>312837.7250886282</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-26T07:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1.048063279605414</v>
+      </c>
+      <c r="E7" t="n">
+        <v>18.36412645</v>
+      </c>
+      <c r="F7" t="n">
+        <v>27.65824394</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3196068.97115671</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33145</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CHEEMS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Cheems</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>6.86148692764553e-09</v>
+      </c>
+      <c r="E8" t="n">
+        <v>48.23801427</v>
+      </c>
+      <c r="F8" t="n">
+        <v>26.23018384</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2886558.935591198</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-24T07:29:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0142259452843911</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-3.0109566</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-0.50640011</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8698628.72535985</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>33103</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BABYCATE</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>BabyCate</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>4.366511130326921e-06</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-24.44442475</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1197.85386709</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2962111.76007665</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-09-23T04:22:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>33094</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.001476351874058549</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-6.8095865</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-8.56184981</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1476351.874058549</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-09-21T13:43:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.163050751438256</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6.93107742</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-23.29109379</v>
+      </c>
+      <c r="G12" t="n">
+        <v>161415644.4529447</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0008294784461641791</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-2.02558223</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-24.23218398</v>
+      </c>
+      <c r="G13" t="n">
+        <v>606982.7559963405</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.004748868459190485</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-8.397617690000001</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-27.654598</v>
+      </c>
+      <c r="G14" t="n">
+        <v>4748868.459190485</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0001758585731391825</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-21.81020282</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-32.95672404</v>
+      </c>
+      <c r="G15" t="n">
+        <v>167065.6444822234</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.01796238049517205</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.08121560999999999</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-4.07761678</v>
+      </c>
+      <c r="G16" t="n">
+        <v>17962380.49517205</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0002724069972740271</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-49.45280829</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-42.86462492</v>
+      </c>
+      <c r="G17" t="n">
+        <v>272406.9972740271</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.006271373132734287</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-9.018684759999999</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-21.13354567</v>
+      </c>
+      <c r="G18" t="n">
+        <v>6271373.132734288</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>6.465105625855984e-07</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-13.27686551</v>
+      </c>
+      <c r="G19" t="n">
+        <v>420749.6125880202</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0007411501195605878</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.68021688</v>
+      </c>
+      <c r="F20" t="n">
+        <v>14.78119274</v>
+      </c>
+      <c r="G20" t="n">
+        <v>382989324.2829337</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0003841794765355513</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1.75254994</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1.58558881</v>
+      </c>
+      <c r="G21" t="n">
+        <v>384179.4765355512</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.007488606720136745</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-1.97733523</v>
+      </c>
+      <c r="F22" t="n">
+        <v>22.39581821</v>
+      </c>
+      <c r="G22" t="n">
+        <v>7040929.617871218</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0005599153308227767</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-37.88486833</v>
+      </c>
+      <c r="F23" t="n">
+        <v>555.61362287</v>
+      </c>
+      <c r="G23" t="n">
+        <v>5599153.308227767</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.01037993564143366</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-9.42628547</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-25.49324059</v>
+      </c>
+      <c r="G24" t="n">
+        <v>10163344.80044024</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0005479199451981269</v>
+      </c>
+      <c r="E25" t="n">
+        <v>42.21004029</v>
+      </c>
+      <c r="F25" t="n">
+        <v>83.69685987</v>
+      </c>
+      <c r="G25" t="n">
+        <v>547919.945198127</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.001564538107594465</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-15.83399137</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-54.83211633</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1486299.258530828</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2.628647042222052e-05</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-10.36854354</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-9.33926301</v>
+      </c>
+      <c r="G27" t="n">
+        <v>177432498.9121489</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.2439284071145464</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-6.11007223</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1.32984948</v>
+      </c>
+      <c r="G28" t="n">
+        <v>243302081.4128778</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>3.524565736213056e-05</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-4.50901168</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-13.48915048</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3524565.736213055</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1.914906200046353e-06</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-13.01950904</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2.76498156</v>
+      </c>
+      <c r="G30" t="n">
+        <v>616254.6745441194</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.01150753413336784</v>
+      </c>
+      <c r="E31" t="n">
+        <v>6.56093431</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-16.31577974</v>
+      </c>
+      <c r="G31" t="n">
+        <v>11507516.17010705</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32576</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>JHH</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Jen-Hsun Huang</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>4.563946929737634e-06</v>
+      </c>
+      <c r="E32" t="n">
+        <v>4.07533652</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.7947930600000001</v>
+      </c>
+      <c r="G32" t="n">
+        <v>44068917.80778901</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-08-06T06:01:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32538</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ONI</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Onigiri</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>3.274884912107008e-06</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-17.66370927</v>
+      </c>
+      <c r="F33" t="n">
+        <v>36.56515874</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1336097.69858137</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-08-02T11:10:58.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>2.165158258667422e-06</v>
+      </c>
+      <c r="E34" t="n">
+        <v>23.99113269</v>
+      </c>
+      <c r="F34" t="n">
+        <v>2.73875584</v>
+      </c>
+      <c r="G34" t="n">
+        <v>14939588.4386852</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.001734990704370407</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.88565022</v>
+      </c>
+      <c r="F35" t="n">
+        <v>75.74761411</v>
+      </c>
+      <c r="G35" t="n">
+        <v>729846994.5642188</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>3.634700794310904e-05</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-0.87129231</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.37274676</v>
+      </c>
+      <c r="G36" t="n">
+        <v>233185.5751342911</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.002710368475151536</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-2.41447112</v>
+      </c>
+      <c r="F37" t="n">
+        <v>8.91848815</v>
+      </c>
+      <c r="G37" t="n">
+        <v>2710368.391130114</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.000891205444886154</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-3.21593</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-31.26524919</v>
+      </c>
+      <c r="G38" t="n">
+        <v>891203.8416075587</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.05748139238323929</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-8.227031050000001</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-7.04404411</v>
+      </c>
+      <c r="G39" t="n">
+        <v>57481392.38323928</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.02639341564041776</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-9.728099500000001</v>
+      </c>
+      <c r="F40" t="n">
+        <v>69.19365037999999</v>
+      </c>
+      <c r="G40" t="n">
+        <v>25150432.00967015</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.3718566692268492</v>
+      </c>
+      <c r="E41" t="n">
+        <v>51.53619724</v>
+      </c>
+      <c r="F41" t="n">
+        <v>195.60103318</v>
+      </c>
+      <c r="G41" t="n">
+        <v>26044347.28699179</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.001454397775117054</v>
+      </c>
+      <c r="E42" t="n">
+        <v>56.59554471</v>
+      </c>
+      <c r="F42" t="n">
+        <v>121.77335294</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1347583.877718532</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.0002470687076896059</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-30.46577995</v>
+      </c>
+      <c r="F43" t="n">
+        <v>14.74499561</v>
+      </c>
+      <c r="G43" t="n">
+        <v>216850.047829349</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>8.890287161053739e-07</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-4.3613259</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-27.65184422</v>
+      </c>
+      <c r="G44" t="n">
+        <v>790244.0878232265</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>32289</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>MIGGLES</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Mr Miggles</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.02999628977296711</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-7.84404817</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-4.86307714</v>
+      </c>
+      <c r="G45" t="n">
+        <v>28717580.66589766</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-07-18T13:00:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.002283753596271068</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-0.98967219</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-6.61320505</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1598626.770602322</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.0001574105643502187</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-0.64245263</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1502.31527311</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1574105.643502187</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1.734099119829244e-06</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-15.46201737</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-37.46909753</v>
+      </c>
+      <c r="G48" t="n">
+        <v>5105655.736696511</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.0006422182107590726</v>
+      </c>
+      <c r="E49" t="n">
+        <v>2.52117812</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-2.97872217</v>
+      </c>
+      <c r="G49" t="n">
+        <v>19266546.32277218</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.0003710001510763287</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-3.11691893</v>
+      </c>
+      <c r="F50" t="n">
+        <v>10.70510083</v>
+      </c>
+      <c r="G50" t="n">
+        <v>29880919.38314049</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.007408200718330864</v>
+      </c>
+      <c r="E51" t="n">
+        <v>4.85028555</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-14.0924823</v>
+      </c>
+      <c r="G51" t="n">
+        <v>7246978.542661471</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.0007767502063230592</v>
+      </c>
+      <c r="E52" t="n">
+        <v>23.12370282</v>
+      </c>
+      <c r="F52" t="n">
+        <v>6.68331891</v>
+      </c>
+      <c r="G52" t="n">
+        <v>667010.6559901627</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.1109300646203428</v>
+      </c>
+      <c r="E53" t="n">
+        <v>34.14540144</v>
+      </c>
+      <c r="F53" t="n">
+        <v>67.23271549</v>
+      </c>
+      <c r="G53" t="n">
+        <v>108231276.4746616</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.04127013889346231</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-4.50803734</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-2.12618138</v>
+      </c>
+      <c r="G54" t="n">
+        <v>38634531.12779038</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>1.391221470938375e-05</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-17.71350893</v>
+      </c>
+      <c r="F55" t="n">
+        <v>25.82942166</v>
+      </c>
+      <c r="G55" t="n">
+        <v>5830406.09131548</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>9.209933777026265e-07</v>
+      </c>
+      <c r="E56" t="n">
+        <v>6.61225271</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-0.29425487</v>
+      </c>
+      <c r="G56" t="n">
+        <v>19340860.93175516</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.06705420116078804</v>
+      </c>
+      <c r="E57" t="n">
+        <v>12.48999246</v>
+      </c>
+      <c r="F57" t="n">
+        <v>66.72944305999999</v>
+      </c>
+      <c r="G57" t="n">
+        <v>67054201.16078804</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.002187364713962921</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-6.16819128</v>
+      </c>
+      <c r="F58" t="n">
+        <v>-6.36669161</v>
+      </c>
+      <c r="G58" t="n">
+        <v>21873294.92714327</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.1522894704434861</v>
+      </c>
+      <c r="E59" t="n">
+        <v>3.54218608</v>
+      </c>
+      <c r="F59" t="n">
+        <v>2.47197047</v>
+      </c>
+      <c r="G59" t="n">
+        <v>91326218.05833849</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.0001978230020077335</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-13.05106407</v>
+      </c>
+      <c r="F60" t="n">
+        <v>38.9858095</v>
+      </c>
+      <c r="G60" t="n">
+        <v>190814.6992160312</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>9.259794596832561e-09</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-12.32356427</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-14.44528238</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3724791.224255907</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.005545784766010199</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-3.63717134</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-18.69650954</v>
+      </c>
+      <c r="G62" t="n">
+        <v>5545784.7660102</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31670</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Doug The Duck</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.002079236052127724</v>
+      </c>
+      <c r="E63" t="n">
+        <v>5.34359947</v>
+      </c>
+      <c r="F63" t="n">
+        <v>75.96305135999999</v>
+      </c>
+      <c r="G63" t="n">
+        <v>2079154.776869682</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-06-06T17:28:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>1.377131279535319e-07</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-12.93265044</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-20.15604558</v>
+      </c>
+      <c r="G64" t="n">
+        <v>56621626.16374145</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31601</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>SELFIE</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>SelfieDogCoin</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.0321530737328685</v>
+      </c>
+      <c r="E65" t="n">
+        <v>13.11840027</v>
+      </c>
+      <c r="F65" t="n">
+        <v>73.30122295</v>
+      </c>
+      <c r="G65" t="n">
+        <v>31629555.19994092</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-06-03T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>3.554127385069849e-06</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-0.59853567</v>
+      </c>
+      <c r="F66" t="n">
+        <v>12.87251787</v>
+      </c>
+      <c r="G66" t="n">
+        <v>1495185.849625035</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.01127701649247274</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-2.01730816</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-3.18701867</v>
+      </c>
+      <c r="G67" t="n">
+        <v>746075.72815291</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.007268773642670858</v>
+      </c>
+      <c r="E68" t="n">
+        <v>34.37859438</v>
+      </c>
+      <c r="F68" t="n">
+        <v>50.57902449</v>
+      </c>
+      <c r="G68" t="n">
+        <v>7267619.710317537</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.08014477393564395</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-5.90659459</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-17.28141273</v>
+      </c>
+      <c r="G69" t="n">
+        <v>79034220.17035779</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>7.830966421901476e-09</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-5.5949615</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-21.4321266</v>
+      </c>
+      <c r="G70" t="n">
+        <v>248283.258550469</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.00714597809748944</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-3.39805227</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-17.26223438</v>
+      </c>
+      <c r="G71" t="n">
+        <v>714597.809748944</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.000160942195580415</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-10.28767469</v>
+      </c>
+      <c r="F72" t="n">
+        <v>95.38405127</v>
+      </c>
+      <c r="G72" t="n">
+        <v>62809123.54127808</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.02500587432416685</v>
+      </c>
+      <c r="E73" t="n">
+        <v>37.55622492</v>
+      </c>
+      <c r="F73" t="n">
+        <v>85.14282025999999</v>
+      </c>
+      <c r="G73" t="n">
+        <v>23553064.28327566</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.0006944713232458865</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-1.64748408</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-30.03923122</v>
+      </c>
+      <c r="G74" t="n">
+        <v>694471.3232458866</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.0786381805943358</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.031615</v>
+      </c>
+      <c r="F75" t="n">
+        <v>-2.29417159</v>
+      </c>
+      <c r="G75" t="n">
+        <v>15982483.98220096</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.004765378320050912</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-1.36499677</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-11.10138328</v>
+      </c>
+      <c r="G76" t="n">
+        <v>8077879.291465566</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>4.606999773359663e-05</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-2.24275108</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-6.90386933</v>
+      </c>
+      <c r="G77" t="n">
+        <v>43694082.59465531</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>1.64286396485642e-05</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.92591675</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-6.56201498</v>
+      </c>
+      <c r="G78" t="n">
+        <v>142511.2526978406</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.02568062217323911</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-0.8459871</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-9.58098734</v>
+      </c>
+      <c r="G79" t="n">
+        <v>2439659.106457715</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.0008029370332517438</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-1.13439738</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-0.39179012</v>
+      </c>
+      <c r="G80" t="n">
+        <v>13158356.77962837</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.01197393636775401</v>
+      </c>
+      <c r="E81" t="n">
+        <v>7.88688806</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.99425957</v>
+      </c>
+      <c r="G81" t="n">
+        <v>11972168.97726771</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.00107207201585366</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-7.63700853</v>
+      </c>
+      <c r="F82" t="n">
+        <v>81.56201013</v>
+      </c>
+      <c r="G82" t="n">
+        <v>993737.6605380139</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>8.170732957485517e-06</v>
+      </c>
+      <c r="E83" t="n">
+        <v>22.88120722</v>
+      </c>
+      <c r="F83" t="n">
+        <v>31.10372551</v>
+      </c>
+      <c r="G83" t="n">
+        <v>5598747.853792221</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>1.265924762646124e-06</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.5776711</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-0.4371728</v>
+      </c>
+      <c r="G84" t="n">
+        <v>992122.7508460215</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.9322756781799439</v>
+      </c>
+      <c r="E85" t="n">
+        <v>69.64083825</v>
+      </c>
+      <c r="F85" t="n">
+        <v>84.91268604</v>
+      </c>
+      <c r="G85" t="n">
+        <v>80605558.26406768</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.2477144269078203</v>
+      </c>
+      <c r="E86" t="n">
+        <v>3.83916261</v>
+      </c>
+      <c r="F86" t="n">
+        <v>31.55994668</v>
+      </c>
+      <c r="G86" t="n">
+        <v>137672076.0900915</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.003794727152833458</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.24084517</v>
+      </c>
+      <c r="F87" t="n">
+        <v>7.57065228</v>
+      </c>
+      <c r="G87" t="n">
+        <v>379472715.2833458</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.004705357889289531</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-4.47918049</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-6.8597393</v>
+      </c>
+      <c r="G88" t="n">
+        <v>39632698.79358011</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>2.541215615960404e-07</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-6.02148711</v>
+      </c>
+      <c r="F89" t="n">
+        <v>13.50405162</v>
+      </c>
+      <c r="G89" t="n">
+        <v>106731055.8703369</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.0001423309554830197</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-11.91227173</v>
+      </c>
+      <c r="F90" t="n">
+        <v>8.95844125</v>
+      </c>
+      <c r="G90" t="n">
+        <v>59877209.66215158</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.0002674625163810997</v>
+      </c>
+      <c r="E91" t="n">
+        <v>1.30605775</v>
+      </c>
+      <c r="F91" t="n">
+        <v>3.72285814</v>
+      </c>
+      <c r="G91" t="n">
+        <v>5182799.499850865</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>3.335695816700198e-07</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0.4313467</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-2.46596538</v>
+      </c>
+      <c r="G92" t="n">
+        <v>295576.9519945736</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.01005478215624792</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.99774662</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-19.6350059</v>
+      </c>
+      <c r="G93" t="n">
+        <v>955703.3639010953</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.0007431760212781149</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-3.03224852</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-9.3307193</v>
+      </c>
+      <c r="G94" t="n">
+        <v>737656.2053461622</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.008068373339719914</v>
+      </c>
+      <c r="E95" t="n">
+        <v>12.72534601</v>
+      </c>
+      <c r="F95" t="n">
+        <v>-4.20985311</v>
+      </c>
+      <c r="G95" t="n">
+        <v>5621371.417394456</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.002760204191853755</v>
+      </c>
+      <c r="E96" t="n">
+        <v>12.48226714</v>
+      </c>
+      <c r="F96" t="n">
+        <v>21.98838688</v>
+      </c>
+      <c r="G96" t="n">
+        <v>2655967.107254166</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.0301377245044013</v>
+      </c>
+      <c r="E97" t="n">
+        <v>45.80190875</v>
+      </c>
+      <c r="F97" t="n">
+        <v>64.27960874</v>
+      </c>
+      <c r="G97" t="n">
+        <v>28630845.90402554</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals) [Old]</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.1751113526461127</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-14.623021</v>
+      </c>
+      <c r="F98" t="n">
+        <v>-97.02209246</v>
+      </c>
+      <c r="G98" t="n">
+        <v>1360615.210060296</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.0001603901280073179</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-1.84063413</v>
+      </c>
+      <c r="F99" t="n">
+        <v>1.38001626</v>
+      </c>
+      <c r="G99" t="n">
+        <v>103164.76359347</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.003454361627069841</v>
+      </c>
+      <c r="E100" t="n">
+        <v>21.54903147</v>
+      </c>
+      <c r="F100" t="n">
+        <v>7.34902557</v>
+      </c>
+      <c r="G100" t="n">
+        <v>3237233.481589927</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30402</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>CAW</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>crow with knife</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>2.927163700778407e-08</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-0.33538853</v>
+      </c>
+      <c r="F101" t="n">
+        <v>-12.28619591</v>
+      </c>
+      <c r="G101" t="n">
+        <v>22535103.38070403</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-04-04T16:24:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>62083.72</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>142.59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-10 12:21:39
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -31,6 +31,7 @@
     <sheet name="Portfolio_22" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="Portfolio_23" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="Portfolio_24" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="Portfolio_25" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53061,6 +53062,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33307</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>POCHITA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pochita</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.009394264020431642</v>
+      </c>
+      <c r="E2" t="n">
+        <v>21.11073052</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-33.00892413</v>
+      </c>
+      <c r="G2" t="n">
+        <v>9394264.020431641</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-10-04T09:21:54.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33287</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MANYU</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>littlemanyu</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.02319929875871627</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-0.09693901000000001</v>
+      </c>
+      <c r="F3" t="n">
+        <v>39.7055478</v>
+      </c>
+      <c r="G3" t="n">
+        <v>23183474.67826808</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-10-03T09:11:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33211</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BABYBNB</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Baby BNB</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0738294643460032</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-10.11867578</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4.39857296</v>
+      </c>
+      <c r="G4" t="n">
+        <v>40963444.73391145</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-09-29T01:27:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33210</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>HANA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Hana</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0005450033150720774</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.2999381</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-45.02726051</v>
+      </c>
+      <c r="G5" t="n">
+        <v>4749813.581490366</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-28T04:03:56.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.003861637658102634</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-26.45199688</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-50.67765587</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3861637.658102634</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33180</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>LAIKA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>laikaCTO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0001851361080763213</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-5.51450015</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.08502870999999999</v>
+      </c>
+      <c r="G7" t="n">
+        <v>295682.7851106059</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-26T07:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1.078630405586442</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2.93300667</v>
+      </c>
+      <c r="F8" t="n">
+        <v>32.24802342</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3289283.421835853</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>33145</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CHEEMS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Cheems</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4.368236264357359e-09</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-36.04429481</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-19.7752561</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1837673.314052497</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-09-24T07:29:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.01405624681227</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-1.19288011</v>
+      </c>
+      <c r="F10" t="n">
+        <v>6.59596014</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8594864.513229644</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>33103</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BABYCATE</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>BabyCate</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>5.312717395696094e-06</v>
+      </c>
+      <c r="E11" t="n">
+        <v>22.42091119</v>
+      </c>
+      <c r="F11" t="n">
+        <v>996.21627601</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3603990.052025122</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-09-23T04:22:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>33094</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.001414886433486341</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-4.16333272</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-7.01742827</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1414886.433486341</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-09-21T13:43:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.1344993995828515</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-17.59085425</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-28.48094529</v>
+      </c>
+      <c r="G13" t="n">
+        <v>133150611.5163251</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0004984401816786534</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-39.96668711</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-54.74326094</v>
+      </c>
+      <c r="G14" t="n">
+        <v>364740.7555599617</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.004021520619326609</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-15.5777979</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-23.56442634</v>
+      </c>
+      <c r="G15" t="n">
+        <v>4021520.619326609</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0001694085130293439</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-3.6593404</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-32.52340005</v>
+      </c>
+      <c r="G16" t="n">
+        <v>160938.0873778767</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.01739068511509629</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-3.26830486</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-5.17231994</v>
+      </c>
+      <c r="G17" t="n">
+        <v>17390685.11509629</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0003038364102551987</v>
+      </c>
+      <c r="E18" t="n">
+        <v>11.53766728</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-39.29143685</v>
+      </c>
+      <c r="G18" t="n">
+        <v>303836.4102551987</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.005820821588141268</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-7.28170057</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-29.10062535</v>
+      </c>
+      <c r="G19" t="n">
+        <v>5820821.588141268</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>6.42186382742625e-07</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.66884906</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-3.623165</v>
+      </c>
+      <c r="G20" t="n">
+        <v>417935.4327447464</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0006639048313527802</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-10.79340498</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.73181637</v>
+      </c>
+      <c r="G21" t="n">
+        <v>343072821.6015492</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0004310840561270523</v>
+      </c>
+      <c r="E22" t="n">
+        <v>12.20902793</v>
+      </c>
+      <c r="F22" t="n">
+        <v>14.37873119</v>
+      </c>
+      <c r="G22" t="n">
+        <v>431084.0561270523</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.007348115998073827</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-1.95105195</v>
+      </c>
+      <c r="F23" t="n">
+        <v>25.73951037</v>
+      </c>
+      <c r="G23" t="n">
+        <v>6908837.584870072</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0009111492002210004</v>
+      </c>
+      <c r="E24" t="n">
+        <v>62.72981825</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1177.22309939</v>
+      </c>
+      <c r="G24" t="n">
+        <v>9111492.002210004</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.008327370030784362</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-19.77435778</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-42.82690957</v>
+      </c>
+      <c r="G25" t="n">
+        <v>8153608.637598895</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.0005810570773531274</v>
+      </c>
+      <c r="E26" t="n">
+        <v>5.908307</v>
+      </c>
+      <c r="F26" t="n">
+        <v>127.33602851</v>
+      </c>
+      <c r="G26" t="n">
+        <v>581057.0773531274</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.001647840521150131</v>
+      </c>
+      <c r="E27" t="n">
+        <v>5.35835244</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-42.38993353</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1565435.915478086</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2.416326861551074e-05</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-7.883768</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-15.50812308</v>
+      </c>
+      <c r="G28" t="n">
+        <v>163100981.4817362</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.2213185678079859</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-9.272397610000001</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-6.80201529</v>
+      </c>
+      <c r="G29" t="n">
+        <v>220750296.5315309</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>3.471328951801262e-05</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-1.41580737</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-7.49582985</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3471328.951801262</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>2.021608246260002e-06</v>
+      </c>
+      <c r="E31" t="n">
+        <v>5.23354125</v>
+      </c>
+      <c r="F31" t="n">
+        <v>10.70451529</v>
+      </c>
+      <c r="G31" t="n">
+        <v>650593.5026083828</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.01376416951819862</v>
+      </c>
+      <c r="E32" t="n">
+        <v>19.2654963</v>
+      </c>
+      <c r="F32" t="n">
+        <v>37.78195317</v>
+      </c>
+      <c r="G32" t="n">
+        <v>13764148.03233001</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32576</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>JHH</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Jen-Hsun Huang</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>3.307500196736562e-06</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-27.70147902</v>
+      </c>
+      <c r="F33" t="n">
+        <v>43.41392287</v>
+      </c>
+      <c r="G33" t="n">
+        <v>31936820.59918446</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-08-06T06:01:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32538</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ONI</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Onigiri</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>2.771271058936958e-06</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-15.37806264</v>
+      </c>
+      <c r="F34" t="n">
+        <v>11.86593178</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1130631.757562611</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-08-02T11:10:58.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1.97393817041554e-06</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-9.11769657</v>
+      </c>
+      <c r="F35" t="n">
+        <v>18.15499468</v>
+      </c>
+      <c r="G35" t="n">
+        <v>13620170.14292958</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.001743324274919254</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.41857245</v>
+      </c>
+      <c r="F36" t="n">
+        <v>94.24618635</v>
+      </c>
+      <c r="G36" t="n">
+        <v>733351668.1995444</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>3.676269666075466e-05</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.10748773</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1.40434906</v>
+      </c>
+      <c r="G37" t="n">
+        <v>235852.44149239</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>0.003049915821692189</v>
+      </c>
+      <c r="E38" t="n">
+        <v>12.67177733</v>
+      </c>
+      <c r="F38" t="n">
+        <v>37.11066821</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3049915.727144798</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.0003308116204686744</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-62.86953287</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-73.93912927</v>
+      </c>
+      <c r="G39" t="n">
+        <v>330811.0253385692</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.06043732309399569</v>
+      </c>
+      <c r="E40" t="n">
+        <v>4.63689409</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.74810977</v>
+      </c>
+      <c r="G40" t="n">
+        <v>60437323.09399569</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.02638061159475594</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-0.86630776</v>
+      </c>
+      <c r="F41" t="n">
+        <v>114.41030908</v>
+      </c>
+      <c r="G41" t="n">
+        <v>25138230.96361179</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.5148950600001549</v>
+      </c>
+      <c r="E42" t="n">
+        <v>37.57067868</v>
+      </c>
+      <c r="F42" t="n">
+        <v>388.34287443</v>
+      </c>
+      <c r="G42" t="n">
+        <v>36062566.22177117</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.001721437277324213</v>
+      </c>
+      <c r="E43" t="n">
+        <v>18.40707883</v>
+      </c>
+      <c r="F43" t="n">
+        <v>200.93549921</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1595011.461867159</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.0004897093280440649</v>
+      </c>
+      <c r="E44" t="n">
+        <v>98.20775064</v>
+      </c>
+      <c r="F44" t="n">
+        <v>121.86494424</v>
+      </c>
+      <c r="G44" t="n">
+        <v>429813.6020618419</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>8.783302591319495e-07</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-0.12099017</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-25.55517989</v>
+      </c>
+      <c r="G45" t="n">
+        <v>780734.3915548329</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>32289</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>MIGGLES</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Mr Miggles</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.02521474764207074</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-15.79090191</v>
+      </c>
+      <c r="F46" t="n">
+        <v>-9.93565536</v>
+      </c>
+      <c r="G46" t="n">
+        <v>24139870.45937894</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-07-18T13:00:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.00222117739413358</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-2.65664939</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.75384863</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1554823.449568498</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.0001800955038087661</v>
+      </c>
+      <c r="E48" t="n">
+        <v>14.41131952</v>
+      </c>
+      <c r="F48" t="n">
+        <v>1733.23004757</v>
+      </c>
+      <c r="G48" t="n">
+        <v>1800955.038087661</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>1.816211396088599e-06</v>
+      </c>
+      <c r="E49" t="n">
+        <v>4.77525486</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-24.8353865</v>
+      </c>
+      <c r="G49" t="n">
+        <v>5347416.435114986</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.0006442372416707397</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.31779157</v>
+      </c>
+      <c r="F50" t="n">
+        <v>2.6191145</v>
+      </c>
+      <c r="G50" t="n">
+        <v>19327117.25012219</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.0003670826400763278</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-1.02892112</v>
+      </c>
+      <c r="F51" t="n">
+        <v>9.434915159999999</v>
+      </c>
+      <c r="G51" t="n">
+        <v>29565397.05778836</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.007115329262614811</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-3.95348643</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-24.39594449</v>
+      </c>
+      <c r="G52" t="n">
+        <v>6960480.749738486</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.0008510430934482413</v>
+      </c>
+      <c r="E53" t="n">
+        <v>9.56457883</v>
+      </c>
+      <c r="F53" t="n">
+        <v>39.07754727</v>
+      </c>
+      <c r="G53" t="n">
+        <v>730807.417128274</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.1053833799332892</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-5.43013922</v>
+      </c>
+      <c r="F54" t="n">
+        <v>81.64832417</v>
+      </c>
+      <c r="G54" t="n">
+        <v>102819535.6094879</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.03525528905490818</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-14.65315414</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-9.0304278</v>
+      </c>
+      <c r="G55" t="n">
+        <v>33003803.69271949</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>1.458199850443329e-05</v>
+      </c>
+      <c r="E56" t="n">
+        <v>4.85257367</v>
+      </c>
+      <c r="F56" t="n">
+        <v>37.20895809</v>
+      </c>
+      <c r="G56" t="n">
+        <v>6131517.5000846</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>9.286657775180675e-07</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1.14479128</v>
+      </c>
+      <c r="F57" t="n">
+        <v>4.73708035</v>
+      </c>
+      <c r="G57" t="n">
+        <v>19501981.32787942</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.08634091550400549</v>
+      </c>
+      <c r="E58" t="n">
+        <v>27.98909731</v>
+      </c>
+      <c r="F58" t="n">
+        <v>116.22940211</v>
+      </c>
+      <c r="G58" t="n">
+        <v>86340915.50400549</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.002420694289365821</v>
+      </c>
+      <c r="E59" t="n">
+        <v>11.01614108</v>
+      </c>
+      <c r="F59" t="n">
+        <v>13.86118342</v>
+      </c>
+      <c r="G59" t="n">
+        <v>24206553.08105714</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.1497680095340833</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-0.7538577400000001</v>
+      </c>
+      <c r="F60" t="n">
+        <v>11.97854586</v>
+      </c>
+      <c r="G60" t="n">
+        <v>89814127.37887718</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.0002377557470588682</v>
+      </c>
+      <c r="E61" t="n">
+        <v>20.15898977</v>
+      </c>
+      <c r="F61" t="n">
+        <v>73.01928689</v>
+      </c>
+      <c r="G61" t="n">
+        <v>229332.7413975206</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>8.400440883187757e-09</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-8.66611513</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-0.1670777</v>
+      </c>
+      <c r="G62" t="n">
+        <v>3379074.055744876</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.005192574483755555</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-6.20639334</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-20.51748891</v>
+      </c>
+      <c r="G63" t="n">
+        <v>5192574.483755555</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31670</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Doug The Duck</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.002349783418209682</v>
+      </c>
+      <c r="E64" t="n">
+        <v>13.02371443</v>
+      </c>
+      <c r="F64" t="n">
+        <v>111.37467022</v>
+      </c>
+      <c r="G64" t="n">
+        <v>2349691.567525648</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-06-06T17:28:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>1.363005283716116e-07</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-1.03932551</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-11.34537865</v>
+      </c>
+      <c r="G65" t="n">
+        <v>56040826.88457951</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31601</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>SELFIE</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>SelfieDogCoin</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.03660220636585211</v>
+      </c>
+      <c r="E66" t="n">
+        <v>13.89043648</v>
+      </c>
+      <c r="F66" t="n">
+        <v>115.78871516</v>
+      </c>
+      <c r="G66" t="n">
+        <v>36006246.75285327</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-06-03T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>3.40849834410299e-06</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-4.09746262</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.21357721</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1433921.168380687</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.01125944422383617</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-0.03703235</v>
+      </c>
+      <c r="F68" t="n">
+        <v>6.89164443</v>
+      </c>
+      <c r="G68" t="n">
+        <v>744913.1650647854</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.006052919355162467</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-16.76823734</v>
+      </c>
+      <c r="F69" t="n">
+        <v>39.83300176</v>
+      </c>
+      <c r="G69" t="n">
+        <v>6051958.442108997</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.07534868445869229</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-6.18046466</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-7.43717157</v>
+      </c>
+      <c r="G70" t="n">
+        <v>74304589.36520369</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>6.889270167394809e-09</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-12.05248554</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-15.99516752</v>
+      </c>
+      <c r="G71" t="n">
+        <v>218426.4819999044</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.007068215645968332</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-1.08819885</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-17.92407489</v>
+      </c>
+      <c r="G72" t="n">
+        <v>706821.5645968332</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0001629021824885702</v>
+      </c>
+      <c r="E73" t="n">
+        <v>1.66135549</v>
+      </c>
+      <c r="F73" t="n">
+        <v>98.39434989999999</v>
+      </c>
+      <c r="G73" t="n">
+        <v>63574025.86791557</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.02778861500254983</v>
+      </c>
+      <c r="E74" t="n">
+        <v>11.17821427</v>
+      </c>
+      <c r="F74" t="n">
+        <v>128.28657086</v>
+      </c>
+      <c r="G74" t="n">
+        <v>26174131.20667044</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.0007275331609876831</v>
+      </c>
+      <c r="E75" t="n">
+        <v>4.93185534</v>
+      </c>
+      <c r="F75" t="n">
+        <v>-18.90054316</v>
+      </c>
+      <c r="G75" t="n">
+        <v>727533.1609876831</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.0768214848371678</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-2.4380543</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-0.11449044</v>
+      </c>
+      <c r="G76" t="n">
+        <v>15613257.34674188</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.004661312350340138</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-2.18341697</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-8.92484024</v>
+      </c>
+      <c r="G77" t="n">
+        <v>7901475.177203351</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>4.553927289426154e-05</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-1.37026894</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-2.14469618</v>
+      </c>
+      <c r="G78" t="n">
+        <v>43190728.21858092</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>1.738461082131561e-05</v>
+      </c>
+      <c r="E79" t="n">
+        <v>5.86733294</v>
+      </c>
+      <c r="F79" t="n">
+        <v>10.06309436</v>
+      </c>
+      <c r="G79" t="n">
+        <v>150803.8838764502</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.02390315902415312</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-6.92920988</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-12.61099855</v>
+      </c>
+      <c r="G80" t="n">
+        <v>2270800.107294546</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0008187186767056146</v>
+      </c>
+      <c r="E81" t="n">
+        <v>1.95562503</v>
+      </c>
+      <c r="F81" t="n">
+        <v>5.22559434</v>
+      </c>
+      <c r="G81" t="n">
+        <v>13416982.90662855</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.01165758530347598</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-2.62308387</v>
+      </c>
+      <c r="F82" t="n">
+        <v>9.736801679999999</v>
+      </c>
+      <c r="G82" t="n">
+        <v>11655864.60739695</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.0009355462163138891</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-12.73476012</v>
+      </c>
+      <c r="F83" t="n">
+        <v>77.754679</v>
+      </c>
+      <c r="G83" t="n">
+        <v>867187.5532397621</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>7.216048177980613e-06</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-11.68415225</v>
+      </c>
+      <c r="F84" t="n">
+        <v>38.54036246</v>
+      </c>
+      <c r="G84" t="n">
+        <v>4944578.957548416</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>1.255767405357652e-06</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-0.80236659</v>
+      </c>
+      <c r="F85" t="n">
+        <v>6.45200096</v>
+      </c>
+      <c r="G85" t="n">
+        <v>984162.2894096711</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.8777792265499241</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-5.82352016</v>
+      </c>
+      <c r="F86" t="n">
+        <v>53.96673025</v>
+      </c>
+      <c r="G86" t="n">
+        <v>75893736.41795421</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.2504665570592648</v>
+      </c>
+      <c r="E87" t="n">
+        <v>1.01638844</v>
+      </c>
+      <c r="F87" t="n">
+        <v>44.60353247</v>
+      </c>
+      <c r="G87" t="n">
+        <v>139201624.7001408</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.004019931170701303</v>
+      </c>
+      <c r="E88" t="n">
+        <v>5.91844859</v>
+      </c>
+      <c r="F88" t="n">
+        <v>28.29597616</v>
+      </c>
+      <c r="G88" t="n">
+        <v>401993117.0701303</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.00452625349604874</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-3.73438088</v>
+      </c>
+      <c r="F89" t="n">
+        <v>-0.32754267</v>
+      </c>
+      <c r="G89" t="n">
+        <v>38124122.69013923</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>2.540950529698733e-07</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.02493608</v>
+      </c>
+      <c r="F90" t="n">
+        <v>12.99268747</v>
+      </c>
+      <c r="G90" t="n">
+        <v>106719922.2473468</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.000137373215033587</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-3.4832482</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.33310608</v>
+      </c>
+      <c r="G91" t="n">
+        <v>57791537.83247969</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.0002603390012911321</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-2.61515912</v>
+      </c>
+      <c r="F92" t="n">
+        <v>3.53766727</v>
+      </c>
+      <c r="G92" t="n">
+        <v>5044762.398633817</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>3.254679968952052e-07</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-2.42875407</v>
+      </c>
+      <c r="F93" t="n">
+        <v>1.91731188</v>
+      </c>
+      <c r="G93" t="n">
+        <v>288398.1147574474</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.009759098859428883</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-2.8729202</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-14.70683689</v>
+      </c>
+      <c r="G94" t="n">
+        <v>927598.7747585328</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.0007452631794320153</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.37467317</v>
+      </c>
+      <c r="F95" t="n">
+        <v>-1.11130745</v>
+      </c>
+      <c r="G95" t="n">
+        <v>739727.8614810247</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.007288361987133605</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-9.612710399999999</v>
+      </c>
+      <c r="F96" t="n">
+        <v>19.11076137</v>
+      </c>
+      <c r="G96" t="n">
+        <v>5077924.388104648</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30550</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>HAMI</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.002994556295119956</v>
+      </c>
+      <c r="E97" t="n">
+        <v>7.12704645</v>
+      </c>
+      <c r="F97" t="n">
+        <v>37.7415548</v>
+      </c>
+      <c r="G97" t="n">
+        <v>2881469.075415744</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-04-11T12:01:43.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30493</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>NUB</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>nubcat</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.03307342605342971</v>
+      </c>
+      <c r="E98" t="n">
+        <v>9.419040409999999</v>
+      </c>
+      <c r="F98" t="n">
+        <v>120.90476983</v>
+      </c>
+      <c r="G98" t="n">
+        <v>31419763.11833501</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-04-10T02:49:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30484</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>PUPS</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>PUPS (Ordinals) [Old]</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.3021026984454845</v>
+      </c>
+      <c r="E99" t="n">
+        <v>72.54426857</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-95.09457218</v>
+      </c>
+      <c r="G99" t="n">
+        <v>2347337.966921414</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-04-09T08:40:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30409</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>NSO</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>NeverSurrenderOne's</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.0002061434898360477</v>
+      </c>
+      <c r="E100" t="n">
+        <v>28.64320473</v>
+      </c>
+      <c r="F100" t="n">
+        <v>41.00632343</v>
+      </c>
+      <c r="G100" t="n">
+        <v>132593.8488826347</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-04-05T06:29:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30407</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>ROOST</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Roost Coin</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.003030591806383384</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-12.26573024</v>
+      </c>
+      <c r="F101" t="n">
+        <v>-2.194488</v>
+      </c>
+      <c r="G101" t="n">
+        <v>2840100.233795826</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-04-05T05:40:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>61168.13</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>140.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-11 12:21:44
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -32,6 +32,7 @@
     <sheet name="Portfolio_23" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="Portfolio_24" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="Portfolio_25" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="Portfolio_26" sheetId="26" state="visible" r:id="rId26"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -56343,6 +56344,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33307</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>POCHITA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pochita</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.008828271441185205</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-8.465754159999999</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-40.45883066</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8828271.441185204</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-10-04T09:21:54.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33294</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>IZZY</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Izzy</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>5.40185144466662e-06</v>
+      </c>
+      <c r="E3" t="n">
+        <v>125.79815728</v>
+      </c>
+      <c r="F3" t="n">
+        <v>32.44633006</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2208178.082303762</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-10-03T12:07:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33287</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MANYU</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>littlemanyu</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.01996226494517522</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-12.54307992</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-19.41444233</v>
+      </c>
+      <c r="G4" t="n">
+        <v>19948648.82299386</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-10-03T09:11:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33211</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BABYBNB</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Baby BNB</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.05611095728244885</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-24.03000092</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-46.1794471</v>
+      </c>
+      <c r="G5" t="n">
+        <v>31132531.13735872</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-09-29T01:27:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33210</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>HANA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Hana</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0007364327654572107</v>
+      </c>
+      <c r="E6" t="n">
+        <v>35.42602971</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-25.89455547</v>
+      </c>
+      <c r="G6" t="n">
+        <v>6418159.769836564</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-28T04:03:56.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.003119175218779938</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-18.28293146</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-52.39141081</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3119175.218779938</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33180</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>LAIKA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>laikaCTO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0001891791587913703</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2.16106238</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-8.38850819</v>
+      </c>
+      <c r="G8" t="n">
+        <v>302139.9830510331</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-26T07:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.8929808412347261</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-17.19512846</v>
+      </c>
+      <c r="F9" t="n">
+        <v>6.74277289</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2723145.075345297</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>33145</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CHEEMS</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Cheems</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>3.870289752366268e-09</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-11.54211717</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-20.16571548</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1628192.195922965</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-09-24T07:29:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.01380063202389603</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-1.51745677</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-3.54172846</v>
+      </c>
+      <c r="G11" t="n">
+        <v>8438565.715763001</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>33103</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BABYCATE</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>BabyCate</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>5.502721781303326e-06</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.0433085</v>
+      </c>
+      <c r="F12" t="n">
+        <v>243.86503094</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3732883.396911932</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-09-23T04:22:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>33094</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.001448977180498218</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.40943345</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-19.17541537</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1448977.180498218</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-09-21T13:43:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.1176333922822024</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-12.39314849</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-26.45170363</v>
+      </c>
+      <c r="G14" t="n">
+        <v>116453740.0590152</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0004544533574688702</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-8.84044495</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-59.59518981</v>
+      </c>
+      <c r="G15" t="n">
+        <v>332552.7657335254</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.003644029384745906</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-9.646467790000001</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-1.97868415</v>
+      </c>
+      <c r="G16" t="n">
+        <v>3644029.384745906</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0001527943330420449</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-9.807708249999999</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-2.89422432</v>
+      </c>
+      <c r="G17" t="n">
+        <v>145154.6163899426</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32949</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>PUFFY</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Puffy</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0004859765829139108</v>
+      </c>
+      <c r="E18" t="n">
+        <v>9.17641074</v>
+      </c>
+      <c r="F18" t="n">
+        <v>131.17843546</v>
+      </c>
+      <c r="G18" t="n">
+        <v>21598915.09088764</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:11:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.01729487203529807</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-0.55115545</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-9.57821453</v>
+      </c>
+      <c r="G19" t="n">
+        <v>17294872.03529807</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0003212493578531934</v>
+      </c>
+      <c r="E20" t="n">
+        <v>5.73102729</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-35.69340044</v>
+      </c>
+      <c r="G20" t="n">
+        <v>321249.3578531934</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.005331521601088187</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-8.42284136</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-34.3428444</v>
+      </c>
+      <c r="G21" t="n">
+        <v>5331521.601088187</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>5.953098681990307e-07</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-7.29951861</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-9.063709080000001</v>
+      </c>
+      <c r="G22" t="n">
+        <v>387428.1580378732</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0006773504903830797</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2.20435537</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1.5327557</v>
+      </c>
+      <c r="G23" t="n">
+        <v>350020865.9054564</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0004269474295819913</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-0.959587</v>
+      </c>
+      <c r="F24" t="n">
+        <v>10.74096206</v>
+      </c>
+      <c r="G24" t="n">
+        <v>426947.4295819913</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>2.837288861862532e-07</v>
+      </c>
+      <c r="E25" t="n">
+        <v>37.88234978</v>
+      </c>
+      <c r="F25" t="n">
+        <v>15.30458784</v>
+      </c>
+      <c r="G25" t="n">
+        <v>116974.5751003605</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.007362692768731796</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.09077424000000001</v>
+      </c>
+      <c r="F26" t="n">
+        <v>27.55946471</v>
+      </c>
+      <c r="G26" t="n">
+        <v>6922542.94023112</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.0007379272920749124</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-19.84080952</v>
+      </c>
+      <c r="F27" t="n">
+        <v>941.34555916</v>
+      </c>
+      <c r="G27" t="n">
+        <v>7379272.920749124</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.007824922951482953</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-6.12236176</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-44.91816995</v>
+      </c>
+      <c r="G28" t="n">
+        <v>7661645.769300315</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.0004981675296725652</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-14.26530214</v>
+      </c>
+      <c r="F29" t="n">
+        <v>124.2245282</v>
+      </c>
+      <c r="G29" t="n">
+        <v>498167.5296725652</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.001428599619344854</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-12.44490377</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-36.05251057</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1357158.732448118</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>2.416788403528056e-05</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.35808448</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-17.84164716</v>
+      </c>
+      <c r="G31" t="n">
+        <v>163132134.7536155</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.2118854315292034</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-4.2622435</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-12.07813084</v>
+      </c>
+      <c r="G32" t="n">
+        <v>211341381.3583123</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>3.949097427650205e-05</v>
+      </c>
+      <c r="E33" t="n">
+        <v>13.7252673</v>
+      </c>
+      <c r="F33" t="n">
+        <v>18.15620905</v>
+      </c>
+      <c r="G33" t="n">
+        <v>3949097.427650205</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>1.781966199553108e-06</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-11.70558426</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-5.06182702</v>
+      </c>
+      <c r="G34" t="n">
+        <v>573471.9540453939</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.01308967386994731</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-4.90037301</v>
+      </c>
+      <c r="F35" t="n">
+        <v>12.10012379</v>
+      </c>
+      <c r="G35" t="n">
+        <v>13089653.4369664</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32576</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>JHH</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Jen-Hsun Huang</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>3.12778713760547e-06</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-5.55082535</v>
+      </c>
+      <c r="F36" t="n">
+        <v>28.31300276</v>
+      </c>
+      <c r="G36" t="n">
+        <v>30201533.10488187</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-08-06T06:01:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32538</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ONI</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Onigiri</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>2.860620899558923e-06</v>
+      </c>
+      <c r="E37" t="n">
+        <v>3.22414656</v>
+      </c>
+      <c r="F37" t="n">
+        <v>16.55495278</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1167084.982523977</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-08-02T11:10:58.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2.263668815814663e-06</v>
+      </c>
+      <c r="E38" t="n">
+        <v>14.77487921</v>
+      </c>
+      <c r="F38" t="n">
+        <v>25.46479378</v>
+      </c>
+      <c r="G38" t="n">
+        <v>15619311.12165949</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0.001749096929817144</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-0.05362503</v>
+      </c>
+      <c r="F39" t="n">
+        <v>76.88498859000001</v>
+      </c>
+      <c r="G39" t="n">
+        <v>735778753.5186015</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>4.797511157263407e-05</v>
+      </c>
+      <c r="E40" t="n">
+        <v>30.49943538</v>
+      </c>
+      <c r="F40" t="n">
+        <v>32.41072795</v>
+      </c>
+      <c r="G40" t="n">
+        <v>307786.1044767897</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.003417859936103454</v>
+      </c>
+      <c r="E41" t="n">
+        <v>13.12230252</v>
+      </c>
+      <c r="F41" t="n">
+        <v>42.50795448</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3417859.830149796</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.0003682993769675962</v>
+      </c>
+      <c r="E42" t="n">
+        <v>11.33199529</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-71.3132748</v>
+      </c>
+      <c r="G42" t="n">
+        <v>368298.7143970171</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.08613435703872251</v>
+      </c>
+      <c r="E43" t="n">
+        <v>43.75534118</v>
+      </c>
+      <c r="F43" t="n">
+        <v>37.76295831</v>
+      </c>
+      <c r="G43" t="n">
+        <v>86134357.0387225</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.03553730516505045</v>
+      </c>
+      <c r="E44" t="n">
+        <v>33.47838536</v>
+      </c>
+      <c r="F44" t="n">
+        <v>141.63585581</v>
+      </c>
+      <c r="G44" t="n">
+        <v>33863695.0039845</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.5581792509486712</v>
+      </c>
+      <c r="E45" t="n">
+        <v>8.40641022</v>
+      </c>
+      <c r="F45" t="n">
+        <v>334.90929205</v>
+      </c>
+      <c r="G45" t="n">
+        <v>39094133.47439967</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.002015879405280413</v>
+      </c>
+      <c r="E46" t="n">
+        <v>17.16458225</v>
+      </c>
+      <c r="F46" t="n">
+        <v>188.60255559</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1867829.167823135</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.0003997315855918492</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-18.37370401</v>
+      </c>
+      <c r="F47" t="n">
+        <v>89.08355039</v>
+      </c>
+      <c r="G47" t="n">
+        <v>350840.9230172238</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>9.405863993368248e-07</v>
+      </c>
+      <c r="E48" t="n">
+        <v>8.24831021</v>
+      </c>
+      <c r="F48" t="n">
+        <v>-10.31728558</v>
+      </c>
+      <c r="G48" t="n">
+        <v>836072.9258653393</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>32289</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>MIGGLES</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Mr Miggles</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.02570828596958136</v>
+      </c>
+      <c r="E49" t="n">
+        <v>2.014493</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-12.4486296</v>
+      </c>
+      <c r="G49" t="n">
+        <v>24612369.7864381</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-07-18T13:00:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.002285440194753342</v>
+      </c>
+      <c r="E50" t="n">
+        <v>2.95126278</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-1.19429717</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1599807.388988396</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.0002011191949519058</v>
+      </c>
+      <c r="E51" t="n">
+        <v>11.67355519</v>
+      </c>
+      <c r="F51" t="n">
+        <v>48.82053009</v>
+      </c>
+      <c r="G51" t="n">
+        <v>2011191.949519058</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>32200</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>BUB</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Lil Bub</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.01165616297359491</v>
+      </c>
+      <c r="E52" t="n">
+        <v>4.30136881</v>
+      </c>
+      <c r="F52" t="n">
+        <v>-18.86875492</v>
+      </c>
+      <c r="G52" t="n">
+        <v>11656162.97359491</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-07-12T14:00:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>32183</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MATT</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Matt Furie</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>4.626656264181787e-06</v>
+      </c>
+      <c r="E53" t="n">
+        <v>6.73515977</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-7.2467628</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1946388.023778636</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-07-11T08:17:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1.863004728924309e-06</v>
+      </c>
+      <c r="E54" t="n">
+        <v>2.59086002</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-16.08918311</v>
+      </c>
+      <c r="G54" t="n">
+        <v>5485188.633658814</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.0006629790671597962</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2.90159372</v>
+      </c>
+      <c r="F55" t="n">
+        <v>31.12138564</v>
+      </c>
+      <c r="G55" t="n">
+        <v>19889372.01479389</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.0003610444190153377</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-1.66554815</v>
+      </c>
+      <c r="F56" t="n">
+        <v>3.68099526</v>
+      </c>
+      <c r="G56" t="n">
+        <v>29079069.50180873</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.007102756299267397</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-0.17670248</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-10.23652121</v>
+      </c>
+      <c r="G57" t="n">
+        <v>6948181.407555314</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.001299609930031727</v>
+      </c>
+      <c r="E58" t="n">
+        <v>52.70788749</v>
+      </c>
+      <c r="F58" t="n">
+        <v>108.30913441</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1116000.56865805</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.1099154017511115</v>
+      </c>
+      <c r="E59" t="n">
+        <v>4.50504908</v>
+      </c>
+      <c r="F59" t="n">
+        <v>77.21928124</v>
+      </c>
+      <c r="G59" t="n">
+        <v>107241299.0694902</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.03812378489036412</v>
+      </c>
+      <c r="E60" t="n">
+        <v>9.41736751</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-15.16515854</v>
+      </c>
+      <c r="G60" t="n">
+        <v>35689110.66323747</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>1.53396563141586e-05</v>
+      </c>
+      <c r="E61" t="n">
+        <v>5.15023958</v>
+      </c>
+      <c r="F61" t="n">
+        <v>12.46264151</v>
+      </c>
+      <c r="G61" t="n">
+        <v>6447677.783470507</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>8.97021820493709e-07</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-3.53283315</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.52660549</v>
+      </c>
+      <c r="G62" t="n">
+        <v>18837458.23036789</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.09020779884749869</v>
+      </c>
+      <c r="E63" t="n">
+        <v>1.86546035</v>
+      </c>
+      <c r="F63" t="n">
+        <v>120.62694342</v>
+      </c>
+      <c r="G63" t="n">
+        <v>90207798.84749869</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.002878776672254458</v>
+      </c>
+      <c r="E64" t="n">
+        <v>19.78406604</v>
+      </c>
+      <c r="F64" t="n">
+        <v>22.94043954</v>
+      </c>
+      <c r="G64" t="n">
+        <v>28787303.08371393</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.1441940379759024</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-3.72173709</v>
+      </c>
+      <c r="F65" t="n">
+        <v>9.174046479999999</v>
+      </c>
+      <c r="G65" t="n">
+        <v>86471481.68911943</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.0001317063736074352</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-41.82956125</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-39.56239529</v>
+      </c>
+      <c r="G66" t="n">
+        <v>127040.393734165</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>9.79851843384759e-09</v>
+      </c>
+      <c r="E67" t="n">
+        <v>16.64290082</v>
+      </c>
+      <c r="F67" t="n">
+        <v>28.50036699</v>
+      </c>
+      <c r="G67" t="n">
+        <v>3941450.203026478</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.005019102689500227</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-3.49267525</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-17.69734768</v>
+      </c>
+      <c r="G68" t="n">
+        <v>5019102.689500227</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31670</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Doug The Duck</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.002341834090417816</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-0.69497493</v>
+      </c>
+      <c r="F69" t="n">
+        <v>82.21008432000001</v>
+      </c>
+      <c r="G69" t="n">
+        <v>2341742.550465055</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-06-06T17:28:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1.363470239994074e-07</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.1348922</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-15.39467255</v>
+      </c>
+      <c r="G70" t="n">
+        <v>56059943.85690034</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>31601</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>SELFIE</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>SelfieDogCoin</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.04249667834466261</v>
+      </c>
+      <c r="E71" t="n">
+        <v>17.8182379</v>
+      </c>
+      <c r="F71" t="n">
+        <v>88.71145765</v>
+      </c>
+      <c r="G71" t="n">
+        <v>41804744.53808069</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-06-03T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>3.045267059283984e-06</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-10.65663668</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-13.90849702</v>
+      </c>
+      <c r="G72" t="n">
+        <v>1281113.399170179</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.01162745977652913</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3.39002617</v>
+      </c>
+      <c r="F73" t="n">
+        <v>2.37854486</v>
+      </c>
+      <c r="G73" t="n">
+        <v>769260.6927668391</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.005888078542552415</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-2.86157383</v>
+      </c>
+      <c r="F74" t="n">
+        <v>34.02654287</v>
+      </c>
+      <c r="G74" t="n">
+        <v>5887143.798307627</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.08204390640460396</v>
+      </c>
+      <c r="E75" t="n">
+        <v>8.70234982</v>
+      </c>
+      <c r="F75" t="n">
+        <v>-10.92113759</v>
+      </c>
+      <c r="G75" t="n">
+        <v>80907036.65375055</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>6.398602556537314e-09</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-7.11027228</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-21.652945</v>
+      </c>
+      <c r="G76" t="n">
+        <v>202869.7107502977</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.00685859966251597</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-2.96561387</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-22.42281434</v>
+      </c>
+      <c r="G77" t="n">
+        <v>685859.966251597</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.0001857130718280868</v>
+      </c>
+      <c r="E78" t="n">
+        <v>12.00859089</v>
+      </c>
+      <c r="F78" t="n">
+        <v>88.73351531</v>
+      </c>
+      <c r="G78" t="n">
+        <v>72476178.35468376</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.03067390469698785</v>
+      </c>
+      <c r="E79" t="n">
+        <v>10.12641758</v>
+      </c>
+      <c r="F79" t="n">
+        <v>138.44669907</v>
+      </c>
+      <c r="G79" t="n">
+        <v>28891789.17647373</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.0006668487105446543</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-8.35606057</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-29.51193236</v>
+      </c>
+      <c r="G80" t="n">
+        <v>666848.7105446543</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.07899044487246783</v>
+      </c>
+      <c r="E81" t="n">
+        <v>2.77851799</v>
+      </c>
+      <c r="F81" t="n">
+        <v>3.14665461</v>
+      </c>
+      <c r="G81" t="n">
+        <v>16054078.44357069</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.00488866612901268</v>
+      </c>
+      <c r="E82" t="n">
+        <v>5.415868</v>
+      </c>
+      <c r="F82" t="n">
+        <v>-5.71035311</v>
+      </c>
+      <c r="G82" t="n">
+        <v>8286866.694356968</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>4.347523620687301e-05</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-5.29502225</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-15.13614972</v>
+      </c>
+      <c r="G83" t="n">
+        <v>41233137.72728849</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>2.727283399035122e-05</v>
+      </c>
+      <c r="E84" t="n">
+        <v>57.0357695</v>
+      </c>
+      <c r="F84" t="n">
+        <v>63.6411505</v>
+      </c>
+      <c r="G84" t="n">
+        <v>236579.8885195513</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.02222258578038682</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-7.03075791</v>
+      </c>
+      <c r="F85" t="n">
+        <v>-18.78612413</v>
+      </c>
+      <c r="G85" t="n">
+        <v>2111145.649136748</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.001188495257249148</v>
+      </c>
+      <c r="E86" t="n">
+        <v>44.78618628</v>
+      </c>
+      <c r="F86" t="n">
+        <v>40.29134154</v>
+      </c>
+      <c r="G86" t="n">
+        <v>19476800.76785962</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.01144742310739151</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-1.76351252</v>
+      </c>
+      <c r="F87" t="n">
+        <v>-0.64275121</v>
+      </c>
+      <c r="G87" t="n">
+        <v>11445733.43191042</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.0009591293505373554</v>
+      </c>
+      <c r="E88" t="n">
+        <v>2.52078773</v>
+      </c>
+      <c r="F88" t="n">
+        <v>63.59240019</v>
+      </c>
+      <c r="G88" t="n">
+        <v>889047.5106724914</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>6.300649281234922e-06</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-12.68559846</v>
+      </c>
+      <c r="F89" t="n">
+        <v>4.31053353</v>
+      </c>
+      <c r="G89" t="n">
+        <v>4317329.525314381</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>1.247503422339397e-06</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-0.6580823</v>
+      </c>
+      <c r="F90" t="n">
+        <v>3.39511749</v>
+      </c>
+      <c r="G90" t="n">
+        <v>977685.6915841592</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.9583416170175103</v>
+      </c>
+      <c r="E91" t="n">
+        <v>9.161223</v>
+      </c>
+      <c r="F91" t="n">
+        <v>66.84843669999999</v>
+      </c>
+      <c r="G91" t="n">
+        <v>82859247.38291386</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.2764994686024189</v>
+      </c>
+      <c r="E92" t="n">
+        <v>10.38853709</v>
+      </c>
+      <c r="F92" t="n">
+        <v>38.79703558</v>
+      </c>
+      <c r="G92" t="n">
+        <v>153669917.8895858</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.005170237408993799</v>
+      </c>
+      <c r="E93" t="n">
+        <v>28.48308181</v>
+      </c>
+      <c r="F93" t="n">
+        <v>54.63020981</v>
+      </c>
+      <c r="G93" t="n">
+        <v>517023740.8993799</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.004533683051435639</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.01108624</v>
+      </c>
+      <c r="F94" t="n">
+        <v>-3.34195285</v>
+      </c>
+      <c r="G94" t="n">
+        <v>38186700.99719838</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>2.648500291412623e-07</v>
+      </c>
+      <c r="E95" t="n">
+        <v>4.05591786</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0.61639772</v>
+      </c>
+      <c r="G95" t="n">
+        <v>111237012.2393302</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.000160174665284974</v>
+      </c>
+      <c r="E96" t="n">
+        <v>16.59817763</v>
+      </c>
+      <c r="F96" t="n">
+        <v>1.15166965</v>
+      </c>
+      <c r="G96" t="n">
+        <v>67383879.93873572</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.0002600450347917859</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-0.08949615</v>
+      </c>
+      <c r="F97" t="n">
+        <v>2.777628</v>
+      </c>
+      <c r="G97" t="n">
+        <v>5039066.013785582</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>3.344237407991296e-07</v>
+      </c>
+      <c r="E98" t="n">
+        <v>2.75165116</v>
+      </c>
+      <c r="F98" t="n">
+        <v>1.9017508</v>
+      </c>
+      <c r="G98" t="n">
+        <v>296333.8248204368</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.01250558553349766</v>
+      </c>
+      <c r="E99" t="n">
+        <v>28.31919616</v>
+      </c>
+      <c r="F99" t="n">
+        <v>10.30335611</v>
+      </c>
+      <c r="G99" t="n">
+        <v>1188651.327914647</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.0007544001128380552</v>
+      </c>
+      <c r="E100" t="n">
+        <v>1.2171932</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-1.5544259</v>
+      </c>
+      <c r="G100" t="n">
+        <v>748797.134853367</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30601</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>MOUTAI</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Moutai</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.007320644409550893</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.12605687</v>
+      </c>
+      <c r="F101" t="n">
+        <v>25.8060839</v>
+      </c>
+      <c r="G101" t="n">
+        <v>5100416.092737205</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-04-12T08:03:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>61137.85</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>142.26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-12 12:19:45
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -33,6 +33,7 @@
     <sheet name="Portfolio_24" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="Portfolio_25" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="Portfolio_26" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="Portfolio_27" sheetId="27" state="visible" r:id="rId27"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -59625,6 +59626,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33384</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>WAP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Wet Ass Pussy</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.02644857610187722</v>
+      </c>
+      <c r="E2" t="n">
+        <v>297.95523002</v>
+      </c>
+      <c r="F2" t="n">
+        <v>62.78998332</v>
+      </c>
+      <c r="G2" t="n">
+        <v>26448576.10187722</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-10-09T13:06:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33307</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>POCHITA</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Pochita</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.006907749381520891</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-22.11765482</v>
+      </c>
+      <c r="F3" t="n">
+        <v>12.10445761</v>
+      </c>
+      <c r="G3" t="n">
+        <v>6907749.381520891</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-10-04T09:21:54.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33294</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>IZZY</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Izzy</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>5.794934218773857e-06</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6.48872876</v>
+      </c>
+      <c r="F4" t="n">
+        <v>236.14402624</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2368863.131718026</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-10-03T12:07:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33287</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MANYU</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>littlemanyu</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.02017735232269784</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.54943413</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.47181894</v>
+      </c>
+      <c r="G5" t="n">
+        <v>20163589.49091113</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-10-03T09:11:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33211</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BABYBNB</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Baby BNB</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.04807086463178029</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-14.3316854</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-58.56807533</v>
+      </c>
+      <c r="G6" t="n">
+        <v>26671576.50537487</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-29T01:27:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33210</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>HANA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Hana</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.000816532506860289</v>
+      </c>
+      <c r="E7" t="n">
+        <v>11.1615419</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-5.02527461</v>
+      </c>
+      <c r="G7" t="n">
+        <v>7116245.137518944</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-28T04:03:56.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.003429175174692003</v>
+      </c>
+      <c r="E8" t="n">
+        <v>10.37775618</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-15.95218533</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3429175.174692003</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>33180</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>LAIKA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>laikaCTO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0001546547277652445</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-18.25001811</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-33.76448038</v>
+      </c>
+      <c r="G9" t="n">
+        <v>247000.658657568</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-09-26T07:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.992943812090576</v>
+      </c>
+      <c r="E10" t="n">
+        <v>11.19427626</v>
+      </c>
+      <c r="F10" t="n">
+        <v>18.86085782</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3027982.154970211</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>33145</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CHEEMS</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Cheems</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4.310215670253868e-09</v>
+      </c>
+      <c r="E11" t="n">
+        <v>11.81256304</v>
+      </c>
+      <c r="F11" t="n">
+        <v>17.94368259</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1813264.6303191</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-09-24T07:29:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01143502752701314</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-17.08286712</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-18.81607774</v>
+      </c>
+      <c r="G12" t="n">
+        <v>6992087.832004802</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>33103</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BABYCATE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BabyCate</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>6.153274967459434e-06</v>
+      </c>
+      <c r="E13" t="n">
+        <v>12.3348215</v>
+      </c>
+      <c r="F13" t="n">
+        <v>13.67525812</v>
+      </c>
+      <c r="G13" t="n">
+        <v>4174199.400868634</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-09-23T04:22:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>33094</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.001490154687180219</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2.84040397</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-17.03373297</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1490154.687180219</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-09-21T13:43:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.1499777756056259</v>
+      </c>
+      <c r="E15" t="n">
+        <v>27.28878059</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-2.93358711</v>
+      </c>
+      <c r="G15" t="n">
+        <v>148473767.1519938</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0004466150355708905</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-1.72478028</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-65.3003035</v>
+      </c>
+      <c r="G16" t="n">
+        <v>326816.9612047595</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.00415444225516788</v>
+      </c>
+      <c r="E17" t="n">
+        <v>13.91807947</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-16.5325041</v>
+      </c>
+      <c r="G17" t="n">
+        <v>4154442.25516788</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0001385365002937565</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-9.332078060000001</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2.89399408</v>
+      </c>
+      <c r="G18" t="n">
+        <v>131609.6752790687</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32949</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>PUFFY</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Puffy</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0004863512264802081</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1.01762389</v>
+      </c>
+      <c r="F19" t="n">
+        <v>99.78599708</v>
+      </c>
+      <c r="G19" t="n">
+        <v>21615565.882021</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:11:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.01797352885767315</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.92352289</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-5.48006019</v>
+      </c>
+      <c r="G20" t="n">
+        <v>17973528.85767315</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0002689986106691155</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-15.24239936</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-42.61466145</v>
+      </c>
+      <c r="G21" t="n">
+        <v>268998.6106691156</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.00574561839240146</v>
+      </c>
+      <c r="E22" t="n">
+        <v>7.56507836</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-13.38096122</v>
+      </c>
+      <c r="G22" t="n">
+        <v>5745618.392401461</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>5.561358403197522e-07</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-6.58044322</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-16.7284635</v>
+      </c>
+      <c r="G23" t="n">
+        <v>361933.6680672837</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.000788745553163895</v>
+      </c>
+      <c r="E24" t="n">
+        <v>16.23549775</v>
+      </c>
+      <c r="F24" t="n">
+        <v>12.04196648</v>
+      </c>
+      <c r="G24" t="n">
+        <v>407584264.5974427</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0004269474295819913</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>11.86647548</v>
+      </c>
+      <c r="G25" t="n">
+        <v>426947.4295819913</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2.460050973467416e-07</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-19.34605799</v>
+      </c>
+      <c r="F26" t="n">
+        <v>4.11886523</v>
+      </c>
+      <c r="G26" t="n">
+        <v>101421.9670103232</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.00750225454803487</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.89580862</v>
+      </c>
+      <c r="F27" t="n">
+        <v>3.67783911</v>
+      </c>
+      <c r="G27" t="n">
+        <v>7053761.56368687</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.0007565497135645262</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2.52361145</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1131.67958405</v>
+      </c>
+      <c r="G28" t="n">
+        <v>7565497.135645262</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.009285339485289146</v>
+      </c>
+      <c r="E29" t="n">
+        <v>18.66365385</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-43.42264737</v>
+      </c>
+      <c r="G29" t="n">
+        <v>9091588.815005565</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0005074890600440125</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1.87116378</v>
+      </c>
+      <c r="F30" t="n">
+        <v>87.51482776</v>
+      </c>
+      <c r="G30" t="n">
+        <v>507489.0600440125</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.001479262857875918</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3.52912971</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-26.31918155</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1405288.422289465</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2.549524573921407e-05</v>
+      </c>
+      <c r="E32" t="n">
+        <v>5.82871851</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-21.5725461</v>
+      </c>
+      <c r="G32" t="n">
+        <v>172091766.8023612</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.2317302436687359</v>
+      </c>
+      <c r="E33" t="n">
+        <v>9.3658219</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-4.60572678</v>
+      </c>
+      <c r="G33" t="n">
+        <v>231132863.2610891</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>3.800669630720992e-05</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-4.04663957</v>
+      </c>
+      <c r="F34" t="n">
+        <v>11.19138757</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3800669.630720992</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1.959160633047577e-06</v>
+      </c>
+      <c r="E35" t="n">
+        <v>10.44252257</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-12.64290572</v>
+      </c>
+      <c r="G35" t="n">
+        <v>630496.6260327318</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.01340811750987596</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.43278513</v>
+      </c>
+      <c r="F36" t="n">
+        <v>40.50722852</v>
+      </c>
+      <c r="G36" t="n">
+        <v>13408096.57980453</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32576</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>JHH</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Jen-Hsun Huang</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>3.628020836660652e-06</v>
+      </c>
+      <c r="E37" t="n">
+        <v>16.09206824</v>
+      </c>
+      <c r="F37" t="n">
+        <v>52.8595398</v>
+      </c>
+      <c r="G37" t="n">
+        <v>35031729.00937639</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-08-06T06:01:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32538</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ONI</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Onigiri</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2.978569712511909e-06</v>
+      </c>
+      <c r="E38" t="n">
+        <v>4.12318923</v>
+      </c>
+      <c r="F38" t="n">
+        <v>15.13868871</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1215206.104873739</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-08-02T11:10:58.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>2.150426494186976e-06</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-4.61905792</v>
+      </c>
+      <c r="F39" t="n">
+        <v>15.1374708</v>
+      </c>
+      <c r="G39" t="n">
+        <v>14837939.28789797</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.002073150210361442</v>
+      </c>
+      <c r="E40" t="n">
+        <v>19.01141823</v>
+      </c>
+      <c r="F40" t="n">
+        <v>101.6162799</v>
+      </c>
+      <c r="G40" t="n">
+        <v>872105618.0570689</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>7.997233152527449e-05</v>
+      </c>
+      <c r="E41" t="n">
+        <v>66.7030982</v>
+      </c>
+      <c r="F41" t="n">
+        <v>120.66609676</v>
+      </c>
+      <c r="G41" t="n">
+        <v>513065.4537160285</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.00388332614961029</v>
+      </c>
+      <c r="E42" t="n">
+        <v>13.40534307</v>
+      </c>
+      <c r="F42" t="n">
+        <v>58.24216469</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3883326.029227179</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.0003039453212550892</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-17.47330018</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-78.45239363</v>
+      </c>
+      <c r="G43" t="n">
+        <v>303944.7744574563</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.1158248725754505</v>
+      </c>
+      <c r="E44" t="n">
+        <v>35.75005543</v>
+      </c>
+      <c r="F44" t="n">
+        <v>84.60065964</v>
+      </c>
+      <c r="G44" t="n">
+        <v>115824872.5754505</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.03327410802357635</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-6.43916556</v>
+      </c>
+      <c r="F45" t="n">
+        <v>109.22433961</v>
+      </c>
+      <c r="G45" t="n">
+        <v>31707081.90749846</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.6199533395423197</v>
+      </c>
+      <c r="E46" t="n">
+        <v>11.06707003</v>
+      </c>
+      <c r="F46" t="n">
+        <v>355.71510563</v>
+      </c>
+      <c r="G46" t="n">
+        <v>43420708.60350916</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.002245179498726821</v>
+      </c>
+      <c r="E47" t="n">
+        <v>11.57929457</v>
+      </c>
+      <c r="F47" t="n">
+        <v>240.25132404</v>
+      </c>
+      <c r="G47" t="n">
+        <v>2080289.001284352</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.000354368655537443</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-11.34834766</v>
+      </c>
+      <c r="F48" t="n">
+        <v>69.09599919</v>
+      </c>
+      <c r="G48" t="n">
+        <v>311026.2753268509</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>1.05984470672621e-06</v>
+      </c>
+      <c r="E49" t="n">
+        <v>12.67122619</v>
+      </c>
+      <c r="F49" t="n">
+        <v>48.73336897</v>
+      </c>
+      <c r="G49" t="n">
+        <v>942079.8181577233</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>32289</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>MIGGLES</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Mr Miggles</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.02601104547381591</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1.23656193</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-10.2423767</v>
+      </c>
+      <c r="G50" t="n">
+        <v>24902222.98331775</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-07-18T13:00:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.00232220292990809</v>
+      </c>
+      <c r="E51" t="n">
+        <v>1.60856255</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-0.5750429500000001</v>
+      </c>
+      <c r="G51" t="n">
+        <v>1625541.291575305</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.0002170078997064987</v>
+      </c>
+      <c r="E52" t="n">
+        <v>7.76683333</v>
+      </c>
+      <c r="F52" t="n">
+        <v>31.76461975</v>
+      </c>
+      <c r="G52" t="n">
+        <v>2170078.997064988</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>32200</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>BUB</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Lil Bub</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.01115917694110521</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-4.69756871</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-14.90824508</v>
+      </c>
+      <c r="G53" t="n">
+        <v>11159176.94110521</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-07-12T14:00:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>32183</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MATT</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Matt Furie</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>4.676632084538599e-06</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1.08045847</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-12.72903121</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1967412.351644543</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-07-11T08:17:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>1.672294994808799e-06</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-10.23941033</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-25.95944873</v>
+      </c>
+      <c r="G55" t="n">
+        <v>4923687.715460667</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.0006579370197527686</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-0.75830698</v>
+      </c>
+      <c r="F56" t="n">
+        <v>21.77915265</v>
+      </c>
+      <c r="G56" t="n">
+        <v>19738110.59258306</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.0003639907639402598</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.80855513</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-2.16189456</v>
+      </c>
+      <c r="G57" t="n">
+        <v>29316372.62667568</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.009403945612518946</v>
+      </c>
+      <c r="E58" t="n">
+        <v>32.39853961</v>
+      </c>
+      <c r="F58" t="n">
+        <v>3.91110615</v>
+      </c>
+      <c r="G58" t="n">
+        <v>9199290.713283367</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.001301358211082149</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-0.52452537</v>
+      </c>
+      <c r="F59" t="n">
+        <v>137.77236555</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1117501.851928791</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.1277176497168143</v>
+      </c>
+      <c r="E60" t="n">
+        <v>16.70829434</v>
+      </c>
+      <c r="F60" t="n">
+        <v>59.95375064</v>
+      </c>
+      <c r="G60" t="n">
+        <v>124610440.8620311</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.03840651526447907</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.9432861</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-11.33505123</v>
+      </c>
+      <c r="G61" t="n">
+        <v>35953785.21322417</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>1.597467471282283e-05</v>
+      </c>
+      <c r="E62" t="n">
+        <v>4.08511494</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-4.50364149</v>
+      </c>
+      <c r="G62" t="n">
+        <v>6714593.412954541</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>8.903106542196295e-07</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-0.79013602</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.60851046</v>
+      </c>
+      <c r="G63" t="n">
+        <v>18696523.73861222</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0914504761002279</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1.37571372</v>
+      </c>
+      <c r="F64" t="n">
+        <v>99.60832506</v>
+      </c>
+      <c r="G64" t="n">
+        <v>91450476.10022789</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.002787481525463082</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-3.39406174</v>
+      </c>
+      <c r="F65" t="n">
+        <v>29.50473254</v>
+      </c>
+      <c r="G65" t="n">
+        <v>27874366.27527523</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.1443698325627512</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.1219153</v>
+      </c>
+      <c r="F66" t="n">
+        <v>5.85780722</v>
+      </c>
+      <c r="G66" t="n">
+        <v>86576903.65115842</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.0002139676633876914</v>
+      </c>
+      <c r="E67" t="n">
+        <v>62.4549028</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-10.1799079</v>
+      </c>
+      <c r="G67" t="n">
+        <v>206387.4014493181</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1.155217228351825e-08</v>
+      </c>
+      <c r="E68" t="n">
+        <v>17.89713273</v>
+      </c>
+      <c r="F68" t="n">
+        <v>43.10083315</v>
+      </c>
+      <c r="G68" t="n">
+        <v>4646856.777345539</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.00518311003655832</v>
+      </c>
+      <c r="E69" t="n">
+        <v>4.01090712</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-13.48174085</v>
+      </c>
+      <c r="G69" t="n">
+        <v>5183110.03655832</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>31670</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Doug The Duck</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.002291585985532758</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-1.55595908</v>
+      </c>
+      <c r="F70" t="n">
+        <v>93.51316496</v>
+      </c>
+      <c r="G70" t="n">
+        <v>2291496.409728169</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-06-06T17:28:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1.515641354860492e-07</v>
+      </c>
+      <c r="E71" t="n">
+        <v>11.33835204</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-12.57596491</v>
+      </c>
+      <c r="G71" t="n">
+        <v>62316555.77685716</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>31601</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>SELFIE</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>SelfieDogCoin</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.04309246887917553</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1.11517017</v>
+      </c>
+      <c r="F72" t="n">
+        <v>102.73241833</v>
+      </c>
+      <c r="G72" t="n">
+        <v>42390834.37059691</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-06-03T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>2.875961007611475e-06</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-5.55964546</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-20.54817586</v>
+      </c>
+      <c r="G73" t="n">
+        <v>1209888.036292071</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.01285481142806484</v>
+      </c>
+      <c r="E74" t="n">
+        <v>10.66900662</v>
+      </c>
+      <c r="F74" t="n">
+        <v>7.21467943</v>
+      </c>
+      <c r="G74" t="n">
+        <v>850461.00649613</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.005593242192590203</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-5.05246624</v>
+      </c>
+      <c r="F75" t="n">
+        <v>13.74400188</v>
+      </c>
+      <c r="G75" t="n">
+        <v>5592354.254205645</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.08373381754712358</v>
+      </c>
+      <c r="E76" t="n">
+        <v>2.48801995</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-22.14928126</v>
+      </c>
+      <c r="G76" t="n">
+        <v>82573530.95833847</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>5.045968229346698e-09</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-21.14043122</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-42.26035125</v>
+      </c>
+      <c r="G77" t="n">
+        <v>159984.0130868717</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.007744922745387364</v>
+      </c>
+      <c r="E78" t="n">
+        <v>12.9227995</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-16.62426429</v>
+      </c>
+      <c r="G78" t="n">
+        <v>774492.2745387364</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.0001788179509391211</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-3.48695307</v>
+      </c>
+      <c r="F79" t="n">
+        <v>58.98159891</v>
+      </c>
+      <c r="G79" t="n">
+        <v>69785296.08987269</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.02668173081977241</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-12.92691409</v>
+      </c>
+      <c r="F80" t="n">
+        <v>97.85827872</v>
+      </c>
+      <c r="G80" t="n">
+        <v>25131555.61130716</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.000698820105480492</v>
+      </c>
+      <c r="E81" t="n">
+        <v>4.79277041</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-25.56836789</v>
+      </c>
+      <c r="G81" t="n">
+        <v>698820.105480492</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.0823693432467261</v>
+      </c>
+      <c r="E82" t="n">
+        <v>4.23347965</v>
+      </c>
+      <c r="F82" t="n">
+        <v>4.26656902</v>
+      </c>
+      <c r="G82" t="n">
+        <v>16740808.3340122</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.005246999037880522</v>
+      </c>
+      <c r="E83" t="n">
+        <v>6.79389073</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.24714224</v>
+      </c>
+      <c r="G83" t="n">
+        <v>8894283.312637808</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>4.001812618288851e-05</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-7.95261807</v>
+      </c>
+      <c r="F84" t="n">
+        <v>-19.56436323</v>
+      </c>
+      <c r="G84" t="n">
+        <v>37954317.27237381</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>3.350622544723215e-05</v>
+      </c>
+      <c r="E85" t="n">
+        <v>22.80486434</v>
+      </c>
+      <c r="F85" t="n">
+        <v>104.89872843</v>
+      </c>
+      <c r="G85" t="n">
+        <v>290651.8289893001</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.02162492111498548</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-2.68944699</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-19.86526994</v>
+      </c>
+      <c r="G86" t="n">
+        <v>2054367.505923621</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.001352630290790747</v>
+      </c>
+      <c r="E87" t="n">
+        <v>13.87952583</v>
+      </c>
+      <c r="F87" t="n">
+        <v>47.49585401</v>
+      </c>
+      <c r="G87" t="n">
+        <v>22166609.85865477</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.01205313708945814</v>
+      </c>
+      <c r="E88" t="n">
+        <v>5.13317188</v>
+      </c>
+      <c r="F88" t="n">
+        <v>5.9718311</v>
+      </c>
+      <c r="G88" t="n">
+        <v>12051358.00869742</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.001262054947265922</v>
+      </c>
+      <c r="E89" t="n">
+        <v>31.58339348</v>
+      </c>
+      <c r="F89" t="n">
+        <v>90.60586766</v>
+      </c>
+      <c r="G89" t="n">
+        <v>1169838.884160986</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>8.120961136290319e-06</v>
+      </c>
+      <c r="E90" t="n">
+        <v>28.89086146</v>
+      </c>
+      <c r="F90" t="n">
+        <v>28.58565605</v>
+      </c>
+      <c r="G90" t="n">
+        <v>5564643.217335996</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>1.266428614912581e-06</v>
+      </c>
+      <c r="E91" t="n">
+        <v>1.51704534</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.95832189</v>
+      </c>
+      <c r="G91" t="n">
+        <v>992517.6268381559</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.9352625011995438</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-2.41079671</v>
+      </c>
+      <c r="F92" t="n">
+        <v>62.72054535</v>
+      </c>
+      <c r="G92" t="n">
+        <v>80863802.19616385</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.2736728348600895</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-1.032349</v>
+      </c>
+      <c r="F93" t="n">
+        <v>7.1627571</v>
+      </c>
+      <c r="G93" t="n">
+        <v>152098961.3060518</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.005560461426567463</v>
+      </c>
+      <c r="E94" t="n">
+        <v>7.25001993</v>
+      </c>
+      <c r="F94" t="n">
+        <v>45.97891661</v>
+      </c>
+      <c r="G94" t="n">
+        <v>556046142.6567463</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.005597724615628983</v>
+      </c>
+      <c r="E95" t="n">
+        <v>23.57330629</v>
+      </c>
+      <c r="F95" t="n">
+        <v>15.99686498</v>
+      </c>
+      <c r="G95" t="n">
+        <v>47149003.08127897</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>2.691294165860409e-07</v>
+      </c>
+      <c r="E96" t="n">
+        <v>1.47119773</v>
+      </c>
+      <c r="F96" t="n">
+        <v>1.70157444</v>
+      </c>
+      <c r="G96" t="n">
+        <v>113034354.9661372</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.0001676197984732492</v>
+      </c>
+      <c r="E97" t="n">
+        <v>4.46804382</v>
+      </c>
+      <c r="F97" t="n">
+        <v>8.967404050000001</v>
+      </c>
+      <c r="G97" t="n">
+        <v>70515973.01971121</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.0002554275932455304</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-1.82952257</v>
+      </c>
+      <c r="F98" t="n">
+        <v>-2.47282622</v>
+      </c>
+      <c r="G98" t="n">
+        <v>4949590.770449336</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>3.459133976152619e-07</v>
+      </c>
+      <c r="E99" t="n">
+        <v>3.43565824</v>
+      </c>
+      <c r="F99" t="n">
+        <v>2.77781963</v>
+      </c>
+      <c r="G99" t="n">
+        <v>306514.84229863</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.01426315972632581</v>
+      </c>
+      <c r="E100" t="n">
+        <v>14.03584098</v>
+      </c>
+      <c r="F100" t="n">
+        <v>33.64590325</v>
+      </c>
+      <c r="G100" t="n">
+        <v>1355708.111670808</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.0007701909223400832</v>
+      </c>
+      <c r="E101" t="n">
+        <v>2.03247974</v>
+      </c>
+      <c r="F101" t="n">
+        <v>-1.70013682</v>
+      </c>
+      <c r="G101" t="n">
+        <v>764470.6650012503</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>62926.65</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>146.26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-13 12:20:05
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -34,6 +34,7 @@
     <sheet name="Portfolio_25" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="Portfolio_26" sheetId="26" state="visible" r:id="rId26"/>
     <sheet name="Portfolio_27" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="Portfolio_28" sheetId="28" state="visible" r:id="rId28"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -62907,6 +62908,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33384</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>WAP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Wet Ass Pussy</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.02244533298197518</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-15.13594949</v>
+      </c>
+      <c r="F2" t="n">
+        <v>38.15017367</v>
+      </c>
+      <c r="G2" t="n">
+        <v>22445332.98197518</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-10-09T13:06:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33307</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>POCHITA</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Pochita</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.005318290979801255</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-23.00978675</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.5707551</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5318290.979801254</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-10-04T09:21:54.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33294</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>IZZY</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Izzy</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>5.071190064642539e-06</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-12.48925573</v>
+      </c>
+      <c r="F4" t="n">
+        <v>638.56301849</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2073009.75723729</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-10-03T12:07:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33287</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MANYU</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>littlemanyu</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.02207491454513095</v>
+      </c>
+      <c r="E5" t="n">
+        <v>9.404416360000001</v>
+      </c>
+      <c r="F5" t="n">
+        <v>32.68994212</v>
+      </c>
+      <c r="G5" t="n">
+        <v>22059857.39934037</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-10-03T09:11:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33211</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BABYBNB</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Baby BNB</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.04465866596691516</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-7.09826772</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-51.60756873</v>
+      </c>
+      <c r="G6" t="n">
+        <v>24778356.60099809</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-09-29T01:27:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33210</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>HANA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Hana</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.001255861996733378</v>
+      </c>
+      <c r="E7" t="n">
+        <v>53.80428656</v>
+      </c>
+      <c r="F7" t="n">
+        <v>89.19812824</v>
+      </c>
+      <c r="G7" t="n">
+        <v>10945090.06385202</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-28T04:03:56.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.003731832644844233</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8.82595536</v>
+      </c>
+      <c r="F8" t="n">
+        <v>37.09495131</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3731832.644844233</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>33180</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>LAIKA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>laikaCTO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0001587055034060533</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.61923816</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-25.98230396</v>
+      </c>
+      <c r="G9" t="n">
+        <v>253470.1941564928</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-09-26T07:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.9898131665301703</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-0.3152893</v>
+      </c>
+      <c r="F10" t="n">
+        <v>18.05438375</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3018435.251333754</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>33145</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CHEEMS</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Cheems</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>3.818886397240025e-09</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-11.3991807</v>
+      </c>
+      <c r="F11" t="n">
+        <v>16.29543322</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1606567.318454906</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-09-24T07:29:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01047645106558194</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-8.382808519999999</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-21.21190298</v>
+      </c>
+      <c r="G12" t="n">
+        <v>6405954.497722398</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>33103</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BABYCATE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BabyCate</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>4.805683389963109e-06</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-21.90039588</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-42.81733478</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3260033.207232195</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-09-23T04:22:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>33094</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.001516235372114611</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.75019984</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-13.83810879</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1516235.37211461</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-09-21T13:43:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.1328963435913196</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-11.38930881</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.41035115</v>
+      </c>
+      <c r="G15" t="n">
+        <v>131563631.3050424</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0004373997023625914</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-2.06337281</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-65.33810265</v>
+      </c>
+      <c r="G16" t="n">
+        <v>320073.5088895551</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.003858868133635665</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-7.1146523</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-16.31290767</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3858868.133635665</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0001127433094778732</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-18.61833579</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-16.49421964</v>
+      </c>
+      <c r="G18" t="n">
+        <v>107106.1440039795</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32949</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>PUFFY</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Puffy</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0003628253773488243</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-25.3984862</v>
+      </c>
+      <c r="F19" t="n">
+        <v>47.78028495</v>
+      </c>
+      <c r="G19" t="n">
+        <v>16125539.3648561</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:11:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.01749542223656786</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-2.66005983</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-6.98319536</v>
+      </c>
+      <c r="G20" t="n">
+        <v>17495422.23656786</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0002858070653001712</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6.24852842</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-34.77876299</v>
+      </c>
+      <c r="G21" t="n">
+        <v>285807.0653001712</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.005569195848716289</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-3.07055797</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-11.1484982</v>
+      </c>
+      <c r="G22" t="n">
+        <v>5569195.848716289</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>5.561358403197522e-07</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-14.00143419</v>
+      </c>
+      <c r="G23" t="n">
+        <v>361933.6680672837</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0007654289990961822</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-2.95615664</v>
+      </c>
+      <c r="F24" t="n">
+        <v>13.70230538</v>
+      </c>
+      <c r="G24" t="n">
+        <v>395535435.2829521</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0004401105350144874</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.08307406</v>
+      </c>
+      <c r="F25" t="n">
+        <v>16.02878077</v>
+      </c>
+      <c r="G25" t="n">
+        <v>440110.5350144874</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2.549122261422993e-07</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3.62070904</v>
+      </c>
+      <c r="F26" t="n">
+        <v>7.7631529</v>
+      </c>
+      <c r="G26" t="n">
+        <v>105094.1613372011</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0.007191871011690526</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-4.13720348</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.27843273</v>
+      </c>
+      <c r="G27" t="n">
+        <v>6761933.09470478</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.0005131110521336451</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-32.17748379</v>
+      </c>
+      <c r="F28" t="n">
+        <v>498.77289173</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5131110.521336451</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.009749672954984761</v>
+      </c>
+      <c r="E29" t="n">
+        <v>5.00071613</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-11.08623954</v>
+      </c>
+      <c r="G29" t="n">
+        <v>9546233.36367345</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0003870180841084646</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-23.73863506</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-1.58373831</v>
+      </c>
+      <c r="G30" t="n">
+        <v>387018.0841084646</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.001300203497889639</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-12.10463435</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-32.27044257</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1235183.397241654</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2.552071572878326e-05</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.09990093999999999</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-17.38191244</v>
+      </c>
+      <c r="G32" t="n">
+        <v>172263688.0911472</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.229493425780228</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-0.965268</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.96484375</v>
+      </c>
+      <c r="G33" t="n">
+        <v>228901811.6944946</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>3.648626417685928e-05</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-4.00043223</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-5.52439212</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3648626.417685928</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1.811704677077874e-06</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-7.52648627</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-9.744637900000001</v>
+      </c>
+      <c r="G35" t="n">
+        <v>583042.3840685557</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0.01182847339725373</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-11.781252</v>
+      </c>
+      <c r="F36" t="n">
+        <v>13.19592455</v>
+      </c>
+      <c r="G36" t="n">
+        <v>11828454.93300675</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32576</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>JHH</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Jen-Hsun Huang</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>3.258387319279083e-06</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-10.18829643</v>
+      </c>
+      <c r="F37" t="n">
+        <v>49.03932046</v>
+      </c>
+      <c r="G37" t="n">
+        <v>31462592.61334281</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-08-06T06:01:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32538</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ONI</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Onigiri</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2.788620945853187e-06</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-6.37718049</v>
+      </c>
+      <c r="F38" t="n">
+        <v>27.78862999</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1137710.218211327</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-08-02T11:10:58.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>1.936550534349811e-06</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-9.94574613</v>
+      </c>
+      <c r="F39" t="n">
+        <v>12.56030708</v>
+      </c>
+      <c r="G39" t="n">
+        <v>13362195.51530993</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.002001601372693308</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-3.45121339</v>
+      </c>
+      <c r="F40" t="n">
+        <v>104.57048071</v>
+      </c>
+      <c r="G40" t="n">
+        <v>842009506.8061429</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>2.709421505281398e-05</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-66.12051375999999</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-25.2949465</v>
+      </c>
+      <c r="G41" t="n">
+        <v>173823.939780452</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.004885607488001775</v>
+      </c>
+      <c r="E42" t="n">
+        <v>25.80986762</v>
+      </c>
+      <c r="F42" t="n">
+        <v>89.74930111</v>
+      </c>
+      <c r="G42" t="n">
+        <v>4885607.336547943</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.0003433568596239547</v>
+      </c>
+      <c r="E43" t="n">
+        <v>12.96665407</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-72.90456856</v>
+      </c>
+      <c r="G43" t="n">
+        <v>343356.2419249642</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.125554128625444</v>
+      </c>
+      <c r="E44" t="n">
+        <v>8.399971300000001</v>
+      </c>
+      <c r="F44" t="n">
+        <v>108.2218335</v>
+      </c>
+      <c r="G44" t="n">
+        <v>125554128.625444</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.02899923470062149</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-12.84744679</v>
+      </c>
+      <c r="F45" t="n">
+        <v>104.01584934</v>
+      </c>
+      <c r="G45" t="n">
+        <v>27633531.43098169</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.6848888034240541</v>
+      </c>
+      <c r="E46" t="n">
+        <v>10.4742502</v>
+      </c>
+      <c r="F46" t="n">
+        <v>443.20204582</v>
+      </c>
+      <c r="G46" t="n">
+        <v>47968702.2594898</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.001744541599589095</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-22.29834628</v>
+      </c>
+      <c r="F47" t="n">
+        <v>182.20307083</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1616418.956242115</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.0003276616191385347</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-7.53651204</v>
+      </c>
+      <c r="F48" t="n">
+        <v>73.37853135</v>
+      </c>
+      <c r="G48" t="n">
+        <v>287585.7426319568</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>9.396491298319155e-07</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-11.34086684</v>
+      </c>
+      <c r="F49" t="n">
+        <v>14.77646701</v>
+      </c>
+      <c r="G49" t="n">
+        <v>835239.767452838</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>32289</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>MIGGLES</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Mr Miggles</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.02412497927454262</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-7.25102035</v>
+      </c>
+      <c r="F50" t="n">
+        <v>-18.33751237</v>
+      </c>
+      <c r="G50" t="n">
+        <v>23096557.72842126</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-07-18T13:00:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.002949820198914958</v>
+      </c>
+      <c r="E51" t="n">
+        <v>27.02680549</v>
+      </c>
+      <c r="F51" t="n">
+        <v>25.63217303</v>
+      </c>
+      <c r="G51" t="n">
+        <v>2064873.174649266</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.0002347852588887103</v>
+      </c>
+      <c r="E52" t="n">
+        <v>8.192033199999999</v>
+      </c>
+      <c r="F52" t="n">
+        <v>40.62532903</v>
+      </c>
+      <c r="G52" t="n">
+        <v>2347852.588887103</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>32200</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>BUB</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Lil Bub</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.01111148055542833</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-0.42741849</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-5.6380821</v>
+      </c>
+      <c r="G53" t="n">
+        <v>11111480.55542833</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-07-12T14:00:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>32183</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>MATT</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Matt Furie</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>4.265414770233689e-06</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-8.793022560000001</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-6.84735637</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1794417.339689611</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-07-11T08:17:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>1.673163685482763e-06</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.05194602</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-22.22548067</v>
+      </c>
+      <c r="G55" t="n">
+        <v>4926245.375211613</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.0006596004656709274</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.25282753</v>
+      </c>
+      <c r="F56" t="n">
+        <v>22.04691512</v>
+      </c>
+      <c r="G56" t="n">
+        <v>19788013.97012782</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.000357479187651644</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-1.78893998</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-5.38677218</v>
+      </c>
+      <c r="G57" t="n">
+        <v>28791920.31695879</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.00945601407591957</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.55368742</v>
+      </c>
+      <c r="F58" t="n">
+        <v>25.57650313</v>
+      </c>
+      <c r="G58" t="n">
+        <v>9250226.028262075</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.000926363450765906</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-28.81564485</v>
+      </c>
+      <c r="F59" t="n">
+        <v>65.47696206000001</v>
+      </c>
+      <c r="G59" t="n">
+        <v>795486.4870981296</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.1824569261688876</v>
+      </c>
+      <c r="E60" t="n">
+        <v>42.85960208</v>
+      </c>
+      <c r="F60" t="n">
+        <v>95.99977584</v>
+      </c>
+      <c r="G60" t="n">
+        <v>178017979.9632102</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.03369774660480313</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-12.26033819</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-16.54158947</v>
+      </c>
+      <c r="G61" t="n">
+        <v>31545729.55280011</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>1.620082893487585e-05</v>
+      </c>
+      <c r="E62" t="n">
+        <v>1.41570471</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-4.41270559</v>
+      </c>
+      <c r="G62" t="n">
+        <v>6809652.228048292</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>8.775028142359795e-07</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-1.43858101</v>
+      </c>
+      <c r="F63" t="n">
+        <v>2.28636411</v>
+      </c>
+      <c r="G63" t="n">
+        <v>18427559.09895557</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.08899653778095497</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-2.68335215</v>
+      </c>
+      <c r="F64" t="n">
+        <v>89.28965596</v>
+      </c>
+      <c r="G64" t="n">
+        <v>88996537.78095497</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.002524834542097414</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-9.42237575</v>
+      </c>
+      <c r="F65" t="n">
+        <v>9.249461289999999</v>
+      </c>
+      <c r="G65" t="n">
+        <v>25247938.74295822</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.144107441342259</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-0.18174934</v>
+      </c>
+      <c r="F66" t="n">
+        <v>10.12295761</v>
+      </c>
+      <c r="G66" t="n">
+        <v>86419550.69859065</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.0002144731478829418</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.23624341</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-6.93543977</v>
+      </c>
+      <c r="G67" t="n">
+        <v>206874.9780755984</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1.548059875538833e-08</v>
+      </c>
+      <c r="E68" t="n">
+        <v>34.00595469</v>
+      </c>
+      <c r="F68" t="n">
+        <v>36.49573839</v>
+      </c>
+      <c r="G68" t="n">
+        <v>6227064.787328014</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.006173627194339813</v>
+      </c>
+      <c r="E69" t="n">
+        <v>19.11047905</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-3.14816122</v>
+      </c>
+      <c r="G69" t="n">
+        <v>6173627.194339814</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>31670</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Doug The Duck</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.002180461121619439</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-4.8492557</v>
+      </c>
+      <c r="F70" t="n">
+        <v>95.40266520999999</v>
+      </c>
+      <c r="G70" t="n">
+        <v>2180375.889574656</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-06-06T17:28:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1.461001435520155e-07</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-3.60506918</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-15.50779262</v>
+      </c>
+      <c r="G71" t="n">
+        <v>60070000.83145685</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>31601</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>SELFIE</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>SelfieDogCoin</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.03624851406565124</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-15.88202067</v>
+      </c>
+      <c r="F72" t="n">
+        <v>64.8107904</v>
+      </c>
+      <c r="G72" t="n">
+        <v>35658313.29473536</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-06-03T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>2.791717138698991e-06</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-2.92924239</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-27.77852108</v>
+      </c>
+      <c r="G73" t="n">
+        <v>1174447.483079279</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.01193577925366756</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-7.14932443</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.48544067</v>
+      </c>
+      <c r="G74" t="n">
+        <v>789658.7899553392</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.005048693194205098</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-9.73583799</v>
+      </c>
+      <c r="F75" t="n">
+        <v>2.59275636</v>
+      </c>
+      <c r="G75" t="n">
+        <v>5047891.704063131</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.07734703122648927</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-7.73942821</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-21.97189543</v>
+      </c>
+      <c r="G76" t="n">
+        <v>76275245.35020418</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>5.291415895858657e-09</v>
+      </c>
+      <c r="E77" t="n">
+        <v>4.86423329</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-40.27460887</v>
+      </c>
+      <c r="G77" t="n">
+        <v>167766.0087132047</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0.007734575720527323</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-0.13359752</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-7.12301686</v>
+      </c>
+      <c r="G78" t="n">
+        <v>773457.5720527323</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>0.0001602467882477397</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-10.38551364</v>
+      </c>
+      <c r="F79" t="n">
+        <v>42.57819072</v>
+      </c>
+      <c r="G79" t="n">
+        <v>62537734.64346917</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.02474776309335569</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-7.24828438</v>
+      </c>
+      <c r="F80" t="n">
+        <v>90.45271941999999</v>
+      </c>
+      <c r="G80" t="n">
+        <v>23309948.9923356</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0006982352322257183</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-0.08369438999999999</v>
+      </c>
+      <c r="F81" t="n">
+        <v>-15.6018685</v>
+      </c>
+      <c r="G81" t="n">
+        <v>698235.2322257183</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.08184459886589433</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-0.67420533</v>
+      </c>
+      <c r="F82" t="n">
+        <v>3.58850828</v>
+      </c>
+      <c r="G82" t="n">
+        <v>16634158.8846225</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.00542963361311048</v>
+      </c>
+      <c r="E83" t="n">
+        <v>3.48074345</v>
+      </c>
+      <c r="F83" t="n">
+        <v>5.85332963</v>
+      </c>
+      <c r="G83" t="n">
+        <v>9203870.496292919</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>4.632636086414023e-05</v>
+      </c>
+      <c r="E84" t="n">
+        <v>15.5989007</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.06879686</v>
+      </c>
+      <c r="G84" t="n">
+        <v>43937224.60358204</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>3.187178314529021e-05</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-4.87802574</v>
+      </c>
+      <c r="F85" t="n">
+        <v>100.48380292</v>
+      </c>
+      <c r="G85" t="n">
+        <v>276473.7579563496</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0.02109314767854065</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-2.45907688</v>
+      </c>
+      <c r="F86" t="n">
+        <v>-17.10403457</v>
+      </c>
+      <c r="G86" t="n">
+        <v>2003849.029461362</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0.00133762260184775</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-1.09804465</v>
+      </c>
+      <c r="F87" t="n">
+        <v>62.85555748</v>
+      </c>
+      <c r="G87" t="n">
+        <v>21920667.12918581</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.01169206834233897</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-2.99564125</v>
+      </c>
+      <c r="F88" t="n">
+        <v>5.20229265</v>
+      </c>
+      <c r="G88" t="n">
+        <v>11690342.55645547</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.001286873200139271</v>
+      </c>
+      <c r="E89" t="n">
+        <v>1.96649543</v>
+      </c>
+      <c r="F89" t="n">
+        <v>55.06503802</v>
+      </c>
+      <c r="G89" t="n">
+        <v>1192843.712366826</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>9.314120206825853e-06</v>
+      </c>
+      <c r="E90" t="n">
+        <v>14.69233814</v>
+      </c>
+      <c r="F90" t="n">
+        <v>2.90049954</v>
+      </c>
+      <c r="G90" t="n">
+        <v>6382219.415230649</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>1.265119547256643e-06</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-0.10336687</v>
+      </c>
+      <c r="F91" t="n">
+        <v>2.18858226</v>
+      </c>
+      <c r="G91" t="n">
+        <v>991491.6924049447</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0.928181260181426</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-0.75713941</v>
+      </c>
+      <c r="F92" t="n">
+        <v>60.55383853</v>
+      </c>
+      <c r="G92" t="n">
+        <v>80251550.47832204</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0.2392741154997088</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-12.52481829</v>
+      </c>
+      <c r="F93" t="n">
+        <v>-2.14435202</v>
+      </c>
+      <c r="G93" t="n">
+        <v>132981208.791664</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.005274348868388538</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-5.14548229</v>
+      </c>
+      <c r="F94" t="n">
+        <v>42.81210782</v>
+      </c>
+      <c r="G94" t="n">
+        <v>527434886.8388538</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.00531337500060182</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-5.07973569</v>
+      </c>
+      <c r="F95" t="n">
+        <v>16.45271659</v>
+      </c>
+      <c r="G95" t="n">
+        <v>44753958.34512956</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>2.697519236357233e-07</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.3857933</v>
+      </c>
+      <c r="F96" t="n">
+        <v>3.91771821</v>
+      </c>
+      <c r="G96" t="n">
+        <v>113295807.9270038</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.0001596786479938061</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-4.73759696</v>
+      </c>
+      <c r="F97" t="n">
+        <v>4.41962148</v>
+      </c>
+      <c r="G97" t="n">
+        <v>67175210.42451431</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.0002428522761649712</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-4.92324142</v>
+      </c>
+      <c r="F98" t="n">
+        <v>-6.56965369</v>
+      </c>
+      <c r="G98" t="n">
+        <v>4705910.46728969</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>3.671519600477463e-07</v>
+      </c>
+      <c r="E99" t="n">
+        <v>6.13984962</v>
+      </c>
+      <c r="F99" t="n">
+        <v>10.32543082</v>
+      </c>
+      <c r="G99" t="n">
+        <v>325334.3926818249</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30645</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>POWSCHE</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Powsche</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.01205562718302703</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-15.47716345</v>
+      </c>
+      <c r="F100" t="n">
+        <v>18.47188086</v>
+      </c>
+      <c r="G100" t="n">
+        <v>1145882.95138717</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:16:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30629</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>KITTENWIF</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>KittenWifHat</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0.0007715998243429439</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.18292893</v>
+      </c>
+      <c r="F101" t="n">
+        <v>-1.10133048</v>
+      </c>
+      <c r="G101" t="n">
+        <v>765869.1029986447</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-04-15T03:51:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>62627.77</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>146.81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-14 12:22:29
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -35,6 +35,7 @@
     <sheet name="Portfolio_26" sheetId="26" state="visible" r:id="rId26"/>
     <sheet name="Portfolio_27" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="Portfolio_28" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="Portfolio_29" sheetId="29" state="visible" r:id="rId29"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -66189,6 +66190,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33440</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Goatseus Maximus</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1242264895797538</v>
+      </c>
+      <c r="E2" t="n">
+        <v>26.88455481</v>
+      </c>
+      <c r="F2" t="n">
+        <v>26.88455481</v>
+      </c>
+      <c r="G2" t="n">
+        <v>124226489.5797538</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-10-14T10:15:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33384</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>WAP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Wet Ass Pussy</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0212715533967031</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-4.41937058</v>
+      </c>
+      <c r="F3" t="n">
+        <v>30.92560481</v>
+      </c>
+      <c r="G3" t="n">
+        <v>21271553.3967031</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-10-09T13:06:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33307</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>POCHITA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Pochita</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.004304495654054276</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-21.04702159</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-59.71990248</v>
+      </c>
+      <c r="G4" t="n">
+        <v>4304495.654054277</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-10-04T09:21:54.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33294</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>IZZY</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Izzy</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4.120720077609411e-06</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-18.74254954</v>
+      </c>
+      <c r="F5" t="n">
+        <v>614.53103808</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1684475.008595452</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-10-03T12:07:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33287</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MANYU</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>littlemanyu</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.01780590602902583</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-19.91565865</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-25.32393129</v>
+      </c>
+      <c r="G6" t="n">
+        <v>17793760.74427448</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-10-03T09:11:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33211</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BABYBNB</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Baby BNB</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.04305017442017053</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-3.59090981</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-57.7052151</v>
+      </c>
+      <c r="G7" t="n">
+        <v>23885903.22667527</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-09-29T01:27:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33210</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>HANA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Hana</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0009408418091803626</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-24.35172704</v>
+      </c>
+      <c r="F8" t="n">
+        <v>23.29785946</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8199625.726474427</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-09-28T04:03:56.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.00331948360211186</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-11.52182703</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-17.17724498</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3319483.60211186</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>33180</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>LAIKA</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>laikaCTO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0001851314947739079</v>
+      </c>
+      <c r="E10" t="n">
+        <v>16.65266934</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-6.7400568</v>
+      </c>
+      <c r="G10" t="n">
+        <v>295675.4171578045</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-09-26T07:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1.009131595421981</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2.37358358</v>
+      </c>
+      <c r="F11" t="n">
+        <v>21.20994241</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3077346.80023933</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>33145</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CHEEMS</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Cheems</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>3.438114071468846e-09</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-7.97059687</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-20.90387397</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1446380.208726229</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-09-24T07:29:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.01078874053188403</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.98087076</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-30.82952409</v>
+      </c>
+      <c r="G13" t="n">
+        <v>6596907.722123115</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>33103</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BABYCATE</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>BabyCate</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>5.079620028458004e-06</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6.12987164</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-4.25125099</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3445863.705353665</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-09-23T04:22:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>33094</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.001565638746736863</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.25829192</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-0.63972117</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1565638.746736862</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-09-21T13:43:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.1234316088009479</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-6.67782854</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4.73121384</v>
+      </c>
+      <c r="G16" t="n">
+        <v>122193810.8516691</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0004592355945802533</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4.99220555</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-56.36539986</v>
+      </c>
+      <c r="G17" t="n">
+        <v>336052.2363648826</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.004104590093584022</v>
+      </c>
+      <c r="E18" t="n">
+        <v>6.43002812</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-11.30380916</v>
+      </c>
+      <c r="G18" t="n">
+        <v>4104590.093584022</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0001080803149358669</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-4.13343264</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-29.75814535</v>
+      </c>
+      <c r="G19" t="n">
+        <v>102676.2991890736</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>32949</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PUFFY</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Puffy</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.000451251091504004</v>
+      </c>
+      <c r="E20" t="n">
+        <v>24.37841011</v>
+      </c>
+      <c r="F20" t="n">
+        <v>27.99154304</v>
+      </c>
+      <c r="G20" t="n">
+        <v>20055563.07183616</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:11:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.01773932037629632</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1.39842819</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-4.66664062</v>
+      </c>
+      <c r="G21" t="n">
+        <v>17739320.37629632</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0002772147864752363</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-4.24845273</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-48.46435763</v>
+      </c>
+      <c r="G22" t="n">
+        <v>277214.7864752363</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.005160223589661188</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-7.70532399</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-23.56241852</v>
+      </c>
+      <c r="G23" t="n">
+        <v>5160223.589661188</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>5.837671019269118e-07</v>
+      </c>
+      <c r="E24" t="n">
+        <v>4.96843749</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-10.5771297</v>
+      </c>
+      <c r="G24" t="n">
+        <v>379916.1161343891</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0007760132706501416</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1.31954081</v>
+      </c>
+      <c r="F25" t="n">
+        <v>9.37256747</v>
+      </c>
+      <c r="G25" t="n">
+        <v>401004857.6084607</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.0004307334174274098</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-2.13062784</v>
+      </c>
+      <c r="F26" t="n">
+        <v>14.08267813</v>
+      </c>
+      <c r="G26" t="n">
+        <v>430733.4174274098</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2.610649219524319e-07</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2.41365269</v>
+      </c>
+      <c r="F27" t="n">
+        <v>18.08040091</v>
+      </c>
+      <c r="G27" t="n">
+        <v>107630.7693921158</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.006308106284470953</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-12.30056949</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-15.92774844</v>
+      </c>
+      <c r="G28" t="n">
+        <v>5931000.789717004</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.0005395057199119868</v>
+      </c>
+      <c r="E29" t="n">
+        <v>5.06361576</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-65.11721162000001</v>
+      </c>
+      <c r="G29" t="n">
+        <v>5395057.199119868</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.01129438991885599</v>
+      </c>
+      <c r="E30" t="n">
+        <v>15.67567753</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-2.53791614</v>
+      </c>
+      <c r="G30" t="n">
+        <v>11058717.80146175</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.0004115625365053078</v>
+      </c>
+      <c r="E31" t="n">
+        <v>5.75518579</v>
+      </c>
+      <c r="F31" t="n">
+        <v>20.66742397</v>
+      </c>
+      <c r="G31" t="n">
+        <v>411562.5365053078</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.001215167418067493</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-5.85323663</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-42.9399469</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1154399.770576049</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2.576295539952e-05</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.84936531</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-17.34267097</v>
+      </c>
+      <c r="G33" t="n">
+        <v>173898794.9273671</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.2259710510321159</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-1.56641948</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-5.78564635</v>
+      </c>
+      <c r="G34" t="n">
+        <v>225388517.3220365</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>4.458139394314506e-05</v>
+      </c>
+      <c r="E35" t="n">
+        <v>22.21024337</v>
+      </c>
+      <c r="F35" t="n">
+        <v>4.50650327</v>
+      </c>
+      <c r="G35" t="n">
+        <v>4458139.394314506</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>2.01530966248473e-06</v>
+      </c>
+      <c r="E36" t="n">
+        <v>11.29309711</v>
+      </c>
+      <c r="F36" t="n">
+        <v>4.24502261</v>
+      </c>
+      <c r="G36" t="n">
+        <v>648566.493820994</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.01141348711091202</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-3.5576406</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-4.16643813</v>
+      </c>
+      <c r="G37" t="n">
+        <v>11413469.29445864</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32576</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>JHH</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Jen-Hsun Huang</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2.88609498629269e-06</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-11.41522675</v>
+      </c>
+      <c r="F38" t="n">
+        <v>12.13277244</v>
+      </c>
+      <c r="G38" t="n">
+        <v>27867783.01642435</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-08-06T06:01:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32538</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ONI</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Onigiri</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>3.114200796580168e-06</v>
+      </c>
+      <c r="E39" t="n">
+        <v>11.67529962</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-17.09491043</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1270541.295008132</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-08-02T11:10:58.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>2.156878557387629e-06</v>
+      </c>
+      <c r="E40" t="n">
+        <v>11.17161498</v>
+      </c>
+      <c r="F40" t="n">
+        <v>19.25014871</v>
+      </c>
+      <c r="G40" t="n">
+        <v>14882458.51341522</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>0.002000424559303374</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-0.32053115</v>
+      </c>
+      <c r="F41" t="n">
+        <v>34.96114359</v>
+      </c>
+      <c r="G41" t="n">
+        <v>841519122.9445862</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>2.698229071746905e-05</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-0.40498305</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-25.84564104</v>
+      </c>
+      <c r="G42" t="n">
+        <v>173105.8850632719</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.006739479047305339</v>
+      </c>
+      <c r="E43" t="n">
+        <v>38.81812882</v>
+      </c>
+      <c r="F43" t="n">
+        <v>142.20688054</v>
+      </c>
+      <c r="G43" t="n">
+        <v>6739478.838381489</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.0003921876499517573</v>
+      </c>
+      <c r="E44" t="n">
+        <v>13.98771707</v>
+      </c>
+      <c r="F44" t="n">
+        <v>-66.95233851</v>
+      </c>
+      <c r="G44" t="n">
+        <v>392186.9444061751</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.126130851862695</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.32449672</v>
+      </c>
+      <c r="F45" t="n">
+        <v>84.21118137000001</v>
+      </c>
+      <c r="G45" t="n">
+        <v>126130851.862695</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.03086479880839789</v>
+      </c>
+      <c r="E46" t="n">
+        <v>5.91807244</v>
+      </c>
+      <c r="F46" t="n">
+        <v>40.89588076</v>
+      </c>
+      <c r="G46" t="n">
+        <v>29411237.80637255</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.6305114908103309</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-9.98655012</v>
+      </c>
+      <c r="F47" t="n">
+        <v>265.07879502</v>
+      </c>
+      <c r="G47" t="n">
+        <v>44160187.49709578</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.002668040948838095</v>
+      </c>
+      <c r="E48" t="n">
+        <v>52.91484274</v>
+      </c>
+      <c r="F48" t="n">
+        <v>172.20234573</v>
+      </c>
+      <c r="G48" t="n">
+        <v>2472094.656125078</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.0003834926162151173</v>
+      </c>
+      <c r="E49" t="n">
+        <v>17.03922395</v>
+      </c>
+      <c r="F49" t="n">
+        <v>105.06396617</v>
+      </c>
+      <c r="G49" t="n">
+        <v>336588.1213614689</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>1.616856815502367e-06</v>
+      </c>
+      <c r="E50" t="n">
+        <v>72.08877562000001</v>
+      </c>
+      <c r="F50" t="n">
+        <v>57.00022556</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1437199.341445998</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>32289</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MIGGLES</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Mr Miggles</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.0273660984566079</v>
+      </c>
+      <c r="E51" t="n">
+        <v>13.45648637</v>
+      </c>
+      <c r="F51" t="n">
+        <v>-13.53934815</v>
+      </c>
+      <c r="G51" t="n">
+        <v>26199511.53581613</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-07-18T13:00:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.003896284755984773</v>
+      </c>
+      <c r="E52" t="n">
+        <v>32.07929213</v>
+      </c>
+      <c r="F52" t="n">
+        <v>65.79254143</v>
+      </c>
+      <c r="G52" t="n">
+        <v>2727398.055104226</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.0002055280147490002</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-13.18619446</v>
+      </c>
+      <c r="F53" t="n">
+        <v>28.49660184</v>
+      </c>
+      <c r="G53" t="n">
+        <v>2055280.147490002</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>32200</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>BUB</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Lil Bub</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.01069777110043429</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-3.73802563</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-12.9913518</v>
+      </c>
+      <c r="G54" t="n">
+        <v>10697771.10043429</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-07-12T14:00:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>32183</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>MATT</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Matt Furie</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>4.760160304974093e-06</v>
+      </c>
+      <c r="E55" t="n">
+        <v>11.59900177</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-4.77090652</v>
+      </c>
+      <c r="G55" t="n">
+        <v>2002551.838699551</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-07-11T08:17:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>1.844570806670423e-06</v>
+      </c>
+      <c r="E56" t="n">
+        <v>10.27539157</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-12.41552654</v>
+      </c>
+      <c r="G56" t="n">
+        <v>5430914.192348542</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.0006473379772746154</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-1.8613723</v>
+      </c>
+      <c r="F57" t="n">
+        <v>6.86277032</v>
+      </c>
+      <c r="G57" t="n">
+        <v>19420139.31823846</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.0003500044297453863</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-2.03214935</v>
+      </c>
+      <c r="F58" t="n">
+        <v>-11.9931961</v>
+      </c>
+      <c r="G58" t="n">
+        <v>28189891.88716597</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.008845205581084682</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-6.4603564</v>
+      </c>
+      <c r="F59" t="n">
+        <v>4.16324029</v>
+      </c>
+      <c r="G59" t="n">
+        <v>8652710.352857817</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.001064874456171138</v>
+      </c>
+      <c r="E60" t="n">
+        <v>14.95212334</v>
+      </c>
+      <c r="F60" t="n">
+        <v>69.02538379000001</v>
+      </c>
+      <c r="G60" t="n">
+        <v>914428.6075187268</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.1659026191619551</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-9.133222460000001</v>
+      </c>
+      <c r="F61" t="n">
+        <v>88.28232408</v>
+      </c>
+      <c r="G61" t="n">
+        <v>161866418.304558</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.03926365057662294</v>
+      </c>
+      <c r="E62" t="n">
+        <v>16.21570336</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-15.42752767</v>
+      </c>
+      <c r="G62" t="n">
+        <v>36756181.8560665</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>1.482227760214368e-05</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-8.583285200000001</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-28.55859837</v>
+      </c>
+      <c r="G63" t="n">
+        <v>6232619.43939889</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>8.768368998771398e-07</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-0.08064949</v>
+      </c>
+      <c r="F64" t="n">
+        <v>3.01298875</v>
+      </c>
+      <c r="G64" t="n">
+        <v>18413574.89741994</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.07537998285030109</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-15.29625063</v>
+      </c>
+      <c r="F65" t="n">
+        <v>30.1760276</v>
+      </c>
+      <c r="G65" t="n">
+        <v>75379982.85030109</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.002611712721208795</v>
+      </c>
+      <c r="E66" t="n">
+        <v>3.42736108</v>
+      </c>
+      <c r="F66" t="n">
+        <v>3.97409775</v>
+      </c>
+      <c r="G66" t="n">
+        <v>26116706.53190743</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>0.1549992789242663</v>
+      </c>
+      <c r="E67" t="n">
+        <v>7.72804723</v>
+      </c>
+      <c r="F67" t="n">
+        <v>8.120246720000001</v>
+      </c>
+      <c r="G67" t="n">
+        <v>92951258.57815504</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.0002298642385271213</v>
+      </c>
+      <c r="E68" t="n">
+        <v>7.24455107</v>
+      </c>
+      <c r="F68" t="n">
+        <v>3.19730753</v>
+      </c>
+      <c r="G68" t="n">
+        <v>221720.806427556</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1.934925436308885e-08</v>
+      </c>
+      <c r="E69" t="n">
+        <v>24.46165918</v>
+      </c>
+      <c r="F69" t="n">
+        <v>59.64922765</v>
+      </c>
+      <c r="G69" t="n">
+        <v>7783121.31511909</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.006419149366963848</v>
+      </c>
+      <c r="E70" t="n">
+        <v>4.66712031</v>
+      </c>
+      <c r="F70" t="n">
+        <v>3.40095744</v>
+      </c>
+      <c r="G70" t="n">
+        <v>6419149.366963848</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>31670</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>DOUG</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Doug The Duck</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.002071078308586584</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-5.25933694</v>
+      </c>
+      <c r="F71" t="n">
+        <v>38.24528945</v>
+      </c>
+      <c r="G71" t="n">
+        <v>2070997.35220658</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-06-06T17:28:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>31632</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>PEIPEI</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>PeiPei (ETH)</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>1.65958290211869e-07</v>
+      </c>
+      <c r="E72" t="n">
+        <v>13.63245346</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-4.24991238</v>
+      </c>
+      <c r="G72" t="n">
+        <v>68234803.80404185</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-06-05T11:23:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>31601</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>SELFIE</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>SelfieDogCoin</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0.04298708818647849</v>
+      </c>
+      <c r="E73" t="n">
+        <v>18.61722882</v>
+      </c>
+      <c r="F73" t="n">
+        <v>49.81868747</v>
+      </c>
+      <c r="G73" t="n">
+        <v>42287169.49350426</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-06-03T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>31569</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>TROG</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Trog</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>2.69856026244197e-06</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-3.34578228</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-27.15783997</v>
+      </c>
+      <c r="G74" t="n">
+        <v>1135257.316806712</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-06-01T10:59:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>31561</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>SOLCAT</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>CatSolHat</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>0.01192032002572427</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-0.76770817</v>
+      </c>
+      <c r="F75" t="n">
+        <v>-3.95062309</v>
+      </c>
+      <c r="G75" t="n">
+        <v>788636.0234503711</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>2024-05-31T10:24:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>31530</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>LFGO</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Lets Fuckin Go</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0.005769744176389665</v>
+      </c>
+      <c r="E76" t="n">
+        <v>14.78692706</v>
+      </c>
+      <c r="F76" t="n">
+        <v>3.69090787</v>
+      </c>
+      <c r="G76" t="n">
+        <v>5768828.217962175</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>2024-05-30T08:07:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>31510</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>MOTHER</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Mother Iggy</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>0.08894976863822271</v>
+      </c>
+      <c r="E77" t="n">
+        <v>14.97346228</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-2.11865066</v>
+      </c>
+      <c r="G77" t="n">
+        <v>87717205.42004165</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>2024-05-29T09:13:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>31496</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>PAPU</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Papu Token</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>4.324602373120853e-09</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-18.26589161</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-48.23340779</v>
+      </c>
+      <c r="G78" t="n">
+        <v>137112.8812569751</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>2024-05-28T12:30:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>31414</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>MAGE</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>MAGE</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>1.598950561035203e-05</v>
+      </c>
+      <c r="E79" t="n">
+        <v>221.16911608</v>
+      </c>
+      <c r="F79" t="n">
+        <v>180.6034298</v>
+      </c>
+      <c r="G79" t="n">
+        <v>196827.1112137242</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>2024-05-24T01:39:49.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>31317</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>MEOW</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>MeowCat</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0.007649885919007981</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-1.09495084</v>
+      </c>
+      <c r="F80" t="n">
+        <v>-1.97153723</v>
+      </c>
+      <c r="G80" t="n">
+        <v>764988.5919007981</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>2024-05-20T09:46:05.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>31305</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>MAGA</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>0.0001595496307857002</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-0.36563276</v>
+      </c>
+      <c r="F81" t="n">
+        <v>2.74793832</v>
+      </c>
+      <c r="G81" t="n">
+        <v>62265662.74210705</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>2024-05-17T14:17:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>31284</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>HAMMY</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>SAD HAMSTER</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>0.02758504911817948</v>
+      </c>
+      <c r="E82" t="n">
+        <v>11.32899315</v>
+      </c>
+      <c r="F82" t="n">
+        <v>43.94627797</v>
+      </c>
+      <c r="G82" t="n">
+        <v>25982392.24572465</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>2024-05-16T10:22:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>31267</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>UTYAB</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>UTYABSWAP</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>0.0006816525217987027</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-2.12960486</v>
+      </c>
+      <c r="F83" t="n">
+        <v>-16.33695345</v>
+      </c>
+      <c r="G83" t="n">
+        <v>681652.5217987027</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>2024-05-15T13:51:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>31259</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>FOXSY</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Foxsy AI</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>0.08316128190838952</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1.6117222</v>
+      </c>
+      <c r="F84" t="n">
+        <v>4.76022686</v>
+      </c>
+      <c r="G84" t="n">
+        <v>16901762.55344174</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>2024-05-15T07:38:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>31163</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>SLOTH</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Slothana</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>0.005554282432801742</v>
+      </c>
+      <c r="E85" t="n">
+        <v>2.43597828</v>
+      </c>
+      <c r="F85" t="n">
+        <v>8.58747885</v>
+      </c>
+      <c r="G85" t="n">
+        <v>9415164.973176952</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>2024-05-09T14:28:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>31152</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>KENDU</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Kendu Inu</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>5.137861333128987e-05</v>
+      </c>
+      <c r="E86" t="n">
+        <v>10.95544319</v>
+      </c>
+      <c r="F86" t="n">
+        <v>12.26311834</v>
+      </c>
+      <c r="G86" t="n">
+        <v>48728923.05048043</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>2024-05-08T16:37:26.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>31106</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>DOKY</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Donkey King</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>3.18266022006996e-05</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-0.1612469</v>
+      </c>
+      <c r="F87" t="n">
+        <v>84.4712528</v>
+      </c>
+      <c r="G87" t="n">
+        <v>276081.8330526805</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>2024-05-06T10:43:36.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>31061</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>DUREV</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Povel Durev</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>0.01948543293570043</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-7.61149008</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-26.81514831</v>
+      </c>
+      <c r="G88" t="n">
+        <v>1851116.128891541</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>2024-05-03T08:27:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>31051</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>LOBO</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>LOBO•THE•WOLF•PUP</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>0.001422710713125477</v>
+      </c>
+      <c r="E89" t="n">
+        <v>8.874440030000001</v>
+      </c>
+      <c r="F89" t="n">
+        <v>64.13207531</v>
+      </c>
+      <c r="G89" t="n">
+        <v>23315072.51781611</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>2024-05-03T05:34:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>31044</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>HEGE</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Hege</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>0.01208022162869304</v>
+      </c>
+      <c r="E90" t="n">
+        <v>3.39316454</v>
+      </c>
+      <c r="F90" t="n">
+        <v>4.5699557</v>
+      </c>
+      <c r="G90" t="n">
+        <v>12078438.55016955</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>2024-05-02T13:06:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>31036</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>CARLO</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Carlo</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>0.001272617912686127</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-1.10793988</v>
+      </c>
+      <c r="F91" t="n">
+        <v>5.29150078</v>
+      </c>
+      <c r="G91" t="n">
+        <v>1179630.032880281</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>2024-05-02T12:04:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>30979</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>ELON</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>ELON Coin</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>8.770053407754047e-06</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-5.84130663</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-1.34311813</v>
+      </c>
+      <c r="G92" t="n">
+        <v>6009414.081918141</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>2024-04-29T12:35:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>30968</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>LONG</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>1.344145559256228e-06</v>
+      </c>
+      <c r="E93" t="n">
+        <v>6.24652525</v>
+      </c>
+      <c r="F93" t="n">
+        <v>6.24569016</v>
+      </c>
+      <c r="G93" t="n">
+        <v>1053425.471352072</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>2024-04-29T08:37:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>30953</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>SHIBTC</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>ShibaBitcoin</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0.8865753884431371</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-4.47486057</v>
+      </c>
+      <c r="F94" t="n">
+        <v>56.53320667</v>
+      </c>
+      <c r="G94" t="n">
+        <v>76654262.0399116</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>2024-04-26T11:08:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>30943</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>$MICHI</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>michi (SOL)</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0.281462636236694</v>
+      </c>
+      <c r="E95" t="n">
+        <v>18.21404317</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0.02853134</v>
+      </c>
+      <c r="G95" t="n">
+        <v>156428293.6226316</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>2024-04-26T07:32:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>30933</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>DOG</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Dog (Runes)</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.005556100612702664</v>
+      </c>
+      <c r="E96" t="n">
+        <v>5.27385291</v>
+      </c>
+      <c r="F96" t="n">
+        <v>41.21643881</v>
+      </c>
+      <c r="G96" t="n">
+        <v>555610061.2702664</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>2024-04-26T04:38:28.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>30912</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>MANEKI</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.005992033282718307</v>
+      </c>
+      <c r="E97" t="n">
+        <v>12.94234278</v>
+      </c>
+      <c r="F97" t="n">
+        <v>23.03021859</v>
+      </c>
+      <c r="G97" t="n">
+        <v>50470220.51088641</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>2024-04-25T07:28:11.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>30867</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>WHY</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>2.829831634168157e-07</v>
+      </c>
+      <c r="E98" t="n">
+        <v>4.64364682</v>
+      </c>
+      <c r="F98" t="n">
+        <v>6.29510496</v>
+      </c>
+      <c r="G98" t="n">
+        <v>118852928.6350626</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>2024-04-24T05:44:18.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>30859</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>HOPPY</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Hoppy</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.0001726989831743256</v>
+      </c>
+      <c r="E99" t="n">
+        <v>7.98474691</v>
+      </c>
+      <c r="F99" t="n">
+        <v>-5.76228739</v>
+      </c>
+      <c r="G99" t="n">
+        <v>72652735.23160703</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>2024-04-23T14:16:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>30828</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>CATA</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>CATAMOTO</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0.0002467083669382604</v>
+      </c>
+      <c r="E100" t="n">
+        <v>1.61685172</v>
+      </c>
+      <c r="F100" t="n">
+        <v>-6.5762469</v>
+      </c>
+      <c r="G100" t="n">
+        <v>4780632.509097993</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>2024-04-22T04:35:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>30647</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Sonic The Goat</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>5.698796744240477e-07</v>
+      </c>
+      <c r="E101" t="n">
+        <v>55.24506335</v>
+      </c>
+      <c r="F101" t="n">
+        <v>63.39258736</v>
+      </c>
+      <c r="G101" t="n">
+        <v>504971.9951279931</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>2024-04-15T09:23:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>BTC Price</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>64828.56</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SOL Price</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>153.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update portfolios at 2024-10-15 12:22:37
</commit_message>
<xml_diff>
--- a/portfolios.xlsx
+++ b/portfolios.xlsx
@@ -36,6 +36,7 @@
     <sheet name="Portfolio_27" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="Portfolio_28" sheetId="28" state="visible" r:id="rId28"/>
     <sheet name="Portfolio_29" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Portfolio_30" sheetId="30" state="visible" r:id="rId30"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -72752,6 +72753,3287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Change 24h</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Change 7d</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Market Cap</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Date Added</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33440</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>GOAT</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Goatseus Maximus</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.113444034319561</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-8.679674759999999</v>
+      </c>
+      <c r="F2" t="n">
+        <v>15.87138814</v>
+      </c>
+      <c r="G2" t="n">
+        <v>113444034.319561</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2024-10-14T10:15:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>33399</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>KLAUS</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Klaus</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0233963097928685</v>
+      </c>
+      <c r="E3" t="n">
+        <v>133.6430109</v>
+      </c>
+      <c r="F3" t="n">
+        <v>285.00757053</v>
+      </c>
+      <c r="G3" t="n">
+        <v>23396309.7928685</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2024-10-11T08:21:20.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>33384</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>WAP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Wet Ass Pussy</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.01263207142530763</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-40.61519067</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-22.25007922</v>
+      </c>
+      <c r="G4" t="n">
+        <v>12632071.42530763</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2024-10-09T13:06:13.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>33356</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MSTR</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MSTR2100</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.5725456660258633</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-32.42944202</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1078.37041018</v>
+      </c>
+      <c r="G5" t="n">
+        <v>11820671.89982176</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2024-10-08T07:11:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>33307</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>POCHITA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Pochita</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.003615830276966241</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-15.99874718</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-63.2054356</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3615830.276966241</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2024-10-04T09:21:54.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>33294</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>IZZY</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Izzy</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>2.719739154595053e-06</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-33.99844922</v>
+      </c>
+      <c r="F7" t="n">
+        <v>131.29235097</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1111779.628203161</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2024-10-03T12:07:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>33287</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MANYU</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>littlemanyu</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.01007496004286974</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-43.4178748</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-66.28592617</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10068087.98264547</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-10-03T09:11:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>33258</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>HIPPO</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>sudeng</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0105850562026491</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-11.28065355</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-31.44602377</v>
+      </c>
+      <c r="G9" t="n">
+        <v>105850562.026491</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-10-01T17:13:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>33211</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BABYBNB</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Baby BNB</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.04281741050702937</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-0.54068053</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-48.19263088</v>
+      </c>
+      <c r="G10" t="n">
+        <v>23756756.79744856</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2024-09-29T01:27:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>33210</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>HANA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Hana</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0007533131385006205</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-19.93200864</v>
+      </c>
+      <c r="F11" t="n">
+        <v>14.54001959</v>
+      </c>
+      <c r="G11" t="n">
+        <v>6565275.618355041</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>2024-09-28T04:03:56.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>33195</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PESTO</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Pesto the Baby King Penguin</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.001937165707642991</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-41.64255831</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-57.66148173</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1937165.707642991</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2024-09-27T08:22:34.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>33180</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>LAIKA</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>laikaCTO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0002090284838690549</v>
+      </c>
+      <c r="E13" t="n">
+        <v>12.90811654</v>
+      </c>
+      <c r="F13" t="n">
+        <v>16.2061229</v>
+      </c>
+      <c r="G13" t="n">
+        <v>333841.5445806515</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2024-09-26T07:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>33148</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ABDS</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ABDS Token</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1.003406821969616</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.56729702</v>
+      </c>
+      <c r="F14" t="n">
+        <v>13.32080254</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3059889.103596344</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2024-09-25T06:00:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>33145</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CHEEMS</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Cheems</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>3.545206469034114e-09</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.11485877</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-23.40809322</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1491432.909457961</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2024-09-24T07:29:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>33128</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>TCAT</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>TON Cat</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.01283698698673182</v>
+      </c>
+      <c r="E16" t="n">
+        <v>18.98503768</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-12.48053728</v>
+      </c>
+      <c r="G16" t="n">
+        <v>7849333.138682563</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2024-09-23T22:02:10.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>33103</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BABYCATE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>BabyCate</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>4.068785517045033e-06</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-19.89980561</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-29.59609603</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2760143.526387003</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2024-09-23T04:22:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>33094</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>MCOIN</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.001591871861456236</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.67555349</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.48227635</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1591871.861456236</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2024-09-21T13:43:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>33093</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>MOODENG</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Moo Deng (moodengsol.com)</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.1084868879378759</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-12.10769349</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-28.82614199</v>
+      </c>
+      <c r="G19" t="n">
+        <v>107398958.770318</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2024-09-21T02:09:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>33017</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>BL00P</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>BLOOP</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0004390579508071248</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-4.39374561</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-48.14036785</v>
+      </c>
+      <c r="G20" t="n">
+        <v>321286.9559847076</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2024-09-14T12:13:45.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>32981</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>CATE</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Cate</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.003964870139271569</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-3.40399287</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-23.52794572</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3964870.139271569</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>2024-09-10T14:18:52.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32950</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SUNPUMP</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>To The Sun</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0001215604042658433</v>
+      </c>
+      <c r="E22" t="n">
+        <v>12.47228909</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-45.95211831</v>
+      </c>
+      <c r="G22" t="n">
+        <v>115482.3840525512</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:13:16.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32949</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>PUFFY</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Puffy</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0003676803830892166</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-18.51977978</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.5632132399999999</v>
+      </c>
+      <c r="G23" t="n">
+        <v>16341316.95669756</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>2024-09-06T06:11:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>32940</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>PHIL</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Philtoken</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.01937215395533447</v>
+      </c>
+      <c r="E24" t="n">
+        <v>9.204600539999999</v>
+      </c>
+      <c r="F24" t="n">
+        <v>7.93599863</v>
+      </c>
+      <c r="G24" t="n">
+        <v>19372153.95533447</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>2024-09-05T05:24:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>32902</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>BRUH</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Bruh</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0002583023284319508</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-6.82231214</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-52.06837132</v>
+      </c>
+      <c r="G25" t="n">
+        <v>258302.3284319508</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>2024-08-30T13:00:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>32862</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>MUNCAT</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0.004961567240490061</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-3.84976243</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-28.05934697</v>
+      </c>
+      <c r="G26" t="n">
+        <v>4961567.240490061</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>2024-08-28T05:37:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32844</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>WIWI</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Wiggly Willy</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>5.837671019269118e-07</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-9.70493976</v>
+      </c>
+      <c r="G27" t="n">
+        <v>379916.1161343891</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2024-08-27T12:03:55.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>32698</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>DOGS</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0.0007892382897349737</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1.70422589</v>
+      </c>
+      <c r="F28" t="n">
+        <v>7.48792275</v>
+      </c>
+      <c r="G28" t="n">
+        <v>407838886.2205477</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>2024-08-26T12:00:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32821</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>BULLS</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0.0004291005059215203</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-0.37910026</v>
+      </c>
+      <c r="F29" t="n">
+        <v>13.6501904</v>
+      </c>
+      <c r="G29" t="n">
+        <v>429100.5059215203</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>2024-08-25T10:26:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32813</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>BUFFI</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Bufficorn</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>2.66036357668687e-07</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1.90429096</v>
+      </c>
+      <c r="F30" t="n">
+        <v>43.63450621</v>
+      </c>
+      <c r="G30" t="n">
+        <v>109680.3724070374</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>2024-08-24T13:15:14.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>32797</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>IVfun</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Invest Zone</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0.006083245894523979</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-3.56462589</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-20.37290843</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5719582.799878327</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2024-08-22T15:01:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>32790</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>EBULL</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ETHEREUM IS GOOD</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0.0005181038837173696</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-3.96693407</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-42.52329024</v>
+      </c>
+      <c r="G32" t="n">
+        <v>5181038.837173696</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>2024-08-22T12:43:06.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32778</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Department Of Government Efficiency (dogegov.com)</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>0.01204098540146955</v>
+      </c>
+      <c r="E33" t="n">
+        <v>6.61032148</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5.06777808</v>
+      </c>
+      <c r="G33" t="n">
+        <v>11789734.59948158</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>2024-08-21T13:37:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32732</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>SUNPEPE</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>sunpepe</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0004116576768280519</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.02311686</v>
+      </c>
+      <c r="F34" t="n">
+        <v>6.84381053</v>
+      </c>
+      <c r="G34" t="n">
+        <v>411657.6768280519</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>2024-08-19T09:50:17.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32727</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>FOFAR</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Fofar (fofar.meme)</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.00171579662778286</v>
+      </c>
+      <c r="E35" t="n">
+        <v>41.19837335</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-7.69699357</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1629993.698002261</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>2024-08-19T06:51:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>32724</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Simon's Cat</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>2.931163861218748e-05</v>
+      </c>
+      <c r="E36" t="n">
+        <v>13.77436384</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-0.05433079</v>
+      </c>
+      <c r="G36" t="n">
+        <v>197852247.6540426</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>2024-08-19T02:07:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>32717</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>SUNDOG</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>0.2375745225319649</v>
+      </c>
+      <c r="E37" t="n">
+        <v>5.13493717</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-8.803956230000001</v>
+      </c>
+      <c r="G37" t="n">
+        <v>236962076.0818609</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>2024-08-17T02:02:00.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>32638</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CATDOG</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>CatDog</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>3.81203541438613e-05</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-14.49268232</v>
+      </c>
+      <c r="F38" t="n">
+        <v>3.2793215</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3812035.41438613</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>2024-08-12T19:10:15.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>32625</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>FUKU</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Fuku-Kun</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>1.859114678759804e-06</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-7.75042102</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-15.55371877</v>
+      </c>
+      <c r="G39" t="n">
+        <v>598299.8599469704</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>2024-08-12T03:43:25.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>32618</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>WDOG</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Wrapped Dog</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>0.0104029207659094</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-8.8541419</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-3.47071627</v>
+      </c>
+      <c r="G40" t="n">
+        <v>10402904.52695009</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>2024-08-10T10:22:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>32576</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>JHH</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Jen-Hsun Huang</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>3.342740093032495e-06</v>
+      </c>
+      <c r="E41" t="n">
+        <v>15.82224802</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-24.07837999</v>
+      </c>
+      <c r="G41" t="n">
+        <v>32277092.76214533</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>2024-08-06T06:01:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>32538</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ONI</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Onigiri</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>3.451473265076914e-06</v>
+      </c>
+      <c r="E42" t="n">
+        <v>10.83014521</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-13.22397158</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1408142.76224975</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2024-08-02T11:10:58.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>32524</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>GINNAN</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Ginnan The Cat</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>1.955600113583474e-06</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-9.331932159999999</v>
+      </c>
+      <c r="F43" t="n">
+        <v>11.99045755</v>
+      </c>
+      <c r="G43" t="n">
+        <v>13493637.58082259</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2024-08-02T04:03:50.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>32521</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>First Neiro On Ethereum</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.001943629011668356</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-2.83917468</v>
+      </c>
+      <c r="F44" t="n">
+        <v>14.71939764</v>
+      </c>
+      <c r="G44" t="n">
+        <v>817628595.464066</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>2024-08-01T17:05:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>32495</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>$YAWN</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>YAWN [Old]</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>2.69993304952008e-05</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.06315171</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-26.36508775</v>
+      </c>
+      <c r="G45" t="n">
+        <v>173215.2043881736</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>2024-07-31T10:49:23.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>32464</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Neiro (neiro.lol)</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.005564432380043609</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-17.43527443</v>
+      </c>
+      <c r="F46" t="n">
+        <v>100.04105855</v>
+      </c>
+      <c r="G46" t="n">
+        <v>5564432.207546205</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>2024-07-29T12:52:31.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>32462</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>YOUNES</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.0003064765481747556</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-21.8546152</v>
+      </c>
+      <c r="F47" t="n">
+        <v>-66.45879141</v>
+      </c>
+      <c r="G47" t="n">
+        <v>306475.9968234454</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:48:04.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>32461</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>NEIRO</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Neiro Ethereum</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.1048413128402294</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-16.87893066</v>
+      </c>
+      <c r="F48" t="n">
+        <v>67.47886742</v>
+      </c>
+      <c r="G48" t="n">
+        <v>104841312.8402294</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>2024-07-29T10:41:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>32448</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>BRAINLET</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Brainlet</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.02645222542569339</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-14.29645925</v>
+      </c>
+      <c r="F49" t="n">
+        <v>-9.70372109</v>
+      </c>
+      <c r="G49" t="n">
+        <v>25206472.17992431</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>2024-07-27T21:56:48.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>32415</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SKBDI</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Skibidi Toilet</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.5024782086833066</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-20.30625674</v>
+      </c>
+      <c r="F50" t="n">
+        <v>104.73778367</v>
+      </c>
+      <c r="G50" t="n">
+        <v>35192906.44511767</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>2024-07-25T21:05:24.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>32412</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>NPCS</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Non-Playable Coin Solana</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.01729175107616965</v>
+      </c>
+      <c r="E51" t="n">
+        <v>34.25025244</v>
+      </c>
+      <c r="F51" t="n">
+        <v>43.14935716</v>
+      </c>
+      <c r="G51" t="n">
+        <v>16768066.46960036</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>2024-07-25T17:01:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>32350</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SOY</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Soyjak</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.002708953549791417</v>
+      </c>
+      <c r="E52" t="n">
+        <v>1.53343227</v>
+      </c>
+      <c r="F52" t="n">
+        <v>191.67402755</v>
+      </c>
+      <c r="G52" t="n">
+        <v>2510002.553389147</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>2024-07-23T12:49:35.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>32310</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>SAITAMA</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>SAITAMA INU</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.0003806046510775651</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-0.75306929</v>
+      </c>
+      <c r="F53" t="n">
+        <v>7.11614518</v>
+      </c>
+      <c r="G53" t="n">
+        <v>334053.3795721749</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>2024-07-22T03:29:32.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>32297</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>BILL</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>BILL THE BEAR</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1.394798111722436e-06</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-13.73397456</v>
+      </c>
+      <c r="F54" t="n">
+        <v>50.01008092</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1239814.748984568</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>2024-07-19T11:16:53.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>32289</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>MIGGLES</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Mr Miggles</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.02727173689403742</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-0.34481189</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-16.21355417</v>
+      </c>
+      <c r="G55" t="n">
+        <v>26109172.50370956</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>2024-07-18T13:00:51.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>32288</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>torsy</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>TORSY</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.005992420368907524</v>
+      </c>
+      <c r="E56" t="n">
+        <v>53.79831671</v>
+      </c>
+      <c r="F56" t="n">
+        <v>159.77321455</v>
+      </c>
+      <c r="G56" t="n">
+        <v>4194692.298713806</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>2024-07-18T12:49:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>32259</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>MOBY</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Moby</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.0002118052938453607</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3.05422066</v>
+      </c>
+      <c r="F57" t="n">
+        <v>33.55684463</v>
+      </c>
+      <c r="G57" t="n">
+        <v>2118052.938453607</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>2024-07-17T06:04:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>32200</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>BUB</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Lil Bub</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.01225434433835944</v>
+      </c>
+      <c r="E58" t="n">
+        <v>14.55044442</v>
+      </c>
+      <c r="F58" t="n">
+        <v>2.04012569</v>
+      </c>
+      <c r="G58" t="n">
+        <v>12254344.33835944</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>2024-07-12T14:00:21.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>32183</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>MATT</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Matt Furie</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>4.836533204023057e-06</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.60441864</v>
+      </c>
+      <c r="F59" t="n">
+        <v>10.36859366</v>
+      </c>
+      <c r="G59" t="n">
+        <v>2034681.15360046</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>2024-07-11T08:17:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>32128</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>MSI</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>monkey shit inu</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1.965780370140827e-06</v>
+      </c>
+      <c r="E60" t="n">
+        <v>6.57115265</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-4.1677889</v>
+      </c>
+      <c r="G60" t="n">
+        <v>5787787.85429705</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>2024-07-05T08:16:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>32125</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>8-Bit Coin</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.000655759953289363</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1.30101683</v>
+      </c>
+      <c r="F61" t="n">
+        <v>4.6829284</v>
+      </c>
+      <c r="G61" t="n">
+        <v>19672798.59868089</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>2024-07-05T07:47:30.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>32074</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>FEG</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>FEED EVERY GORILLA</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.0003416769417509148</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-2.37925217</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-10.7743142</v>
+      </c>
+      <c r="G62" t="n">
+        <v>27519183.27234474</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>2024-07-03T08:17:41.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>32019</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>CRASH</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Crash</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.009254366019244009</v>
+      </c>
+      <c r="E63" t="n">
+        <v>4.62578777</v>
+      </c>
+      <c r="F63" t="n">
+        <v>30.97956664</v>
+      </c>
+      <c r="G63" t="n">
+        <v>9052966.370288551</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>2024-06-27T10:08:47.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>31923</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>HAWKTUAH</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Hawk Tuah</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.001286019339672106</v>
+      </c>
+      <c r="E64" t="n">
+        <v>20.76722587</v>
+      </c>
+      <c r="F64" t="n">
+        <v>103.84862689</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1104330.06182423</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>2024-06-20T13:31:09.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>31921</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>RETARDIO</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.1528816929580212</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-7.84853565</v>
+      </c>
+      <c r="F65" t="n">
+        <v>85.03158899</v>
+      </c>
+      <c r="G65" t="n">
+        <v>149162274.7636941</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2024-06-20T11:11:46.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>31914</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>BILLY</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Billy</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>0.0450651318128366</v>
+      </c>
+      <c r="E66" t="n">
+        <v>14.77570514</v>
+      </c>
+      <c r="F66" t="n">
+        <v>4.46643958</v>
+      </c>
+      <c r="G66" t="n">
+        <v>42187166.90766501</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>2024-06-20T06:10:19.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>31908</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Wat</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>1.371097077307854e-05</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-7.4975443</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-18.9038052</v>
+      </c>
+      <c r="G67" t="n">
+        <v>5765326.036058073</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>2024-06-19T13:54:33.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>31900</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>RGOAT</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>RealGOAT</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>8.812051023088752e-07</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.4981773</v>
+      </c>
+      <c r="F68" t="n">
+        <v>2.13372292</v>
+      </c>
+      <c r="G68" t="n">
+        <v>18505307.14848638</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>2024-06-19T08:48:44.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>31668</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>BILLION•DOLLAR•CAT</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.07414470527368888</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-1.63873422</v>
+      </c>
+      <c r="F69" t="n">
+        <v>24.38485708</v>
+      </c>
+      <c r="G69" t="n">
+        <v>74144705.27368888</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2024-06-19T04:29:07.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>31847</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>WOLF</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>LandWolf (SOL)</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.002593715798384947</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-0.68908508</v>
+      </c>
+      <c r="F70" t="n">
+        <v>11.26313006</v>
+      </c>
+      <c r="G70" t="n">
+        <v>25936740.16658625</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>2024-06-17T02:21:40.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>31830</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>DADDY</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Daddy Tate</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>0.1771589678638656</v>
+      </c>
+      <c r="E71" t="n">
+        <v>14.29664002</v>
+      </c>
+      <c r="F71" t="n">
+        <v>20.32288404</v>
+      </c>
+      <c r="G71" t="n">
+        <v>106240165.4100545</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>2024-06-14T06:33:59.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>31798</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>JENNER</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Caitlyn Jenner (ETH)</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>0.0002573586203558239</v>
+      </c>
+      <c r="E72" t="n">
+        <v>11.96113933</v>
+      </c>
+      <c r="F72" t="n">
+        <v>13.25263081</v>
+      </c>
+      <c r="G72" t="n">
+        <v>248241.1409969885</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>2024-06-13T05:34:37.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>31770</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>HONK</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Pepoclown</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>1.670906653439391e-08</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-13.64490734</v>
+      </c>
+      <c r="F73" t="n">
+        <v>58.20992386</v>
+      </c>
+      <c r="G73" t="n">
+        <v>6718509.288355571</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>2024-06-11T19:57:02.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>31678</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>MAGAA</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>MAGA AGAIN</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0.006785331923455193</v>
+      </c>
+      <c r="E74" t="n">
+        <v>5.70453397</v>
+      </c>
+      <c r="F74" t="n">
+        <v>17.90103747</v>
+      </c>
+      <c r="G74" t="n">
+        <v>6785331.923455193</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>2024-06-07T07:02:39.000Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>31670</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+   